<commit_message>
update inconsistency issues file and replace file
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3AD28E68-F2A3-F940-8930-E97363F153D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82A383E-E0E4-274A-896E-8A67A8CC0F95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="460" windowWidth="23460" windowHeight="16540" activeTab="3"/>
+    <workbookView xWindow="180" yWindow="500" windowWidth="23460" windowHeight="16300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,15 @@
     <sheet name="termWithDifferentParent" sheetId="3" r:id="rId3"/>
     <sheet name="units" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">termWithDifferentParent!$A$1:$F$22</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="310">
   <si>
     <t>sid</t>
   </si>
@@ -836,13 +839,130 @@
   </si>
   <si>
     <t>NO_IRI|http://purl.obolibrary.org/obo/NCIT_C64387|http://purl.obolibrary.org/obo/UO_0010003|http://purl.obolibrary.org/obo/NCIT_C67015</t>
+  </si>
+  <si>
+    <t>change</t>
+  </si>
+  <si>
+    <t>Plasmodium, by microscopy result</t>
+  </si>
+  <si>
+    <t>Plasmodium falciparum gametocytes, by microscopy result</t>
+  </si>
+  <si>
+    <t>Plasmodium falciparum asexual stages, by microscopy result</t>
+  </si>
+  <si>
+    <t>Anemia (hemoglobin &lt; 11 g/dL)</t>
+  </si>
+  <si>
+    <t>Room count</t>
+  </si>
+  <si>
+    <t>1-2 convulsions over 24 h</t>
+  </si>
+  <si>
+    <t>More than 3 convulsions over 24h</t>
+  </si>
+  <si>
+    <t>Total female Anopheles count</t>
+  </si>
+  <si>
+    <t>Vacutainer sample (5mL)</t>
+  </si>
+  <si>
+    <t>Mother's living children count</t>
+  </si>
+  <si>
+    <t>Study timepoint</t>
+  </si>
+  <si>
+    <t>Participant</t>
+  </si>
+  <si>
+    <t>Household observation details</t>
+  </si>
+  <si>
+    <t>Maternal clinical history</t>
+  </si>
+  <si>
+    <t>should be in label, not unitLabel</t>
+  </si>
+  <si>
+    <t>should be C</t>
+  </si>
+  <si>
+    <t>Malaria diagnoses in the past year count</t>
+  </si>
+  <si>
+    <t>correct_label</t>
+  </si>
+  <si>
+    <t>PCR DNA sample source</t>
+  </si>
+  <si>
+    <t>Oocysts count</t>
+  </si>
+  <si>
+    <t>one is mg/L and the other is total mannitol (mg). Change label of EUPATH_0036400 to "Total mannitol excreted"</t>
+  </si>
+  <si>
+    <t>one is mg/L and the other is total lacutulose (mg). Change label of EUPATH_0036399 to "Total lactulose excreted"</t>
+  </si>
+  <si>
+    <t>Change to match all other projects</t>
+  </si>
+  <si>
+    <t>leave as is</t>
+  </si>
+  <si>
+    <t>map all variables to 1 IRI, Jay will have to merge the data when loading, so termType should also be updated to "variable,derived"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ontology team to choose IRI and apply </t>
+  </si>
+  <si>
+    <t>Changing the label for 20122 to be "Total female Anopheles count"</t>
+  </si>
+  <si>
+    <t>For EUPATH_0000537, change label to "Plasmodium, by microscopy result" and move under Raw eukaryota data for blood</t>
+  </si>
+  <si>
+    <t>For EUPATH_0000546, change label to "Plasmodium, by microscopy result" and move under Raw eukaryota data for blood</t>
+  </si>
+  <si>
+    <t>correct_parent</t>
+  </si>
+  <si>
+    <t>change label to "Plasmodium, by microscopy result" and move under Raw eukaryota data for blood</t>
+  </si>
+  <si>
+    <t>change label to "Plasmodium falciparum asexual stages, by microscopy result" and move under Raw eukaryota data for blood</t>
+  </si>
+  <si>
+    <t>change label to "Plasmodium vivax asexual stages, by microscopy result" and move under Raw eukaryota data for blood</t>
+  </si>
+  <si>
+    <t>change label to "Plasmodium vivax gametocytes, by microscopy result" and move under Raw eukaryota data for blood</t>
+  </si>
+  <si>
+    <t>Observation details</t>
+  </si>
+  <si>
+    <t>should be /uL</t>
+  </si>
+  <si>
+    <t>replace IRI with EUPATH_0000092, move to "Raw eukaryota data for blood", and add "result" to end of label. Move and add result to the label for the 2nd and 3rd variables too</t>
+  </si>
+  <si>
+    <t>replace IRI with EUPATH_0023018, move to "Raw eukaryota data for blood", and add "result" to end of label. Move and add result to the label for the 2nd and 3rd variables too</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -982,6 +1102,13 @@
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1325,12 +1452,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1685,21 +1813,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1712,8 +1841,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1726,8 +1858,11 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1740,8 +1875,11 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1754,8 +1892,11 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1768,8 +1909,11 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1782,8 +1926,11 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1796,8 +1943,11 @@
       <c r="D7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1810,8 +1960,11 @@
       <c r="D8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1824,8 +1977,11 @@
       <c r="D9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1838,8 +1994,11 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1852,8 +2011,11 @@
       <c r="D11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1866,8 +2028,11 @@
       <c r="D12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1880,8 +2045,11 @@
       <c r="D13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1894,8 +2062,11 @@
       <c r="D14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1907,6 +2078,9 @@
       </c>
       <c r="D15" t="s">
         <v>38</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -1915,21 +2089,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
     <col min="3" max="3" width="47.6640625" customWidth="1"/>
     <col min="4" max="4" width="33.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -1946,7 +2121,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1959,8 +2134,11 @@
       <c r="E2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1976,8 +2154,11 @@
       <c r="E3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -1994,7 +2175,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>54</v>
       </c>
@@ -2011,7 +2192,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>56</v>
       </c>
@@ -2028,7 +2209,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>59</v>
       </c>
@@ -2045,7 +2226,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>62</v>
       </c>
@@ -2062,7 +2243,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -2078,8 +2259,11 @@
       <c r="E9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>67</v>
       </c>
@@ -2096,7 +2280,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -2112,8 +2296,11 @@
       <c r="E11" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>73</v>
       </c>
@@ -2130,12 +2317,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>51</v>
       </c>
@@ -2145,8 +2332,11 @@
       <c r="C15" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="D15" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>54</v>
       </c>
@@ -2156,17 +2346,20 @@
       <c r="C16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="D16" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="D17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
@@ -2177,7 +2370,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="C20" t="s">
         <v>90</v>
@@ -2186,7 +2379,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="C21" t="s">
         <v>91</v>
@@ -2194,11 +2387,15 @@
       <c r="D21" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -2208,24 +2405,34 @@
       <c r="C23" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>79</v>
       </c>
       <c r="D24" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>81</v>
       </c>
       <c r="D25" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E25" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -2235,24 +2442,34 @@
       <c r="C27" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>83</v>
       </c>
       <c r="D28" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>84</v>
       </c>
       <c r="D29" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E29" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -2262,16 +2479,23 @@
       <c r="C31" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>85</v>
       </c>
       <c r="D32" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E32" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -2281,39 +2505,46 @@
       <c r="C34" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>87</v>
       </c>
       <c r="D35" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
     <col min="4" max="4" width="52.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2329,8 +2560,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -2346,8 +2580,11 @@
       <c r="E2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -2363,8 +2600,11 @@
       <c r="E3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -2380,8 +2620,11 @@
       <c r="E4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -2397,8 +2640,11 @@
       <c r="E5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>108</v>
       </c>
@@ -2414,8 +2660,11 @@
       <c r="E6" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>111</v>
       </c>
@@ -2431,8 +2680,11 @@
       <c r="E7" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -2448,8 +2700,11 @@
       <c r="E8" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>117</v>
       </c>
@@ -2465,8 +2720,11 @@
       <c r="E9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>120</v>
       </c>
@@ -2482,8 +2740,11 @@
       <c r="E10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -2499,8 +2760,11 @@
       <c r="E11" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>126</v>
       </c>
@@ -2516,8 +2780,11 @@
       <c r="E12" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>129</v>
       </c>
@@ -2533,8 +2800,11 @@
       <c r="E13" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2550,8 +2820,11 @@
       <c r="E14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -2567,8 +2840,11 @@
       <c r="E15" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>136</v>
       </c>
@@ -2584,8 +2860,11 @@
       <c r="E16" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -2601,8 +2880,11 @@
       <c r="E17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -2618,8 +2900,11 @@
       <c r="E18" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>143</v>
       </c>
@@ -2635,8 +2920,11 @@
       <c r="E19" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>146</v>
       </c>
@@ -2652,8 +2940,11 @@
       <c r="E20" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -2669,8 +2960,11 @@
       <c r="E21" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -2686,29 +2980,34 @@
       <c r="E22" t="s">
         <v>38</v>
       </c>
+      <c r="F22" s="5" t="s">
+        <v>306</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F22" xr:uid="{7BECD99F-9EFF-CC49-9661-6B01821D2C04}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
     <col min="3" max="3" width="62" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>154</v>
       </c>
@@ -2721,8 +3020,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>157</v>
       </c>
@@ -2735,8 +3037,11 @@
       <c r="D2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>160</v>
       </c>
@@ -2750,7 +3055,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -2764,7 +3069,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>165</v>
       </c>
@@ -2778,7 +3083,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -2791,8 +3096,11 @@
       <c r="D6" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>170</v>
       </c>
@@ -2806,7 +3114,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -2820,7 +3128,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>175</v>
       </c>
@@ -2834,7 +3142,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>177</v>
       </c>
@@ -2848,7 +3156,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -2862,7 +3170,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>180</v>
       </c>
@@ -2876,7 +3184,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>181</v>
       </c>
@@ -2890,7 +3198,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>183</v>
       </c>
@@ -2904,7 +3212,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>184</v>
       </c>
@@ -2918,7 +3226,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>185</v>
       </c>
@@ -2932,7 +3240,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>188</v>
       </c>
@@ -2946,7 +3254,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>191</v>
       </c>
@@ -2960,7 +3268,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>194</v>
       </c>
@@ -2974,7 +3282,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>195</v>
       </c>
@@ -2988,7 +3296,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>198</v>
       </c>
@@ -3002,7 +3310,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>200</v>
       </c>
@@ -3016,7 +3324,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>202</v>
       </c>
@@ -3030,7 +3338,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>204</v>
       </c>
@@ -3044,7 +3352,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>207</v>
       </c>
@@ -3058,7 +3366,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>209</v>
       </c>
@@ -3072,7 +3380,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>211</v>
       </c>
@@ -3086,7 +3394,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>213</v>
       </c>
@@ -3100,7 +3408,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>216</v>
       </c>
@@ -3114,7 +3422,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>218</v>
       </c>
@@ -3128,7 +3436,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>221</v>
       </c>
@@ -3142,7 +3450,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>224</v>
       </c>
@@ -3156,7 +3464,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>226</v>
       </c>
@@ -3170,7 +3478,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>229</v>
       </c>
@@ -3183,8 +3491,11 @@
       <c r="D34" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>230</v>
       </c>
@@ -3198,7 +3509,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>232</v>
       </c>
@@ -3212,7 +3523,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>233</v>
       </c>
@@ -3226,7 +3537,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>235</v>
       </c>
@@ -3240,7 +3551,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>237</v>
       </c>
@@ -3254,7 +3565,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>239</v>
       </c>
@@ -3268,7 +3579,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>241</v>
       </c>
@@ -3282,7 +3593,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>244</v>
       </c>
@@ -3296,7 +3607,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>245</v>
       </c>
@@ -3310,7 +3621,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>248</v>
       </c>
@@ -3323,8 +3634,11 @@
       <c r="D44" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>251</v>
       </c>
@@ -3338,7 +3652,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>253</v>
       </c>
@@ -3352,7 +3666,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>256</v>
       </c>
@@ -3366,7 +3680,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>258</v>
       </c>
@@ -3380,7 +3694,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>261</v>
       </c>
@@ -3394,7 +3708,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>263</v>
       </c>
@@ -3408,7 +3722,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>266</v>
       </c>
@@ -3422,7 +3736,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>269</v>
       </c>

</xml_diff>

<commit_message>
fix same ID with different labels and other noticed label issues, refs #45330
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82A383E-E0E4-274A-896E-8A67A8CC0F95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F629F4-87A1-A64D-87EE-948D7CCF65A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="500" windowWidth="23460" windowHeight="16300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6440" yWindow="460" windowWidth="21820" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="312">
   <si>
     <t>sid</t>
   </si>
@@ -956,13 +956,19 @@
   </si>
   <si>
     <t>replace IRI with EUPATH_0023018, move to "Raw eukaryota data for blood", and add "result" to end of label. Move and add result to the label for the 2nd and 3rd variables too</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>fixed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1814,21 +1820,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="3.6640625" customWidth="1"/>
+    <col min="3" max="3" width="61.1640625" customWidth="1"/>
+    <col min="4" max="4" width="56.83203125" customWidth="1"/>
+    <col min="5" max="5" width="55.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1845,7 +1852,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1861,8 +1868,11 @@
       <c r="E2" s="5" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1878,8 +1888,11 @@
       <c r="E3" s="5" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1895,8 +1908,11 @@
       <c r="E4" s="5" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1912,8 +1928,11 @@
       <c r="E5" s="5" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1929,8 +1948,11 @@
       <c r="E6" s="5" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1946,8 +1968,11 @@
       <c r="E7" s="5" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1963,8 +1988,11 @@
       <c r="E8" s="5" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1980,8 +2008,11 @@
       <c r="E9" s="5" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1997,8 +2028,11 @@
       <c r="E10" s="5" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2014,8 +2048,11 @@
       <c r="E11" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -2031,8 +2068,11 @@
       <c r="E12" s="5" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2049,7 +2089,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -2065,8 +2105,11 @@
       <c r="E14" s="5" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2082,9 +2125,13 @@
       <c r="E15" s="5" t="s">
         <v>282</v>
       </c>
+      <c r="F15" t="s">
+        <v>310</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2093,10 +2140,10 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
     <col min="3" max="3" width="47.6640625" customWidth="1"/>
@@ -2104,7 +2151,7 @@
     <col min="6" max="6" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -2121,7 +2168,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -2138,7 +2185,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -2158,7 +2205,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -2175,7 +2222,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>54</v>
       </c>
@@ -2192,7 +2239,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>56</v>
       </c>
@@ -2209,7 +2256,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>59</v>
       </c>
@@ -2226,7 +2273,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>62</v>
       </c>
@@ -2243,7 +2290,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -2263,7 +2310,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
         <v>67</v>
       </c>
@@ -2280,7 +2327,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -2300,7 +2347,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>73</v>
       </c>
@@ -2317,12 +2364,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
         <v>51</v>
       </c>
@@ -2336,7 +2383,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
         <v>54</v>
       </c>
@@ -2350,16 +2397,16 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="D17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
@@ -2370,7 +2417,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="1"/>
       <c r="C20" t="s">
         <v>90</v>
@@ -2379,7 +2426,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="1"/>
       <c r="C21" t="s">
         <v>91</v>
@@ -2391,11 +2438,11 @@
         <v>294</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" s="1"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -2407,7 +2454,7 @@
       </c>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="C24" t="s">
         <v>79</v>
       </c>
@@ -2418,7 +2465,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="C25" t="s">
         <v>81</v>
       </c>
@@ -2429,10 +2476,10 @@
         <v>295</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -2444,7 +2491,7 @@
       </c>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="C28" t="s">
         <v>83</v>
       </c>
@@ -2455,7 +2502,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="C29" t="s">
         <v>84</v>
       </c>
@@ -2466,10 +2513,10 @@
         <v>295</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -2481,7 +2528,7 @@
       </c>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -2492,10 +2539,10 @@
         <v>296</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -2507,7 +2554,7 @@
       </c>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>87</v>
       </c>
@@ -2518,7 +2565,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" s="3"/>
     </row>
   </sheetData>
@@ -2531,11 +2578,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
@@ -2544,7 +2591,7 @@
     <col min="6" max="6" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2564,7 +2611,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -2584,7 +2631,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -2604,7 +2651,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -2624,7 +2671,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -2644,7 +2691,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>108</v>
       </c>
@@ -2664,7 +2711,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>111</v>
       </c>
@@ -2684,7 +2731,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -2704,7 +2751,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>117</v>
       </c>
@@ -2724,7 +2771,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>120</v>
       </c>
@@ -2744,7 +2791,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -2764,7 +2811,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>126</v>
       </c>
@@ -2784,7 +2831,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>129</v>
       </c>
@@ -2804,7 +2851,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2824,7 +2871,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -2844,7 +2891,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>136</v>
       </c>
@@ -2864,7 +2911,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -2884,7 +2931,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -2904,7 +2951,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>143</v>
       </c>
@@ -2924,7 +2971,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>146</v>
       </c>
@@ -2944,7 +2991,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -2964,7 +3011,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -2992,22 +3039,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="62" customWidth="1"/>
+    <col min="3" max="3" width="47.83203125" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>154</v>
       </c>
@@ -3024,7 +3071,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>157</v>
       </c>
@@ -3041,7 +3088,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>160</v>
       </c>
@@ -3055,7 +3102,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -3069,7 +3116,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>165</v>
       </c>
@@ -3083,7 +3130,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -3100,7 +3147,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>170</v>
       </c>
@@ -3114,7 +3161,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -3128,7 +3175,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>175</v>
       </c>
@@ -3142,7 +3189,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>177</v>
       </c>
@@ -3156,7 +3203,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -3170,7 +3217,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>180</v>
       </c>
@@ -3184,7 +3231,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>181</v>
       </c>
@@ -3198,7 +3245,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>183</v>
       </c>
@@ -3212,7 +3259,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>184</v>
       </c>
@@ -3226,7 +3273,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>185</v>
       </c>
@@ -3240,7 +3287,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>188</v>
       </c>
@@ -3254,7 +3301,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>191</v>
       </c>
@@ -3268,7 +3315,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>194</v>
       </c>
@@ -3282,7 +3329,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>195</v>
       </c>
@@ -3296,7 +3343,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>198</v>
       </c>
@@ -3310,7 +3357,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>200</v>
       </c>
@@ -3324,7 +3371,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>202</v>
       </c>
@@ -3338,7 +3385,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>204</v>
       </c>
@@ -3352,7 +3399,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>207</v>
       </c>
@@ -3366,7 +3413,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>209</v>
       </c>
@@ -3380,7 +3427,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>211</v>
       </c>
@@ -3394,7 +3441,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>213</v>
       </c>
@@ -3408,7 +3455,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>216</v>
       </c>
@@ -3422,7 +3469,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>218</v>
       </c>
@@ -3436,7 +3483,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>221</v>
       </c>
@@ -3450,7 +3497,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>224</v>
       </c>
@@ -3464,7 +3511,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>226</v>
       </c>
@@ -3478,7 +3525,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>229</v>
       </c>
@@ -3494,8 +3541,11 @@
       <c r="E34" s="5" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>230</v>
       </c>
@@ -3509,7 +3559,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>232</v>
       </c>
@@ -3523,7 +3573,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>233</v>
       </c>
@@ -3537,7 +3587,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>235</v>
       </c>
@@ -3551,7 +3601,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>237</v>
       </c>
@@ -3565,7 +3615,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>239</v>
       </c>
@@ -3579,7 +3629,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>241</v>
       </c>
@@ -3593,7 +3643,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>244</v>
       </c>
@@ -3607,7 +3657,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>245</v>
       </c>
@@ -3621,7 +3671,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>248</v>
       </c>
@@ -3638,7 +3688,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>251</v>
       </c>
@@ -3652,7 +3702,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>253</v>
       </c>
@@ -3666,7 +3716,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>256</v>
       </c>
@@ -3680,7 +3730,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>258</v>
       </c>
@@ -3694,7 +3744,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>261</v>
       </c>
@@ -3708,7 +3758,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>263</v>
       </c>
@@ -3722,7 +3772,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>266</v>
       </c>
@@ -3736,7 +3786,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>269</v>
       </c>

</xml_diff>

<commit_message>
fixed issues of different terms with same labels and same term under different parents issues, fixed some unitLabel issues, refs #45330
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F629F4-87A1-A64D-87EE-948D7CCF65A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF41E40F-A72E-9F42-8E09-7E682EB30E8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="460" windowWidth="21820" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="340" yWindow="460" windowWidth="25180" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
     <sheet name="LabelsUsedMultipleTerms" sheetId="2" r:id="rId2"/>
     <sheet name="termWithDifferentParent" sheetId="3" r:id="rId3"/>
     <sheet name="units" sheetId="4" r:id="rId4"/>
+    <sheet name="units_latest" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">termWithDifferentParent!$A$1:$F$22</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="318">
   <si>
     <t>sid</t>
   </si>
@@ -961,7 +962,25 @@
     <t>Fixed</t>
   </si>
   <si>
-    <t>fixed</t>
+    <t>JZ comment</t>
+  </si>
+  <si>
+    <t>Any rule of using whitespace for value with unit? I saw two kinds, e.g. '1-2 convulsions over 24 h', 'More than 3 convulsions over 24h'</t>
+  </si>
+  <si>
+    <t>gates_provide | icemr_india_behavior | icemr_meghalaya</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000316|http://purl.obolibrary.org/obo/EUPATH_0024232</t>
+  </si>
+  <si>
+    <t>icemr_indian | icemr_prism | icemr_india_feverSurv | general/general_crompton | icemr_prism2 | gates_gamin | icemr_indian_cx | icemr_southAsia | icemr_india_behavior | icemr_westAfrica | icemr_prism2_border_cohort</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0024232|http://purl.obolibrary.org/obo/UO_0000316</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0010003|http://purl.obolibrary.org/obo/NCIT_C67015|NO_IRI|http://purl.obolibrary.org/obo/NCIT_C64387</t>
   </si>
 </sst>
 </file>
@@ -1820,10 +1839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1851,6 +1870,9 @@
       <c r="E1" s="5" t="s">
         <v>289</v>
       </c>
+      <c r="F1" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
@@ -2127,6 +2149,11 @@
       </c>
       <c r="F15" t="s">
         <v>310</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -2137,21 +2164,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1"/>
+    <col min="1" max="1" width="37" customWidth="1"/>
     <col min="3" max="3" width="47.6640625" customWidth="1"/>
     <col min="4" max="4" width="33.83203125" customWidth="1"/>
+    <col min="5" max="5" width="39.1640625" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -2168,7 +2196,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -2184,8 +2212,11 @@
       <c r="F2" s="5" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -2204,8 +2235,11 @@
       <c r="F3" s="5" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -2221,8 +2255,11 @@
       <c r="E4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>54</v>
       </c>
@@ -2238,8 +2275,11 @@
       <c r="E5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>56</v>
       </c>
@@ -2255,8 +2295,11 @@
       <c r="E6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>59</v>
       </c>
@@ -2272,8 +2315,11 @@
       <c r="E7" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>62</v>
       </c>
@@ -2289,8 +2335,11 @@
       <c r="E8" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -2309,8 +2358,11 @@
       <c r="F9" s="5" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>67</v>
       </c>
@@ -2326,8 +2378,11 @@
       <c r="E10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -2346,8 +2401,11 @@
       <c r="F11" s="5" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>73</v>
       </c>
@@ -2363,13 +2421,16 @@
       <c r="E12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G12" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
         <v>51</v>
       </c>
@@ -2383,7 +2444,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" s="4" t="s">
         <v>54</v>
       </c>
@@ -2576,10 +2637,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2587,11 +2648,11 @@
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
     <col min="4" max="4" width="52.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="5"/>
+    <col min="5" max="5" width="33" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2611,7 +2672,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -2630,8 +2691,11 @@
       <c r="F2" s="5" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -2650,8 +2714,11 @@
       <c r="F3" s="5" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -2670,8 +2737,11 @@
       <c r="F4" s="5" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -2690,8 +2760,11 @@
       <c r="F5" s="5" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>108</v>
       </c>
@@ -2710,8 +2783,11 @@
       <c r="F6" s="5" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>111</v>
       </c>
@@ -2730,8 +2806,11 @@
       <c r="F7" s="5" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -2750,8 +2829,11 @@
       <c r="F8" s="5" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>117</v>
       </c>
@@ -2770,8 +2852,11 @@
       <c r="F9" s="5" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>120</v>
       </c>
@@ -2790,8 +2875,11 @@
       <c r="F10" s="5" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -2810,8 +2898,11 @@
       <c r="F11" s="5" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>126</v>
       </c>
@@ -2830,8 +2921,11 @@
       <c r="F12" s="5" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>129</v>
       </c>
@@ -2850,8 +2944,11 @@
       <c r="F13" s="5" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2870,8 +2967,11 @@
       <c r="F14" s="5" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -2890,8 +2990,11 @@
       <c r="F15" s="5" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>136</v>
       </c>
@@ -2910,8 +3013,11 @@
       <c r="F16" s="5" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -2930,8 +3036,11 @@
       <c r="F17" s="5" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -2950,8 +3059,11 @@
       <c r="F18" s="5" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>143</v>
       </c>
@@ -2970,8 +3082,11 @@
       <c r="F19" s="5" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>146</v>
       </c>
@@ -2990,8 +3105,11 @@
       <c r="F20" s="5" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -3010,8 +3128,11 @@
       <c r="F21" s="5" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -3029,11 +3150,15 @@
       </c>
       <c r="F22" s="5" t="s">
         <v>306</v>
+      </c>
+      <c r="G22" t="s">
+        <v>310</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F22" xr:uid="{7BECD99F-9EFF-CC49-9661-6B01821D2C04}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3041,20 +3166,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="47.83203125" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="3" max="3" width="84.5" customWidth="1"/>
+    <col min="4" max="4" width="65.1640625" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>154</v>
       </c>
@@ -3070,8 +3195,11 @@
       <c r="E1" s="5" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>157</v>
       </c>
@@ -3087,8 +3215,11 @@
       <c r="E2" s="5" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>160</v>
       </c>
@@ -3102,7 +3233,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -3116,7 +3247,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>165</v>
       </c>
@@ -3130,7 +3261,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -3146,8 +3277,11 @@
       <c r="E6" s="5" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>170</v>
       </c>
@@ -3161,7 +3295,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -3175,7 +3309,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>175</v>
       </c>
@@ -3189,7 +3323,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>177</v>
       </c>
@@ -3203,7 +3337,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -3217,7 +3351,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>180</v>
       </c>
@@ -3231,7 +3365,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>181</v>
       </c>
@@ -3245,7 +3379,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>183</v>
       </c>
@@ -3259,7 +3393,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>184</v>
       </c>
@@ -3273,7 +3407,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>185</v>
       </c>
@@ -3541,8 +3675,8 @@
       <c r="E34" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>311</v>
+      <c r="F34" s="4" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -3687,6 +3821,9 @@
       <c r="E44" s="5" t="s">
         <v>286</v>
       </c>
+      <c r="F44" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
@@ -3797,6 +3934,684 @@
         <v>270</v>
       </c>
       <c r="D52" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{905C8918-D215-6643-9522-53B380C55A89}">
+  <dimension ref="A1:D47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="119.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>158</v>
+      </c>
+      <c r="D12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>192</v>
+      </c>
+      <c r="D15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>195</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>198</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>199</v>
+      </c>
+      <c r="D18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>203</v>
+      </c>
+      <c r="D19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>204</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>205</v>
+      </c>
+      <c r="D20" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>207</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>208</v>
+      </c>
+      <c r="D21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>209</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>210</v>
+      </c>
+      <c r="D22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>211</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>212</v>
+      </c>
+      <c r="D23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>213</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>214</v>
+      </c>
+      <c r="D24" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>216</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>217</v>
+      </c>
+      <c r="D25" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>218</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>219</v>
+      </c>
+      <c r="D26" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>221</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>222</v>
+      </c>
+      <c r="D27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>224</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>225</v>
+      </c>
+      <c r="D28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>230</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>231</v>
+      </c>
+      <c r="D29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>232</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>164</v>
+      </c>
+      <c r="D30" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>233</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>234</v>
+      </c>
+      <c r="D31" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>235</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>236</v>
+      </c>
+      <c r="D32" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>237</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>238</v>
+      </c>
+      <c r="D33" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>239</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>240</v>
+      </c>
+      <c r="D34" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>241</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>242</v>
+      </c>
+      <c r="D35" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>244</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>164</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>160</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>314</v>
+      </c>
+      <c r="D37" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>245</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>246</v>
+      </c>
+      <c r="D38" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>251</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>252</v>
+      </c>
+      <c r="D39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>253</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>254</v>
+      </c>
+      <c r="D40" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>256</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>257</v>
+      </c>
+      <c r="D41" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>258</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>259</v>
+      </c>
+      <c r="D42" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>261</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>262</v>
+      </c>
+      <c r="D43" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>226</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>316</v>
+      </c>
+      <c r="D44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>263</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>267</v>
+      </c>
+      <c r="D45" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>266</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>267</v>
+      </c>
+      <c r="D46" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>269</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>317</v>
+      </c>
+      <c r="D47" t="s">
         <v>159</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update the inconsistent issue summarized information
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF41E40F-A72E-9F42-8E09-7E682EB30E8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE779E2-4F58-224C-928E-681648ED8E90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="25180" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6080" yWindow="520" windowWidth="25180" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="319">
   <si>
     <t>sid</t>
   </si>
@@ -981,6 +981,9 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/UO_0010003|http://purl.obolibrary.org/obo/NCIT_C67015|NO_IRI|http://purl.obolibrary.org/obo/NCIT_C64387</t>
+  </si>
+  <si>
+    <t>Basically, units should have a space between what comes before and the unit</t>
   </si>
 </sst>
 </file>
@@ -1839,10 +1842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2110,6 +2113,9 @@
       <c r="E13" s="5" t="s">
         <v>280</v>
       </c>
+      <c r="F13" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
@@ -2154,6 +2160,11 @@
     <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>312</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed unit label and IRIs
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE779E2-4F58-224C-928E-681648ED8E90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB2053E-6920-A445-A12D-45BB7CDB565A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="520" windowWidth="25180" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="900" windowWidth="25180" windowHeight="11920" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="termWithDifferentParent" sheetId="3" r:id="rId3"/>
     <sheet name="units" sheetId="4" r:id="rId4"/>
     <sheet name="units_latest" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">termWithDifferentParent!$A$1:$F$22</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="346">
   <si>
     <t>sid</t>
   </si>
@@ -962,9 +963,6 @@
     <t>Fixed</t>
   </si>
   <si>
-    <t>JZ comment</t>
-  </si>
-  <si>
     <t>Any rule of using whitespace for value with unit? I saw two kinds, e.g. '1-2 convulsions over 24 h', 'More than 3 convulsions over 24h'</t>
   </si>
   <si>
@@ -984,13 +982,97 @@
   </si>
   <si>
     <t>Basically, units should have a space between what comes before and the unit</t>
+  </si>
+  <si>
+    <t>JZ comments</t>
+  </si>
+  <si>
+    <t>EUPATH_0023011</t>
+  </si>
+  <si>
+    <t>Creatinine</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0010003</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>gates_elicit.owl</t>
+  </si>
+  <si>
+    <t>icemr_southAsia.owl</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0004374</t>
+  </si>
+  <si>
+    <t>EUPATH_0023005</t>
+  </si>
+  <si>
+    <t>Bicarbonate</t>
+  </si>
+  <si>
+    <t>Plasmodium asexual stages, by microscopy result</t>
+  </si>
+  <si>
+    <t>Plasmodium asexual stages, by microscopy result, 2nd</t>
+  </si>
+  <si>
+    <t>Plasmodium asexual stages, by microscopy result, 3rd</t>
+  </si>
+  <si>
+    <t>Plasmodium gametocytes, by microscopy result</t>
+  </si>
+  <si>
+    <t>Plasmodium gametocytes, by microscopy result, 2nd</t>
+  </si>
+  <si>
+    <t>Plasmodium gametocytes, by microscopy result, 3rd</t>
+  </si>
+  <si>
+    <t>icemr_southernAfrica.owl</t>
+  </si>
+  <si>
+    <t>in other OWL files, the unit is /uL</t>
+  </si>
+  <si>
+    <t>EFO_0004309</t>
+  </si>
+  <si>
+    <t>Platelet count</t>
+  </si>
+  <si>
+    <t>EUPATH_0024244</t>
+  </si>
+  <si>
+    <t>EUPATH_0024243</t>
+  </si>
+  <si>
+    <t>EUPATH_0023018</t>
+  </si>
+  <si>
+    <t>EUPATH_0024242</t>
+  </si>
+  <si>
+    <t>EUPATH_0024241</t>
+  </si>
+  <si>
+    <t>EUPATH_0000092</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1137,6 +1219,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF808080"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1436,7 +1532,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1479,16 +1575,19 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1522,6 +1621,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1844,8 +1944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1874,7 +1974,7 @@
         <v>289</v>
       </c>
       <c r="F1" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2159,12 +2259,12 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -2177,8 +2277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2206,6 +2306,9 @@
       <c r="E1" t="s">
         <v>43</v>
       </c>
+      <c r="G1" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
@@ -2650,8 +2753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2682,6 +2785,9 @@
       <c r="F1" s="5" t="s">
         <v>301</v>
       </c>
+      <c r="G1" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
@@ -3177,17 +3283,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="84.5" customWidth="1"/>
-    <col min="4" max="4" width="65.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="4" max="4" width="48" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="5"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3207,7 +3314,7 @@
         <v>271</v>
       </c>
       <c r="F1" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3958,8 +4065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{905C8918-D215-6643-9522-53B380C55A89}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3984,91 +4091,91 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>164</v>
+        <v>313</v>
       </c>
       <c r="D2" t="s">
-        <v>159</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>158</v>
+        <v>186</v>
       </c>
       <c r="D4" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="D5" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
-        <v>174</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>245</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>178</v>
+        <v>246</v>
       </c>
       <c r="D7" t="s">
-        <v>174</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -4077,40 +4184,40 @@
         <v>158</v>
       </c>
       <c r="D8" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>180</v>
+        <v>263</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>267</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="D10" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -4119,158 +4226,158 @@
         <v>158</v>
       </c>
       <c r="D11" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="D12" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="D13" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="D14" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="D15" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="D16" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>195</v>
+        <v>251</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>196</v>
+        <v>252</v>
       </c>
       <c r="D17" t="s">
-        <v>197</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D18" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D19" t="s">
-        <v>171</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D20" t="s">
-        <v>206</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>207</v>
+        <v>256</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>208</v>
+        <v>257</v>
       </c>
       <c r="D21" t="s">
-        <v>174</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D22" t="s">
         <v>174</v>
@@ -4278,13 +4385,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D23" t="s">
         <v>174</v>
@@ -4301,7 +4408,7 @@
         <v>214</v>
       </c>
       <c r="D24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -4320,83 +4427,83 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>218</v>
+        <v>253</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>219</v>
+        <v>254</v>
       </c>
       <c r="D26" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D27" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D28" t="s">
-        <v>174</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>230</v>
+        <v>258</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>231</v>
+        <v>259</v>
       </c>
       <c r="D29" t="s">
-        <v>174</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>232</v>
+        <v>261</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>164</v>
+        <v>262</v>
       </c>
       <c r="D30" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D31" t="s">
         <v>174</v>
@@ -4404,27 +4511,27 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>236</v>
+        <v>315</v>
       </c>
       <c r="D32" t="s">
-        <v>174</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="D33" t="s">
         <v>174</v>
@@ -4432,201 +4539,447 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>240</v>
+        <v>164</v>
       </c>
       <c r="D34" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="D35" t="s">
-        <v>243</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>244</v>
+        <v>179</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>314</v>
+        <v>158</v>
       </c>
       <c r="D37" t="s">
-        <v>315</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>245</v>
+        <v>181</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>246</v>
+        <v>182</v>
       </c>
       <c r="D38" t="s">
-        <v>247</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="D39" t="s">
-        <v>97</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="D40" t="s">
-        <v>255</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="D41" t="s">
-        <v>223</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>259</v>
+        <v>316</v>
       </c>
       <c r="D42" t="s">
-        <v>260</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>261</v>
+        <v>183</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>262</v>
+        <v>158</v>
       </c>
       <c r="D43" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>226</v>
+        <v>184</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>316</v>
+        <v>158</v>
       </c>
       <c r="D44" t="s">
-        <v>228</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>263</v>
+        <v>241</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="D45" t="s">
-        <v>265</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>266</v>
+        <v>244</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>267</v>
+        <v>164</v>
       </c>
       <c r="D46" t="s">
-        <v>268</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
+        <v>266</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="D47" t="s">
+        <v>268</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D47">
+    <sortCondition ref="A2:A47"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="C47" r:id="rId1" xr:uid="{FA0A87BC-A58C-754C-B782-FF9D321AE679}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="41.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C2" t="s">
         <v>269</v>
       </c>
-      <c r="B47">
-        <v>4</v>
-      </c>
-      <c r="C47" t="s">
-        <v>317</v>
-      </c>
-      <c r="D47" t="s">
-        <v>159</v>
+      <c r="D2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="C3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="E3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D4" t="s">
+        <v>321</v>
+      </c>
+      <c r="E4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="C5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>343</v>
+      </c>
+      <c r="B7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D7" t="s">
+        <v>227</v>
+      </c>
+      <c r="E7" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>342</v>
+      </c>
+      <c r="B8" t="s">
+        <v>329</v>
+      </c>
+      <c r="C8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>341</v>
+      </c>
+      <c r="B9" t="s">
+        <v>330</v>
+      </c>
+      <c r="C9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D9" t="s">
+        <v>227</v>
+      </c>
+      <c r="E9" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>340</v>
+      </c>
+      <c r="B10" t="s">
+        <v>331</v>
+      </c>
+      <c r="C10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D10" t="s">
+        <v>227</v>
+      </c>
+      <c r="E10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>339</v>
+      </c>
+      <c r="B11" t="s">
+        <v>332</v>
+      </c>
+      <c r="C11" t="s">
+        <v>226</v>
+      </c>
+      <c r="D11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>338</v>
+      </c>
+      <c r="B12" t="s">
+        <v>333</v>
+      </c>
+      <c r="C12" t="s">
+        <v>226</v>
+      </c>
+      <c r="D12" t="s">
+        <v>227</v>
+      </c>
+      <c r="E12" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>336</v>
+      </c>
+      <c r="B15" t="s">
+        <v>337</v>
+      </c>
+      <c r="C15" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E15" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>336</v>
+      </c>
+      <c r="B16" t="s">
+        <v>337</v>
+      </c>
+      <c r="C16" t="s">
+        <v>244</v>
+      </c>
+      <c r="D16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E16" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update unit checking information
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB2053E-6920-A445-A12D-45BB7CDB565A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D1E144-3DCE-8542-9651-AD2D982E56CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="900" windowWidth="25180" windowHeight="11920" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3620" yWindow="900" windowWidth="25180" windowHeight="11920" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
     <sheet name="LabelsUsedMultipleTerms" sheetId="2" r:id="rId2"/>
     <sheet name="termWithDifferentParent" sheetId="3" r:id="rId3"/>
-    <sheet name="units" sheetId="4" r:id="rId4"/>
-    <sheet name="units_latest" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="units_issues" sheetId="6" r:id="rId4"/>
+    <sheet name="units" sheetId="4" r:id="rId5"/>
+    <sheet name="units_latest" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">termWithDifferentParent!$A$1:$F$22</definedName>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="356">
   <si>
     <t>sid</t>
   </si>
@@ -969,18 +969,9 @@
     <t>gates_provide | icemr_india_behavior | icemr_meghalaya</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000316|http://purl.obolibrary.org/obo/EUPATH_0024232</t>
-  </si>
-  <si>
-    <t>icemr_indian | icemr_prism | icemr_india_feverSurv | general/general_crompton | icemr_prism2 | gates_gamin | icemr_indian_cx | icemr_southAsia | icemr_india_behavior | icemr_westAfrica | icemr_prism2_border_cohort</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/EUPATH_0024232|http://purl.obolibrary.org/obo/UO_0000316</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/UO_0010003|http://purl.obolibrary.org/obo/NCIT_C67015|NO_IRI|http://purl.obolibrary.org/obo/NCIT_C64387</t>
-  </si>
-  <si>
     <t>Basically, units should have a space between what comes before and the unit</t>
   </si>
   <si>
@@ -1066,6 +1057,45 @@
   </si>
   <si>
     <t>Label</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000179</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000015</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000009</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000035</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000275</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000033|http://purl.obolibrary.org/obo/UO_0000036</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0004374|http://purl.obolibrary.org/obo/UO_0010003</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0010003|http://purl.obolibrary.org/obo/NCIT_C64387</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0023059|http://purl.obolibrary.org/obo/UO_0000316</t>
+  </si>
+  <si>
+    <t>gates_elicit | general/general_crompton | icemr_southAsia</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000316|http://purl.obolibrary.org/obo/EUPATH_0024232|http://purl.obolibrary.org/obo/EUPATH_0023059</t>
+  </si>
+  <si>
+    <t>icemr_indian | icemr_prism | gates_elicit | icemr_india_feverSurv | general/general_crompton | icemr_prism2 | gates_gamin | icemr_indian_cx | icemr_southAsia | icemr_india_behavior | icemr_westAfrica | icemr_prism2_border_cohort</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0010003|http://www.ebi.ac.uk/efo/EFO_0004374|http://purl.obolibrary.org/obo/NCIT_C64387</t>
   </si>
 </sst>
 </file>
@@ -1974,7 +2004,7 @@
         <v>289</v>
       </c>
       <c r="F1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2264,7 +2294,7 @@
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -2307,7 +2337,7 @@
         <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2786,7 +2816,7 @@
         <v>301</v>
       </c>
       <c r="G1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3280,6 +3310,246 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="41.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="C3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="E3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B4" t="s">
+        <v>324</v>
+      </c>
+      <c r="C4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="C5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>340</v>
+      </c>
+      <c r="B7" t="s">
+        <v>325</v>
+      </c>
+      <c r="C7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D7" t="s">
+        <v>227</v>
+      </c>
+      <c r="E7" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>339</v>
+      </c>
+      <c r="B8" t="s">
+        <v>326</v>
+      </c>
+      <c r="C8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E8" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>338</v>
+      </c>
+      <c r="B9" t="s">
+        <v>327</v>
+      </c>
+      <c r="C9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D9" t="s">
+        <v>227</v>
+      </c>
+      <c r="E9" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>337</v>
+      </c>
+      <c r="B10" t="s">
+        <v>328</v>
+      </c>
+      <c r="C10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D10" t="s">
+        <v>227</v>
+      </c>
+      <c r="E10" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>336</v>
+      </c>
+      <c r="B11" t="s">
+        <v>329</v>
+      </c>
+      <c r="C11" t="s">
+        <v>226</v>
+      </c>
+      <c r="D11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E11" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>335</v>
+      </c>
+      <c r="B12" t="s">
+        <v>330</v>
+      </c>
+      <c r="C12" t="s">
+        <v>226</v>
+      </c>
+      <c r="D12" t="s">
+        <v>227</v>
+      </c>
+      <c r="E12" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>333</v>
+      </c>
+      <c r="B15" t="s">
+        <v>334</v>
+      </c>
+      <c r="C15" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E15" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>333</v>
+      </c>
+      <c r="B16" t="s">
+        <v>334</v>
+      </c>
+      <c r="C16" t="s">
+        <v>244</v>
+      </c>
+      <c r="D16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E16" t="s">
+        <v>321</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
@@ -3314,7 +3584,7 @@
         <v>271</v>
       </c>
       <c r="F1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -4061,18 +4331,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{905C8918-D215-6643-9522-53B380C55A89}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="119.83203125" customWidth="1"/>
+    <col min="3" max="3" width="47.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4091,133 +4361,133 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>313</v>
+        <v>166</v>
       </c>
       <c r="D2" t="s">
-        <v>314</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D3" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="D4" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="D5" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>245</v>
+        <v>179</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>246</v>
+        <v>158</v>
       </c>
       <c r="D7" t="s">
-        <v>247</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>158</v>
+        <v>343</v>
       </c>
       <c r="D8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>263</v>
+        <v>181</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>267</v>
+        <v>182</v>
       </c>
       <c r="D9" t="s">
-        <v>265</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>192</v>
+        <v>158</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -4226,172 +4496,172 @@
         <v>158</v>
       </c>
       <c r="D11" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="D12" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="D13" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>245</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>176</v>
+        <v>344</v>
       </c>
       <c r="D14" t="s">
-        <v>174</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D15" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="D16" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>251</v>
+        <v>195</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>252</v>
+        <v>196</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D18" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>205</v>
+        <v>345</v>
       </c>
       <c r="D19" t="s">
-        <v>206</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D20" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>256</v>
+        <v>204</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>257</v>
+        <v>205</v>
       </c>
       <c r="D21" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="D22" t="s">
-        <v>174</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D23" t="s">
         <v>174</v>
@@ -4399,72 +4669,72 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D24" t="s">
-        <v>312</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D25" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>253</v>
+        <v>213</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>254</v>
+        <v>214</v>
       </c>
       <c r="D26" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D27" t="s">
-        <v>220</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D28" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -4472,10 +4742,10 @@
         <v>258</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>259</v>
+        <v>346</v>
       </c>
       <c r="D29" t="s">
         <v>260</v>
@@ -4486,10 +4756,10 @@
         <v>261</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>262</v>
+        <v>347</v>
       </c>
       <c r="D30" t="s">
         <v>174</v>
@@ -4511,27 +4781,27 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>315</v>
+        <v>231</v>
       </c>
       <c r="D32" t="s">
-        <v>228</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D33" t="s">
         <v>174</v>
@@ -4539,27 +4809,27 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>164</v>
+        <v>236</v>
       </c>
       <c r="D34" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D35" t="s">
         <v>174</v>
@@ -4567,142 +4837,142 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>158</v>
+        <v>240</v>
       </c>
       <c r="D36" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>180</v>
+        <v>241</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>242</v>
       </c>
       <c r="D37" t="s">
-        <v>159</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>181</v>
+        <v>263</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>182</v>
+        <v>348</v>
       </c>
       <c r="D38" t="s">
-        <v>174</v>
+        <v>265</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>237</v>
+        <v>256</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>238</v>
+        <v>349</v>
       </c>
       <c r="D39" t="s">
-        <v>174</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>236</v>
+        <v>350</v>
       </c>
       <c r="D40" t="s">
-        <v>174</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>240</v>
+        <v>313</v>
       </c>
       <c r="D41" t="s">
-        <v>174</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>316</v>
+        <v>351</v>
       </c>
       <c r="D42" t="s">
-        <v>159</v>
+        <v>352</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>183</v>
+        <v>266</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>158</v>
+        <v>348</v>
       </c>
       <c r="D43" t="s">
-        <v>159</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>158</v>
+        <v>353</v>
       </c>
       <c r="D44" t="s">
-        <v>159</v>
+        <v>354</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>241</v>
+        <v>269</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>242</v>
+        <v>355</v>
       </c>
       <c r="D45" t="s">
-        <v>243</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -4742,244 +5012,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
-  <dimension ref="A1:E16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="41.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>319</v>
-      </c>
-      <c r="B2" t="s">
-        <v>320</v>
-      </c>
-      <c r="C2" t="s">
-        <v>269</v>
-      </c>
-      <c r="D2" t="s">
-        <v>321</v>
-      </c>
-      <c r="E2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="C3" t="s">
-        <v>256</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="E3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>326</v>
-      </c>
-      <c r="B4" t="s">
-        <v>327</v>
-      </c>
-      <c r="C4" t="s">
-        <v>269</v>
-      </c>
-      <c r="D4" t="s">
-        <v>321</v>
-      </c>
-      <c r="E4" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="C5" t="s">
-        <v>221</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="E5" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>343</v>
-      </c>
-      <c r="B7" t="s">
-        <v>328</v>
-      </c>
-      <c r="C7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D7" t="s">
-        <v>227</v>
-      </c>
-      <c r="E7" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>342</v>
-      </c>
-      <c r="B8" t="s">
-        <v>329</v>
-      </c>
-      <c r="C8" t="s">
-        <v>226</v>
-      </c>
-      <c r="D8" t="s">
-        <v>227</v>
-      </c>
-      <c r="E8" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>341</v>
-      </c>
-      <c r="B9" t="s">
-        <v>330</v>
-      </c>
-      <c r="C9" t="s">
-        <v>226</v>
-      </c>
-      <c r="D9" t="s">
-        <v>227</v>
-      </c>
-      <c r="E9" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>340</v>
-      </c>
-      <c r="B10" t="s">
-        <v>331</v>
-      </c>
-      <c r="C10" t="s">
-        <v>226</v>
-      </c>
-      <c r="D10" t="s">
-        <v>227</v>
-      </c>
-      <c r="E10" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>339</v>
-      </c>
-      <c r="B11" t="s">
-        <v>332</v>
-      </c>
-      <c r="C11" t="s">
-        <v>226</v>
-      </c>
-      <c r="D11" t="s">
-        <v>227</v>
-      </c>
-      <c r="E11" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>338</v>
-      </c>
-      <c r="B12" t="s">
-        <v>333</v>
-      </c>
-      <c r="C12" t="s">
-        <v>226</v>
-      </c>
-      <c r="D12" t="s">
-        <v>227</v>
-      </c>
-      <c r="E12" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="B13" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>336</v>
-      </c>
-      <c r="B15" t="s">
-        <v>337</v>
-      </c>
-      <c r="C15" t="s">
-        <v>160</v>
-      </c>
-      <c r="D15" t="s">
-        <v>161</v>
-      </c>
-      <c r="E15" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>336</v>
-      </c>
-      <c r="B16" t="s">
-        <v>337</v>
-      </c>
-      <c r="C16" t="s">
-        <v>244</v>
-      </c>
-      <c r="D16" t="s">
-        <v>164</v>
-      </c>
-      <c r="E16" t="s">
-        <v>324</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update unit inconsistency issues
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D1E144-3DCE-8542-9651-AD2D982E56CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E990BCDB-CB7B-DE4C-9017-C0A75A2BDE47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="900" windowWidth="25180" windowHeight="11920" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9980" yWindow="10220" windowWidth="25180" windowHeight="11920" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="358">
   <si>
     <t>sid</t>
   </si>
@@ -1096,13 +1096,19 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/UO_0010003|http://www.ebi.ac.uk/efo/EFO_0004374|http://purl.obolibrary.org/obo/NCIT_C64387</t>
+  </si>
+  <si>
+    <t>correct</t>
+  </si>
+  <si>
+    <t>/500 WBC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1974,11 +1980,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" customWidth="1"/>
@@ -1987,7 +1993,7 @@
     <col min="5" max="5" width="55.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2007,7 +2013,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2027,7 +2033,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2047,7 +2053,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2067,7 +2073,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2087,7 +2093,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2107,7 +2113,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2127,7 +2133,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2147,7 +2153,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2167,7 +2173,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2187,7 +2193,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2207,7 +2213,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -2227,7 +2233,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2247,7 +2253,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -2267,7 +2273,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2287,12 +2293,12 @@
         <v>310</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>314</v>
       </c>
@@ -2307,11 +2313,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
     <col min="3" max="3" width="47.6640625" customWidth="1"/>
@@ -2320,7 +2326,7 @@
     <col min="6" max="6" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -2340,7 +2346,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -2360,7 +2366,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -2383,7 +2389,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -2403,7 +2409,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>54</v>
       </c>
@@ -2423,7 +2429,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>56</v>
       </c>
@@ -2443,7 +2449,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>59</v>
       </c>
@@ -2463,7 +2469,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>62</v>
       </c>
@@ -2483,7 +2489,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -2506,7 +2512,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>67</v>
       </c>
@@ -2526,7 +2532,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -2549,7 +2555,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>73</v>
       </c>
@@ -2569,12 +2575,12 @@
         <v>310</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>51</v>
       </c>
@@ -2588,7 +2594,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>54</v>
       </c>
@@ -2602,16 +2608,16 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="D17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
@@ -2622,7 +2628,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="C20" t="s">
         <v>90</v>
@@ -2631,7 +2637,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="C21" t="s">
         <v>91</v>
@@ -2643,11 +2649,11 @@
         <v>294</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -2659,7 +2665,7 @@
       </c>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>79</v>
       </c>
@@ -2670,7 +2676,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>81</v>
       </c>
@@ -2681,10 +2687,10 @@
         <v>295</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -2696,7 +2702,7 @@
       </c>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>83</v>
       </c>
@@ -2707,7 +2713,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>84</v>
       </c>
@@ -2718,10 +2724,10 @@
         <v>295</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -2733,7 +2739,7 @@
       </c>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -2744,10 +2750,10 @@
         <v>296</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -2759,7 +2765,7 @@
       </c>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>87</v>
       </c>
@@ -2770,7 +2776,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
     </row>
   </sheetData>
@@ -2783,11 +2789,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
@@ -2796,7 +2802,7 @@
     <col min="6" max="6" width="29.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2819,7 +2825,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -2842,7 +2848,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -2865,7 +2871,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -2888,7 +2894,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -2911,7 +2917,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>108</v>
       </c>
@@ -2934,7 +2940,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>111</v>
       </c>
@@ -2957,7 +2963,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -2980,7 +2986,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>117</v>
       </c>
@@ -3003,7 +3009,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>120</v>
       </c>
@@ -3026,7 +3032,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3049,7 +3055,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>126</v>
       </c>
@@ -3072,7 +3078,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>129</v>
       </c>
@@ -3095,7 +3101,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -3118,7 +3124,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -3141,7 +3147,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>136</v>
       </c>
@@ -3164,7 +3170,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -3187,7 +3193,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -3210,7 +3216,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>143</v>
       </c>
@@ -3233,7 +3239,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>146</v>
       </c>
@@ -3256,7 +3262,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -3279,7 +3285,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -3311,13 +3317,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
@@ -3326,7 +3332,7 @@
     <col min="5" max="5" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>341</v>
       </c>
@@ -3343,7 +3349,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>316</v>
       </c>
@@ -3359,8 +3365,11 @@
       <c r="E2" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>256</v>
       </c>
@@ -3370,8 +3379,11 @@
       <c r="E3" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>323</v>
       </c>
@@ -3387,8 +3399,11 @@
       <c r="E4" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>221</v>
       </c>
@@ -3398,11 +3413,15 @@
       <c r="E5" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>340</v>
       </c>
@@ -3418,8 +3437,11 @@
       <c r="E7" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>339</v>
       </c>
@@ -3435,8 +3457,11 @@
       <c r="E8" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>338</v>
       </c>
@@ -3452,8 +3477,11 @@
       <c r="E9" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>337</v>
       </c>
@@ -3469,8 +3497,11 @@
       <c r="E10" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>336</v>
       </c>
@@ -3486,8 +3517,11 @@
       <c r="E11" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>335</v>
       </c>
@@ -3503,13 +3537,20 @@
       <c r="E12" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>333</v>
       </c>
@@ -3525,8 +3566,11 @@
       <c r="E15" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>333</v>
       </c>
@@ -3541,6 +3585,9 @@
       </c>
       <c r="E16" t="s">
         <v>321</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -3553,11 +3600,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -3567,7 +3614,7 @@
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>154</v>
       </c>
@@ -3587,7 +3634,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>157</v>
       </c>
@@ -3607,7 +3654,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>160</v>
       </c>
@@ -3621,7 +3668,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -3635,7 +3682,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>165</v>
       </c>
@@ -3649,7 +3696,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -3669,7 +3716,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>170</v>
       </c>
@@ -3683,7 +3730,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -3697,7 +3744,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>175</v>
       </c>
@@ -3711,7 +3758,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>177</v>
       </c>
@@ -3725,7 +3772,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -3739,7 +3786,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>180</v>
       </c>
@@ -3753,7 +3800,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>181</v>
       </c>
@@ -3767,7 +3814,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>183</v>
       </c>
@@ -3781,7 +3828,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>184</v>
       </c>
@@ -3795,7 +3842,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>185</v>
       </c>
@@ -3809,7 +3856,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>188</v>
       </c>
@@ -3823,7 +3870,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>191</v>
       </c>
@@ -3837,7 +3884,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>194</v>
       </c>
@@ -3851,7 +3898,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>195</v>
       </c>
@@ -3865,7 +3912,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>198</v>
       </c>
@@ -3879,7 +3926,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>200</v>
       </c>
@@ -3893,7 +3940,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>202</v>
       </c>
@@ -3907,7 +3954,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>204</v>
       </c>
@@ -3921,7 +3968,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>207</v>
       </c>
@@ -3935,7 +3982,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>209</v>
       </c>
@@ -3949,7 +3996,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>211</v>
       </c>
@@ -3963,7 +4010,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>213</v>
       </c>
@@ -3977,7 +4024,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>216</v>
       </c>
@@ -3991,7 +4038,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>218</v>
       </c>
@@ -4005,7 +4052,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>221</v>
       </c>
@@ -4019,7 +4066,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>224</v>
       </c>
@@ -4033,7 +4080,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>226</v>
       </c>
@@ -4047,7 +4094,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>229</v>
       </c>
@@ -4067,7 +4114,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>230</v>
       </c>
@@ -4081,7 +4128,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>232</v>
       </c>
@@ -4095,7 +4142,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>233</v>
       </c>
@@ -4109,7 +4156,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>235</v>
       </c>
@@ -4123,7 +4170,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>237</v>
       </c>
@@ -4137,7 +4184,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>239</v>
       </c>
@@ -4151,7 +4198,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>241</v>
       </c>
@@ -4165,7 +4212,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>244</v>
       </c>
@@ -4179,7 +4226,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>245</v>
       </c>
@@ -4193,7 +4240,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>248</v>
       </c>
@@ -4213,7 +4260,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>251</v>
       </c>
@@ -4227,7 +4274,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>253</v>
       </c>
@@ -4241,7 +4288,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>256</v>
       </c>
@@ -4255,7 +4302,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>258</v>
       </c>
@@ -4269,7 +4316,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>261</v>
       </c>
@@ -4283,7 +4330,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>263</v>
       </c>
@@ -4297,7 +4344,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>266</v>
       </c>
@@ -4311,7 +4358,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>269</v>
       </c>
@@ -4339,13 +4386,13 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="3" max="3" width="47.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>154</v>
       </c>
@@ -4359,7 +4406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -4373,7 +4420,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>170</v>
       </c>
@@ -4387,7 +4434,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>172</v>
       </c>
@@ -4401,7 +4448,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>175</v>
       </c>
@@ -4415,7 +4462,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>177</v>
       </c>
@@ -4429,7 +4476,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>179</v>
       </c>
@@ -4443,7 +4490,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>180</v>
       </c>
@@ -4457,7 +4504,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>181</v>
       </c>
@@ -4471,7 +4518,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>183</v>
       </c>
@@ -4485,7 +4532,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>184</v>
       </c>
@@ -4499,7 +4546,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>185</v>
       </c>
@@ -4513,7 +4560,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>188</v>
       </c>
@@ -4527,7 +4574,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>245</v>
       </c>
@@ -4541,7 +4588,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>191</v>
       </c>
@@ -4555,7 +4602,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>194</v>
       </c>
@@ -4569,7 +4616,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>195</v>
       </c>
@@ -4583,7 +4630,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>198</v>
       </c>
@@ -4597,7 +4644,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>251</v>
       </c>
@@ -4611,7 +4658,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>202</v>
       </c>
@@ -4625,7 +4672,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>204</v>
       </c>
@@ -4639,7 +4686,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>253</v>
       </c>
@@ -4653,7 +4700,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>207</v>
       </c>
@@ -4667,7 +4714,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>209</v>
       </c>
@@ -4681,7 +4728,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>211</v>
       </c>
@@ -4695,7 +4742,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>213</v>
       </c>
@@ -4709,7 +4756,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>216</v>
       </c>
@@ -4723,7 +4770,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>218</v>
       </c>
@@ -4737,7 +4784,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>258</v>
       </c>
@@ -4751,7 +4798,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>261</v>
       </c>
@@ -4765,7 +4812,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>224</v>
       </c>
@@ -4779,7 +4826,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>230</v>
       </c>
@@ -4793,7 +4840,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>233</v>
       </c>
@@ -4807,7 +4854,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>235</v>
       </c>
@@ -4821,7 +4868,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>237</v>
       </c>
@@ -4835,7 +4882,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>239</v>
       </c>
@@ -4849,7 +4896,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>241</v>
       </c>
@@ -4863,7 +4910,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>263</v>
       </c>
@@ -4877,7 +4924,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>256</v>
       </c>
@@ -4891,7 +4938,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>221</v>
       </c>
@@ -4905,7 +4952,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>226</v>
       </c>
@@ -4919,7 +4966,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>244</v>
       </c>
@@ -4933,7 +4980,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>266</v>
       </c>
@@ -4947,7 +4994,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>160</v>
       </c>
@@ -4961,7 +5008,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>269</v>
       </c>
@@ -4975,7 +5022,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>244</v>
       </c>
@@ -4989,7 +5036,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>266</v>
       </c>

</xml_diff>

<commit_message>
update issues and unitList
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC4DB16-0F56-2144-963A-BBD0AF3E721B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F605E5-8A58-F847-91FE-A2626C56A482}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="1300" windowWidth="25180" windowHeight="14380" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1300" windowWidth="25180" windowHeight="14380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="206">
   <si>
     <t>sid</t>
   </si>
@@ -612,7 +612,37 @@
     <t>Relocation|Participant</t>
   </si>
   <si>
-    <t>See comments on 'LabelsUsedMultipleTerms'</t>
+    <t>copies/rxn</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0022272</t>
+  </si>
+  <si>
+    <t>days/week</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C170633</t>
+  </si>
+  <si>
+    <t>hrs/day</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176380</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000080</t>
+  </si>
+  <si>
+    <t>sols</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0022271</t>
+  </si>
+  <si>
+    <t>See comments on 'TermWithDifferentLabels'</t>
   </si>
 </sst>
 </file>
@@ -1766,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1817,7 +1847,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1830,7 +1860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -2897,16 +2927,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E96E553-B9B7-3A43-9A19-9B2DEFC1133B}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
@@ -2918,352 +2945,422 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>195</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>197</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>199</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>201</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B26" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>169</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="B31" t="s">
-        <v>165</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>130</v>
+        <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>140</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>204</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>127</v>
-      </c>
-      <c r="B39" t="s">
-        <v>173</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="B42" t="s">
-        <v>174</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>127</v>
+      </c>
+      <c r="B50" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B53" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>40</v>
+      </c>
+      <c r="B55" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B44">
-    <sortCondition ref="A2:A44"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
assigned IDs to few units and updated unit list
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F605E5-8A58-F847-91FE-A2626C56A482}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC2CB8F-7CDD-6D42-A388-7B060DC71BB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1300" windowWidth="25180" windowHeight="14380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2420" yWindow="1560" windowWidth="25180" windowHeight="14380" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="213">
   <si>
     <t>sid</t>
   </si>
@@ -643,6 +643,27 @@
   </si>
   <si>
     <t>See comments on 'TermWithDifferentLabels'</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0015721</t>
+  </si>
+  <si>
+    <t>-&gt; epg</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0030176</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C173109</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0049454</t>
+  </si>
+  <si>
+    <t>epg</t>
+  </si>
+  <si>
+    <t>Assigned IDs to following units</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1173,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1161,6 +1182,8 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1796,7 +1819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -2147,7 +2170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -2927,13 +2950,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E96E553-B9B7-3A43-9A19-9B2DEFC1133B}">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="47.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
@@ -2945,422 +2972,440 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>195</v>
       </c>
       <c r="B8" t="s">
-        <v>166</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>195</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>124</v>
+      </c>
+      <c r="B10" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>197</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>198</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>211</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>199</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>199</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>200</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>112</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>167</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>201</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>201</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>202</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="B25" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="B26" t="s">
-        <v>144</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="B32" t="s">
-        <v>83</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B33" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>169</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>94</v>
+        <v>203</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>204</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>203</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>165</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B43" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>130</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>140</v>
+        <v>209</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>102</v>
+      </c>
+      <c r="B46" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>105</v>
+      </c>
+      <c r="B47" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="B48" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
-        <v>105</v>
-      </c>
-      <c r="B49" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
-        <v>127</v>
-      </c>
-      <c r="B50" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="50" spans="1:4">
+      <c r="B50" s="8"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>31</v>
       </c>
       <c r="B53" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="D53" s="8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>55</v>
       </c>
       <c r="B54" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>40</v>
       </c>
       <c r="B55" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="D55" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>44</v>
       </c>
       <c r="B56" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" t="s">
-        <v>45</v>
-      </c>
-      <c r="B57" t="s">
-        <v>20</v>
-      </c>
+      <c r="D56" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="D57" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update eda inconsistency file
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F605E5-8A58-F847-91FE-A2626C56A482}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A3A260-33B7-6949-A7E1-56D7A7939FDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1300" windowWidth="25180" windowHeight="14380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="12100" windowWidth="25180" windowHeight="14380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="211">
   <si>
     <t>sid</t>
   </si>
@@ -643,13 +643,30 @@
   </si>
   <si>
     <t>See comments on 'TermWithDifferentLabels'</t>
+  </si>
+  <si>
+    <t>change to Time living in dwelling with units years</t>
+  </si>
+  <si>
+    <t>EUPATH_0022264 should be "Plasmodium falciparum, by qPCR result" and be moved under 'Raw eukaryota data for blood' with unit "/uL"
+EUPATH_0022062 should be "Plasmodium falciparum copies, by qPCR", moved under 'Raw eukaryota data for blood", with unit "/rxn"</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>EUPATH_0022247 should be "Plasmodium vivax, by qPCR result" and be moved under 'Raw eukaryota data for blood' with unit "/uL"
+EUPATH_0022061 should be "Plasmodium vivax copies, by qPCR", moved under 'Raw eukaryota data for blood", with unit "/rxn"</t>
+  </si>
+  <si>
+    <t>should be under Relocation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1152,7 +1169,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1161,6 +1178,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1519,10 +1539,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" customWidth="1"/>
@@ -1531,7 +1551,7 @@
     <col min="5" max="5" width="55.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1545,7 +1565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>185</v>
       </c>
@@ -1560,7 +1580,7 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>188</v>
       </c>
@@ -1571,12 +1591,15 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>189</v>
       </c>
       <c r="C5" t="s">
         <v>190</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1589,20 +1612,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
     <col min="4" max="4" width="33.83203125" customWidth="1"/>
     <col min="5" max="5" width="39.1640625" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="5"/>
+    <col min="6" max="6" width="47.5" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1619,10 +1642,10 @@
         <v>9</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="97" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>175</v>
       </c>
@@ -1638,9 +1661,11 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>177</v>
       </c>
@@ -1656,9 +1681,11 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -1678,7 +1705,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>182</v>
       </c>
@@ -1698,92 +1725,92 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
     </row>
   </sheetData>
@@ -1796,11 +1823,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
@@ -1809,7 +1836,7 @@
     <col min="6" max="6" width="29.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1827,7 +1854,7 @@
       </c>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>185</v>
       </c>
@@ -1843,9 +1870,11 @@
       <c r="E2" t="s">
         <v>187</v>
       </c>
-      <c r="F2"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F2" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>205</v>
       </c>
@@ -1864,7 +1893,7 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
@@ -1873,7 +1902,7 @@
     <col min="5" max="5" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>163</v>
       </c>
@@ -1890,7 +1919,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -1910,7 +1939,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>117</v>
       </c>
@@ -1924,7 +1953,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -1944,7 +1973,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>82</v>
       </c>
@@ -1958,11 +1987,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D6" s="6"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>162</v>
       </c>
@@ -1985,7 +2014,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>161</v>
       </c>
@@ -2005,7 +2034,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>160</v>
       </c>
@@ -2025,7 +2054,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>159</v>
       </c>
@@ -2045,7 +2074,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>158</v>
       </c>
@@ -2065,7 +2094,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>157</v>
       </c>
@@ -2085,16 +2114,16 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>154</v>
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2117,7 +2146,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -2151,7 +2180,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -2161,7 +2190,7 @@
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2181,7 +2210,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2201,7 +2230,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2215,7 +2244,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2229,7 +2258,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2243,7 +2272,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2263,7 +2292,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -2277,7 +2306,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -2291,7 +2320,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2305,7 +2334,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2319,7 +2348,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -2333,7 +2362,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -2347,7 +2376,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -2361,7 +2390,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2375,7 +2404,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -2389,7 +2418,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2403,7 +2432,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2417,7 +2446,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -2431,7 +2460,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -2445,7 +2474,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -2459,7 +2488,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -2473,7 +2502,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -2487,7 +2516,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -2501,7 +2530,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -2515,7 +2544,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -2529,7 +2558,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>70</v>
       </c>
@@ -2543,7 +2572,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -2557,7 +2586,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -2571,7 +2600,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -2585,7 +2614,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -2599,7 +2628,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -2613,7 +2642,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -2627,7 +2656,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -2641,7 +2670,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>90</v>
       </c>
@@ -2661,7 +2690,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -2675,7 +2704,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -2689,7 +2718,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>94</v>
       </c>
@@ -2703,7 +2732,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>96</v>
       </c>
@@ -2717,7 +2746,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -2731,7 +2760,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>100</v>
       </c>
@@ -2745,7 +2774,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -2759,7 +2788,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>105</v>
       </c>
@@ -2773,7 +2802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>106</v>
       </c>
@@ -2787,7 +2816,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>109</v>
       </c>
@@ -2807,7 +2836,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>112</v>
       </c>
@@ -2821,7 +2850,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>114</v>
       </c>
@@ -2835,7 +2864,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>117</v>
       </c>
@@ -2849,7 +2878,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>119</v>
       </c>
@@ -2863,7 +2892,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>122</v>
       </c>
@@ -2877,7 +2906,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>124</v>
       </c>
@@ -2891,7 +2920,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>127</v>
       </c>
@@ -2905,7 +2934,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>130</v>
       </c>
@@ -2933,9 +2962,9 @@
       <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2943,7 +2972,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2951,7 +2980,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>171</v>
       </c>
@@ -2959,7 +2988,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2967,7 +2996,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -2975,7 +3004,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -2983,7 +3012,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2991,7 +3020,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -2999,7 +3028,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>195</v>
       </c>
@@ -3007,12 +3036,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -3020,7 +3049,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>197</v>
       </c>
@@ -3028,7 +3057,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -3036,12 +3065,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -3049,7 +3078,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -3057,7 +3086,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -3065,7 +3094,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -3073,7 +3102,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>199</v>
       </c>
@@ -3081,7 +3110,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -3089,7 +3118,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>112</v>
       </c>
@@ -3097,7 +3126,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -3105,7 +3134,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -3113,7 +3142,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>201</v>
       </c>
@@ -3121,7 +3150,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -3129,7 +3158,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>117</v>
       </c>
@@ -3137,7 +3166,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -3145,7 +3174,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -3153,7 +3182,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -3161,7 +3190,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>114</v>
       </c>
@@ -3169,7 +3198,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -3177,7 +3206,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -3185,7 +3214,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>119</v>
       </c>
@@ -3193,7 +3222,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>122</v>
       </c>
@@ -3201,7 +3230,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -3209,7 +3238,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>91</v>
       </c>
@@ -3217,7 +3246,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>94</v>
       </c>
@@ -3225,7 +3254,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>203</v>
       </c>
@@ -3233,12 +3262,12 @@
         <v>204</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -3246,7 +3275,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -3254,7 +3283,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -3262,7 +3291,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -3270,7 +3299,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>100</v>
       </c>
@@ -3278,7 +3307,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>130</v>
       </c>
@@ -3286,17 +3315,17 @@
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>102</v>
       </c>
@@ -3304,7 +3333,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>105</v>
       </c>
@@ -3312,7 +3341,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>127</v>
       </c>
@@ -3320,7 +3349,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -3328,7 +3357,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -3336,7 +3365,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>40</v>
       </c>
@@ -3344,7 +3373,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -3352,7 +3381,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Revert "update eda inconsistency file"
This reverts commit d0a27e1ae6ad09d7ccd0fc5dd6350893ff9b3d88.
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A3A260-33B7-6949-A7E1-56D7A7939FDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F605E5-8A58-F847-91FE-A2626C56A482}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12100" windowWidth="25180" windowHeight="14380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1300" windowWidth="25180" windowHeight="14380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="206">
   <si>
     <t>sid</t>
   </si>
@@ -643,30 +643,13 @@
   </si>
   <si>
     <t>See comments on 'TermWithDifferentLabels'</t>
-  </si>
-  <si>
-    <t>change to Time living in dwelling with units years</t>
-  </si>
-  <si>
-    <t>EUPATH_0022264 should be "Plasmodium falciparum, by qPCR result" and be moved under 'Raw eukaryota data for blood' with unit "/uL"
-EUPATH_0022062 should be "Plasmodium falciparum copies, by qPCR", moved under 'Raw eukaryota data for blood", with unit "/rxn"</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>EUPATH_0022247 should be "Plasmodium vivax, by qPCR result" and be moved under 'Raw eukaryota data for blood' with unit "/uL"
-EUPATH_0022061 should be "Plasmodium vivax copies, by qPCR", moved under 'Raw eukaryota data for blood", with unit "/rxn"</t>
-  </si>
-  <si>
-    <t>should be under Relocation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1169,7 +1152,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1178,9 +1161,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1539,10 +1519,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" customWidth="1"/>
@@ -1551,7 +1531,7 @@
     <col min="5" max="5" width="55.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1565,7 +1545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>185</v>
       </c>
@@ -1580,7 +1560,7 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>188</v>
       </c>
@@ -1591,15 +1571,12 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>189</v>
       </c>
       <c r="C5" t="s">
         <v>190</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1612,20 +1589,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
     <col min="4" max="4" width="33.83203125" customWidth="1"/>
     <col min="5" max="5" width="39.1640625" customWidth="1"/>
-    <col min="6" max="6" width="47.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1642,10 +1619,10 @@
         <v>9</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="97" customHeight="1" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>175</v>
       </c>
@@ -1661,11 +1638,9 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="F2"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>177</v>
       </c>
@@ -1681,11 +1656,9 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F3"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -1705,7 +1678,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="7" t="s">
         <v>182</v>
       </c>
@@ -1725,92 +1698,92 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="4"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="4"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="1"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" s="1"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" s="3"/>
     </row>
   </sheetData>
@@ -1823,11 +1796,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
@@ -1836,7 +1809,7 @@
     <col min="6" max="6" width="29.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1854,7 +1827,7 @@
       </c>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>185</v>
       </c>
@@ -1870,11 +1843,9 @@
       <c r="E2" t="s">
         <v>187</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>205</v>
       </c>
@@ -1893,7 +1864,7 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
@@ -1902,7 +1873,7 @@
     <col min="5" max="5" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>163</v>
       </c>
@@ -1919,7 +1890,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -1939,7 +1910,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="C3" t="s">
         <v>117</v>
       </c>
@@ -1953,7 +1924,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -1973,7 +1944,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="C5" t="s">
         <v>82</v>
       </c>
@@ -1987,11 +1958,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="D6" s="6"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>162</v>
       </c>
@@ -2014,7 +1985,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>161</v>
       </c>
@@ -2034,7 +2005,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>160</v>
       </c>
@@ -2054,7 +2025,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>159</v>
       </c>
@@ -2074,7 +2045,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>158</v>
       </c>
@@ -2094,7 +2065,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>157</v>
       </c>
@@ -2114,16 +2085,16 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="B13" t="s">
         <v>154</v>
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2146,7 +2117,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -2180,7 +2151,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -2190,7 +2161,7 @@
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2210,7 +2181,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2230,7 +2201,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2244,7 +2215,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2258,7 +2229,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2272,7 +2243,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2292,7 +2263,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -2306,7 +2277,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -2320,7 +2291,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2334,7 +2305,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2348,7 +2319,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -2362,7 +2333,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -2376,7 +2347,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -2390,7 +2361,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2404,7 +2375,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -2418,7 +2389,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2432,7 +2403,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2446,7 +2417,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -2460,7 +2431,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -2474,7 +2445,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -2488,7 +2459,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -2502,7 +2473,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -2516,7 +2487,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -2530,7 +2501,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -2544,7 +2515,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -2558,7 +2529,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>70</v>
       </c>
@@ -2572,7 +2543,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -2586,7 +2557,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -2600,7 +2571,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -2614,7 +2585,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -2628,7 +2599,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -2642,7 +2613,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -2656,7 +2627,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -2670,7 +2641,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>90</v>
       </c>
@@ -2690,7 +2661,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -2704,7 +2675,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -2718,7 +2689,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>94</v>
       </c>
@@ -2732,7 +2703,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>96</v>
       </c>
@@ -2746,7 +2717,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -2760,7 +2731,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>100</v>
       </c>
@@ -2774,7 +2745,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -2788,7 +2759,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>105</v>
       </c>
@@ -2802,7 +2773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>106</v>
       </c>
@@ -2816,7 +2787,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>109</v>
       </c>
@@ -2836,7 +2807,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>112</v>
       </c>
@@ -2850,7 +2821,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>114</v>
       </c>
@@ -2864,7 +2835,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>117</v>
       </c>
@@ -2878,7 +2849,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>119</v>
       </c>
@@ -2892,7 +2863,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>122</v>
       </c>
@@ -2906,7 +2877,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>124</v>
       </c>
@@ -2920,7 +2891,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>127</v>
       </c>
@@ -2934,7 +2905,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>130</v>
       </c>
@@ -2962,9 +2933,9 @@
       <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2972,7 +2943,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2980,7 +2951,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>171</v>
       </c>
@@ -2988,7 +2959,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2996,7 +2967,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -3004,7 +2975,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -3012,7 +2983,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -3020,7 +2991,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -3028,7 +2999,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>195</v>
       </c>
@@ -3036,12 +3007,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -3049,7 +3020,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>197</v>
       </c>
@@ -3057,7 +3028,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -3065,12 +3036,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -3078,7 +3049,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -3086,7 +3057,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -3094,7 +3065,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -3102,7 +3073,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>199</v>
       </c>
@@ -3110,7 +3081,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -3118,7 +3089,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>112</v>
       </c>
@@ -3126,7 +3097,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -3134,7 +3105,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -3142,7 +3113,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>201</v>
       </c>
@@ -3150,7 +3121,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -3158,7 +3129,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>117</v>
       </c>
@@ -3166,7 +3137,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -3174,7 +3145,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -3182,7 +3153,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -3190,7 +3161,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>114</v>
       </c>
@@ -3198,7 +3169,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -3206,7 +3177,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -3214,7 +3185,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>119</v>
       </c>
@@ -3222,7 +3193,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>122</v>
       </c>
@@ -3230,7 +3201,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -3238,7 +3209,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>91</v>
       </c>
@@ -3246,7 +3217,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>94</v>
       </c>
@@ -3254,7 +3225,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>203</v>
       </c>
@@ -3262,12 +3233,12 @@
         <v>204</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -3275,7 +3246,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -3283,7 +3254,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -3291,7 +3262,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -3299,7 +3270,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>100</v>
       </c>
@@ -3307,7 +3278,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>130</v>
       </c>
@@ -3315,17 +3286,17 @@
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>102</v>
       </c>
@@ -3333,7 +3304,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>105</v>
       </c>
@@ -3341,7 +3312,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>127</v>
       </c>
@@ -3349,7 +3320,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -3357,7 +3328,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -3365,7 +3336,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>40</v>
       </c>
@@ -3373,7 +3344,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -3381,7 +3352,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
respond to Jie's inconsistency issues
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC2CB8F-7CDD-6D42-A388-7B060DC71BB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632B746E-48FA-9D4C-93BC-F2976CFEB0EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="1560" windowWidth="25180" windowHeight="14380" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2420" yWindow="1560" windowWidth="25180" windowHeight="14380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="220">
   <si>
     <t>sid</t>
   </si>
@@ -579,9 +579,6 @@
     <t>EUPATH_0000367|EUPATH_0000355|EUPATH_0000351</t>
   </si>
   <si>
-    <t>Shall I merge the terms?</t>
-  </si>
-  <si>
     <t>EUPATH_0000377</t>
   </si>
   <si>
@@ -664,13 +661,39 @@
   </si>
   <si>
     <t>Assigned IDs to following units</t>
+  </si>
+  <si>
+    <t>change to Time living in dwelling with units years</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>EUPATH_0022264 should be "Plasmodium falciparum, by qPCR result" and be moved under 'Raw eukaryota data for blood' with unit "/uL"
+EUPATH_0022062 should be "Plasmodium falciparum copies, by qPCR", moved under 'Raw eukaryota data for blood", with unit "/rxn"</t>
+  </si>
+  <si>
+    <t>EUPATH_0022247 should be "Plasmodium vivax, by qPCR result" and be moved under 'Raw eukaryota data for blood' with unit "/uL"
+EUPATH_0022061 should be "Plasmodium vivax copies, by qPCR", moved under 'Raw eukaryota data for blood", with unit "/rxn"</t>
+  </si>
+  <si>
+    <t>should be under Relocation</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>For EUPATH_0000350, change label to "Time spent in occupation every week" with units "days", for EUPATH_0000366 - change label to "Time spent in occupation every day" with unit "hrs"</t>
+  </si>
+  <si>
+    <t>For EUPATH_0000351, change label to "Time spent in secoondary occupation every week" with unit "days", for EUPATH_0000367 - change label to "Time spent in secondary occupation every day" with unit "hrs", and leave label for EUPATH_0000355 as is</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1173,7 +1196,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1184,6 +1207,9 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1542,10 +1568,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" customWidth="1"/>
@@ -1554,7 +1580,7 @@
     <col min="5" max="5" width="55.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1568,38 +1594,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" t="s">
         <v>186</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>187</v>
       </c>
-      <c r="E2"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>188</v>
       </c>
-      <c r="C4" t="s">
-        <v>191</v>
-      </c>
-      <c r="D4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
         <v>189</v>
       </c>
-      <c r="C5" t="s">
-        <v>190</v>
+      <c r="D5" s="5" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -1612,20 +1641,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
     <col min="4" max="4" width="33.83203125" customWidth="1"/>
     <col min="5" max="5" width="39.1640625" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="5"/>
+    <col min="6" max="6" width="75.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1642,10 +1671,10 @@
         <v>9</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="184" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>175</v>
       </c>
@@ -1661,9 +1690,11 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" s="10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>177</v>
       </c>
@@ -1679,9 +1710,11 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -1697,11 +1730,11 @@
       <c r="E4" t="s">
         <v>181</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>182</v>
       </c>
@@ -1717,96 +1750,96 @@
       <c r="E5" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="F5" s="10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
     </row>
   </sheetData>
@@ -1820,10 +1853,10 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
@@ -1832,7 +1865,7 @@
     <col min="6" max="6" width="29.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1848,29 +1881,33 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="F1" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" t="s">
         <v>193</v>
       </c>
-      <c r="D2" t="s">
-        <v>194</v>
-      </c>
       <c r="E2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F2"/>
-    </row>
-    <row r="4" spans="1:6">
+        <v>186</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -1887,7 +1924,7 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
@@ -1896,7 +1933,7 @@
     <col min="5" max="5" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>163</v>
       </c>
@@ -1913,7 +1950,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -1933,7 +1970,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>117</v>
       </c>
@@ -1947,7 +1984,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -1967,7 +2004,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>82</v>
       </c>
@@ -1981,11 +2018,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D6" s="6"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>162</v>
       </c>
@@ -2008,7 +2045,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>161</v>
       </c>
@@ -2028,7 +2065,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>160</v>
       </c>
@@ -2048,7 +2085,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>159</v>
       </c>
@@ -2068,7 +2105,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>158</v>
       </c>
@@ -2088,7 +2125,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>157</v>
       </c>
@@ -2108,16 +2145,16 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>154</v>
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2140,7 +2177,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -2170,11 +2207,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -2184,7 +2221,7 @@
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2204,7 +2241,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2224,7 +2261,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2238,7 +2275,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2252,7 +2289,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2266,7 +2303,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2286,7 +2323,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -2300,7 +2337,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -2314,7 +2351,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2328,7 +2365,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2342,7 +2379,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -2356,7 +2393,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -2370,7 +2407,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -2384,7 +2421,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2398,7 +2435,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -2412,7 +2449,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2426,7 +2463,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2440,7 +2477,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -2454,7 +2491,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -2468,7 +2505,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -2482,7 +2519,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -2496,7 +2533,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -2510,7 +2547,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -2524,7 +2561,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -2538,7 +2575,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -2552,7 +2589,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>70</v>
       </c>
@@ -2566,7 +2603,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -2580,7 +2617,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -2594,7 +2631,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -2608,7 +2645,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -2622,7 +2659,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -2636,7 +2673,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -2650,7 +2687,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -2664,7 +2701,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>90</v>
       </c>
@@ -2684,7 +2721,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -2698,7 +2735,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -2712,7 +2749,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>94</v>
       </c>
@@ -2726,7 +2763,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>96</v>
       </c>
@@ -2740,7 +2777,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -2754,7 +2791,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>100</v>
       </c>
@@ -2768,7 +2805,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -2782,7 +2819,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>105</v>
       </c>
@@ -2796,7 +2833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>106</v>
       </c>
@@ -2810,7 +2847,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>109</v>
       </c>
@@ -2830,7 +2867,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>112</v>
       </c>
@@ -2844,7 +2881,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>114</v>
       </c>
@@ -2858,7 +2895,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>117</v>
       </c>
@@ -2872,7 +2909,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>119</v>
       </c>
@@ -2886,7 +2923,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>122</v>
       </c>
@@ -2900,7 +2937,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>124</v>
       </c>
@@ -2914,7 +2951,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>127</v>
       </c>
@@ -2928,7 +2965,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>130</v>
       </c>
@@ -2952,17 +2989,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E96E553-B9B7-3A43-9A19-9B2DEFC1133B}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="47.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2970,7 +3007,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -2978,7 +3015,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2986,7 +3023,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -2994,7 +3031,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -3002,7 +3039,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -3010,7 +3047,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -3018,23 +3055,23 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8" t="s">
         <v>195</v>
       </c>
-      <c r="B8" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -3042,15 +3079,15 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" t="s">
         <v>197</v>
       </c>
-      <c r="B11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -3058,15 +3095,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -3074,7 +3111,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -3082,7 +3119,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -3090,7 +3127,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -3098,15 +3135,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>198</v>
+      </c>
+      <c r="B18" t="s">
         <v>199</v>
       </c>
-      <c r="B18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -3114,7 +3151,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>112</v>
       </c>
@@ -3122,7 +3159,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -3130,7 +3167,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -3138,15 +3175,15 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B23" t="s">
         <v>201</v>
       </c>
-      <c r="B23" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -3154,7 +3191,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -3162,7 +3199,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -3170,7 +3207,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -3178,7 +3215,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -3186,7 +3223,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -3194,7 +3231,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -3202,7 +3239,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -3210,7 +3247,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>119</v>
       </c>
@@ -3218,7 +3255,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>122</v>
       </c>
@@ -3226,7 +3263,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -3234,7 +3271,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -3242,7 +3279,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>94</v>
       </c>
@@ -3250,23 +3287,23 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" t="s">
         <v>203</v>
       </c>
-      <c r="B37" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -3274,7 +3311,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -3282,7 +3319,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -3290,7 +3327,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>96</v>
       </c>
@@ -3298,7 +3335,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>100</v>
       </c>
@@ -3306,7 +3343,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>130</v>
       </c>
@@ -3314,15 +3351,15 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>102</v>
       </c>
@@ -3330,7 +3367,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>105</v>
       </c>
@@ -3338,7 +3375,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>127</v>
       </c>
@@ -3346,15 +3383,15 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B50" s="8"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -3362,10 +3399,10 @@
         <v>174</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -3373,13 +3410,13 @@
         <v>54</v>
       </c>
       <c r="C54" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="D54" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="D54" s="8" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>40</v>
       </c>
@@ -3387,10 +3424,10 @@
         <v>20</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -3398,10 +3435,10 @@
         <v>20</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D57" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix inconsistent issues in icemr_amazoniaPeru_long, refs #45330
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632B746E-48FA-9D4C-93BC-F2976CFEB0EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E296F80E-E51A-2B46-A8C6-5BF1ACD2AA19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="1560" windowWidth="25180" windowHeight="14380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="1460" windowWidth="23440" windowHeight="14380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="220">
   <si>
     <t>sid</t>
   </si>
@@ -693,7 +693,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1567,11 +1567,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" customWidth="1"/>
@@ -1580,7 +1580,7 @@
     <col min="5" max="5" width="55.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>188</v>
       </c>
@@ -1629,6 +1629,9 @@
       </c>
       <c r="D5" s="5" t="s">
         <v>212</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1639,13 +1642,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
@@ -1654,7 +1657,7 @@
     <col min="6" max="6" width="75.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1674,7 +1677,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="184" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="184" customHeight="1">
       <c r="A2" t="s">
         <v>175</v>
       </c>
@@ -1694,7 +1697,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="66" customHeight="1">
       <c r="A3" t="s">
         <v>177</v>
       </c>
@@ -1714,7 +1717,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="51">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -1734,7 +1737,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="68">
       <c r="A5" s="7" t="s">
         <v>182</v>
       </c>
@@ -1753,93 +1756,96 @@
       <c r="F5" s="10" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="4"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="4"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="1"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" s="1"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" s="3"/>
     </row>
   </sheetData>
@@ -1850,13 +1856,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
@@ -1865,7 +1871,7 @@
     <col min="6" max="6" width="29.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1885,7 +1891,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -1904,8 +1910,11 @@
       <c r="F2" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>204</v>
       </c>
@@ -1924,7 +1933,7 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
@@ -1933,7 +1942,7 @@
     <col min="5" max="5" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>163</v>
       </c>
@@ -1950,7 +1959,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -1970,7 +1979,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="C3" t="s">
         <v>117</v>
       </c>
@@ -1984,7 +1993,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -2004,7 +2013,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="C5" t="s">
         <v>82</v>
       </c>
@@ -2018,11 +2027,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="D6" s="6"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>162</v>
       </c>
@@ -2045,7 +2054,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>161</v>
       </c>
@@ -2065,7 +2074,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>160</v>
       </c>
@@ -2085,7 +2094,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>159</v>
       </c>
@@ -2105,7 +2114,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>158</v>
       </c>
@@ -2125,7 +2134,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>157</v>
       </c>
@@ -2145,16 +2154,16 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="B13" t="s">
         <v>154</v>
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2177,7 +2186,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -2211,7 +2220,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -2221,7 +2230,7 @@
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2241,7 +2250,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2261,7 +2270,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2275,7 +2284,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2289,7 +2298,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2303,7 +2312,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2323,7 +2332,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -2337,7 +2346,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -2351,7 +2360,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2365,7 +2374,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2379,7 +2388,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -2393,7 +2402,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -2407,7 +2416,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -2421,7 +2430,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2435,7 +2444,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -2449,7 +2458,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2463,7 +2472,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2477,7 +2486,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -2491,7 +2500,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -2505,7 +2514,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -2519,7 +2528,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -2533,7 +2542,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -2547,7 +2556,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -2561,7 +2570,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -2575,7 +2584,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -2589,7 +2598,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>70</v>
       </c>
@@ -2603,7 +2612,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -2617,7 +2626,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -2631,7 +2640,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -2645,7 +2654,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -2659,7 +2668,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -2673,7 +2682,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -2687,7 +2696,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -2701,7 +2710,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>90</v>
       </c>
@@ -2721,7 +2730,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -2735,7 +2744,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -2749,7 +2758,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>94</v>
       </c>
@@ -2763,7 +2772,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>96</v>
       </c>
@@ -2777,7 +2786,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -2791,7 +2800,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>100</v>
       </c>
@@ -2805,7 +2814,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -2819,7 +2828,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>105</v>
       </c>
@@ -2833,7 +2842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>106</v>
       </c>
@@ -2847,7 +2856,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>109</v>
       </c>
@@ -2867,7 +2876,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>112</v>
       </c>
@@ -2881,7 +2890,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>114</v>
       </c>
@@ -2895,7 +2904,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>117</v>
       </c>
@@ -2909,7 +2918,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>119</v>
       </c>
@@ -2923,7 +2932,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>122</v>
       </c>
@@ -2937,7 +2946,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>124</v>
       </c>
@@ -2951,7 +2960,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>127</v>
       </c>
@@ -2965,7 +2974,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>130</v>
       </c>
@@ -2993,13 +3002,13 @@
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="47.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3007,7 +3016,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -3015,7 +3024,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3023,7 +3032,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -3031,7 +3040,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -3039,7 +3048,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -3047,7 +3056,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -3055,7 +3064,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>194</v>
       </c>
@@ -3063,7 +3072,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -3071,7 +3080,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -3079,7 +3088,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>196</v>
       </c>
@@ -3087,7 +3096,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -3095,7 +3104,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>210</v>
       </c>
@@ -3103,7 +3112,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -3111,7 +3120,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -3119,7 +3128,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -3127,7 +3136,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -3135,7 +3144,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>198</v>
       </c>
@@ -3143,7 +3152,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -3151,7 +3160,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>112</v>
       </c>
@@ -3159,7 +3168,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -3167,7 +3176,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -3175,7 +3184,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>200</v>
       </c>
@@ -3183,7 +3192,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -3191,7 +3200,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -3199,7 +3208,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -3207,7 +3216,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -3215,7 +3224,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -3223,7 +3232,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -3231,7 +3240,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -3239,7 +3248,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -3247,7 +3256,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>119</v>
       </c>
@@ -3255,7 +3264,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>122</v>
       </c>
@@ -3263,7 +3272,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -3271,7 +3280,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -3279,7 +3288,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>94</v>
       </c>
@@ -3287,7 +3296,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>202</v>
       </c>
@@ -3295,7 +3304,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -3303,7 +3312,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -3311,7 +3320,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -3319,7 +3328,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -3327,7 +3336,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>96</v>
       </c>
@@ -3335,7 +3344,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>100</v>
       </c>
@@ -3343,7 +3352,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>130</v>
       </c>
@@ -3351,7 +3360,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -3359,7 +3368,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>102</v>
       </c>
@@ -3367,7 +3376,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>105</v>
       </c>
@@ -3375,7 +3384,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>127</v>
       </c>
@@ -3383,15 +3392,15 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="B50" s="8"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -3402,7 +3411,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -3416,7 +3425,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>40</v>
       </c>
@@ -3427,7 +3436,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -3438,7 +3447,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="D57" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update inconsistency issue tracker
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BD4D11-6362-194A-9428-E7F9AE453077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDC8ED8-F056-984E-8B2F-50ED991A8E54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="1240" windowWidth="24820" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6720" yWindow="4080" windowWidth="24820" windowHeight="13380" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,15 @@
     <sheet name="units" sheetId="4" r:id="rId5"/>
     <sheet name="unit list" sheetId="7" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">termWithDifferentParent!$A$1:$F$30</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="562">
   <si>
     <t>sid</t>
   </si>
@@ -1429,13 +1432,295 @@
   </si>
   <si>
     <t>wrong IRI, need change to http://purl.obolibrary.org/obo/UO_0000036</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Platelets</t>
+  </si>
+  <si>
+    <t>Hematocrit (%)</t>
+  </si>
+  <si>
+    <t>Persons living in house count</t>
+  </si>
+  <si>
+    <t>Sleeping rooms in dwelling count</t>
+  </si>
+  <si>
+    <t>Time living in settlement and put the unit as Years</t>
+  </si>
+  <si>
+    <t>Persons sleeping in dwelling count</t>
+  </si>
+  <si>
+    <t>Water trips per day</t>
+  </si>
+  <si>
+    <t>Water trips per week</t>
+  </si>
+  <si>
+    <t>Children under 60 months in dwelling count</t>
+  </si>
+  <si>
+    <t>Households sharing human waste disposal facility count</t>
+  </si>
+  <si>
+    <t>Max loose stools at episode count</t>
+  </si>
+  <si>
+    <t>Pharmacy, transport expenses amount</t>
+  </si>
+  <si>
+    <t>Traditional healer, transport expenses amount</t>
+  </si>
+  <si>
+    <t>Unlicensed doctor, total expenses amount</t>
+  </si>
+  <si>
+    <t>Unlicensed doctor, transport expenses amount</t>
+  </si>
+  <si>
+    <t>Licensed doctor, transport expenses amount</t>
+  </si>
+  <si>
+    <t>Bought remedy or medicine, transport expenses amount</t>
+  </si>
+  <si>
+    <t>1st choice hospital or health center, total expenses amount</t>
+  </si>
+  <si>
+    <t>Licensed doctor, total expenses amount</t>
+  </si>
+  <si>
+    <t>Pharmacy, total expenses amount</t>
+  </si>
+  <si>
+    <t>Traditional healer, total expenses amount</t>
+  </si>
+  <si>
+    <t>Bought remedy or medicine, total expenses amount</t>
+  </si>
+  <si>
+    <t>1st choice hospital or health center, transport expenses amount</t>
+  </si>
+  <si>
+    <t>2nd choice hospital or health center, total expenses amount</t>
+  </si>
+  <si>
+    <t>2nd choice hospital or health center, transport expenses amount</t>
+  </si>
+  <si>
+    <t>3rd choice hospital or health center, total expenses amount</t>
+  </si>
+  <si>
+    <t>3rd choice hospital or health center, transport expenses amount</t>
+  </si>
+  <si>
+    <t>Other total medical expenses amount</t>
+  </si>
+  <si>
+    <t>Other transportation expenses amount</t>
+  </si>
+  <si>
+    <t>Payment for initial transportation to clinic amount</t>
+  </si>
+  <si>
+    <t>Payment for trips to clinic after initial visit amount</t>
+  </si>
+  <si>
+    <t>Payment for transportation by other household members amount</t>
+  </si>
+  <si>
+    <t>Hospitalization or visit, consultation expenses amount</t>
+  </si>
+  <si>
+    <t>Hospitalization or visit, drug expenses amount</t>
+  </si>
+  <si>
+    <t>Hospitalization or visit, diagnostic expenses amount</t>
+  </si>
+  <si>
+    <t>Hospitalization or visit, food expenses amount</t>
+  </si>
+  <si>
+    <t>Hospitalization or visit, other expenses amount</t>
+  </si>
+  <si>
+    <t>Hospitalization or visit, other expenses</t>
+  </si>
+  <si>
+    <t>Hospitalization or visit, total expenses amount</t>
+  </si>
+  <si>
+    <t>Lost earnings due to care, other caregivers</t>
+  </si>
+  <si>
+    <t>Lost earnings due to care amount, other caregivers</t>
+  </si>
+  <si>
+    <t>Earning time lost due to care</t>
+  </si>
+  <si>
+    <t>Earning time lost due to care, other caregivers</t>
+  </si>
+  <si>
+    <t>Diarrhea treament</t>
+  </si>
+  <si>
+    <t>Anemia (hemoglobin &lt;11 g/dL)</t>
+  </si>
+  <si>
+    <t>Anemia (hemoglobin &lt;10 g/dL)</t>
+  </si>
+  <si>
+    <t>Plasmodium vivax, by qPCR result</t>
+  </si>
+  <si>
+    <t>Plasmodium falciparum, by qPCR result</t>
+  </si>
+  <si>
+    <t>School-age children treated in village (%)</t>
+  </si>
+  <si>
+    <t>Total population treated in village (%)</t>
+  </si>
+  <si>
+    <t>Mean Schistosoma mansoni count, by microscopy</t>
+  </si>
+  <si>
+    <t>EUPATH_0030133</t>
+  </si>
+  <si>
+    <t>Percent school-age children treated in village, second treatment</t>
+  </si>
+  <si>
+    <t>School-age children treated in village, second treatment (%)</t>
+  </si>
+  <si>
+    <t>gates_scoreNig</t>
+  </si>
+  <si>
+    <t>Percent total population treated in village, second treatment</t>
+  </si>
+  <si>
+    <t>Total population treated in village, second treatment (%)</t>
+  </si>
+  <si>
+    <t>EUPATH_0030135</t>
+  </si>
+  <si>
+    <t>Schistosoma haematobium egg count, by microscopy</t>
+  </si>
+  <si>
+    <t>School ID</t>
+  </si>
+  <si>
+    <t>Schistosoma mansoni, by CCA</t>
+  </si>
+  <si>
+    <t>Diarrhea onset date</t>
+  </si>
+  <si>
+    <t>O2 saturation (%)</t>
+  </si>
+  <si>
+    <t>Low birth weight (&lt;2500 g)</t>
+  </si>
+  <si>
+    <t>Malaria diagnoses in the past year count</t>
+  </si>
+  <si>
+    <t>Campylobacter jejuni or C. coli, by TAC result</t>
+  </si>
+  <si>
+    <t>CMO_0000105</t>
+  </si>
+  <si>
+    <t>EUPATH_0033152 - used to have 2 terms because of different units</t>
+  </si>
+  <si>
+    <t>EUPATH_0042171</t>
+  </si>
+  <si>
+    <t>EUPATH_0000156</t>
+  </si>
+  <si>
+    <t>EUPATH_0024160, and change label to "Time since last personal bednet treatment"</t>
+  </si>
+  <si>
+    <t>EUPATH_0010097</t>
+  </si>
+  <si>
+    <t>EUPATH_0022187 - used to have 2 terms because of different units</t>
+  </si>
+  <si>
+    <t>EUPATH_0021223 - used to have 2 terms because of different units</t>
+  </si>
+  <si>
+    <t>EUPATH_0024266</t>
+  </si>
+  <si>
+    <t>EUPATH_0000427 - used to have 2 terms because of different units</t>
+  </si>
+  <si>
+    <t>IAO_0000414</t>
+  </si>
+  <si>
+    <t>EUPATH_0024002</t>
+  </si>
+  <si>
+    <t>OBI_0001169</t>
+  </si>
+  <si>
+    <t>ENVO_00000004</t>
+  </si>
+  <si>
+    <t>drop end_age and EUPATH_0031204 entirely from VIDA</t>
+  </si>
+  <si>
+    <t>Participant</t>
+  </si>
+  <si>
+    <t>Entomology - although I believe we might be changing this label and IRI to Specimen collection</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Relocation</t>
+  </si>
+  <si>
+    <t>Household observation details</t>
+  </si>
+  <si>
+    <t>Household water</t>
+  </si>
+  <si>
+    <t>Socioeconomic factors</t>
+  </si>
+  <si>
+    <t>Labor and delivery</t>
+  </si>
+  <si>
+    <t>Raw eukaryota data for blood</t>
+  </si>
+  <si>
+    <t>Clinical history - also change label to "Diagnosis prior to 60 day follow-up visit"</t>
+  </si>
+  <si>
+    <t>Yes, for EFO_0004348, label should be Hematocrit (%) and for EUPATH_0032049 label should be O2 saturation (%) with no units</t>
+  </si>
+  <si>
+    <t>agree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1940,7 +2225,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1950,6 +2235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2306,13 +2592,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
@@ -2321,7 +2607,7 @@
     <col min="5" max="5" width="55.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2334,8 +2620,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="E1" s="4" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -2348,9 +2637,11 @@
       <c r="D2" t="s">
         <v>116</v>
       </c>
-      <c r="E2"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="4" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>117</v>
       </c>
@@ -2363,8 +2654,11 @@
       <c r="D3" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" s="4" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>120</v>
       </c>
@@ -2377,8 +2671,11 @@
       <c r="D4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -2391,8 +2688,11 @@
       <c r="D5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>126</v>
       </c>
@@ -2405,8 +2705,11 @@
       <c r="D6" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -2419,8 +2722,11 @@
       <c r="D7" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7" s="4" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -2433,8 +2739,11 @@
       <c r="D8" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -2447,8 +2756,11 @@
       <c r="D9" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9" s="4" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -2461,8 +2773,11 @@
       <c r="D10" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="E10" s="4" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>140</v>
       </c>
@@ -2475,8 +2790,11 @@
       <c r="D11" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="E11" s="4" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>143</v>
       </c>
@@ -2489,8 +2807,11 @@
       <c r="D12" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="E12" s="4" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>145</v>
       </c>
@@ -2503,8 +2824,11 @@
       <c r="D13" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="E13" s="4" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>148</v>
       </c>
@@ -2517,8 +2841,11 @@
       <c r="D14" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="E14" s="4" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>151</v>
       </c>
@@ -2531,8 +2858,11 @@
       <c r="D15" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="E15" s="4" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>153</v>
       </c>
@@ -2545,8 +2875,11 @@
       <c r="D16" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="4" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>156</v>
       </c>
@@ -2559,8 +2892,11 @@
       <c r="D17" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="4" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>158</v>
       </c>
@@ -2573,8 +2909,11 @@
       <c r="D18" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="4" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>160</v>
       </c>
@@ -2587,8 +2926,11 @@
       <c r="D19" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="4" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>162</v>
       </c>
@@ -2601,8 +2943,11 @@
       <c r="D20" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="4" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>164</v>
       </c>
@@ -2615,8 +2960,11 @@
       <c r="D21" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="4" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -2629,8 +2977,11 @@
       <c r="D22" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="4" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>168</v>
       </c>
@@ -2643,8 +2994,11 @@
       <c r="D23" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="4" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>170</v>
       </c>
@@ -2657,8 +3011,11 @@
       <c r="D24" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="4" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>172</v>
       </c>
@@ -2671,8 +3028,11 @@
       <c r="D25" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" s="4" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>174</v>
       </c>
@@ -2685,8 +3045,11 @@
       <c r="D26" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" s="4" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>176</v>
       </c>
@@ -2699,8 +3062,11 @@
       <c r="D27" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" s="4" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>178</v>
       </c>
@@ -2713,8 +3079,11 @@
       <c r="D28" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" s="4" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>180</v>
       </c>
@@ -2727,8 +3096,11 @@
       <c r="D29" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" s="4" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>182</v>
       </c>
@@ -2741,8 +3113,11 @@
       <c r="D30" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" s="4" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>184</v>
       </c>
@@ -2755,8 +3130,11 @@
       <c r="D31" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" s="4" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>186</v>
       </c>
@@ -2769,8 +3147,11 @@
       <c r="D32" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" s="4" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>188</v>
       </c>
@@ -2783,8 +3164,11 @@
       <c r="D33" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" s="4" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>190</v>
       </c>
@@ -2797,8 +3181,11 @@
       <c r="D34" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" s="4" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>192</v>
       </c>
@@ -2811,8 +3198,11 @@
       <c r="D35" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" s="4" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>194</v>
       </c>
@@ -2825,8 +3215,11 @@
       <c r="D36" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" s="4" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>196</v>
       </c>
@@ -2839,8 +3232,11 @@
       <c r="D37" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" s="4" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>198</v>
       </c>
@@ -2853,8 +3249,11 @@
       <c r="D38" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38" s="4" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>200</v>
       </c>
@@ -2867,8 +3266,11 @@
       <c r="D39" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39" s="4" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>202</v>
       </c>
@@ -2881,8 +3283,11 @@
       <c r="D40" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40" s="4" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>204</v>
       </c>
@@ -2895,8 +3300,11 @@
       <c r="D41" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41" s="4" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>206</v>
       </c>
@@ -2909,8 +3317,11 @@
       <c r="D42" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42" s="4" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>208</v>
       </c>
@@ -2923,8 +3334,11 @@
       <c r="D43" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43" s="4" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>210</v>
       </c>
@@ -2937,8 +3351,11 @@
       <c r="D44" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44" s="4" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>212</v>
       </c>
@@ -2951,8 +3368,11 @@
       <c r="D45" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45" s="4" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>214</v>
       </c>
@@ -2965,8 +3385,11 @@
       <c r="D46" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46" s="4" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>217</v>
       </c>
@@ -2979,8 +3402,11 @@
       <c r="D47" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47" s="4" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>220</v>
       </c>
@@ -2993,8 +3419,11 @@
       <c r="D48" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48" s="4" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>223</v>
       </c>
@@ -3007,8 +3436,11 @@
       <c r="D49" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49" s="4" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>226</v>
       </c>
@@ -3021,8 +3453,11 @@
       <c r="D50" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50" s="4" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>228</v>
       </c>
@@ -3035,8 +3470,11 @@
       <c r="D51" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51" s="4" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>230</v>
       </c>
@@ -3049,8 +3487,11 @@
       <c r="D52" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52" s="4" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>233</v>
       </c>
@@ -3063,103 +3504,161 @@
       <c r="D53" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53" s="4" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>520</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>521</v>
+      </c>
+      <c r="D54" t="s">
+        <v>523</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>526</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>524</v>
+      </c>
+      <c r="D55" t="s">
+        <v>523</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>235</v>
       </c>
-      <c r="B54">
-        <v>2</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
         <v>236</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D56" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" t="s">
+      <c r="E56" s="4" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>238</v>
       </c>
-      <c r="B55">
+      <c r="B57">
         <v>3</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C57" t="s">
         <v>239</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D57" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
+      <c r="E57" s="4" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>241</v>
       </c>
-      <c r="B56">
-        <v>2</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58" t="s">
         <v>242</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D58" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
+      <c r="E58" s="9" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>244</v>
       </c>
-      <c r="B57">
-        <v>2</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
         <v>245</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D59" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
+      <c r="E59" s="9" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>246</v>
       </c>
-      <c r="B58">
-        <v>2</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
         <v>247</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D60" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
+      <c r="E60" s="9" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>249</v>
       </c>
-      <c r="B59">
-        <v>2</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61" t="s">
         <v>250</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D61" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" t="s">
+      <c r="E61" s="9" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>252</v>
       </c>
-      <c r="B60">
-        <v>2</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62" t="s">
         <v>253</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D62" t="s">
         <v>254</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>532</v>
       </c>
     </row>
   </sheetData>
@@ -3172,20 +3671,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="48" customWidth="1"/>
-    <col min="4" max="4" width="33.83203125" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="39.1640625" customWidth="1"/>
-    <col min="6" max="6" width="75.1640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="30.1640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3205,7 +3704,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>344</v>
       </c>
@@ -3221,9 +3720,11 @@
       <c r="E2" t="s">
         <v>346</v>
       </c>
-      <c r="F2"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" s="4" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>347</v>
       </c>
@@ -3239,9 +3740,11 @@
       <c r="E3" t="s">
         <v>349</v>
       </c>
-      <c r="F3"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="4" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>350</v>
       </c>
@@ -3257,9 +3760,11 @@
       <c r="E4" t="s">
         <v>352</v>
       </c>
-      <c r="F4"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4" s="4" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>353</v>
       </c>
@@ -3275,9 +3780,11 @@
       <c r="E5" t="s">
         <v>326</v>
       </c>
-      <c r="F5"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="F5" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>355</v>
       </c>
@@ -3293,9 +3800,11 @@
       <c r="E6" t="s">
         <v>326</v>
       </c>
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="F6" s="4" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>357</v>
       </c>
@@ -3311,9 +3820,11 @@
       <c r="E7" t="s">
         <v>315</v>
       </c>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="F7" s="4" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>359</v>
       </c>
@@ -3329,9 +3840,11 @@
       <c r="E8" t="s">
         <v>361</v>
       </c>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="F8" s="4" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>362</v>
       </c>
@@ -3347,9 +3860,11 @@
       <c r="E9" t="s">
         <v>364</v>
       </c>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9" s="4" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>365</v>
       </c>
@@ -3365,9 +3880,11 @@
       <c r="E10" t="s">
         <v>367</v>
       </c>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="F10" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>368</v>
       </c>
@@ -3383,9 +3900,11 @@
       <c r="E11" t="s">
         <v>315</v>
       </c>
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="F11" s="4" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>370</v>
       </c>
@@ -3401,9 +3920,11 @@
       <c r="E12" t="s">
         <v>372</v>
       </c>
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="F12" s="4" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>373</v>
       </c>
@@ -3419,9 +3940,11 @@
       <c r="E13" t="s">
         <v>349</v>
       </c>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="F13" s="4" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>375</v>
       </c>
@@ -3437,9 +3960,11 @@
       <c r="E14" t="s">
         <v>378</v>
       </c>
-      <c r="F14"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="F14" s="4" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>338</v>
       </c>
@@ -3455,9 +3980,11 @@
       <c r="E15" t="s">
         <v>381</v>
       </c>
-      <c r="F15"/>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="F15" s="4" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>382</v>
       </c>
@@ -3473,68 +4000,70 @@
       <c r="E16" t="s">
         <v>385</v>
       </c>
-      <c r="F16"/>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="4" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
     </row>
   </sheetData>
@@ -3545,20 +4074,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="C11" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="34.5" customWidth="1"/>
     <col min="4" max="4" width="45.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3574,8 +4104,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>255</v>
       </c>
@@ -3591,8 +4124,11 @@
       <c r="E2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="4" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>259</v>
       </c>
@@ -3608,8 +4144,11 @@
       <c r="E3" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="4" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>263</v>
       </c>
@@ -3625,8 +4164,11 @@
       <c r="E4" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="4" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>267</v>
       </c>
@@ -3642,8 +4184,11 @@
       <c r="E5" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>271</v>
       </c>
@@ -3659,8 +4204,11 @@
       <c r="E6" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="4" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>274</v>
       </c>
@@ -3676,8 +4224,11 @@
       <c r="E7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="4" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>276</v>
       </c>
@@ -3693,8 +4244,11 @@
       <c r="E8" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="4" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>280</v>
       </c>
@@ -3710,8 +4264,11 @@
       <c r="E9" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="4" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>283</v>
       </c>
@@ -3727,8 +4284,11 @@
       <c r="E10" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="4" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>286</v>
       </c>
@@ -3744,8 +4304,11 @@
       <c r="E11" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="4" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>289</v>
       </c>
@@ -3761,8 +4324,11 @@
       <c r="E12" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="4" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>293</v>
       </c>
@@ -3778,8 +4344,11 @@
       <c r="E13" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="4" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>296</v>
       </c>
@@ -3795,8 +4364,11 @@
       <c r="E14" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" s="4" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>300</v>
       </c>
@@ -3812,8 +4384,11 @@
       <c r="E15" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="4" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>252</v>
       </c>
@@ -3829,8 +4404,11 @@
       <c r="E16" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>305</v>
       </c>
@@ -3846,8 +4424,11 @@
       <c r="E17" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="4" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>308</v>
       </c>
@@ -3863,8 +4444,11 @@
       <c r="E18" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>312</v>
       </c>
@@ -3880,8 +4464,11 @@
       <c r="E19" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="4" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>314</v>
       </c>
@@ -3897,8 +4484,11 @@
       <c r="E20" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="4" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>228</v>
       </c>
@@ -3914,8 +4504,11 @@
       <c r="E21" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" s="4" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>226</v>
       </c>
@@ -3931,8 +4524,11 @@
       <c r="E22" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="4" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>320</v>
       </c>
@@ -3948,8 +4544,11 @@
       <c r="E23" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="4" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>322</v>
       </c>
@@ -3965,8 +4564,11 @@
       <c r="E24" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="4" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>325</v>
       </c>
@@ -3982,8 +4584,11 @@
       <c r="E25" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="4" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>328</v>
       </c>
@@ -3999,8 +4604,11 @@
       <c r="E26" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>126</v>
       </c>
@@ -4016,8 +4624,11 @@
       <c r="E27" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="4" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>334</v>
       </c>
@@ -4033,8 +4644,11 @@
       <c r="E28" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" s="4" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>337</v>
       </c>
@@ -4050,8 +4664,11 @@
       <c r="E29" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>341</v>
       </c>
@@ -4067,8 +4684,12 @@
       <c r="E30" t="s">
         <v>343</v>
       </c>
+      <c r="F30" s="4" t="s">
+        <v>306</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F30" xr:uid="{3F2C9002-1B0A-C348-905C-32E2D16BAD66}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -4078,11 +4699,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="42.83203125" customWidth="1"/>
@@ -4091,7 +4712,7 @@
     <col min="5" max="5" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -4104,9 +4725,11 @@
       <c r="D1" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="E1" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -4119,9 +4742,11 @@
       <c r="D2" t="s">
         <v>462</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E2" s="4" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -4134,8 +4759,11 @@
       <c r="D4" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" s="4" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -4146,7 +4774,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -4157,7 +4785,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -4168,7 +4796,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -4179,7 +4807,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>85</v>
       </c>
@@ -4193,7 +4821,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -4204,7 +4832,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -4215,7 +4843,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -4228,8 +4856,11 @@
       <c r="D14" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="E14" s="4" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -4240,7 +4871,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>89</v>
       </c>
@@ -4253,8 +4884,11 @@
       <c r="D17" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="4" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D18" s="7"/>
     </row>
   </sheetData>
@@ -4271,14 +4905,14 @@
       <selection activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="76.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="4"/>
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -4292,7 +4926,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -4306,7 +4940,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4320,7 +4954,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -4334,7 +4968,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -4348,7 +4982,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -4362,7 +4996,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -4376,7 +5010,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>389</v>
       </c>
@@ -4390,7 +5024,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -4404,7 +5038,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -4418,7 +5052,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -4432,7 +5066,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -4446,7 +5080,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -4460,7 +5094,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -4474,7 +5108,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>395</v>
       </c>
@@ -4488,7 +5122,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>103</v>
       </c>
@@ -4502,7 +5136,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -4516,7 +5150,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>400</v>
       </c>
@@ -4530,7 +5164,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -4544,7 +5178,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -4558,7 +5192,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -4572,7 +5206,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -4586,7 +5220,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>407</v>
       </c>
@@ -4600,7 +5234,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -4614,7 +5248,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>410</v>
       </c>
@@ -4628,7 +5262,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -4642,7 +5276,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -4656,7 +5290,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -4670,7 +5304,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -4684,7 +5318,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -4698,7 +5332,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -4712,7 +5346,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>415</v>
       </c>
@@ -4726,7 +5360,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>417</v>
       </c>
@@ -4740,7 +5374,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -4755,7 +5389,7 @@
       </c>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -4769,7 +5403,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>421</v>
       </c>
@@ -4783,7 +5417,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -4797,7 +5431,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -4811,7 +5445,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -4825,7 +5459,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>425</v>
       </c>
@@ -4839,7 +5473,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>107</v>
       </c>
@@ -4853,7 +5487,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>73</v>
       </c>
@@ -4867,7 +5501,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>427</v>
       </c>
@@ -4881,7 +5515,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>75</v>
       </c>
@@ -4895,7 +5529,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>77</v>
       </c>
@@ -4909,7 +5543,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>79</v>
       </c>
@@ -4923,7 +5557,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>81</v>
       </c>
@@ -4937,7 +5571,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>100</v>
       </c>
@@ -4951,7 +5585,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -4965,7 +5599,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>433</v>
       </c>
@@ -4979,7 +5613,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>32</v>
       </c>
@@ -4993,7 +5627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>88</v>
       </c>
@@ -5007,7 +5641,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -5021,7 +5655,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -5035,7 +5669,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -5049,7 +5683,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>444</v>
       </c>
@@ -5063,7 +5697,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -5077,7 +5711,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>89</v>
       </c>
@@ -5091,7 +5725,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>85</v>
       </c>
@@ -5105,7 +5739,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>90</v>
       </c>
@@ -5129,17 +5763,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E96E553-B9B7-3A43-9A19-9B2DEFC1133B}">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A48" workbookViewId="0">
       <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -5147,7 +5781,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -5155,7 +5789,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -5163,7 +5797,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -5171,7 +5805,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5179,7 +5813,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -5187,7 +5821,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -5195,7 +5829,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -5203,7 +5837,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>395</v>
       </c>
@@ -5211,7 +5845,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>103</v>
       </c>
@@ -5219,7 +5853,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -5227,7 +5861,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>88</v>
       </c>
@@ -5235,7 +5869,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -5243,7 +5877,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -5251,7 +5885,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -5259,7 +5893,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>400</v>
       </c>
@@ -5267,7 +5901,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -5275,7 +5909,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -5283,7 +5917,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -5291,7 +5925,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>433</v>
       </c>
@@ -5299,7 +5933,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -5307,7 +5941,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>83</v>
       </c>
@@ -5315,7 +5949,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -5323,7 +5957,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>48</v>
       </c>
@@ -5331,7 +5965,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>48</v>
       </c>
@@ -5339,7 +5973,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>389</v>
       </c>
@@ -5347,7 +5981,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>407</v>
       </c>
@@ -5355,7 +5989,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>105</v>
       </c>
@@ -5363,7 +5997,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>410</v>
       </c>
@@ -5371,7 +6005,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -5379,7 +6013,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>85</v>
       </c>
@@ -5387,7 +6021,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>85</v>
       </c>
@@ -5395,7 +6029,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -5403,7 +6037,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -5411,7 +6045,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -5419,7 +6053,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>84</v>
       </c>
@@ -5427,7 +6061,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>415</v>
       </c>
@@ -5435,7 +6069,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>417</v>
       </c>
@@ -5443,7 +6077,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -5451,7 +6085,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>62</v>
       </c>
@@ -5459,7 +6093,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -5467,7 +6101,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>421</v>
       </c>
@@ -5475,7 +6109,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -5483,7 +6117,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>65</v>
       </c>
@@ -5491,7 +6125,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>444</v>
       </c>
@@ -5499,7 +6133,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>69</v>
       </c>
@@ -5507,7 +6141,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>69</v>
       </c>
@@ -5515,7 +6149,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>71</v>
       </c>
@@ -5523,7 +6157,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>425</v>
       </c>
@@ -5531,7 +6165,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>107</v>
       </c>
@@ -5539,7 +6173,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -5547,7 +6181,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -5555,7 +6189,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>33</v>
       </c>
@@ -5564,7 +6198,7 @@
       </c>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>427</v>
       </c>
@@ -5574,7 +6208,7 @@
       <c r="C54" s="6"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>75</v>
       </c>
@@ -5583,7 +6217,7 @@
       </c>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -5592,7 +6226,7 @@
       </c>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>77</v>
       </c>
@@ -5601,7 +6235,7 @@
       </c>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>90</v>
       </c>
@@ -5609,7 +6243,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>35</v>
       </c>
@@ -5617,7 +6251,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>79</v>
       </c>
@@ -5625,7 +6259,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>81</v>
       </c>
@@ -5633,7 +6267,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>89</v>
       </c>
@@ -5641,7 +6275,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
conversion file updates and inconsistency tracker
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67931F96-409C-A74B-8D40-B0503B2168FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F053B3-5672-B048-A594-C440E8EF0187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="460" windowWidth="26240" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2560" yWindow="500" windowWidth="26240" windowHeight="13380" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="708">
   <si>
     <t>sid</t>
   </si>
@@ -1617,9 +1617,6 @@
     <t>Participant</t>
   </si>
   <si>
-    <t>Entomology - although I believe we might be changing this label and IRI to Specimen collection</t>
-  </si>
-  <si>
     <t>Activity</t>
   </si>
   <si>
@@ -2101,13 +2098,67 @@
   </si>
   <si>
     <t>wrong IRI, it is 'ng/dL', need change to http://purl.obolibrary.org/obo/NCIT_C67305</t>
+  </si>
+  <si>
+    <t>Diarrhea treatment</t>
+  </si>
+  <si>
+    <t>Edinburgh Postnatal Depression Scale score</t>
+  </si>
+  <si>
+    <t>EUPATH_0036567</t>
+  </si>
+  <si>
+    <t>Arthropod collection</t>
+  </si>
+  <si>
+    <t>Feeding</t>
+  </si>
+  <si>
+    <t>Arthropod collection process</t>
+  </si>
+  <si>
+    <t>Pregnancy</t>
+  </si>
+  <si>
+    <t>Sample details</t>
+  </si>
+  <si>
+    <t>Immunization and prevention</t>
+  </si>
+  <si>
+    <t>use hrs</t>
+  </si>
+  <si>
+    <t>Family income in local currency</t>
+  </si>
+  <si>
+    <t>Cumulative time exclusive breastfeeding with unit days</t>
+  </si>
+  <si>
+    <t>Socioeconomic status</t>
+  </si>
+  <si>
+    <t>Symptoms</t>
+  </si>
+  <si>
+    <t>Family income in USD' - make sure there are no units entered</t>
+  </si>
+  <si>
+    <t>Plesiomonas, by TAC result - should have units of 'CT value'</t>
+  </si>
+  <si>
+    <t>Time living in settlement - should have units of 'years'</t>
+  </si>
+  <si>
+    <t>Arthropod collection' EUPATH_0044177</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2621,7 +2672,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2633,6 +2684,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2991,11 +3043,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
@@ -3004,7 +3056,7 @@
     <col min="5" max="5" width="55.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3021,7 +3073,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -3038,10 +3090,10 @@
         <v>448</v>
       </c>
       <c r="F2" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -3058,10 +3110,10 @@
         <v>449</v>
       </c>
       <c r="F3" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -3078,10 +3130,10 @@
         <v>450</v>
       </c>
       <c r="F4" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -3098,10 +3150,10 @@
         <v>451</v>
       </c>
       <c r="F5" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -3118,10 +3170,10 @@
         <v>452</v>
       </c>
       <c r="F6" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -3138,10 +3190,10 @@
         <v>512</v>
       </c>
       <c r="F7" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -3158,10 +3210,10 @@
         <v>453</v>
       </c>
       <c r="F8" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>134</v>
       </c>
@@ -3178,10 +3230,10 @@
         <v>454</v>
       </c>
       <c r="F9" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>137</v>
       </c>
@@ -3198,10 +3250,10 @@
         <v>455</v>
       </c>
       <c r="F10" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -3218,10 +3270,10 @@
         <v>456</v>
       </c>
       <c r="F11" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>142</v>
       </c>
@@ -3238,10 +3290,10 @@
         <v>457</v>
       </c>
       <c r="F12" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>144</v>
       </c>
@@ -3258,10 +3310,10 @@
         <v>458</v>
       </c>
       <c r="F13" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>147</v>
       </c>
@@ -3278,7 +3330,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>150</v>
       </c>
@@ -3295,7 +3347,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>152</v>
       </c>
@@ -3312,7 +3364,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>155</v>
       </c>
@@ -3329,7 +3381,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>157</v>
       </c>
@@ -3346,7 +3398,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>159</v>
       </c>
@@ -3363,7 +3415,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>161</v>
       </c>
@@ -3380,7 +3432,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>163</v>
       </c>
@@ -3397,7 +3449,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>165</v>
       </c>
@@ -3414,7 +3466,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>167</v>
       </c>
@@ -3431,7 +3483,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>169</v>
       </c>
@@ -3448,7 +3500,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>171</v>
       </c>
@@ -3465,7 +3517,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>173</v>
       </c>
@@ -3482,7 +3534,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>175</v>
       </c>
@@ -3499,7 +3551,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>177</v>
       </c>
@@ -3516,7 +3568,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>179</v>
       </c>
@@ -3533,7 +3585,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>181</v>
       </c>
@@ -3550,7 +3602,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>183</v>
       </c>
@@ -3567,7 +3619,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>185</v>
       </c>
@@ -3584,7 +3636,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>187</v>
       </c>
@@ -3601,7 +3653,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>189</v>
       </c>
@@ -3618,7 +3670,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>191</v>
       </c>
@@ -3635,7 +3687,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>193</v>
       </c>
@@ -3652,7 +3704,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>195</v>
       </c>
@@ -3669,7 +3721,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>197</v>
       </c>
@@ -3686,7 +3738,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>199</v>
       </c>
@@ -3703,7 +3755,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>201</v>
       </c>
@@ -3720,7 +3772,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>203</v>
       </c>
@@ -3737,7 +3789,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>205</v>
       </c>
@@ -3754,7 +3806,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>207</v>
       </c>
@@ -3771,7 +3823,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>209</v>
       </c>
@@ -3788,7 +3840,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>211</v>
       </c>
@@ -3805,7 +3857,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>213</v>
       </c>
@@ -3822,7 +3874,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>216</v>
       </c>
@@ -3839,7 +3891,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>219</v>
       </c>
@@ -3856,7 +3908,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>222</v>
       </c>
@@ -3873,7 +3925,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>225</v>
       </c>
@@ -3890,7 +3942,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>227</v>
       </c>
@@ -3907,7 +3959,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>229</v>
       </c>
@@ -3924,7 +3976,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>232</v>
       </c>
@@ -3941,7 +3993,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>499</v>
       </c>
@@ -3958,7 +4010,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>505</v>
       </c>
@@ -3975,7 +4027,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>234</v>
       </c>
@@ -3992,7 +4044,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>237</v>
       </c>
@@ -4009,7 +4061,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>240</v>
       </c>
@@ -4026,7 +4078,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>243</v>
       </c>
@@ -4043,7 +4095,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>245</v>
       </c>
@@ -4060,7 +4112,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>248</v>
       </c>
@@ -4077,7 +4129,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>251</v>
       </c>
@@ -4094,15 +4146,15 @@
         <v>511</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E63" s="8"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -4115,9 +4167,8 @@
       <c r="D67" t="s">
         <v>3</v>
       </c>
-      <c r="E67"/>
-    </row>
-    <row r="68" spans="1:5">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>125</v>
       </c>
@@ -4130,24 +4181,28 @@
       <c r="D68" t="s">
         <v>127</v>
       </c>
-      <c r="E68"/>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="E68" s="4" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>622</v>
+      </c>
+      <c r="B69">
+        <v>2</v>
+      </c>
+      <c r="C69" t="s">
         <v>623</v>
       </c>
-      <c r="B69">
-        <v>2</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>624</v>
       </c>
-      <c r="D69" t="s">
-        <v>625</v>
-      </c>
-      <c r="E69"/>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="E69" s="4" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>183</v>
       </c>
@@ -4155,29 +4210,33 @@
         <v>2</v>
       </c>
       <c r="C70" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D70" t="s">
         <v>149</v>
       </c>
-      <c r="E70"/>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="E70" s="4" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>626</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71" t="s">
         <v>627</v>
       </c>
-      <c r="B71">
-        <v>2</v>
-      </c>
-      <c r="C71" t="s">
-        <v>628</v>
-      </c>
       <c r="D71" t="s">
-        <v>547</v>
-      </c>
-      <c r="E71"/>
-    </row>
-    <row r="72" spans="1:5">
+        <v>546</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>213</v>
       </c>
@@ -4185,44 +4244,50 @@
         <v>2</v>
       </c>
       <c r="C72" t="s">
+        <v>628</v>
+      </c>
+      <c r="D72" t="s">
         <v>629</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" s="4" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>630</v>
       </c>
-      <c r="E72"/>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" t="s">
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
         <v>631</v>
       </c>
-      <c r="B73">
-        <v>2</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
+        <v>578</v>
+      </c>
+      <c r="E73" s="11" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>632</v>
       </c>
-      <c r="D73" t="s">
-        <v>579</v>
-      </c>
-      <c r="E73"/>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" t="s">
+      <c r="B74">
+        <v>2</v>
+      </c>
+      <c r="C74" t="s">
         <v>633</v>
       </c>
-      <c r="B74">
-        <v>2</v>
-      </c>
-      <c r="C74" t="s">
-        <v>634</v>
-      </c>
       <c r="D74" t="s">
-        <v>617</v>
-      </c>
-      <c r="E74"/>
-    </row>
-    <row r="75" spans="1:5">
+        <v>616</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>219</v>
       </c>
@@ -4235,9 +4300,11 @@
       <c r="D75" t="s">
         <v>221</v>
       </c>
-      <c r="E75"/>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="E75" s="4" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>234</v>
       </c>
@@ -4250,22 +4317,26 @@
       <c r="D76" t="s">
         <v>236</v>
       </c>
-      <c r="E76"/>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="E76" s="4" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>634</v>
+      </c>
+      <c r="B77">
+        <v>2</v>
+      </c>
+      <c r="C77" t="s">
         <v>635</v>
       </c>
-      <c r="B77">
-        <v>2</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>636</v>
       </c>
-      <c r="D77" t="s">
-        <v>637</v>
-      </c>
-      <c r="E77"/>
+      <c r="E77" s="4" t="s">
+        <v>691</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4277,11 +4348,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="42.83203125" customWidth="1"/>
@@ -4290,7 +4361,7 @@
     <col min="6" max="6" width="30.1640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4310,7 +4381,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>343</v>
       </c>
@@ -4330,7 +4401,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>346</v>
       </c>
@@ -4350,7 +4421,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>349</v>
       </c>
@@ -4370,7 +4441,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>352</v>
       </c>
@@ -4390,7 +4461,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>354</v>
       </c>
@@ -4410,7 +4481,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>356</v>
       </c>
@@ -4430,7 +4501,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>358</v>
       </c>
@@ -4450,7 +4521,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>361</v>
       </c>
@@ -4470,7 +4541,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>364</v>
       </c>
@@ -4490,7 +4561,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>367</v>
       </c>
@@ -4510,7 +4581,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>369</v>
       </c>
@@ -4530,7 +4601,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>372</v>
       </c>
@@ -4550,7 +4621,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>374</v>
       </c>
@@ -4570,7 +4641,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>337</v>
       </c>
@@ -4590,7 +4661,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>381</v>
       </c>
@@ -4607,21 +4678,21 @@
         <v>384</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -4639,75 +4710,77 @@
       </c>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>638</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
         <v>639</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>640</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>641</v>
-      </c>
-      <c r="F22"/>
-    </row>
-    <row r="23" spans="1:6">
+        <v>640</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
     </row>
   </sheetData>
@@ -4720,11 +4793,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="34.5" customWidth="1"/>
@@ -4732,7 +4805,7 @@
     <col min="6" max="6" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4752,7 +4825,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>254</v>
       </c>
@@ -4772,7 +4845,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>258</v>
       </c>
@@ -4788,11 +4861,11 @@
       <c r="E3" t="s">
         <v>261</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="11" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>262</v>
       </c>
@@ -4809,10 +4882,10 @@
         <v>265</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>266</v>
       </c>
@@ -4832,7 +4905,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>270</v>
       </c>
@@ -4849,10 +4922,10 @@
         <v>154</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>273</v>
       </c>
@@ -4869,10 +4942,10 @@
         <v>154</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>275</v>
       </c>
@@ -4889,10 +4962,10 @@
         <v>278</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>279</v>
       </c>
@@ -4912,7 +4985,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>282</v>
       </c>
@@ -4929,10 +5002,10 @@
         <v>284</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>285</v>
       </c>
@@ -4948,11 +5021,11 @@
       <c r="E11" t="s">
         <v>261</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="F11" s="11" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>288</v>
       </c>
@@ -4969,10 +5042,10 @@
         <v>291</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>292</v>
       </c>
@@ -4992,7 +5065,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>295</v>
       </c>
@@ -5009,10 +5082,10 @@
         <v>298</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>299</v>
       </c>
@@ -5032,7 +5105,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>251</v>
       </c>
@@ -5049,10 +5122,10 @@
         <v>253</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>304</v>
       </c>
@@ -5072,7 +5145,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>307</v>
       </c>
@@ -5092,7 +5165,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>311</v>
       </c>
@@ -5109,10 +5182,10 @@
         <v>265</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>313</v>
       </c>
@@ -5132,7 +5205,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>227</v>
       </c>
@@ -5149,10 +5222,10 @@
         <v>127</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>225</v>
       </c>
@@ -5169,10 +5242,10 @@
         <v>127</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>319</v>
       </c>
@@ -5189,10 +5262,10 @@
         <v>154</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>321</v>
       </c>
@@ -5209,10 +5282,10 @@
         <v>136</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>324</v>
       </c>
@@ -5232,7 +5305,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>327</v>
       </c>
@@ -5252,7 +5325,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>125</v>
       </c>
@@ -5269,10 +5342,10 @@
         <v>127</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>333</v>
       </c>
@@ -5289,10 +5362,10 @@
         <v>335</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>336</v>
       </c>
@@ -5312,7 +5385,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>340</v>
       </c>
@@ -5332,12 +5405,12 @@
         <v>305</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -5353,9 +5426,8 @@
       <c r="E35" t="s">
         <v>3</v>
       </c>
-      <c r="F35"/>
-    </row>
-    <row r="36" spans="1:6">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>254</v>
       </c>
@@ -5369,29 +5441,33 @@
         <v>256</v>
       </c>
       <c r="E36" t="s">
+        <v>542</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>543</v>
       </c>
-      <c r="F36"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
         <v>544</v>
       </c>
-      <c r="B37">
-        <v>2</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>545</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>546</v>
       </c>
-      <c r="E37" t="s">
-        <v>547</v>
-      </c>
-      <c r="F37"/>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="F37" s="4" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>258</v>
       </c>
@@ -5402,32 +5478,36 @@
         <v>259</v>
       </c>
       <c r="D38" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E38" t="s">
         <v>261</v>
       </c>
-      <c r="F38"/>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="F38" s="4" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>548</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
         <v>549</v>
       </c>
-      <c r="B39">
-        <v>2</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>550</v>
       </c>
-      <c r="D39" t="s">
-        <v>551</v>
-      </c>
       <c r="E39" t="s">
-        <v>547</v>
-      </c>
-      <c r="F39"/>
-    </row>
-    <row r="40" spans="1:6">
+        <v>546</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>262</v>
       </c>
@@ -5443,63 +5523,71 @@
       <c r="E40" t="s">
         <v>265</v>
       </c>
-      <c r="F40"/>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="F40" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>551</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
         <v>552</v>
       </c>
-      <c r="B41">
-        <v>2</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>553</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>554</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" s="4" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>555</v>
       </c>
-      <c r="F41"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" t="s">
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
         <v>556</v>
       </c>
-      <c r="B42">
-        <v>2</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
+        <v>553</v>
+      </c>
+      <c r="E42" t="s">
         <v>557</v>
       </c>
-      <c r="D42" t="s">
-        <v>554</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="F42" s="4" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>558</v>
       </c>
-      <c r="F42"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" t="s">
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
         <v>559</v>
       </c>
-      <c r="B43">
-        <v>2</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>560</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>561</v>
       </c>
-      <c r="E43" t="s">
-        <v>562</v>
-      </c>
-      <c r="F43"/>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="F43" s="4" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>266</v>
       </c>
@@ -5515,9 +5603,11 @@
       <c r="E44" t="s">
         <v>269</v>
       </c>
-      <c r="F44"/>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="F44" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>270</v>
       </c>
@@ -5533,9 +5623,11 @@
       <c r="E45" t="s">
         <v>154</v>
       </c>
-      <c r="F45"/>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="F45" s="4" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>273</v>
       </c>
@@ -5551,27 +5643,31 @@
       <c r="E46" t="s">
         <v>154</v>
       </c>
-      <c r="F46"/>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="F46" s="4" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>562</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
         <v>563</v>
       </c>
-      <c r="B47">
-        <v>2</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>564</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>565</v>
       </c>
-      <c r="E47" t="s">
-        <v>566</v>
-      </c>
-      <c r="F47"/>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="F47" s="4" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>275</v>
       </c>
@@ -5587,9 +5683,11 @@
       <c r="E48" t="s">
         <v>278</v>
       </c>
-      <c r="F48"/>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="F48" s="4" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>279</v>
       </c>
@@ -5603,11 +5701,13 @@
         <v>256</v>
       </c>
       <c r="E49" t="s">
-        <v>567</v>
-      </c>
-      <c r="F49"/>
-    </row>
-    <row r="50" spans="1:6">
+        <v>566</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>282</v>
       </c>
@@ -5623,27 +5723,31 @@
       <c r="E50" t="s">
         <v>284</v>
       </c>
-      <c r="F50"/>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="F50" s="4" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>567</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
         <v>568</v>
       </c>
-      <c r="B51">
-        <v>2</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>569</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>570</v>
       </c>
-      <c r="E51" t="s">
-        <v>571</v>
-      </c>
-      <c r="F51"/>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="F51" s="4" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>288</v>
       </c>
@@ -5657,11 +5761,13 @@
         <v>290</v>
       </c>
       <c r="E52" t="s">
-        <v>572</v>
-      </c>
-      <c r="F52"/>
-    </row>
-    <row r="53" spans="1:6">
+        <v>571</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>292</v>
       </c>
@@ -5677,27 +5783,31 @@
       <c r="E53" t="s">
         <v>294</v>
       </c>
-      <c r="F53"/>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="F53" s="4" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>572</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
         <v>573</v>
-      </c>
-      <c r="B54">
-        <v>2</v>
-      </c>
-      <c r="C54" t="s">
-        <v>574</v>
       </c>
       <c r="D54" t="s">
         <v>290</v>
       </c>
       <c r="E54" t="s">
-        <v>575</v>
-      </c>
-      <c r="F54"/>
-    </row>
-    <row r="55" spans="1:6">
+        <v>574</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>295</v>
       </c>
@@ -5713,27 +5823,31 @@
       <c r="E55" t="s">
         <v>298</v>
       </c>
-      <c r="F55"/>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="F55" s="4" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>575</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
         <v>576</v>
       </c>
-      <c r="B56">
-        <v>2</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>577</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>578</v>
       </c>
-      <c r="E56" t="s">
-        <v>579</v>
-      </c>
-      <c r="F56"/>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="F56" s="4" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>299</v>
       </c>
@@ -5747,11 +5861,13 @@
         <v>256</v>
       </c>
       <c r="E57" t="s">
-        <v>580</v>
-      </c>
-      <c r="F57"/>
-    </row>
-    <row r="58" spans="1:6">
+        <v>579</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>251</v>
       </c>
@@ -5767,9 +5883,8 @@
       <c r="E58" t="s">
         <v>253</v>
       </c>
-      <c r="F58"/>
-    </row>
-    <row r="59" spans="1:6">
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>304</v>
       </c>
@@ -5783,11 +5898,13 @@
         <v>256</v>
       </c>
       <c r="E59" t="s">
-        <v>581</v>
-      </c>
-      <c r="F59"/>
-    </row>
-    <row r="60" spans="1:6">
+        <v>580</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>307</v>
       </c>
@@ -5803,9 +5920,11 @@
       <c r="E60" t="s">
         <v>310</v>
       </c>
-      <c r="F60"/>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="F60" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>311</v>
       </c>
@@ -5821,9 +5940,11 @@
       <c r="E61" t="s">
         <v>265</v>
       </c>
-      <c r="F61"/>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="F61" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>313</v>
       </c>
@@ -5839,9 +5960,11 @@
       <c r="E62" t="s">
         <v>315</v>
       </c>
-      <c r="F62"/>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="F62" s="4" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>319</v>
       </c>
@@ -5857,9 +5980,11 @@
       <c r="E63" t="s">
         <v>154</v>
       </c>
-      <c r="F63"/>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="F63" s="4" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>321</v>
       </c>
@@ -5875,117 +6000,128 @@
       <c r="E64" t="s">
         <v>136</v>
       </c>
-      <c r="F64"/>
-    </row>
-    <row r="65" spans="1:6">
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>581</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65" t="s">
         <v>582</v>
       </c>
-      <c r="B65">
-        <v>2</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
+        <v>550</v>
+      </c>
+      <c r="E65" t="s">
+        <v>546</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>583</v>
       </c>
-      <c r="D65" t="s">
-        <v>551</v>
-      </c>
-      <c r="E65" t="s">
-        <v>547</v>
-      </c>
-      <c r="F65"/>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" t="s">
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s">
         <v>584</v>
       </c>
-      <c r="B66">
-        <v>2</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>585</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>586</v>
       </c>
-      <c r="E66" t="s">
+      <c r="F66" s="4" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>587</v>
       </c>
-      <c r="F66"/>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" t="s">
+      <c r="B67">
+        <v>2</v>
+      </c>
+      <c r="C67" t="s">
         <v>588</v>
       </c>
-      <c r="B67">
-        <v>2</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>589</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>590</v>
       </c>
-      <c r="E67" t="s">
+      <c r="F67" s="4" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>591</v>
       </c>
-      <c r="F67"/>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" t="s">
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68" t="s">
         <v>592</v>
       </c>
-      <c r="B68">
-        <v>2</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
+        <v>589</v>
+      </c>
+      <c r="E68" t="s">
         <v>593</v>
       </c>
-      <c r="D68" t="s">
-        <v>590</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="F68" s="4" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>594</v>
       </c>
-      <c r="F68"/>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" t="s">
+      <c r="B69">
+        <v>2</v>
+      </c>
+      <c r="C69" t="s">
         <v>595</v>
       </c>
-      <c r="B69">
-        <v>2</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
+        <v>585</v>
+      </c>
+      <c r="E69" t="s">
         <v>596</v>
       </c>
-      <c r="D69" t="s">
-        <v>586</v>
-      </c>
-      <c r="E69" t="s">
+      <c r="F69" s="4" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>597</v>
       </c>
-      <c r="F69"/>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" t="s">
+      <c r="B70">
+        <v>2</v>
+      </c>
+      <c r="C70" t="s">
         <v>598</v>
       </c>
-      <c r="B70">
-        <v>2</v>
-      </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>599</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>600</v>
       </c>
-      <c r="E70" t="s">
-        <v>601</v>
-      </c>
-      <c r="F70"/>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="F70" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>324</v>
       </c>
@@ -5999,11 +6135,13 @@
         <v>256</v>
       </c>
       <c r="E71" t="s">
-        <v>602</v>
-      </c>
-      <c r="F71"/>
-    </row>
-    <row r="72" spans="1:6">
+        <v>601</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>327</v>
       </c>
@@ -6017,29 +6155,33 @@
         <v>329</v>
       </c>
       <c r="E72" t="s">
+        <v>602</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>603</v>
       </c>
-      <c r="F72"/>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" t="s">
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
         <v>604</v>
-      </c>
-      <c r="B73">
-        <v>2</v>
-      </c>
-      <c r="C73" t="s">
-        <v>605</v>
       </c>
       <c r="D73" t="s">
         <v>256</v>
       </c>
       <c r="E73" t="s">
-        <v>606</v>
-      </c>
-      <c r="F73"/>
-    </row>
-    <row r="74" spans="1:6">
+        <v>605</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>125</v>
       </c>
@@ -6055,81 +6197,91 @@
       <c r="E74" t="s">
         <v>127</v>
       </c>
-      <c r="F74"/>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="F74" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>606</v>
+      </c>
+      <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75" t="s">
         <v>607</v>
       </c>
-      <c r="B75">
-        <v>2</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>608</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>609</v>
       </c>
-      <c r="E75" t="s">
+      <c r="F75" s="4" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>610</v>
       </c>
-      <c r="F75"/>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" t="s">
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76" t="s">
         <v>611</v>
       </c>
-      <c r="B76">
-        <v>2</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
+        <v>608</v>
+      </c>
+      <c r="E76" t="s">
+        <v>609</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>612</v>
       </c>
-      <c r="D76" t="s">
+      <c r="B77">
+        <v>2</v>
+      </c>
+      <c r="C77" t="s">
+        <v>613</v>
+      </c>
+      <c r="D77" t="s">
+        <v>608</v>
+      </c>
+      <c r="E77" t="s">
         <v>609</v>
       </c>
-      <c r="E76" t="s">
-        <v>610</v>
-      </c>
-      <c r="F76"/>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" t="s">
-        <v>613</v>
-      </c>
-      <c r="B77">
-        <v>2</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="F77" s="4" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>614</v>
       </c>
-      <c r="D77" t="s">
-        <v>609</v>
-      </c>
-      <c r="E77" t="s">
-        <v>610</v>
-      </c>
-      <c r="F77"/>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" t="s">
+      <c r="B78">
+        <v>2</v>
+      </c>
+      <c r="C78" t="s">
         <v>615</v>
       </c>
-      <c r="B78">
-        <v>2</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
+        <v>608</v>
+      </c>
+      <c r="E78" t="s">
         <v>616</v>
       </c>
-      <c r="D78" t="s">
-        <v>609</v>
-      </c>
-      <c r="E78" t="s">
-        <v>617</v>
-      </c>
-      <c r="F78"/>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="F78" s="4" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>333</v>
       </c>
@@ -6145,27 +6297,28 @@
       <c r="E79" t="s">
         <v>335</v>
       </c>
-      <c r="F79"/>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="F79" s="4" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>617</v>
+      </c>
+      <c r="B80">
+        <v>2</v>
+      </c>
+      <c r="C80" t="s">
         <v>618</v>
       </c>
-      <c r="B80">
-        <v>2</v>
-      </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
         <v>619</v>
       </c>
-      <c r="D80" t="s">
-        <v>620</v>
-      </c>
       <c r="E80" t="s">
-        <v>547</v>
-      </c>
-      <c r="F80"/>
-    </row>
-    <row r="81" spans="1:6">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>526</v>
       </c>
@@ -6179,11 +6332,13 @@
         <v>338</v>
       </c>
       <c r="E81" t="s">
-        <v>621</v>
-      </c>
-      <c r="F81"/>
-    </row>
-    <row r="82" spans="1:6">
+        <v>620</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>340</v>
       </c>
@@ -6199,7 +6354,9 @@
       <c r="E82" t="s">
         <v>342</v>
       </c>
-      <c r="F82"/>
+      <c r="F82" s="4" t="s">
+        <v>305</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F30" xr:uid="{3F2C9002-1B0A-C348-905C-32E2D16BAD66}"/>
@@ -6212,11 +6369,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="42.83203125" customWidth="1"/>
@@ -6225,7 +6382,7 @@
     <col min="5" max="5" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -6242,7 +6399,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -6256,10 +6413,10 @@
         <v>441</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -6273,10 +6430,10 @@
         <v>442</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -6287,7 +6444,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -6298,7 +6455,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -6309,7 +6466,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -6320,7 +6477,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -6334,7 +6491,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -6345,7 +6502,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -6356,7 +6513,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -6370,10 +6527,10 @@
         <v>444</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -6384,7 +6541,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -6398,26 +6555,26 @@
         <v>446</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D18" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B22" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>43</v>
       </c>
@@ -6425,18 +6582,21 @@
         <v>44</v>
       </c>
       <c r="D24" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>684</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>84</v>
       </c>
@@ -6444,10 +6604,10 @@
         <v>433</v>
       </c>
       <c r="D27" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>84</v>
       </c>
@@ -6455,7 +6615,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>83</v>
       </c>
@@ -6463,7 +6623,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>83</v>
       </c>
@@ -6471,10 +6631,10 @@
         <v>44</v>
       </c>
       <c r="D31" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>85</v>
       </c>
@@ -6482,7 +6642,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>85</v>
       </c>
@@ -6490,18 +6650,18 @@
         <v>100</v>
       </c>
       <c r="D34" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>416</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>416</v>
       </c>
@@ -6509,10 +6669,10 @@
         <v>417</v>
       </c>
       <c r="D37" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>76</v>
       </c>
@@ -6520,15 +6680,15 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>76</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D40" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
   </sheetData>
@@ -6545,14 +6705,14 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="83.83203125" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="4"/>
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -6566,7 +6726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -6580,7 +6740,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -6594,7 +6754,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -6608,7 +6768,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -6619,10 +6779,10 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -6633,10 +6793,10 @@
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -6644,13 +6804,13 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
+        <v>662</v>
+      </c>
+      <c r="D7" t="s">
         <v>663</v>
       </c>
-      <c r="D7" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>391</v>
       </c>
@@ -6664,7 +6824,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>102</v>
       </c>
@@ -6678,7 +6838,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -6689,10 +6849,10 @@
         <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -6700,13 +6860,13 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
+        <v>679</v>
+      </c>
+      <c r="D11" t="s">
         <v>680</v>
       </c>
-      <c r="D11" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -6720,7 +6880,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>112</v>
       </c>
@@ -6734,7 +6894,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -6748,7 +6908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>396</v>
       </c>
@@ -6759,10 +6919,10 @@
         <v>397</v>
       </c>
       <c r="D15" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -6773,10 +6933,10 @@
         <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -6790,21 +6950,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>645</v>
+      </c>
+      <c r="D18" t="s">
         <v>646</v>
       </c>
-      <c r="D18" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -6818,9 +6978,9 @@
         <v>398</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -6829,10 +6989,10 @@
         <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>422</v>
       </c>
@@ -6843,10 +7003,10 @@
         <v>423</v>
       </c>
       <c r="D21" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -6860,21 +7020,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
+        <v>648</v>
+      </c>
+      <c r="D23" t="s">
         <v>649</v>
       </c>
-      <c r="D23" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -6885,10 +7045,10 @@
         <v>96</v>
       </c>
       <c r="D24" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -6902,7 +7062,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -6916,7 +7076,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>387</v>
       </c>
@@ -6930,7 +7090,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>400</v>
       </c>
@@ -6944,7 +7104,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>104</v>
       </c>
@@ -6958,7 +7118,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>403</v>
       </c>
@@ -6966,13 +7126,13 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D30" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -6983,10 +7143,10 @@
         <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -6997,10 +7157,10 @@
         <v>430</v>
       </c>
       <c r="D32" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -7011,10 +7171,10 @@
         <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -7029,7 +7189,7 @@
       </c>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -7040,10 +7200,10 @@
         <v>56</v>
       </c>
       <c r="D35" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>57</v>
       </c>
@@ -7054,10 +7214,10 @@
         <v>58</v>
       </c>
       <c r="D36" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -7065,13 +7225,13 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
+        <v>665</v>
+      </c>
+      <c r="D37" t="s">
         <v>666</v>
       </c>
-      <c r="D37" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>406</v>
       </c>
@@ -7079,13 +7239,13 @@
         <v>2</v>
       </c>
       <c r="C38" t="s">
+        <v>667</v>
+      </c>
+      <c r="D38" t="s">
         <v>668</v>
       </c>
-      <c r="D38" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>408</v>
       </c>
@@ -7099,7 +7259,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>59</v>
       </c>
@@ -7110,10 +7270,10 @@
         <v>60</v>
       </c>
       <c r="D40" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>61</v>
       </c>
@@ -7124,10 +7284,10 @@
         <v>427</v>
       </c>
       <c r="D41" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -7135,13 +7295,13 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
+        <v>675</v>
+      </c>
+      <c r="D42" t="s">
         <v>676</v>
       </c>
-      <c r="D42" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>410</v>
       </c>
@@ -7155,7 +7315,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -7166,10 +7326,10 @@
         <v>98</v>
       </c>
       <c r="D44" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>64</v>
       </c>
@@ -7180,10 +7340,10 @@
         <v>65</v>
       </c>
       <c r="D45" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>428</v>
       </c>
@@ -7197,7 +7357,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>68</v>
       </c>
@@ -7211,7 +7371,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -7225,7 +7385,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>414</v>
       </c>
@@ -7239,7 +7399,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>106</v>
       </c>
@@ -7253,7 +7413,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>30</v>
       </c>
@@ -7267,7 +7427,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>31</v>
       </c>
@@ -7281,7 +7441,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>32</v>
       </c>
@@ -7292,24 +7452,24 @@
         <v>33</v>
       </c>
       <c r="D53" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D54" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>416</v>
       </c>
@@ -7317,13 +7477,13 @@
         <v>2</v>
       </c>
       <c r="C55" t="s">
+        <v>670</v>
+      </c>
+      <c r="D55" t="s">
         <v>671</v>
       </c>
-      <c r="D55" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>74</v>
       </c>
@@ -7337,7 +7497,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>72</v>
       </c>
@@ -7348,10 +7508,10 @@
         <v>73</v>
       </c>
       <c r="D57" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>76</v>
       </c>
@@ -7359,13 +7519,13 @@
         <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D58" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>89</v>
       </c>
@@ -7373,13 +7533,13 @@
         <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D59" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -7390,10 +7550,10 @@
         <v>110</v>
       </c>
       <c r="D60" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>78</v>
       </c>
@@ -7401,13 +7561,13 @@
         <v>2</v>
       </c>
       <c r="C61" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D61" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>80</v>
       </c>
@@ -7421,7 +7581,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>88</v>
       </c>
@@ -7429,10 +7589,10 @@
         <v>3</v>
       </c>
       <c r="C63" t="s">
+        <v>677</v>
+      </c>
+      <c r="D63" t="s">
         <v>678</v>
-      </c>
-      <c r="D63" t="s">
-        <v>679</v>
       </c>
     </row>
   </sheetData>
@@ -7452,13 +7612,13 @@
       <selection activeCell="A62" sqref="A62:B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>12</v>
       </c>
@@ -7466,7 +7626,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>99</v>
       </c>
@@ -7474,7 +7634,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>17</v>
       </c>
@@ -7482,7 +7642,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
@@ -7490,7 +7650,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
@@ -7498,7 +7658,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>20</v>
       </c>
@@ -7506,7 +7666,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>81</v>
       </c>
@@ -7514,7 +7674,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>391</v>
       </c>
@@ -7522,7 +7682,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>102</v>
       </c>
@@ -7530,7 +7690,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>22</v>
       </c>
@@ -7538,7 +7698,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>87</v>
       </c>
@@ -7546,7 +7706,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>87</v>
       </c>
@@ -7554,7 +7714,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>39</v>
       </c>
@@ -7562,7 +7722,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>112</v>
       </c>
@@ -7570,7 +7730,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>23</v>
       </c>
@@ -7578,7 +7738,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>396</v>
       </c>
@@ -7586,7 +7746,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>41</v>
       </c>
@@ -7594,7 +7754,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>26</v>
       </c>
@@ -7602,13 +7762,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B19" s="9"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>43</v>
       </c>
@@ -7616,15 +7776,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>422</v>
       </c>
@@ -7632,7 +7792,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>28</v>
       </c>
@@ -7640,15 +7800,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
+        <v>647</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>648</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>82</v>
       </c>
@@ -7656,7 +7816,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>45</v>
       </c>
@@ -7664,7 +7824,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>47</v>
       </c>
@@ -7672,7 +7832,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>387</v>
       </c>
@@ -7680,7 +7840,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>400</v>
       </c>
@@ -7688,7 +7848,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>104</v>
       </c>
@@ -7696,7 +7856,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>403</v>
       </c>
@@ -7704,7 +7864,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>49</v>
       </c>
@@ -7712,7 +7872,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>84</v>
       </c>
@@ -7720,7 +7880,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>84</v>
       </c>
@@ -7728,7 +7888,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>53</v>
       </c>
@@ -7736,7 +7896,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>51</v>
       </c>
@@ -7744,7 +7904,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>55</v>
       </c>
@@ -7752,7 +7912,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>83</v>
       </c>
@@ -7760,7 +7920,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>83</v>
       </c>
@@ -7768,7 +7928,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>406</v>
       </c>
@@ -7776,7 +7936,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>408</v>
       </c>
@@ -7784,7 +7944,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>59</v>
       </c>
@@ -7792,7 +7952,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>61</v>
       </c>
@@ -7800,7 +7960,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>85</v>
       </c>
@@ -7808,7 +7968,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>85</v>
       </c>
@@ -7816,7 +7976,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>410</v>
       </c>
@@ -7824,7 +7984,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>86</v>
       </c>
@@ -7832,7 +7992,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>64</v>
       </c>
@@ -7840,7 +8000,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>428</v>
       </c>
@@ -7848,7 +8008,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>68</v>
       </c>
@@ -7856,7 +8016,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>70</v>
       </c>
@@ -7864,7 +8024,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
         <v>414</v>
       </c>
@@ -7872,7 +8032,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
         <v>106</v>
       </c>
@@ -7881,7 +8041,7 @@
       </c>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
         <v>30</v>
       </c>
@@ -7891,7 +8051,7 @@
       <c r="C54" s="6"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
         <v>31</v>
       </c>
@@ -7900,7 +8060,7 @@
       </c>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
         <v>32</v>
       </c>
@@ -7909,24 +8069,24 @@
       </c>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="B57" s="9" t="s">
         <v>660</v>
       </c>
-      <c r="B57" s="9" t="s">
-        <v>661</v>
-      </c>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
         <v>416</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
         <v>416</v>
       </c>
@@ -7934,7 +8094,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
         <v>74</v>
       </c>
@@ -7942,7 +8102,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
         <v>72</v>
       </c>
@@ -7950,7 +8110,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
         <v>76</v>
       </c>
@@ -7958,15 +8118,15 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
         <v>76</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
         <v>89</v>
       </c>
@@ -7974,7 +8134,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
         <v>34</v>
       </c>
@@ -7982,7 +8142,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
         <v>78</v>
       </c>
@@ -7990,7 +8150,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
         <v>80</v>
       </c>
@@ -7998,7 +8158,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Update MALED and inconsistency tracker
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD7C542-BBA6-BF45-BAD7-5D2EF4E5DB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B0490B-8633-9C44-8DDE-14B64C4DE0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1660" windowWidth="26240" windowHeight="13380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="1960" windowWidth="26240" windowHeight="13380" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="812">
   <si>
     <t>sid</t>
   </si>
@@ -2452,6 +2452,18 @@
   </si>
   <si>
     <t>Use EUPATH_0000165 for all and update replaces annottation where needed</t>
+  </si>
+  <si>
+    <t>by qPCR calculation (units /uL), by qPCR result (units CT value)</t>
+  </si>
+  <si>
+    <t>Have Danica check that we can drop one of the terms</t>
+  </si>
+  <si>
+    <t>shouldn't be a unit</t>
+  </si>
+  <si>
+    <t>Should be days</t>
   </si>
 </sst>
 </file>
@@ -3334,8 +3346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView topLeftCell="C60" workbookViewId="0">
+      <selection activeCell="C80" sqref="A80:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4739,8 +4751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5194,6 +5206,9 @@
       <c r="E26" t="s">
         <v>529</v>
       </c>
+      <c r="F26" s="4" t="s">
+        <v>808</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -5230,6 +5245,9 @@
       </c>
       <c r="E28" t="s">
         <v>675</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>809</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -5275,8 +5293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="F102" sqref="F102"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107:XFD108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7340,8 +7358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7558,6 +7576,9 @@
       <c r="C22" t="s">
         <v>622</v>
       </c>
+      <c r="E22" s="4" t="s">
+        <v>810</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -7653,6 +7674,9 @@
       </c>
       <c r="D32" t="s">
         <v>786</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>811</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -7685,8 +7709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
some inconsistency issue tracker updates
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12032E0-C3FA-A641-8277-7DEDBFAA3438}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF24A69B-59DE-384B-9535-5B9D78F0A0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="2500" windowWidth="26240" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="2500" windowWidth="26240" windowHeight="13380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1578" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="881">
   <si>
     <t>sid</t>
   </si>
@@ -2632,13 +2632,52 @@
   </si>
   <si>
     <t>Fixed</t>
+  </si>
+  <si>
+    <t>Fever at episode &gt;37.5 C</t>
+  </si>
+  <si>
+    <t>Persistent diarrheal episode (&gt;14 days)</t>
+  </si>
+  <si>
+    <t>Maximum loose stools at episode count</t>
+  </si>
+  <si>
+    <t>Severe anemia (hemoglobin &lt;5 mg/dL)</t>
+  </si>
+  <si>
+    <t>Persons enrolled in study count</t>
+  </si>
+  <si>
+    <t>Persons &lt;=18 years living in house</t>
+  </si>
+  <si>
+    <t>Eukaryota in stool</t>
+  </si>
+  <si>
+    <t>Eukaryota in urine</t>
+  </si>
+  <si>
+    <t>Schistosoma haematobium infection intensity, by microscopy</t>
+  </si>
+  <si>
+    <t>Use EUPATH_0033152, should be under Breastfeeding. Remove Breastfeeding summary category</t>
+  </si>
+  <si>
+    <t>Shouldn't exist anymore. All variables should be moved under Breastfeeding EUPATH_0011730 instead</t>
+  </si>
+  <si>
+    <t>Village observation details</t>
+  </si>
+  <si>
+    <t>remove unit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3506,11 +3545,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
@@ -3519,7 +3558,7 @@
     <col min="5" max="5" width="55.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3536,7 +3575,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -3556,7 +3595,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -3576,7 +3615,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3596,7 +3635,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -3616,7 +3655,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>122</v>
       </c>
@@ -3636,7 +3675,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -3656,7 +3695,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -3676,7 +3715,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>131</v>
       </c>
@@ -3696,7 +3735,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -3716,7 +3755,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -3736,7 +3775,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>139</v>
       </c>
@@ -3756,7 +3795,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -3776,7 +3815,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>144</v>
       </c>
@@ -3793,7 +3832,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>147</v>
       </c>
@@ -3810,7 +3849,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>149</v>
       </c>
@@ -3827,7 +3866,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>152</v>
       </c>
@@ -3844,7 +3883,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>154</v>
       </c>
@@ -3861,7 +3900,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>156</v>
       </c>
@@ -3878,7 +3917,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>158</v>
       </c>
@@ -3895,7 +3934,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>160</v>
       </c>
@@ -3912,7 +3951,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>162</v>
       </c>
@@ -3929,7 +3968,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>164</v>
       </c>
@@ -3946,7 +3985,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>166</v>
       </c>
@@ -3963,7 +4002,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>168</v>
       </c>
@@ -3980,7 +4019,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>170</v>
       </c>
@@ -3997,7 +4036,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>172</v>
       </c>
@@ -4014,7 +4053,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>174</v>
       </c>
@@ -4031,7 +4070,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>176</v>
       </c>
@@ -4048,7 +4087,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>178</v>
       </c>
@@ -4065,7 +4104,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>180</v>
       </c>
@@ -4082,7 +4121,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>182</v>
       </c>
@@ -4099,7 +4138,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>184</v>
       </c>
@@ -4116,7 +4155,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>186</v>
       </c>
@@ -4133,7 +4172,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>188</v>
       </c>
@@ -4150,7 +4189,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>190</v>
       </c>
@@ -4167,7 +4206,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>192</v>
       </c>
@@ -4184,7 +4223,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>194</v>
       </c>
@@ -4201,7 +4240,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>196</v>
       </c>
@@ -4218,7 +4257,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>198</v>
       </c>
@@ -4235,7 +4274,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>200</v>
       </c>
@@ -4252,7 +4291,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>202</v>
       </c>
@@ -4269,7 +4308,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>204</v>
       </c>
@@ -4286,7 +4325,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>206</v>
       </c>
@@ -4303,7 +4342,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>208</v>
       </c>
@@ -4320,7 +4359,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>210</v>
       </c>
@@ -4337,7 +4376,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>213</v>
       </c>
@@ -4354,7 +4393,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>216</v>
       </c>
@@ -4371,7 +4410,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>219</v>
       </c>
@@ -4388,7 +4427,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>222</v>
       </c>
@@ -4405,7 +4444,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>224</v>
       </c>
@@ -4422,7 +4461,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>226</v>
       </c>
@@ -4439,7 +4478,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>229</v>
       </c>
@@ -4456,7 +4495,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>486</v>
       </c>
@@ -4473,7 +4512,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>492</v>
       </c>
@@ -4490,7 +4529,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>231</v>
       </c>
@@ -4507,7 +4546,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>234</v>
       </c>
@@ -4524,7 +4563,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>237</v>
       </c>
@@ -4541,7 +4580,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>240</v>
       </c>
@@ -4558,7 +4597,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>242</v>
       </c>
@@ -4575,7 +4614,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>245</v>
       </c>
@@ -4592,7 +4631,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>248</v>
       </c>
@@ -4609,15 +4648,15 @@
         <v>498</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E63" s="6"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -4632,7 +4671,7 @@
       </c>
       <c r="E67"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>662</v>
       </c>
@@ -4649,7 +4688,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>664</v>
       </c>
@@ -4666,7 +4705,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>666</v>
       </c>
@@ -4683,7 +4722,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>669</v>
       </c>
@@ -4700,7 +4739,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>136</v>
       </c>
@@ -4717,7 +4756,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>180</v>
       </c>
@@ -4734,7 +4773,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>672</v>
       </c>
@@ -4751,7 +4790,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>216</v>
       </c>
@@ -4768,7 +4807,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>675</v>
       </c>
@@ -4785,7 +4824,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>678</v>
       </c>
@@ -4802,7 +4841,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>680</v>
       </c>
@@ -4819,7 +4858,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>683</v>
       </c>
@@ -4836,7 +4875,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>231</v>
       </c>
@@ -4850,7 +4889,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>685</v>
       </c>
@@ -4867,7 +4906,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>688</v>
       </c>
@@ -4881,7 +4920,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>610</v>
       </c>
@@ -4898,15 +4937,15 @@
         <v>775</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E84"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>814</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -4923,7 +4962,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>662</v>
       </c>
@@ -4940,7 +4979,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>136</v>
       </c>
@@ -4954,10 +4993,10 @@
         <v>138</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>141</v>
       </c>
@@ -4971,10 +5010,10 @@
         <v>817</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>180</v>
       </c>
@@ -4991,7 +5030,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>818</v>
       </c>
@@ -5004,8 +5043,11 @@
       <c r="D93" t="s">
         <v>820</v>
       </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="E93" s="2" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>821</v>
       </c>
@@ -5018,8 +5060,11 @@
       <c r="D94" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="E94" s="2" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>672</v>
       </c>
@@ -5036,7 +5081,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>216</v>
       </c>
@@ -5050,10 +5095,10 @@
         <v>218</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>823</v>
       </c>
@@ -5066,8 +5111,11 @@
       <c r="D97" t="s">
         <v>825</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="E97" s="2" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>826</v>
       </c>
@@ -5080,8 +5128,11 @@
       <c r="D98" t="s">
         <v>825</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="E98" s="2" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>680</v>
       </c>
@@ -5098,7 +5149,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>683</v>
       </c>
@@ -5115,7 +5166,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>231</v>
       </c>
@@ -5129,10 +5180,10 @@
         <v>233</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>830</v>
       </c>
@@ -5145,8 +5196,11 @@
       <c r="D102" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="E102" s="2" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>234</v>
       </c>
@@ -5160,10 +5214,10 @@
         <v>236</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>834</v>
       </c>
@@ -5176,8 +5230,11 @@
       <c r="D104" t="s">
         <v>836</v>
       </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="E104" s="2" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>685</v>
       </c>
@@ -5194,7 +5251,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>837</v>
       </c>
@@ -5206,6 +5263,9 @@
       </c>
       <c r="D106" t="s">
         <v>592</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>873</v>
       </c>
     </row>
   </sheetData>
@@ -5218,11 +5278,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45.1640625" customWidth="1"/>
     <col min="3" max="3" width="42.83203125" customWidth="1"/>
@@ -5231,7 +5291,7 @@
     <col min="6" max="6" width="30.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5251,7 +5311,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>340</v>
       </c>
@@ -5271,7 +5331,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>343</v>
       </c>
@@ -5291,7 +5351,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>346</v>
       </c>
@@ -5311,7 +5371,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>349</v>
       </c>
@@ -5331,7 +5391,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>351</v>
       </c>
@@ -5351,7 +5411,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>353</v>
       </c>
@@ -5371,7 +5431,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>355</v>
       </c>
@@ -5391,7 +5451,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>358</v>
       </c>
@@ -5411,7 +5471,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>361</v>
       </c>
@@ -5431,7 +5491,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>364</v>
       </c>
@@ -5451,7 +5511,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>366</v>
       </c>
@@ -5471,7 +5531,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>369</v>
       </c>
@@ -5491,7 +5551,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>371</v>
       </c>
@@ -5511,7 +5571,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>334</v>
       </c>
@@ -5531,7 +5591,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>378</v>
       </c>
@@ -5551,18 +5611,18 @@
         <v>528</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -5580,7 +5640,7 @@
       </c>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>643</v>
       </c>
@@ -5600,7 +5660,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>646</v>
       </c>
@@ -5617,7 +5677,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>649</v>
       </c>
@@ -5637,7 +5697,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>652</v>
       </c>
@@ -5657,7 +5717,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>481</v>
       </c>
@@ -5677,7 +5737,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>656</v>
       </c>
@@ -5697,7 +5757,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>658</v>
       </c>
@@ -5717,19 +5777,19 @@
         <v>784</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>814</v>
       </c>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -5749,7 +5809,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>346</v>
       </c>
@@ -5766,10 +5826,10 @@
         <v>532</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>646</v>
       </c>
@@ -5786,7 +5846,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>840</v>
       </c>
@@ -5803,7 +5863,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>482</v>
       </c>
@@ -5820,7 +5880,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>481</v>
       </c>
@@ -5840,7 +5900,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>842</v>
       </c>
@@ -5857,7 +5917,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>844</v>
       </c>
@@ -5874,7 +5934,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>656</v>
       </c>
@@ -5894,7 +5954,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>658</v>
       </c>
@@ -5914,7 +5974,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>378</v>
       </c>
@@ -5944,11 +6004,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F138"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="F117" sqref="F117"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="F137" sqref="F137"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="34.5" customWidth="1"/>
@@ -5957,7 +6017,7 @@
     <col min="6" max="6" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5977,7 +6037,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>251</v>
       </c>
@@ -5997,7 +6057,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>255</v>
       </c>
@@ -6017,7 +6077,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>259</v>
       </c>
@@ -6037,7 +6097,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>263</v>
       </c>
@@ -6057,7 +6117,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>267</v>
       </c>
@@ -6077,7 +6137,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>270</v>
       </c>
@@ -6097,7 +6157,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>272</v>
       </c>
@@ -6117,7 +6177,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>276</v>
       </c>
@@ -6137,7 +6197,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>279</v>
       </c>
@@ -6157,7 +6217,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>282</v>
       </c>
@@ -6177,7 +6237,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>285</v>
       </c>
@@ -6197,7 +6257,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>289</v>
       </c>
@@ -6217,7 +6277,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>292</v>
       </c>
@@ -6237,7 +6297,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>296</v>
       </c>
@@ -6257,7 +6317,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>248</v>
       </c>
@@ -6277,7 +6337,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>301</v>
       </c>
@@ -6297,7 +6357,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>304</v>
       </c>
@@ -6317,7 +6377,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>308</v>
       </c>
@@ -6337,7 +6397,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>310</v>
       </c>
@@ -6357,7 +6417,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>224</v>
       </c>
@@ -6377,7 +6437,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>222</v>
       </c>
@@ -6397,7 +6457,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>316</v>
       </c>
@@ -6417,7 +6477,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>318</v>
       </c>
@@ -6437,7 +6497,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>321</v>
       </c>
@@ -6457,7 +6517,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>324</v>
       </c>
@@ -6477,7 +6537,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>122</v>
       </c>
@@ -6497,7 +6557,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>330</v>
       </c>
@@ -6517,7 +6577,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>333</v>
       </c>
@@ -6537,7 +6597,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>337</v>
       </c>
@@ -6557,12 +6617,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -6579,7 +6639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>251</v>
       </c>
@@ -6599,7 +6659,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>530</v>
       </c>
@@ -6619,7 +6679,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>255</v>
       </c>
@@ -6639,7 +6699,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>535</v>
       </c>
@@ -6659,7 +6719,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>259</v>
       </c>
@@ -6679,7 +6739,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>538</v>
       </c>
@@ -6699,7 +6759,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>542</v>
       </c>
@@ -6719,7 +6779,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>545</v>
       </c>
@@ -6739,7 +6799,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>263</v>
       </c>
@@ -6759,7 +6819,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>267</v>
       </c>
@@ -6779,7 +6839,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>270</v>
       </c>
@@ -6799,7 +6859,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>549</v>
       </c>
@@ -6819,7 +6879,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>272</v>
       </c>
@@ -6839,7 +6899,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>276</v>
       </c>
@@ -6859,7 +6919,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>279</v>
       </c>
@@ -6879,7 +6939,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>554</v>
       </c>
@@ -6899,7 +6959,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>285</v>
       </c>
@@ -6919,7 +6979,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>289</v>
       </c>
@@ -6939,7 +6999,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>559</v>
       </c>
@@ -6959,7 +7019,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>292</v>
       </c>
@@ -6979,7 +7039,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>562</v>
       </c>
@@ -6999,7 +7059,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>296</v>
       </c>
@@ -7019,7 +7079,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>248</v>
       </c>
@@ -7036,7 +7096,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>301</v>
       </c>
@@ -7056,7 +7116,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>304</v>
       </c>
@@ -7076,7 +7136,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>308</v>
       </c>
@@ -7096,7 +7156,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>310</v>
       </c>
@@ -7116,7 +7176,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>316</v>
       </c>
@@ -7136,7 +7196,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>318</v>
       </c>
@@ -7153,7 +7213,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>568</v>
       </c>
@@ -7173,7 +7233,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>570</v>
       </c>
@@ -7193,7 +7253,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>574</v>
       </c>
@@ -7213,7 +7273,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>578</v>
       </c>
@@ -7233,7 +7293,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>581</v>
       </c>
@@ -7253,7 +7313,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>584</v>
       </c>
@@ -7273,7 +7333,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>321</v>
       </c>
@@ -7293,7 +7353,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>324</v>
       </c>
@@ -7313,7 +7373,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>590</v>
       </c>
@@ -7333,7 +7393,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>122</v>
       </c>
@@ -7353,7 +7413,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>593</v>
       </c>
@@ -7373,7 +7433,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>597</v>
       </c>
@@ -7393,7 +7453,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>599</v>
       </c>
@@ -7413,7 +7473,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>601</v>
       </c>
@@ -7433,7 +7493,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>330</v>
       </c>
@@ -7453,7 +7513,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>604</v>
       </c>
@@ -7470,7 +7530,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>513</v>
       </c>
@@ -7490,7 +7550,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>337</v>
       </c>
@@ -7510,12 +7570,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -7533,7 +7593,7 @@
       </c>
       <c r="F89"/>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>255</v>
       </c>
@@ -7553,7 +7613,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>692</v>
       </c>
@@ -7573,7 +7633,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>672</v>
       </c>
@@ -7593,7 +7653,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>697</v>
       </c>
@@ -7613,7 +7673,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>701</v>
       </c>
@@ -7633,7 +7693,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>705</v>
       </c>
@@ -7653,7 +7713,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>272</v>
       </c>
@@ -7673,7 +7733,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>708</v>
       </c>
@@ -7693,7 +7753,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>711</v>
       </c>
@@ -7713,7 +7773,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>554</v>
       </c>
@@ -7733,7 +7793,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>714</v>
       </c>
@@ -7753,7 +7813,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>289</v>
       </c>
@@ -7773,7 +7833,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>719</v>
       </c>
@@ -7793,7 +7853,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>562</v>
       </c>
@@ -7810,7 +7870,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>722</v>
       </c>
@@ -7830,7 +7890,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>688</v>
       </c>
@@ -7847,7 +7907,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>728</v>
       </c>
@@ -7867,7 +7927,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>570</v>
       </c>
@@ -7884,7 +7944,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>581</v>
       </c>
@@ -7901,7 +7961,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>732</v>
       </c>
@@ -7921,7 +7981,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>324</v>
       </c>
@@ -7941,7 +8001,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>736</v>
       </c>
@@ -7961,7 +8021,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>740</v>
       </c>
@@ -7978,7 +8038,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>742</v>
       </c>
@@ -7998,12 +8058,12 @@
         <v>252</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>814</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -8023,7 +8083,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>787</v>
       </c>
@@ -8039,8 +8099,11 @@
       <c r="E118" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="119" spans="1:6">
+      <c r="F118" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>736</v>
       </c>
@@ -8060,7 +8123,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>672</v>
       </c>
@@ -8076,8 +8139,11 @@
       <c r="E120" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="121" spans="1:6">
+      <c r="F120" s="2" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>697</v>
       </c>
@@ -8097,7 +8163,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>272</v>
       </c>
@@ -8117,7 +8183,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>791</v>
       </c>
@@ -8133,8 +8199,11 @@
       <c r="E123" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="124" spans="1:6">
+      <c r="F123" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>794</v>
       </c>
@@ -8150,8 +8219,11 @@
       <c r="E124" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="125" spans="1:6">
+      <c r="F124" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>742</v>
       </c>
@@ -8171,7 +8243,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>711</v>
       </c>
@@ -8191,7 +8263,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>797</v>
       </c>
@@ -8207,8 +8279,11 @@
       <c r="E127" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="128" spans="1:6">
+      <c r="F127" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>719</v>
       </c>
@@ -8228,7 +8303,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>562</v>
       </c>
@@ -8248,7 +8323,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>800</v>
       </c>
@@ -8264,8 +8339,11 @@
       <c r="E130" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="131" spans="1:6">
+      <c r="F130" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>802</v>
       </c>
@@ -8281,8 +8359,11 @@
       <c r="E131" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="132" spans="1:6">
+      <c r="F131" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>324</v>
       </c>
@@ -8302,7 +8383,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>805</v>
       </c>
@@ -8318,8 +8399,11 @@
       <c r="E133" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="134" spans="1:6">
+      <c r="F133" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>590</v>
       </c>
@@ -8339,7 +8423,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>807</v>
       </c>
@@ -8355,8 +8439,11 @@
       <c r="E135" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="136" spans="1:6">
+      <c r="F135" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>809</v>
       </c>
@@ -8372,8 +8459,11 @@
       <c r="E136" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="137" spans="1:6">
+      <c r="F136" s="2" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>812</v>
       </c>
@@ -8389,8 +8479,11 @@
       <c r="E137" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="138" spans="1:6">
+      <c r="F137" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F138"/>
     </row>
   </sheetData>
@@ -8405,10 +8498,10 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="42.83203125" customWidth="1"/>
@@ -8417,7 +8510,7 @@
     <col min="5" max="5" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -8434,7 +8527,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -8451,7 +8544,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -8468,7 +8561,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -8479,7 +8572,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -8490,7 +8583,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -8501,7 +8594,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -8512,7 +8605,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -8526,7 +8619,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -8537,7 +8630,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -8548,7 +8641,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -8565,7 +8658,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -8576,7 +8669,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>87</v>
       </c>
@@ -8593,15 +8686,15 @@
         <v>525</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D18" s="5"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>746</v>
       </c>
@@ -8612,7 +8705,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>613</v>
       </c>
@@ -8626,7 +8719,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>751</v>
       </c>
@@ -8637,7 +8730,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>748</v>
       </c>
@@ -8649,10 +8742,10 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -8669,7 +8762,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -8686,7 +8779,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -8700,7 +8793,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>621</v>
       </c>
@@ -8714,10 +8807,10 @@
         <v>762</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>334</v>
       </c>
@@ -8737,17 +8830,17 @@
         <v>867</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" s="3"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>866</v>
       </c>
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>751</v>
       </c>
@@ -8757,12 +8850,15 @@
       <c r="C36" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="E36" s="2" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
     </row>
@@ -8776,11 +8872,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" customWidth="1"/>
@@ -8790,7 +8886,7 @@
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -8805,7 +8901,7 @@
       </c>
       <c r="E1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>746</v>
       </c>
@@ -8820,7 +8916,7 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>747</v>
       </c>
@@ -8835,7 +8931,7 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -8850,7 +8946,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -8865,7 +8961,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -8880,7 +8976,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -8895,7 +8991,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -8910,7 +9006,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>616</v>
       </c>
@@ -8925,7 +9021,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>384</v>
       </c>
@@ -8940,7 +9036,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -8955,7 +9051,7 @@
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -8970,7 +9066,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -8985,7 +9081,7 @@
       </c>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>750</v>
       </c>
@@ -9000,7 +9096,7 @@
       </c>
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -9015,7 +9111,7 @@
       </c>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -9030,7 +9126,7 @@
       </c>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -9045,7 +9141,7 @@
       </c>
       <c r="E17"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -9060,7 +9156,7 @@
       </c>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>861</v>
       </c>
@@ -9075,7 +9171,7 @@
       </c>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>853</v>
       </c>
@@ -9090,7 +9186,7 @@
       </c>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>390</v>
       </c>
@@ -9105,7 +9201,7 @@
       </c>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -9120,7 +9216,7 @@
       </c>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -9135,7 +9231,7 @@
       </c>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -9150,7 +9246,7 @@
       </c>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -9165,7 +9261,7 @@
       </c>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -9180,7 +9276,7 @@
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>393</v>
       </c>
@@ -9195,7 +9291,7 @@
       </c>
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -9210,7 +9306,7 @@
       </c>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -9225,7 +9321,7 @@
       </c>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -9240,7 +9336,7 @@
       </c>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -9255,7 +9351,7 @@
       </c>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -9270,7 +9366,7 @@
       </c>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -9285,7 +9381,7 @@
       </c>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>399</v>
       </c>
@@ -9300,7 +9396,7 @@
       </c>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>401</v>
       </c>
@@ -9315,7 +9411,7 @@
       </c>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -9330,7 +9426,7 @@
       </c>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>403</v>
       </c>
@@ -9345,7 +9441,7 @@
       </c>
       <c r="E37"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -9360,7 +9456,7 @@
       </c>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -9375,7 +9471,7 @@
       </c>
       <c r="E39"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>751</v>
       </c>
@@ -9390,7 +9486,7 @@
       </c>
       <c r="E40"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>67</v>
       </c>
@@ -9405,7 +9501,7 @@
       </c>
       <c r="E41"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -9420,7 +9516,7 @@
       </c>
       <c r="E42"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>407</v>
       </c>
@@ -9435,7 +9531,7 @@
       </c>
       <c r="E43"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>104</v>
       </c>
@@ -9450,7 +9546,7 @@
       </c>
       <c r="E44"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>623</v>
       </c>
@@ -9465,7 +9561,7 @@
       </c>
       <c r="E45"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>409</v>
       </c>
@@ -9480,7 +9576,7 @@
       </c>
       <c r="E46"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>73</v>
       </c>
@@ -9495,7 +9591,7 @@
       </c>
       <c r="E47"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>75</v>
       </c>
@@ -9510,7 +9606,7 @@
       </c>
       <c r="E48"/>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>77</v>
       </c>
@@ -9525,7 +9621,7 @@
       </c>
       <c r="E49"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -9540,7 +9636,7 @@
       </c>
       <c r="E50"/>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>98</v>
       </c>
@@ -9555,7 +9651,7 @@
       </c>
       <c r="E51"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -9570,7 +9666,7 @@
       </c>
       <c r="E52"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>413</v>
       </c>
@@ -9585,7 +9681,7 @@
       </c>
       <c r="E53"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -9600,7 +9696,7 @@
       </c>
       <c r="E54"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>396</v>
       </c>
@@ -9615,7 +9711,7 @@
       </c>
       <c r="E55"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>83</v>
       </c>
@@ -9630,7 +9726,7 @@
       </c>
       <c r="E56"/>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -9645,7 +9741,7 @@
       </c>
       <c r="E57"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>71</v>
       </c>
@@ -9660,7 +9756,7 @@
       </c>
       <c r="E58"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>86</v>
       </c>
@@ -9675,7 +9771,7 @@
       </c>
       <c r="E59"/>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>84</v>
       </c>
@@ -9690,7 +9786,7 @@
       </c>
       <c r="E60"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>87</v>
       </c>
@@ -9705,7 +9801,7 @@
       </c>
       <c r="E61"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>88</v>
       </c>
@@ -9737,12 +9833,12 @@
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -9753,7 +9849,7 @@
       <c r="F1"/>
       <c r="I1"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -9761,7 +9857,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>746</v>
       </c>
@@ -9769,7 +9865,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>747</v>
       </c>
@@ -9777,7 +9873,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -9785,7 +9881,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -9793,7 +9889,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -9801,7 +9897,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -9809,7 +9905,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -9817,7 +9913,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -9825,7 +9921,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -9833,7 +9929,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -9841,7 +9937,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>861</v>
       </c>
@@ -9849,7 +9945,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>853</v>
       </c>
@@ -9857,7 +9953,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -9865,7 +9961,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>390</v>
       </c>
@@ -9873,7 +9969,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -9881,7 +9977,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -9889,7 +9985,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -9897,7 +9993,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>413</v>
       </c>
@@ -9905,7 +10001,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -9913,7 +10009,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>616</v>
       </c>
@@ -9921,7 +10017,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -9929,7 +10025,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -9937,7 +10033,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -9945,7 +10041,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>384</v>
       </c>
@@ -9953,7 +10049,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>393</v>
       </c>
@@ -9961,7 +10057,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -9969,7 +10065,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>396</v>
       </c>
@@ -9977,7 +10073,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -9985,7 +10081,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -9993,7 +10089,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -10001,7 +10097,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -10009,7 +10105,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -10017,7 +10113,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -10025,7 +10121,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>399</v>
       </c>
@@ -10033,7 +10129,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>401</v>
       </c>
@@ -10041,7 +10137,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -10049,7 +10145,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -10057,7 +10153,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -10065,7 +10161,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>403</v>
       </c>
@@ -10073,7 +10169,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -10081,7 +10177,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -10089,12 +10185,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>67</v>
       </c>
@@ -10102,7 +10198,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>69</v>
       </c>
@@ -10110,7 +10206,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>407</v>
       </c>
@@ -10118,7 +10214,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>104</v>
       </c>
@@ -10126,7 +10222,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>30</v>
       </c>
@@ -10134,7 +10230,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -10142,7 +10238,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>32</v>
       </c>
@@ -10150,7 +10246,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>623</v>
       </c>
@@ -10159,7 +10255,7 @@
       </c>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>409</v>
       </c>
@@ -10169,7 +10265,7 @@
       <c r="C53" s="4"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>73</v>
       </c>
@@ -10178,7 +10274,7 @@
       </c>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>71</v>
       </c>
@@ -10187,7 +10283,7 @@
       </c>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>75</v>
       </c>
@@ -10196,7 +10292,7 @@
       </c>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -10204,7 +10300,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>34</v>
       </c>
@@ -10212,7 +10308,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>77</v>
       </c>
@@ -10220,7 +10316,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>79</v>
       </c>
@@ -10228,7 +10324,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
update consistent checking results
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D539E4-FCDD-BB42-9951-3D998E6F2BD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E182A5-B64F-B14E-B313-3139E358CC2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="1260" windowWidth="22420" windowHeight="11480" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="340" yWindow="2620" windowWidth="22420" windowHeight="11480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="termWithDifferentLabels" sheetId="1" r:id="rId1"/>
+    <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
     <sheet name="LabelsUsedMultipleTerms" sheetId="2" r:id="rId2"/>
     <sheet name="termWithDifferentParent" sheetId="3" r:id="rId3"/>
     <sheet name="units_issues" sheetId="6" r:id="rId4"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="896">
   <si>
     <t>sid</t>
   </si>
@@ -2664,9 +2664,6 @@
     <t>Use IRI EUPATH_0030024 for this label</t>
   </si>
   <si>
-    <t>Checked on Aug 11th, all known issues are fixed</t>
-  </si>
-  <si>
     <t>icemr_india_gujarat | icemr_prism2_border_cohort | gates_gems1a | gates_gems | icemr_southAsia | icemr_southernAfrica | icemr_india_cx | gates_perch | icemr_malawi | general/general_promote | icemr_india_cohort | icemr_india_feverSurv | gates_sip | icemr_southeastAsia | icemr_prism2 | icemr_meghalaya | icemr_prism | gates_provide | icemr_amazoniaPeru | icemr_westAfrica | gates_maled | general/general_crompton</t>
   </si>
   <si>
@@ -2707,6 +2704,18 @@
   </si>
   <si>
     <t>Removed and no unit issues left.</t>
+  </si>
+  <si>
+    <t>Checked on Aug 19th, all known issues are fixed</t>
+  </si>
+  <si>
+    <t>Checked on Aug 19th, two remaining issues need to be addressed in the future.</t>
+  </si>
+  <si>
+    <t>Rotavirus IgA titer, by ELISA result</t>
+  </si>
+  <si>
+    <t>EUPATH_0036335|EUPATH_0011516|EUPATH_0036490</t>
   </si>
 </sst>
 </file>
@@ -3592,8 +3601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5282,20 +5291,11 @@
       </c>
     </row>
     <row r="107" spans="1:5">
-      <c r="D107" s="11" t="s">
-        <v>878</v>
+      <c r="A107" s="11" t="s">
+        <v>892</v>
       </c>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" t="s">
-        <v>0</v>
-      </c>
-      <c r="B108" t="s">
-        <v>1</v>
-      </c>
-      <c r="C108" t="s">
-        <v>2</v>
-      </c>
       <c r="E108"/>
     </row>
     <row r="109" spans="1:5">
@@ -5315,10 +5315,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6056,7 +6056,7 @@
         <v>2</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>9</v>
@@ -6065,7 +6065,7 @@
         <v>647</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1">
@@ -6076,7 +6076,7 @@
     </row>
     <row r="46" spans="1:6" s="3" customFormat="1">
       <c r="A46" s="10" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F46" s="6"/>
     </row>
@@ -6121,10 +6121,48 @@
       </c>
     </row>
     <row r="50" spans="1:6" s="3" customFormat="1">
+      <c r="A50" s="10" t="s">
+        <v>893</v>
+      </c>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="3"/>
+    <row r="51" spans="1:6" s="3" customFormat="1">
+      <c r="A51" s="3" t="s">
+        <v>837</v>
+      </c>
+      <c r="B51" s="3">
+        <v>2</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>838</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>894</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52" t="s">
+        <v>895</v>
+      </c>
+      <c r="D52" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" t="s">
+        <v>568</v>
+      </c>
+      <c r="F52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6137,7 +6175,7 @@
   <dimension ref="A1:F139"/>
   <sheetViews>
     <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="A139" sqref="A139"/>
+      <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8620,7 +8658,7 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" s="1" t="s">
-        <v>878</v>
+        <v>892</v>
       </c>
     </row>
   </sheetData>
@@ -8632,10 +8670,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8973,7 +9011,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B35" s="3"/>
     </row>
@@ -8993,13 +9031,18 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="7" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B38" s="7"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="11" t="s">
+        <v>892</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9078,7 +9121,7 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="E4"/>
     </row>
@@ -9093,7 +9136,7 @@
         <v>106</v>
       </c>
       <c r="D5" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="E5"/>
     </row>
@@ -9258,7 +9301,7 @@
         <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="E16"/>
     </row>
@@ -9273,7 +9316,7 @@
         <v>94</v>
       </c>
       <c r="D17" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="E17"/>
     </row>
@@ -9333,7 +9376,7 @@
         <v>391</v>
       </c>
       <c r="D21" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="E21"/>
     </row>
@@ -9378,7 +9421,7 @@
         <v>95</v>
       </c>
       <c r="D24" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="E24"/>
     </row>
@@ -9393,7 +9436,7 @@
         <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="E25"/>
     </row>
@@ -9888,7 +9931,7 @@
         <v>854</v>
       </c>
       <c r="D58" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E58"/>
     </row>
@@ -9903,7 +9946,7 @@
         <v>750</v>
       </c>
       <c r="D59" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="E59"/>
     </row>
@@ -9953,8 +9996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E96E553-B9B7-3A43-9A19-9B2DEFC1133B}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
fix inconsistent issues in provide study, refs #45330
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2806501-1FA9-DD43-B6D1-6CC29F6008E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80120A72-2BD1-FA43-ACD4-1200456794EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="2620" windowWidth="22420" windowHeight="11480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5960" yWindow="960" windowWidth="21820" windowHeight="11480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="899">
   <si>
     <t>sid</t>
   </si>
@@ -2722,13 +2722,16 @@
   </si>
   <si>
     <t>In PROVIDE, drop EUPATH_0036490. Leave EUPATH_0036335 since that's under a different parent sample type</t>
+  </si>
+  <si>
+    <t>Changed terms in Provide studies as usggested, no more issue found on Aug 20th.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3611,7 +3614,7 @@
       <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
@@ -3620,7 +3623,7 @@
     <col min="5" max="5" width="55.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3637,7 +3640,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -3657,7 +3660,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -3677,7 +3680,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3697,7 +3700,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -3717,7 +3720,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>122</v>
       </c>
@@ -3737,7 +3740,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -3757,7 +3760,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -3777,7 +3780,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>131</v>
       </c>
@@ -3797,7 +3800,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -3817,7 +3820,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -3837,7 +3840,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>139</v>
       </c>
@@ -3857,7 +3860,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -3877,7 +3880,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>144</v>
       </c>
@@ -3894,7 +3897,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>147</v>
       </c>
@@ -3911,7 +3914,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>149</v>
       </c>
@@ -3928,7 +3931,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>152</v>
       </c>
@@ -3945,7 +3948,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>154</v>
       </c>
@@ -3962,7 +3965,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>156</v>
       </c>
@@ -3979,7 +3982,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>158</v>
       </c>
@@ -3996,7 +3999,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>160</v>
       </c>
@@ -4013,7 +4016,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>162</v>
       </c>
@@ -4030,7 +4033,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>164</v>
       </c>
@@ -4047,7 +4050,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>166</v>
       </c>
@@ -4064,7 +4067,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>168</v>
       </c>
@@ -4081,7 +4084,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>170</v>
       </c>
@@ -4098,7 +4101,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>172</v>
       </c>
@@ -4115,7 +4118,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>174</v>
       </c>
@@ -4132,7 +4135,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>176</v>
       </c>
@@ -4149,7 +4152,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>178</v>
       </c>
@@ -4166,7 +4169,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>180</v>
       </c>
@@ -4183,7 +4186,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>182</v>
       </c>
@@ -4200,7 +4203,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>184</v>
       </c>
@@ -4217,7 +4220,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>186</v>
       </c>
@@ -4234,7 +4237,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>188</v>
       </c>
@@ -4251,7 +4254,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>190</v>
       </c>
@@ -4268,7 +4271,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>192</v>
       </c>
@@ -4285,7 +4288,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>194</v>
       </c>
@@ -4302,7 +4305,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>196</v>
       </c>
@@ -4319,7 +4322,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>198</v>
       </c>
@@ -4336,7 +4339,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>200</v>
       </c>
@@ -4353,7 +4356,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>202</v>
       </c>
@@ -4370,7 +4373,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>204</v>
       </c>
@@ -4387,7 +4390,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>206</v>
       </c>
@@ -4404,7 +4407,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>208</v>
       </c>
@@ -4421,7 +4424,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>210</v>
       </c>
@@ -4438,7 +4441,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>213</v>
       </c>
@@ -4455,7 +4458,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>216</v>
       </c>
@@ -4472,7 +4475,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>219</v>
       </c>
@@ -4489,7 +4492,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>222</v>
       </c>
@@ -4506,7 +4509,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>224</v>
       </c>
@@ -4523,7 +4526,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>226</v>
       </c>
@@ -4540,7 +4543,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>229</v>
       </c>
@@ -4557,7 +4560,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>485</v>
       </c>
@@ -4574,7 +4577,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>491</v>
       </c>
@@ -4591,7 +4594,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>231</v>
       </c>
@@ -4608,7 +4611,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>234</v>
       </c>
@@ -4625,7 +4628,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>237</v>
       </c>
@@ -4642,7 +4645,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>240</v>
       </c>
@@ -4659,7 +4662,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>242</v>
       </c>
@@ -4676,7 +4679,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>245</v>
       </c>
@@ -4693,7 +4696,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>248</v>
       </c>
@@ -4710,15 +4713,15 @@
         <v>497</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5">
       <c r="E63" s="6"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -4733,7 +4736,7 @@
       </c>
       <c r="E67"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>658</v>
       </c>
@@ -4750,7 +4753,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>660</v>
       </c>
@@ -4767,7 +4770,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>662</v>
       </c>
@@ -4784,7 +4787,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>665</v>
       </c>
@@ -4801,7 +4804,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>136</v>
       </c>
@@ -4818,7 +4821,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>180</v>
       </c>
@@ -4835,7 +4838,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>668</v>
       </c>
@@ -4852,7 +4855,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>216</v>
       </c>
@@ -4869,7 +4872,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>671</v>
       </c>
@@ -4886,7 +4889,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>674</v>
       </c>
@@ -4903,7 +4906,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>676</v>
       </c>
@@ -4920,7 +4923,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>679</v>
       </c>
@@ -4937,7 +4940,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>231</v>
       </c>
@@ -4951,7 +4954,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>681</v>
       </c>
@@ -4968,7 +4971,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>684</v>
       </c>
@@ -4982,7 +4985,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>609</v>
       </c>
@@ -4999,15 +5002,15 @@
         <v>771</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5">
       <c r="E84"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5">
       <c r="A86" s="1" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -5024,7 +5027,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>658</v>
       </c>
@@ -5041,7 +5044,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>141</v>
       </c>
@@ -5058,7 +5061,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>180</v>
       </c>
@@ -5075,7 +5078,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>813</v>
       </c>
@@ -5092,7 +5095,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>816</v>
       </c>
@@ -5109,7 +5112,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>216</v>
       </c>
@@ -5126,7 +5129,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>818</v>
       </c>
@@ -5143,7 +5146,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>821</v>
       </c>
@@ -5160,7 +5163,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>676</v>
       </c>
@@ -5177,7 +5180,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>679</v>
       </c>
@@ -5194,7 +5197,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>231</v>
       </c>
@@ -5211,7 +5214,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>825</v>
       </c>
@@ -5228,7 +5231,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>234</v>
       </c>
@@ -5245,7 +5248,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>829</v>
       </c>
@@ -5262,7 +5265,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>681</v>
       </c>
@@ -5279,7 +5282,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
         <v>832</v>
       </c>
@@ -5296,21 +5299,21 @@
         <v>861</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5">
       <c r="A107" s="11" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5">
       <c r="E108"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5">
       <c r="E109"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5">
       <c r="E110"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5">
       <c r="E111"/>
     </row>
   </sheetData>
@@ -5321,22 +5324,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="45.1640625" customWidth="1"/>
-    <col min="3" max="3" width="42.83203125" customWidth="1"/>
+    <col min="3" max="3" width="62.33203125" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="39.1640625" customWidth="1"/>
     <col min="6" max="6" width="30.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5356,7 +5359,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>340</v>
       </c>
@@ -5376,7 +5379,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>343</v>
       </c>
@@ -5396,7 +5399,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>346</v>
       </c>
@@ -5416,7 +5419,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>349</v>
       </c>
@@ -5436,7 +5439,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>351</v>
       </c>
@@ -5456,7 +5459,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>353</v>
       </c>
@@ -5476,7 +5479,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>355</v>
       </c>
@@ -5496,7 +5499,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>358</v>
       </c>
@@ -5516,7 +5519,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>361</v>
       </c>
@@ -5536,7 +5539,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>364</v>
       </c>
@@ -5556,7 +5559,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>366</v>
       </c>
@@ -5576,7 +5579,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>369</v>
       </c>
@@ -5596,7 +5599,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>371</v>
       </c>
@@ -5616,7 +5619,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>334</v>
       </c>
@@ -5636,7 +5639,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>378</v>
       </c>
@@ -5656,18 +5659,18 @@
         <v>527</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -5685,7 +5688,7 @@
       </c>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>639</v>
       </c>
@@ -5705,7 +5708,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>642</v>
       </c>
@@ -5722,7 +5725,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>645</v>
       </c>
@@ -5742,7 +5745,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>648</v>
       </c>
@@ -5762,7 +5765,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>480</v>
       </c>
@@ -5782,7 +5785,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>652</v>
       </c>
@@ -5802,7 +5805,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>654</v>
       </c>
@@ -5822,19 +5825,19 @@
         <v>780</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>868</v>
       </c>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -5854,7 +5857,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>346</v>
       </c>
@@ -5874,7 +5877,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" s="3" customFormat="1">
       <c r="A34" s="3" t="s">
         <v>642</v>
       </c>
@@ -5894,7 +5897,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" s="3" customFormat="1">
       <c r="A35" s="3" t="s">
         <v>835</v>
       </c>
@@ -5914,7 +5917,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" s="3" customFormat="1">
       <c r="A36" s="3" t="s">
         <v>481</v>
       </c>
@@ -5934,7 +5937,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" s="3" customFormat="1">
       <c r="A37" s="3" t="s">
         <v>480</v>
       </c>
@@ -5954,7 +5957,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" s="3" customFormat="1">
       <c r="A38" s="3" t="s">
         <v>837</v>
       </c>
@@ -5974,7 +5977,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" s="3" customFormat="1">
       <c r="A39" s="3" t="s">
         <v>839</v>
       </c>
@@ -5994,7 +5997,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" s="3" customFormat="1">
       <c r="A40" s="3" t="s">
         <v>652</v>
       </c>
@@ -6014,7 +6017,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" s="3" customFormat="1">
       <c r="A41" s="3" t="s">
         <v>654</v>
       </c>
@@ -6034,7 +6037,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" s="3" customFormat="1">
       <c r="A42" s="3" t="s">
         <v>378</v>
       </c>
@@ -6054,7 +6057,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" s="3" customFormat="1">
       <c r="A43" s="3" t="s">
         <v>645</v>
       </c>
@@ -6074,19 +6077,19 @@
         <v>889</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" s="3" customFormat="1">
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" s="3" customFormat="1">
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" s="3" customFormat="1">
       <c r="A46" s="10" t="s">
         <v>890</v>
       </c>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" s="3" customFormat="1">
       <c r="A47" s="3" t="s">
         <v>642</v>
       </c>
@@ -6106,7 +6109,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" s="3" customFormat="1">
       <c r="A48" s="3" t="s">
         <v>837</v>
       </c>
@@ -6126,13 +6129,13 @@
         <v>876</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" s="3" customFormat="1">
       <c r="A50" s="10" t="s">
         <v>893</v>
       </c>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" s="3" customFormat="1">
       <c r="A51" s="3" t="s">
         <v>837</v>
       </c>
@@ -6152,7 +6155,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>894</v>
       </c>
@@ -6170,6 +6173,11 @@
       </c>
       <c r="F52" s="6" t="s">
         <v>897</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>898</v>
       </c>
     </row>
   </sheetData>
@@ -6186,7 +6194,7 @@
       <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="34.5" customWidth="1"/>
@@ -6195,7 +6203,7 @@
     <col min="6" max="6" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6215,7 +6223,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>251</v>
       </c>
@@ -6235,7 +6243,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>255</v>
       </c>
@@ -6255,7 +6263,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>259</v>
       </c>
@@ -6275,7 +6283,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>263</v>
       </c>
@@ -6295,7 +6303,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>267</v>
       </c>
@@ -6315,7 +6323,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>270</v>
       </c>
@@ -6335,7 +6343,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>272</v>
       </c>
@@ -6355,7 +6363,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>276</v>
       </c>
@@ -6375,7 +6383,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>279</v>
       </c>
@@ -6395,7 +6403,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>282</v>
       </c>
@@ -6415,7 +6423,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>285</v>
       </c>
@@ -6435,7 +6443,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>289</v>
       </c>
@@ -6455,7 +6463,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>292</v>
       </c>
@@ -6475,7 +6483,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>296</v>
       </c>
@@ -6495,7 +6503,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>248</v>
       </c>
@@ -6515,7 +6523,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>301</v>
       </c>
@@ -6535,7 +6543,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>304</v>
       </c>
@@ -6555,7 +6563,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>308</v>
       </c>
@@ -6575,7 +6583,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>310</v>
       </c>
@@ -6595,7 +6603,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>224</v>
       </c>
@@ -6615,7 +6623,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>222</v>
       </c>
@@ -6635,7 +6643,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>316</v>
       </c>
@@ -6655,7 +6663,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>318</v>
       </c>
@@ -6675,7 +6683,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>321</v>
       </c>
@@ -6695,7 +6703,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>324</v>
       </c>
@@ -6715,7 +6723,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>122</v>
       </c>
@@ -6735,7 +6743,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>330</v>
       </c>
@@ -6755,7 +6763,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>333</v>
       </c>
@@ -6775,7 +6783,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>337</v>
       </c>
@@ -6795,12 +6803,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -6817,7 +6825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>251</v>
       </c>
@@ -6837,7 +6845,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>529</v>
       </c>
@@ -6857,7 +6865,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>255</v>
       </c>
@@ -6877,7 +6885,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>534</v>
       </c>
@@ -6897,7 +6905,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>259</v>
       </c>
@@ -6917,7 +6925,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>537</v>
       </c>
@@ -6937,7 +6945,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>541</v>
       </c>
@@ -6957,7 +6965,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>544</v>
       </c>
@@ -6977,7 +6985,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>263</v>
       </c>
@@ -6997,7 +7005,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>267</v>
       </c>
@@ -7017,7 +7025,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>270</v>
       </c>
@@ -7037,7 +7045,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>548</v>
       </c>
@@ -7057,7 +7065,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>272</v>
       </c>
@@ -7077,7 +7085,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>276</v>
       </c>
@@ -7097,7 +7105,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>279</v>
       </c>
@@ -7117,7 +7125,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>553</v>
       </c>
@@ -7137,7 +7145,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>285</v>
       </c>
@@ -7157,7 +7165,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>289</v>
       </c>
@@ -7177,7 +7185,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>558</v>
       </c>
@@ -7197,7 +7205,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>292</v>
       </c>
@@ -7217,7 +7225,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>561</v>
       </c>
@@ -7237,7 +7245,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>296</v>
       </c>
@@ -7257,7 +7265,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>248</v>
       </c>
@@ -7274,7 +7282,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>301</v>
       </c>
@@ -7294,7 +7302,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>304</v>
       </c>
@@ -7314,7 +7322,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>308</v>
       </c>
@@ -7334,7 +7342,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>310</v>
       </c>
@@ -7354,7 +7362,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>316</v>
       </c>
@@ -7374,7 +7382,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>318</v>
       </c>
@@ -7391,7 +7399,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>567</v>
       </c>
@@ -7411,7 +7419,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>569</v>
       </c>
@@ -7431,7 +7439,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>573</v>
       </c>
@@ -7451,7 +7459,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>577</v>
       </c>
@@ -7471,7 +7479,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>580</v>
       </c>
@@ -7491,7 +7499,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>583</v>
       </c>
@@ -7511,7 +7519,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>321</v>
       </c>
@@ -7531,7 +7539,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>324</v>
       </c>
@@ -7551,7 +7559,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>589</v>
       </c>
@@ -7571,7 +7579,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>122</v>
       </c>
@@ -7591,7 +7599,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>592</v>
       </c>
@@ -7611,7 +7619,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>596</v>
       </c>
@@ -7631,7 +7639,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>598</v>
       </c>
@@ -7651,7 +7659,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>600</v>
       </c>
@@ -7671,7 +7679,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>330</v>
       </c>
@@ -7691,7 +7699,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>603</v>
       </c>
@@ -7708,7 +7716,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>512</v>
       </c>
@@ -7728,7 +7736,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>337</v>
       </c>
@@ -7748,12 +7756,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6">
       <c r="A87" s="1" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -7771,7 +7779,7 @@
       </c>
       <c r="F89"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>255</v>
       </c>
@@ -7791,7 +7799,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>688</v>
       </c>
@@ -7811,7 +7819,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>668</v>
       </c>
@@ -7831,7 +7839,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
         <v>693</v>
       </c>
@@ -7851,7 +7859,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>697</v>
       </c>
@@ -7871,7 +7879,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>701</v>
       </c>
@@ -7891,7 +7899,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>272</v>
       </c>
@@ -7911,7 +7919,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>704</v>
       </c>
@@ -7931,7 +7939,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6">
       <c r="A98" t="s">
         <v>707</v>
       </c>
@@ -7951,7 +7959,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6">
       <c r="A99" t="s">
         <v>553</v>
       </c>
@@ -7971,7 +7979,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
         <v>710</v>
       </c>
@@ -7991,7 +7999,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6">
       <c r="A101" t="s">
         <v>289</v>
       </c>
@@ -8011,7 +8019,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6">
       <c r="A102" t="s">
         <v>715</v>
       </c>
@@ -8031,7 +8039,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6">
       <c r="A103" t="s">
         <v>561</v>
       </c>
@@ -8048,7 +8056,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
         <v>718</v>
       </c>
@@ -8068,7 +8076,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
         <v>684</v>
       </c>
@@ -8085,7 +8093,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
         <v>724</v>
       </c>
@@ -8105,7 +8113,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
         <v>569</v>
       </c>
@@ -8122,7 +8130,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6">
       <c r="A108" t="s">
         <v>580</v>
       </c>
@@ -8139,7 +8147,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6">
       <c r="A109" t="s">
         <v>728</v>
       </c>
@@ -8159,7 +8167,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6">
       <c r="A110" t="s">
         <v>324</v>
       </c>
@@ -8179,7 +8187,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6">
       <c r="A111" t="s">
         <v>732</v>
       </c>
@@ -8199,7 +8207,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6">
       <c r="A112" t="s">
         <v>736</v>
       </c>
@@ -8216,7 +8224,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6">
       <c r="A113" t="s">
         <v>738</v>
       </c>
@@ -8236,12 +8244,12 @@
         <v>252</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6">
       <c r="A116" s="1" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -8261,7 +8269,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6">
       <c r="A118" t="s">
         <v>783</v>
       </c>
@@ -8281,7 +8289,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6">
       <c r="A119" t="s">
         <v>732</v>
       </c>
@@ -8301,7 +8309,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
         <v>693</v>
       </c>
@@ -8321,7 +8329,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
         <v>272</v>
       </c>
@@ -8341,7 +8349,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
         <v>787</v>
       </c>
@@ -8361,7 +8369,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6">
       <c r="A123" t="s">
         <v>790</v>
       </c>
@@ -8381,7 +8389,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6">
       <c r="A124" t="s">
         <v>738</v>
       </c>
@@ -8401,7 +8409,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6">
       <c r="A125" t="s">
         <v>869</v>
       </c>
@@ -8421,7 +8429,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6">
       <c r="A126" t="s">
         <v>707</v>
       </c>
@@ -8441,7 +8449,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6">
       <c r="A127" t="s">
         <v>793</v>
       </c>
@@ -8461,7 +8469,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6">
       <c r="A128" t="s">
         <v>715</v>
       </c>
@@ -8481,7 +8489,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6">
       <c r="A129" t="s">
         <v>561</v>
       </c>
@@ -8501,7 +8509,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6">
       <c r="A130" t="s">
         <v>796</v>
       </c>
@@ -8521,7 +8529,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6">
       <c r="A131" t="s">
         <v>798</v>
       </c>
@@ -8541,7 +8549,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6">
       <c r="A132" t="s">
         <v>324</v>
       </c>
@@ -8561,7 +8569,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6">
       <c r="A133" t="s">
         <v>801</v>
       </c>
@@ -8581,7 +8589,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
         <v>589</v>
       </c>
@@ -8601,7 +8609,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6">
       <c r="A135" t="s">
         <v>803</v>
       </c>
@@ -8621,7 +8629,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6">
       <c r="A136" t="s">
         <v>805</v>
       </c>
@@ -8641,7 +8649,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6">
       <c r="A137" t="s">
         <v>808</v>
       </c>
@@ -8661,10 +8669,10 @@
         <v>637</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6">
       <c r="F138"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6">
       <c r="A139" s="1" t="s">
         <v>892</v>
       </c>
@@ -8684,7 +8692,7 @@
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="42.83203125" customWidth="1"/>
@@ -8693,7 +8701,7 @@
     <col min="5" max="5" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -8710,7 +8718,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -8727,7 +8735,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -8744,7 +8752,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -8755,7 +8763,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -8766,7 +8774,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -8777,7 +8785,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -8788,7 +8796,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -8802,7 +8810,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -8813,7 +8821,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -8824,7 +8832,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -8841,7 +8849,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -8852,7 +8860,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>87</v>
       </c>
@@ -8869,15 +8877,15 @@
         <v>524</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="D18" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>742</v>
       </c>
@@ -8888,7 +8896,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="7" t="s">
         <v>612</v>
       </c>
@@ -8902,7 +8910,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>747</v>
       </c>
@@ -8913,7 +8921,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>744</v>
       </c>
@@ -8925,10 +8933,10 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -8945,7 +8953,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -8962,7 +8970,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -8976,7 +8984,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>617</v>
       </c>
@@ -8990,10 +8998,10 @@
         <v>758</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>334</v>
       </c>
@@ -9013,17 +9021,17 @@
         <v>855</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" s="7"/>
       <c r="B33" s="3"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
         <v>887</v>
       </c>
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>747</v>
       </c>
@@ -9037,17 +9045,17 @@
         <v>867</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" s="7" t="s">
         <v>891</v>
       </c>
       <c r="B38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
         <v>892</v>
       </c>
@@ -9066,14 +9074,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="52.33203125" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="2"/>
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -9088,7 +9096,7 @@
       </c>
       <c r="E1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>742</v>
       </c>
@@ -9103,7 +9111,7 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>743</v>
       </c>
@@ -9118,7 +9126,7 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -9133,7 +9141,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -9148,7 +9156,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -9163,7 +9171,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -9178,7 +9186,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -9193,7 +9201,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>614</v>
       </c>
@@ -9208,7 +9216,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>384</v>
       </c>
@@ -9223,7 +9231,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -9238,7 +9246,7 @@
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -9253,7 +9261,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -9268,7 +9276,7 @@
       </c>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>746</v>
       </c>
@@ -9283,7 +9291,7 @@
       </c>
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -9298,7 +9306,7 @@
       </c>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -9313,7 +9321,7 @@
       </c>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -9328,7 +9336,7 @@
       </c>
       <c r="E17"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -9343,7 +9351,7 @@
       </c>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>852</v>
       </c>
@@ -9358,7 +9366,7 @@
       </c>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>846</v>
       </c>
@@ -9373,7 +9381,7 @@
       </c>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>390</v>
       </c>
@@ -9388,7 +9396,7 @@
       </c>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -9403,7 +9411,7 @@
       </c>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -9418,7 +9426,7 @@
       </c>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -9433,7 +9441,7 @@
       </c>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -9448,7 +9456,7 @@
       </c>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -9463,7 +9471,7 @@
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>392</v>
       </c>
@@ -9478,7 +9486,7 @@
       </c>
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -9493,7 +9501,7 @@
       </c>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -9508,7 +9516,7 @@
       </c>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -9523,7 +9531,7 @@
       </c>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -9538,7 +9546,7 @@
       </c>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -9553,7 +9561,7 @@
       </c>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -9568,7 +9576,7 @@
       </c>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>398</v>
       </c>
@@ -9583,7 +9591,7 @@
       </c>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>400</v>
       </c>
@@ -9598,7 +9606,7 @@
       </c>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -9613,7 +9621,7 @@
       </c>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>402</v>
       </c>
@@ -9628,7 +9636,7 @@
       </c>
       <c r="E37"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -9643,7 +9651,7 @@
       </c>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -9658,7 +9666,7 @@
       </c>
       <c r="E39"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -9673,7 +9681,7 @@
       </c>
       <c r="E40"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -9688,7 +9696,7 @@
       </c>
       <c r="E41"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>406</v>
       </c>
@@ -9703,7 +9711,7 @@
       </c>
       <c r="E42"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -9718,7 +9726,7 @@
       </c>
       <c r="E43"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>619</v>
       </c>
@@ -9733,7 +9741,7 @@
       </c>
       <c r="E44"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>408</v>
       </c>
@@ -9748,7 +9756,7 @@
       </c>
       <c r="E45"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>73</v>
       </c>
@@ -9763,7 +9771,7 @@
       </c>
       <c r="E46"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>75</v>
       </c>
@@ -9778,7 +9786,7 @@
       </c>
       <c r="E47"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>77</v>
       </c>
@@ -9793,7 +9801,7 @@
       </c>
       <c r="E48"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>79</v>
       </c>
@@ -9808,7 +9816,7 @@
       </c>
       <c r="E49"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -9823,7 +9831,7 @@
       </c>
       <c r="E50"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -9838,7 +9846,7 @@
       </c>
       <c r="E51"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>412</v>
       </c>
@@ -9853,7 +9861,7 @@
       </c>
       <c r="E52"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -9868,7 +9876,7 @@
       </c>
       <c r="E53"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>395</v>
       </c>
@@ -9883,7 +9891,7 @@
       </c>
       <c r="E54"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>83</v>
       </c>
@@ -9898,7 +9906,7 @@
       </c>
       <c r="E55"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -9913,7 +9921,7 @@
       </c>
       <c r="E56"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>71</v>
       </c>
@@ -9928,7 +9936,7 @@
       </c>
       <c r="E57"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>86</v>
       </c>
@@ -9943,7 +9951,7 @@
       </c>
       <c r="E58"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>84</v>
       </c>
@@ -9958,7 +9966,7 @@
       </c>
       <c r="E59"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>87</v>
       </c>
@@ -9973,7 +9981,7 @@
       </c>
       <c r="E60"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -9988,7 +9996,7 @@
       </c>
       <c r="E61"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="E62"/>
     </row>
   </sheetData>
@@ -10008,12 +10016,12 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -10021,7 +10029,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -10029,7 +10037,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>742</v>
       </c>
@@ -10037,7 +10045,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>743</v>
       </c>
@@ -10045,7 +10053,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -10053,7 +10061,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -10061,7 +10069,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -10069,7 +10077,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -10077,7 +10085,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -10085,7 +10093,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -10093,7 +10101,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -10101,7 +10109,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -10109,7 +10117,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>852</v>
       </c>
@@ -10117,7 +10125,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>846</v>
       </c>
@@ -10125,7 +10133,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -10133,7 +10141,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>390</v>
       </c>
@@ -10141,7 +10149,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -10149,7 +10157,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -10157,7 +10165,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -10165,7 +10173,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>412</v>
       </c>
@@ -10173,7 +10181,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -10181,7 +10189,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>614</v>
       </c>
@@ -10189,7 +10197,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -10197,7 +10205,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -10205,7 +10213,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -10213,7 +10221,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>384</v>
       </c>
@@ -10221,7 +10229,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>392</v>
       </c>
@@ -10229,7 +10237,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -10237,7 +10245,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>395</v>
       </c>
@@ -10245,7 +10253,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -10253,7 +10261,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -10261,7 +10269,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -10269,7 +10277,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -10277,7 +10285,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -10285,7 +10293,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -10293,7 +10301,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>398</v>
       </c>
@@ -10301,7 +10309,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>400</v>
       </c>
@@ -10309,7 +10317,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -10317,7 +10325,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -10325,7 +10333,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -10333,7 +10341,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>402</v>
       </c>
@@ -10341,7 +10349,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -10349,7 +10357,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -10357,7 +10365,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -10365,7 +10373,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -10373,7 +10381,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>406</v>
       </c>
@@ -10381,7 +10389,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>104</v>
       </c>
@@ -10389,7 +10397,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>30</v>
       </c>
@@ -10397,7 +10405,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -10405,7 +10413,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>32</v>
       </c>
@@ -10413,7 +10421,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>619</v>
       </c>
@@ -10421,7 +10429,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>408</v>
       </c>
@@ -10430,7 +10438,7 @@
       </c>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>73</v>
       </c>
@@ -10440,7 +10448,7 @@
       <c r="C53" s="4"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -10449,7 +10457,7 @@
       </c>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>75</v>
       </c>
@@ -10458,7 +10466,7 @@
       </c>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -10467,7 +10475,7 @@
       </c>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -10475,7 +10483,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -10483,7 +10491,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>79</v>
       </c>
@@ -10491,7 +10499,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
fix same term under different parents, refs #45330
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1072FB-F76F-2948-8227-9082CD103EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F7FCFA-E17A-B34A-B691-217C1A8581FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1240" windowWidth="25240" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8420" yWindow="500" windowWidth="23100" windowHeight="15860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="925">
   <si>
     <t>sid</t>
   </si>
@@ -2800,13 +2800,16 @@
   </si>
   <si>
     <t>Spliting into 2 separate terms (see tab 1)</t>
+  </si>
+  <si>
+    <t>Checked on Sept 10th, all known issues are fixed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3683,22 +3686,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F118"/>
+  <dimension ref="A1:F120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="57.83203125" customWidth="1"/>
+    <col min="3" max="3" width="43.33203125" customWidth="1"/>
     <col min="4" max="4" width="53.83203125" customWidth="1"/>
     <col min="5" max="5" width="55.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3715,7 +3718,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -3735,7 +3738,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -3755,7 +3758,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3775,7 +3778,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -3795,7 +3798,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>122</v>
       </c>
@@ -3815,7 +3818,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -3835,7 +3838,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -3855,7 +3858,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>131</v>
       </c>
@@ -3875,7 +3878,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -3895,7 +3898,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -3915,7 +3918,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>139</v>
       </c>
@@ -3935,7 +3938,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -3955,7 +3958,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>144</v>
       </c>
@@ -3972,7 +3975,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>147</v>
       </c>
@@ -3989,7 +3992,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>149</v>
       </c>
@@ -4006,7 +4009,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>152</v>
       </c>
@@ -4023,7 +4026,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>154</v>
       </c>
@@ -4040,7 +4043,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>156</v>
       </c>
@@ -4057,7 +4060,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>158</v>
       </c>
@@ -4074,7 +4077,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>160</v>
       </c>
@@ -4091,7 +4094,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>162</v>
       </c>
@@ -4108,7 +4111,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>164</v>
       </c>
@@ -4125,7 +4128,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>166</v>
       </c>
@@ -4142,7 +4145,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>168</v>
       </c>
@@ -4159,7 +4162,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>170</v>
       </c>
@@ -4176,7 +4179,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>172</v>
       </c>
@@ -4193,7 +4196,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>174</v>
       </c>
@@ -4210,7 +4213,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>176</v>
       </c>
@@ -4227,7 +4230,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>178</v>
       </c>
@@ -4244,7 +4247,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>180</v>
       </c>
@@ -4261,7 +4264,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>182</v>
       </c>
@@ -4278,7 +4281,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>184</v>
       </c>
@@ -4295,7 +4298,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>186</v>
       </c>
@@ -4312,7 +4315,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>188</v>
       </c>
@@ -4329,7 +4332,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>190</v>
       </c>
@@ -4346,7 +4349,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>192</v>
       </c>
@@ -4363,7 +4366,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>194</v>
       </c>
@@ -4380,7 +4383,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>196</v>
       </c>
@@ -4397,7 +4400,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>198</v>
       </c>
@@ -4414,7 +4417,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>200</v>
       </c>
@@ -4431,7 +4434,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>202</v>
       </c>
@@ -4448,7 +4451,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>204</v>
       </c>
@@ -4465,7 +4468,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>206</v>
       </c>
@@ -4482,7 +4485,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>208</v>
       </c>
@@ -4499,7 +4502,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>210</v>
       </c>
@@ -4516,7 +4519,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>213</v>
       </c>
@@ -4533,7 +4536,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>216</v>
       </c>
@@ -4550,7 +4553,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>219</v>
       </c>
@@ -4567,7 +4570,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>222</v>
       </c>
@@ -4584,7 +4587,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>224</v>
       </c>
@@ -4601,7 +4604,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>226</v>
       </c>
@@ -4618,7 +4621,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>229</v>
       </c>
@@ -4635,7 +4638,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>485</v>
       </c>
@@ -4652,7 +4655,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>491</v>
       </c>
@@ -4669,7 +4672,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>231</v>
       </c>
@@ -4686,7 +4689,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>234</v>
       </c>
@@ -4703,7 +4706,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>237</v>
       </c>
@@ -4720,7 +4723,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>240</v>
       </c>
@@ -4737,7 +4740,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>242</v>
       </c>
@@ -4754,7 +4757,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>245</v>
       </c>
@@ -4771,7 +4774,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>248</v>
       </c>
@@ -4788,15 +4791,15 @@
         <v>497</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5">
       <c r="E63" s="6"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -4811,7 +4814,7 @@
       </c>
       <c r="E67"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>658</v>
       </c>
@@ -4828,7 +4831,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>660</v>
       </c>
@@ -4845,7 +4848,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>662</v>
       </c>
@@ -4862,7 +4865,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>665</v>
       </c>
@@ -4879,7 +4882,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>136</v>
       </c>
@@ -4896,7 +4899,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>180</v>
       </c>
@@ -4913,7 +4916,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>668</v>
       </c>
@@ -4930,7 +4933,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>216</v>
       </c>
@@ -4947,7 +4950,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>671</v>
       </c>
@@ -4964,7 +4967,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>674</v>
       </c>
@@ -4981,7 +4984,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>676</v>
       </c>
@@ -4998,7 +5001,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>679</v>
       </c>
@@ -5015,7 +5018,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>231</v>
       </c>
@@ -5029,7 +5032,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>681</v>
       </c>
@@ -5046,7 +5049,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>684</v>
       </c>
@@ -5060,7 +5063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>609</v>
       </c>
@@ -5077,15 +5080,15 @@
         <v>771</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5">
       <c r="E84"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5">
       <c r="A86" s="1" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -5102,7 +5105,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>658</v>
       </c>
@@ -5119,7 +5122,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>141</v>
       </c>
@@ -5136,7 +5139,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>180</v>
       </c>
@@ -5153,7 +5156,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>813</v>
       </c>
@@ -5170,7 +5173,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>816</v>
       </c>
@@ -5187,7 +5190,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>216</v>
       </c>
@@ -5204,7 +5207,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>818</v>
       </c>
@@ -5221,7 +5224,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>821</v>
       </c>
@@ -5238,7 +5241,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>676</v>
       </c>
@@ -5255,7 +5258,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>679</v>
       </c>
@@ -5272,7 +5275,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>231</v>
       </c>
@@ -5289,7 +5292,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>825</v>
       </c>
@@ -5306,7 +5309,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>234</v>
       </c>
@@ -5323,7 +5326,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>829</v>
       </c>
@@ -5340,7 +5343,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>681</v>
       </c>
@@ -5357,7 +5360,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
         <v>832</v>
       </c>
@@ -5374,24 +5377,24 @@
         <v>861</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5">
       <c r="A107" s="11" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5">
       <c r="E108"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5">
       <c r="E109"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5">
       <c r="A110" s="11" t="s">
         <v>912</v>
       </c>
       <c r="E110"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
         <v>0</v>
       </c>
@@ -5406,7 +5409,7 @@
       </c>
       <c r="E111"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5">
       <c r="A112" t="s">
         <v>899</v>
       </c>
@@ -5423,7 +5426,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
         <v>902</v>
       </c>
@@ -5440,7 +5443,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
         <v>904</v>
       </c>
@@ -5457,7 +5460,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
         <v>905</v>
       </c>
@@ -5474,7 +5477,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
         <v>906</v>
       </c>
@@ -5491,7 +5494,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
         <v>908</v>
       </c>
@@ -5508,7 +5511,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
         <v>832</v>
       </c>
@@ -5523,6 +5526,11 @@
       </c>
       <c r="E118" s="2" t="s">
         <v>922</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="11" t="s">
+        <v>924</v>
       </c>
     </row>
   </sheetData>
@@ -5535,11 +5543,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="45.1640625" customWidth="1"/>
     <col min="3" max="3" width="62.33203125" customWidth="1"/>
@@ -5548,7 +5556,7 @@
     <col min="6" max="6" width="30.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5568,7 +5576,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>340</v>
       </c>
@@ -5588,7 +5596,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>343</v>
       </c>
@@ -5608,7 +5616,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>346</v>
       </c>
@@ -5628,7 +5636,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>349</v>
       </c>
@@ -5648,7 +5656,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>351</v>
       </c>
@@ -5668,7 +5676,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>353</v>
       </c>
@@ -5688,7 +5696,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>355</v>
       </c>
@@ -5708,7 +5716,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>358</v>
       </c>
@@ -5728,7 +5736,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>361</v>
       </c>
@@ -5748,7 +5756,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>364</v>
       </c>
@@ -5768,7 +5776,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>366</v>
       </c>
@@ -5788,7 +5796,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>369</v>
       </c>
@@ -5808,7 +5816,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>371</v>
       </c>
@@ -5828,7 +5836,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>334</v>
       </c>
@@ -5848,7 +5856,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>378</v>
       </c>
@@ -5868,18 +5876,18 @@
         <v>527</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -5897,7 +5905,7 @@
       </c>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>639</v>
       </c>
@@ -5917,7 +5925,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>642</v>
       </c>
@@ -5934,7 +5942,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>645</v>
       </c>
@@ -5954,7 +5962,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>648</v>
       </c>
@@ -5974,7 +5982,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>480</v>
       </c>
@@ -5994,7 +6002,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>652</v>
       </c>
@@ -6014,7 +6022,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>654</v>
       </c>
@@ -6034,19 +6042,19 @@
         <v>780</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>868</v>
       </c>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -6066,7 +6074,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>346</v>
       </c>
@@ -6086,7 +6094,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" s="3" customFormat="1">
       <c r="A34" s="3" t="s">
         <v>642</v>
       </c>
@@ -6106,7 +6114,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" s="3" customFormat="1">
       <c r="A35" s="3" t="s">
         <v>835</v>
       </c>
@@ -6126,7 +6134,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" s="3" customFormat="1">
       <c r="A36" s="3" t="s">
         <v>481</v>
       </c>
@@ -6146,7 +6154,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" s="3" customFormat="1">
       <c r="A37" s="3" t="s">
         <v>480</v>
       </c>
@@ -6166,7 +6174,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" s="3" customFormat="1">
       <c r="A38" s="3" t="s">
         <v>837</v>
       </c>
@@ -6186,7 +6194,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" s="3" customFormat="1">
       <c r="A39" s="3" t="s">
         <v>839</v>
       </c>
@@ -6206,7 +6214,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" s="3" customFormat="1">
       <c r="A40" s="3" t="s">
         <v>652</v>
       </c>
@@ -6226,7 +6234,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" s="3" customFormat="1">
       <c r="A41" s="3" t="s">
         <v>654</v>
       </c>
@@ -6246,7 +6254,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" s="3" customFormat="1">
       <c r="A42" s="3" t="s">
         <v>378</v>
       </c>
@@ -6266,7 +6274,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" s="3" customFormat="1">
       <c r="A43" s="3" t="s">
         <v>645</v>
       </c>
@@ -6286,19 +6294,19 @@
         <v>889</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" s="3" customFormat="1">
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" s="3" customFormat="1">
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" s="3" customFormat="1">
       <c r="A46" s="10" t="s">
         <v>890</v>
       </c>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" s="3" customFormat="1">
       <c r="A47" s="3" t="s">
         <v>642</v>
       </c>
@@ -6318,7 +6326,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" s="3" customFormat="1">
       <c r="A48" s="3" t="s">
         <v>837</v>
       </c>
@@ -6338,13 +6346,13 @@
         <v>876</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" s="3" customFormat="1">
       <c r="A50" s="10" t="s">
         <v>893</v>
       </c>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" s="3" customFormat="1">
       <c r="A51" s="3" t="s">
         <v>837</v>
       </c>
@@ -6364,7 +6372,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>894</v>
       </c>
@@ -6384,7 +6392,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>898</v>
       </c>
@@ -6397,13 +6405,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F145"/>
+  <dimension ref="A1:F148"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="F146" sqref="F146"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="34.5" customWidth="1"/>
@@ -6412,7 +6420,7 @@
     <col min="6" max="6" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6432,7 +6440,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>251</v>
       </c>
@@ -6452,7 +6460,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>255</v>
       </c>
@@ -6472,7 +6480,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>259</v>
       </c>
@@ -6492,7 +6500,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>263</v>
       </c>
@@ -6512,7 +6520,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>267</v>
       </c>
@@ -6532,7 +6540,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>270</v>
       </c>
@@ -6552,7 +6560,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>272</v>
       </c>
@@ -6572,7 +6580,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>276</v>
       </c>
@@ -6592,7 +6600,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>279</v>
       </c>
@@ -6612,7 +6620,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>282</v>
       </c>
@@ -6632,7 +6640,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>285</v>
       </c>
@@ -6652,7 +6660,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>289</v>
       </c>
@@ -6672,7 +6680,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>292</v>
       </c>
@@ -6692,7 +6700,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>296</v>
       </c>
@@ -6712,7 +6720,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>248</v>
       </c>
@@ -6732,7 +6740,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>301</v>
       </c>
@@ -6752,7 +6760,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>304</v>
       </c>
@@ -6772,7 +6780,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>308</v>
       </c>
@@ -6792,7 +6800,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>310</v>
       </c>
@@ -6812,7 +6820,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>224</v>
       </c>
@@ -6832,7 +6840,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>222</v>
       </c>
@@ -6852,7 +6860,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>316</v>
       </c>
@@ -6872,7 +6880,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>318</v>
       </c>
@@ -6892,7 +6900,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>321</v>
       </c>
@@ -6912,7 +6920,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>324</v>
       </c>
@@ -6932,7 +6940,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>122</v>
       </c>
@@ -6952,7 +6960,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>330</v>
       </c>
@@ -6972,7 +6980,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>333</v>
       </c>
@@ -6992,7 +7000,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>337</v>
       </c>
@@ -7012,12 +7020,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -7034,7 +7042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>251</v>
       </c>
@@ -7054,7 +7062,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>529</v>
       </c>
@@ -7074,7 +7082,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>255</v>
       </c>
@@ -7094,7 +7102,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>534</v>
       </c>
@@ -7114,7 +7122,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>259</v>
       </c>
@@ -7134,7 +7142,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>537</v>
       </c>
@@ -7154,7 +7162,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>541</v>
       </c>
@@ -7174,7 +7182,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>544</v>
       </c>
@@ -7194,7 +7202,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>263</v>
       </c>
@@ -7214,7 +7222,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>267</v>
       </c>
@@ -7234,7 +7242,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>270</v>
       </c>
@@ -7254,7 +7262,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>548</v>
       </c>
@@ -7274,7 +7282,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>272</v>
       </c>
@@ -7294,7 +7302,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>276</v>
       </c>
@@ -7314,7 +7322,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>279</v>
       </c>
@@ -7334,7 +7342,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>553</v>
       </c>
@@ -7354,7 +7362,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>285</v>
       </c>
@@ -7374,7 +7382,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>289</v>
       </c>
@@ -7394,7 +7402,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>558</v>
       </c>
@@ -7414,7 +7422,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>292</v>
       </c>
@@ -7434,7 +7442,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>561</v>
       </c>
@@ -7454,7 +7462,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>296</v>
       </c>
@@ -7474,7 +7482,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>248</v>
       </c>
@@ -7491,7 +7499,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>301</v>
       </c>
@@ -7511,7 +7519,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>304</v>
       </c>
@@ -7531,7 +7539,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>308</v>
       </c>
@@ -7551,7 +7559,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>310</v>
       </c>
@@ -7571,7 +7579,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>316</v>
       </c>
@@ -7591,7 +7599,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>318</v>
       </c>
@@ -7608,7 +7616,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>567</v>
       </c>
@@ -7628,7 +7636,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>569</v>
       </c>
@@ -7648,7 +7656,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>573</v>
       </c>
@@ -7668,7 +7676,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>577</v>
       </c>
@@ -7688,7 +7696,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>580</v>
       </c>
@@ -7708,7 +7716,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>583</v>
       </c>
@@ -7728,7 +7736,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>321</v>
       </c>
@@ -7748,7 +7756,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>324</v>
       </c>
@@ -7768,7 +7776,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>589</v>
       </c>
@@ -7788,7 +7796,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>122</v>
       </c>
@@ -7808,7 +7816,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>592</v>
       </c>
@@ -7828,7 +7836,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>596</v>
       </c>
@@ -7848,7 +7856,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>598</v>
       </c>
@@ -7868,7 +7876,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>600</v>
       </c>
@@ -7888,7 +7896,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>330</v>
       </c>
@@ -7908,7 +7916,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>603</v>
       </c>
@@ -7925,7 +7933,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>512</v>
       </c>
@@ -7945,7 +7953,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>337</v>
       </c>
@@ -7965,12 +7973,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6">
       <c r="A87" s="1" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -7988,7 +7996,7 @@
       </c>
       <c r="F89"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>255</v>
       </c>
@@ -8008,7 +8016,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>688</v>
       </c>
@@ -8028,7 +8036,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>668</v>
       </c>
@@ -8048,7 +8056,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
         <v>693</v>
       </c>
@@ -8068,7 +8076,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>697</v>
       </c>
@@ -8088,7 +8096,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>701</v>
       </c>
@@ -8108,7 +8116,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>272</v>
       </c>
@@ -8128,7 +8136,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>704</v>
       </c>
@@ -8148,7 +8156,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6">
       <c r="A98" t="s">
         <v>707</v>
       </c>
@@ -8168,7 +8176,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6">
       <c r="A99" t="s">
         <v>553</v>
       </c>
@@ -8188,7 +8196,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
         <v>710</v>
       </c>
@@ -8208,7 +8216,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6">
       <c r="A101" t="s">
         <v>289</v>
       </c>
@@ -8228,7 +8236,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6">
       <c r="A102" t="s">
         <v>715</v>
       </c>
@@ -8248,7 +8256,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6">
       <c r="A103" t="s">
         <v>561</v>
       </c>
@@ -8265,7 +8273,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
         <v>718</v>
       </c>
@@ -8285,7 +8293,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
         <v>684</v>
       </c>
@@ -8302,7 +8310,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
         <v>724</v>
       </c>
@@ -8322,7 +8330,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
         <v>569</v>
       </c>
@@ -8339,7 +8347,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6">
       <c r="A108" t="s">
         <v>580</v>
       </c>
@@ -8356,7 +8364,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6">
       <c r="A109" t="s">
         <v>728</v>
       </c>
@@ -8376,7 +8384,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6">
       <c r="A110" t="s">
         <v>324</v>
       </c>
@@ -8396,7 +8404,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6">
       <c r="A111" t="s">
         <v>732</v>
       </c>
@@ -8416,7 +8424,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6">
       <c r="A112" t="s">
         <v>736</v>
       </c>
@@ -8433,7 +8441,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6">
       <c r="A113" t="s">
         <v>738</v>
       </c>
@@ -8453,12 +8461,12 @@
         <v>252</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6">
       <c r="A116" s="1" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -8478,7 +8486,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6">
       <c r="A118" t="s">
         <v>783</v>
       </c>
@@ -8498,7 +8506,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6">
       <c r="A119" t="s">
         <v>732</v>
       </c>
@@ -8518,7 +8526,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
         <v>693</v>
       </c>
@@ -8538,7 +8546,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
         <v>272</v>
       </c>
@@ -8558,7 +8566,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
         <v>787</v>
       </c>
@@ -8578,7 +8586,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6">
       <c r="A123" t="s">
         <v>790</v>
       </c>
@@ -8598,7 +8606,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6">
       <c r="A124" t="s">
         <v>738</v>
       </c>
@@ -8618,7 +8626,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6">
       <c r="A125" t="s">
         <v>869</v>
       </c>
@@ -8638,7 +8646,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6">
       <c r="A126" t="s">
         <v>707</v>
       </c>
@@ -8658,7 +8666,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6">
       <c r="A127" t="s">
         <v>793</v>
       </c>
@@ -8678,7 +8686,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6">
       <c r="A128" t="s">
         <v>715</v>
       </c>
@@ -8698,7 +8706,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6">
       <c r="A129" t="s">
         <v>561</v>
       </c>
@@ -8718,7 +8726,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6">
       <c r="A130" t="s">
         <v>796</v>
       </c>
@@ -8738,7 +8746,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6">
       <c r="A131" t="s">
         <v>798</v>
       </c>
@@ -8758,7 +8766,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6">
       <c r="A132" t="s">
         <v>324</v>
       </c>
@@ -8778,7 +8786,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6">
       <c r="A133" t="s">
         <v>801</v>
       </c>
@@ -8798,7 +8806,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
         <v>589</v>
       </c>
@@ -8818,7 +8826,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6">
       <c r="A135" t="s">
         <v>803</v>
       </c>
@@ -8838,7 +8846,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6">
       <c r="A136" t="s">
         <v>805</v>
       </c>
@@ -8858,7 +8866,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6">
       <c r="A137" t="s">
         <v>808</v>
       </c>
@@ -8878,20 +8886,20 @@
         <v>637</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6">
       <c r="F138"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6">
       <c r="A139" s="1" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6">
       <c r="A142" s="11" t="s">
         <v>912</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6">
       <c r="A143" s="7" t="s">
         <v>0</v>
       </c>
@@ -8908,7 +8916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6">
       <c r="A144" s="7" t="s">
         <v>913</v>
       </c>
@@ -8928,7 +8936,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6">
       <c r="A145" s="7" t="s">
         <v>899</v>
       </c>
@@ -8946,6 +8954,11 @@
       </c>
       <c r="F145" s="2" t="s">
         <v>923</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" s="11" t="s">
+        <v>924</v>
       </c>
     </row>
   </sheetData>
@@ -8963,7 +8976,7 @@
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="42.83203125" customWidth="1"/>
@@ -8972,7 +8985,7 @@
     <col min="5" max="5" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -8989,7 +9002,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -9006,7 +9019,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -9023,7 +9036,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -9034,7 +9047,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -9045,7 +9058,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -9056,7 +9069,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -9067,7 +9080,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -9081,7 +9094,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -9092,7 +9105,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -9103,7 +9116,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -9120,7 +9133,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -9131,7 +9144,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>87</v>
       </c>
@@ -9148,15 +9161,15 @@
         <v>524</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="D18" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>742</v>
       </c>
@@ -9167,7 +9180,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="7" t="s">
         <v>612</v>
       </c>
@@ -9181,7 +9194,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>747</v>
       </c>
@@ -9192,7 +9205,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>744</v>
       </c>
@@ -9204,10 +9217,10 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -9224,7 +9237,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -9241,7 +9254,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -9255,7 +9268,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>617</v>
       </c>
@@ -9269,10 +9282,10 @@
         <v>758</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>334</v>
       </c>
@@ -9292,17 +9305,17 @@
         <v>855</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" s="7"/>
       <c r="B33" s="3"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
         <v>887</v>
       </c>
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>747</v>
       </c>
@@ -9316,17 +9329,17 @@
         <v>867</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" s="7" t="s">
         <v>891</v>
       </c>
       <c r="B38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
         <v>892</v>
       </c>
@@ -9345,14 +9358,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="52.33203125" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="2"/>
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -9367,7 +9380,7 @@
       </c>
       <c r="E1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>742</v>
       </c>
@@ -9382,7 +9395,7 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>743</v>
       </c>
@@ -9397,7 +9410,7 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -9412,7 +9425,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -9427,7 +9440,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -9442,7 +9455,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -9457,7 +9470,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -9472,7 +9485,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>614</v>
       </c>
@@ -9487,7 +9500,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>384</v>
       </c>
@@ -9502,7 +9515,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -9517,7 +9530,7 @@
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -9532,7 +9545,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -9547,7 +9560,7 @@
       </c>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>746</v>
       </c>
@@ -9562,7 +9575,7 @@
       </c>
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -9577,7 +9590,7 @@
       </c>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -9592,7 +9605,7 @@
       </c>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -9607,7 +9620,7 @@
       </c>
       <c r="E17"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -9622,7 +9635,7 @@
       </c>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>852</v>
       </c>
@@ -9637,7 +9650,7 @@
       </c>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>846</v>
       </c>
@@ -9652,7 +9665,7 @@
       </c>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>390</v>
       </c>
@@ -9667,7 +9680,7 @@
       </c>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -9682,7 +9695,7 @@
       </c>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -9697,7 +9710,7 @@
       </c>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -9712,7 +9725,7 @@
       </c>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -9727,7 +9740,7 @@
       </c>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -9742,7 +9755,7 @@
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>392</v>
       </c>
@@ -9757,7 +9770,7 @@
       </c>
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -9772,7 +9785,7 @@
       </c>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -9787,7 +9800,7 @@
       </c>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -9802,7 +9815,7 @@
       </c>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -9817,7 +9830,7 @@
       </c>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -9832,7 +9845,7 @@
       </c>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -9847,7 +9860,7 @@
       </c>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>398</v>
       </c>
@@ -9862,7 +9875,7 @@
       </c>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>400</v>
       </c>
@@ -9877,7 +9890,7 @@
       </c>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -9892,7 +9905,7 @@
       </c>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>402</v>
       </c>
@@ -9907,7 +9920,7 @@
       </c>
       <c r="E37"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -9922,7 +9935,7 @@
       </c>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -9937,7 +9950,7 @@
       </c>
       <c r="E39"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -9952,7 +9965,7 @@
       </c>
       <c r="E40"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -9967,7 +9980,7 @@
       </c>
       <c r="E41"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>406</v>
       </c>
@@ -9982,7 +9995,7 @@
       </c>
       <c r="E42"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -9997,7 +10010,7 @@
       </c>
       <c r="E43"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>619</v>
       </c>
@@ -10012,7 +10025,7 @@
       </c>
       <c r="E44"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>408</v>
       </c>
@@ -10027,7 +10040,7 @@
       </c>
       <c r="E45"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>73</v>
       </c>
@@ -10042,7 +10055,7 @@
       </c>
       <c r="E46"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>75</v>
       </c>
@@ -10057,7 +10070,7 @@
       </c>
       <c r="E47"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>77</v>
       </c>
@@ -10072,7 +10085,7 @@
       </c>
       <c r="E48"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>79</v>
       </c>
@@ -10087,7 +10100,7 @@
       </c>
       <c r="E49"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -10102,7 +10115,7 @@
       </c>
       <c r="E50"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -10117,7 +10130,7 @@
       </c>
       <c r="E51"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>412</v>
       </c>
@@ -10132,7 +10145,7 @@
       </c>
       <c r="E52"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -10147,7 +10160,7 @@
       </c>
       <c r="E53"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>395</v>
       </c>
@@ -10162,7 +10175,7 @@
       </c>
       <c r="E54"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>83</v>
       </c>
@@ -10177,7 +10190,7 @@
       </c>
       <c r="E55"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -10192,7 +10205,7 @@
       </c>
       <c r="E56"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>71</v>
       </c>
@@ -10207,7 +10220,7 @@
       </c>
       <c r="E57"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>86</v>
       </c>
@@ -10222,7 +10235,7 @@
       </c>
       <c r="E58"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>84</v>
       </c>
@@ -10237,7 +10250,7 @@
       </c>
       <c r="E59"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>87</v>
       </c>
@@ -10252,7 +10265,7 @@
       </c>
       <c r="E60"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -10267,7 +10280,7 @@
       </c>
       <c r="E61"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="E62"/>
     </row>
   </sheetData>
@@ -10287,12 +10300,12 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -10300,7 +10313,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -10308,7 +10321,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>742</v>
       </c>
@@ -10316,7 +10329,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>743</v>
       </c>
@@ -10324,7 +10337,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -10332,7 +10345,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -10340,7 +10353,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -10348,7 +10361,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -10356,7 +10369,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -10364,7 +10377,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -10372,7 +10385,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -10380,7 +10393,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -10388,7 +10401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>852</v>
       </c>
@@ -10396,7 +10409,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>846</v>
       </c>
@@ -10404,7 +10417,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -10412,7 +10425,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>390</v>
       </c>
@@ -10420,7 +10433,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -10428,7 +10441,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -10436,7 +10449,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -10444,7 +10457,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>412</v>
       </c>
@@ -10452,7 +10465,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -10460,7 +10473,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>614</v>
       </c>
@@ -10468,7 +10481,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -10476,7 +10489,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -10484,7 +10497,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -10492,7 +10505,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>384</v>
       </c>
@@ -10500,7 +10513,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>392</v>
       </c>
@@ -10508,7 +10521,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -10516,7 +10529,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>395</v>
       </c>
@@ -10524,7 +10537,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -10532,7 +10545,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -10540,7 +10553,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -10548,7 +10561,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -10556,7 +10569,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -10564,7 +10577,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -10572,7 +10585,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>398</v>
       </c>
@@ -10580,7 +10593,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>400</v>
       </c>
@@ -10588,7 +10601,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -10596,7 +10609,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -10604,7 +10617,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -10612,7 +10625,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>402</v>
       </c>
@@ -10620,7 +10633,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -10628,7 +10641,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -10636,7 +10649,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -10644,7 +10657,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -10652,7 +10665,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>406</v>
       </c>
@@ -10660,7 +10673,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>104</v>
       </c>
@@ -10668,7 +10681,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>30</v>
       </c>
@@ -10676,7 +10689,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -10684,7 +10697,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>32</v>
       </c>
@@ -10692,7 +10705,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>619</v>
       </c>
@@ -10700,7 +10713,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>408</v>
       </c>
@@ -10709,7 +10722,7 @@
       </c>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>73</v>
       </c>
@@ -10719,7 +10732,7 @@
       <c r="C53" s="4"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -10728,7 +10741,7 @@
       </c>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>75</v>
       </c>
@@ -10737,7 +10750,7 @@
       </c>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -10746,7 +10759,7 @@
       </c>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -10754,7 +10767,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -10762,7 +10775,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>79</v>
       </c>
@@ -10770,7 +10783,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
newly identified inconsistent issues in clinEpi
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F7FCFA-E17A-B34A-B691-217C1A8581FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F2CC79-2868-0A48-8C8D-DFC4AA47BACD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8420" yWindow="500" windowWidth="23100" windowHeight="15860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="660" windowWidth="23100" windowHeight="15860" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="967">
   <si>
     <t>sid</t>
   </si>
@@ -2803,6 +2803,132 @@
   </si>
   <si>
     <t>Checked on Sept 10th, all known issues are fixed</t>
+  </si>
+  <si>
+    <t>Checked on Oct 6th, identified following issues:</t>
+  </si>
+  <si>
+    <t>EUPATH_0020097</t>
+  </si>
+  <si>
+    <t>Household administrative information | Household administrative Information</t>
+  </si>
+  <si>
+    <t>icemr_prism2_border_cohort | gates_washb_kenya | gates_washb_bangladesh | icemr_prism2 | gates_ganc</t>
+  </si>
+  <si>
+    <t>Persons &lt;=18 years living in house count | Persons &lt;=18 years living in house</t>
+  </si>
+  <si>
+    <t>EUPATH_0036132</t>
+  </si>
+  <si>
+    <t>Other adult read with child | Other person read with child</t>
+  </si>
+  <si>
+    <t>gates_provide | gates_ganc</t>
+  </si>
+  <si>
+    <t>EUPATH_0036134</t>
+  </si>
+  <si>
+    <t>Other adult told child stories | Other person told child stories</t>
+  </si>
+  <si>
+    <t>EUPATH_0042144</t>
+  </si>
+  <si>
+    <t>Child still alive | Child vital status</t>
+  </si>
+  <si>
+    <t>general/general_promote | gates_ganc</t>
+  </si>
+  <si>
+    <t>EUPATH_0042219</t>
+  </si>
+  <si>
+    <t>Child delivery location | Infant delivery location</t>
+  </si>
+  <si>
+    <t>EUPATH_0047002</t>
+  </si>
+  <si>
+    <t>Antenatal care | Antenatal and postnatal care</t>
+  </si>
+  <si>
+    <t>icemr_india_meghalaya | gates_sip | gates_ganc</t>
+  </si>
+  <si>
+    <t>Household administrative information</t>
+  </si>
+  <si>
+    <t>wrong IRI, should be</t>
+  </si>
+  <si>
+    <t>gates_score_sm_crt</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>mm Hg</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>gates_ganc</t>
+  </si>
+  <si>
+    <t>all other datasets</t>
+  </si>
+  <si>
+    <t>should change to min</t>
+  </si>
+  <si>
+    <t>Unit IRI</t>
+  </si>
+  <si>
+    <t>should change to mmHg</t>
+  </si>
+  <si>
+    <t>EUPATH_0011730|EUPATH_0015647|EUPATH_0047667</t>
+  </si>
+  <si>
+    <t>category|variable|value</t>
+  </si>
+  <si>
+    <t>Feeding|Proposed way to prevent child from illness|Factors contributing to not using FP</t>
+  </si>
+  <si>
+    <t>icemr_west_africa | icemr_prism2_border_cohort | gates_gems | gates_elicit | icemr_india_cx | general/general_kalifabougou | icemr_amazonia_brazil | gates_washb_bangladesh | general/general_promote | icemr_india_cohort | icemr_south_asia | gates_score_sm_crt | icemr_southeast_asia | icemr_prism | gates_provide | icemr_amazonia_peru | icemr_india_severe_malaria</t>
+  </si>
+  <si>
+    <t>EUPATH_0030005</t>
+  </si>
+  <si>
+    <t>Birth year</t>
+  </si>
+  <si>
+    <t>Demographics|Child demographics</t>
+  </si>
+  <si>
+    <t>gates_gems_huas | gates_score_sm_crt | icemr_southeast_asia | gates_ganc</t>
+  </si>
+  <si>
+    <t>Child still alive|Child vital status</t>
+  </si>
+  <si>
+    <t>Obstetric history|Child observation details</t>
   </si>
 </sst>
 </file>
@@ -3317,7 +3443,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3330,6 +3456,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3686,10 +3813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F120"/>
+  <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="A120" sqref="A120"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5533,6 +5660,129 @@
         <v>924</v>
       </c>
     </row>
+    <row r="122" spans="1:5">
+      <c r="A122" s="11" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" t="s">
+        <v>0</v>
+      </c>
+      <c r="B123" t="s">
+        <v>1</v>
+      </c>
+      <c r="C123" t="s">
+        <v>2</v>
+      </c>
+      <c r="D123" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" t="s">
+        <v>926</v>
+      </c>
+      <c r="B124">
+        <v>2</v>
+      </c>
+      <c r="C124" t="s">
+        <v>927</v>
+      </c>
+      <c r="D124" t="s">
+        <v>928</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" t="s">
+        <v>832</v>
+      </c>
+      <c r="B125">
+        <v>2</v>
+      </c>
+      <c r="C125" t="s">
+        <v>929</v>
+      </c>
+      <c r="D125" t="s">
+        <v>911</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" t="s">
+        <v>930</v>
+      </c>
+      <c r="B126">
+        <v>2</v>
+      </c>
+      <c r="C126" t="s">
+        <v>931</v>
+      </c>
+      <c r="D126" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" t="s">
+        <v>933</v>
+      </c>
+      <c r="B127">
+        <v>2</v>
+      </c>
+      <c r="C127" t="s">
+        <v>934</v>
+      </c>
+      <c r="D127" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" t="s">
+        <v>935</v>
+      </c>
+      <c r="B128">
+        <v>2</v>
+      </c>
+      <c r="C128" t="s">
+        <v>936</v>
+      </c>
+      <c r="D128" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" t="s">
+        <v>938</v>
+      </c>
+      <c r="B129">
+        <v>2</v>
+      </c>
+      <c r="C129" t="s">
+        <v>939</v>
+      </c>
+      <c r="D129" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" t="s">
+        <v>940</v>
+      </c>
+      <c r="B130">
+        <v>2</v>
+      </c>
+      <c r="C130" t="s">
+        <v>941</v>
+      </c>
+      <c r="D130" t="s">
+        <v>942</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -5541,10 +5791,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6397,6 +6647,47 @@
         <v>898</v>
       </c>
     </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="11" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>545</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>957</v>
+      </c>
+      <c r="D60" t="s">
+        <v>958</v>
+      </c>
+      <c r="E60" t="s">
+        <v>959</v>
+      </c>
+      <c r="F60"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6405,10 +6696,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F148"/>
+  <dimension ref="A1:F154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A152" sqref="A152"/>
+    <sheetView topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8961,6 +9252,79 @@
         <v>924</v>
       </c>
     </row>
+    <row r="150" spans="1:6">
+      <c r="A150" s="11" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" t="s">
+        <v>0</v>
+      </c>
+      <c r="B151" t="s">
+        <v>10</v>
+      </c>
+      <c r="C151" t="s">
+        <v>2</v>
+      </c>
+      <c r="D151" t="s">
+        <v>11</v>
+      </c>
+      <c r="E151" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" t="s">
+        <v>732</v>
+      </c>
+      <c r="B152">
+        <v>2</v>
+      </c>
+      <c r="C152" t="s">
+        <v>733</v>
+      </c>
+      <c r="D152" t="s">
+        <v>730</v>
+      </c>
+      <c r="E152" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" t="s">
+        <v>961</v>
+      </c>
+      <c r="B153">
+        <v>2</v>
+      </c>
+      <c r="C153" t="s">
+        <v>962</v>
+      </c>
+      <c r="D153" t="s">
+        <v>963</v>
+      </c>
+      <c r="E153" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" t="s">
+        <v>935</v>
+      </c>
+      <c r="B154">
+        <v>2</v>
+      </c>
+      <c r="C154" t="s">
+        <v>965</v>
+      </c>
+      <c r="D154" t="s">
+        <v>966</v>
+      </c>
+      <c r="E154" t="s">
+        <v>937</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F30" xr:uid="{3F2C9002-1B0A-C348-905C-32E2D16BAD66}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8970,19 +9334,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="42.83203125" customWidth="1"/>
-    <col min="3" max="3" width="56.33203125" customWidth="1"/>
-    <col min="4" max="4" width="41.5" customWidth="1"/>
-    <col min="5" max="5" width="36.1640625" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -9305,17 +9669,17 @@
         <v>855</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:6">
       <c r="A33" s="7"/>
       <c r="B33" s="3"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
         <v>887</v>
       </c>
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>747</v>
       </c>
@@ -9329,19 +9693,136 @@
         <v>867</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:6">
       <c r="A38" s="7" t="s">
         <v>891</v>
       </c>
       <c r="B38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:6">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:6">
       <c r="A40" s="11" t="s">
         <v>892</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="11"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="11" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="12" customFormat="1">
+      <c r="A44" s="12" t="s">
+        <v>948</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>949</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>950</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>334</v>
+      </c>
+      <c r="B45" t="s">
+        <v>512</v>
+      </c>
+      <c r="C45" t="s">
+        <v>752</v>
+      </c>
+      <c r="D45" t="s">
+        <v>84</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="F45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>733</v>
+      </c>
+      <c r="B46" t="s">
+        <v>732</v>
+      </c>
+      <c r="C46" t="s">
+        <v>945</v>
+      </c>
+      <c r="D46" t="s">
+        <v>87</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="F46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="12" customFormat="1">
+      <c r="A49" s="12" t="s">
+        <v>955</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>951</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" t="s">
+        <v>946</v>
+      </c>
+      <c r="C50" t="s">
+        <v>952</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" t="s">
+        <v>947</v>
+      </c>
+      <c r="C52" t="s">
+        <v>952</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="B53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" t="s">
+        <v>953</v>
       </c>
     </row>
   </sheetData>
@@ -9354,7 +9835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -10294,10 +10775,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E96E553-B9B7-3A43-9A19-9B2DEFC1133B}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10305,15 +10786,17 @@
     <col min="1" max="2" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="E1"/>
+      <c r="F1"/>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -10321,7 +10804,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>742</v>
       </c>
@@ -10329,7 +10812,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>743</v>
       </c>
@@ -10337,7 +10820,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -10345,7 +10828,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -10353,7 +10836,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -10361,7 +10844,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -10369,7 +10852,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -10377,7 +10860,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -10385,7 +10868,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -10393,7 +10876,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -10401,7 +10884,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>852</v>
       </c>
@@ -10409,7 +10892,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>846</v>
       </c>
@@ -10417,7 +10900,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -10425,7 +10908,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>390</v>
       </c>

</xml_diff>

<commit_message>
fixed inconsistent issues, refs #45330
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E61D5A-2CE0-AB44-A557-86B783B24502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587622FB-5BF4-A249-B57D-DEAB2231A782}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="660" windowWidth="23100" windowHeight="15860" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="660" windowWidth="23100" windowHeight="15860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="974">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="972">
   <si>
     <t>sid</t>
   </si>
@@ -2901,15 +2901,6 @@
     <t>should change to mmHg</t>
   </si>
   <si>
-    <t>EUPATH_0011730|EUPATH_0015647|EUPATH_0047667</t>
-  </si>
-  <si>
-    <t>category|variable|value</t>
-  </si>
-  <si>
-    <t>Feeding|Proposed way to prevent child from illness|Factors contributing to not using FP</t>
-  </si>
-  <si>
     <t>icemr_west_africa | icemr_prism2_border_cohort | gates_gems | gates_elicit | icemr_india_cx | general/general_kalifabougou | icemr_amazonia_brazil | gates_washb_bangladesh | general/general_promote | icemr_india_cohort | icemr_south_asia | gates_score_sm_crt | icemr_southeast_asia | icemr_prism | gates_provide | icemr_amazonia_peru | icemr_india_severe_malaria</t>
   </si>
   <si>
@@ -2946,17 +2937,20 @@
     <t>Antenatal and postnatal care</t>
   </si>
   <si>
-    <t>I'm seeing that EUPATH_0011730 is a category while EUPATH_0015647 and EUPATH_0047667 are multifilter values, so this should be ok</t>
-  </si>
-  <si>
     <t>Term in Child demographics needs a new IRI with label "Child birth year"</t>
+  </si>
+  <si>
+    <t>Rechecked on Oct 6th, all known issues are fixed</t>
+  </si>
+  <si>
+    <t>Checked on Oct 6th, no issue was found</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3834,13 +3828,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F130"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+    <sheetView topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
@@ -3849,7 +3843,7 @@
     <col min="5" max="5" width="55.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3866,7 +3860,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -3886,7 +3880,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -3906,7 +3900,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3926,7 +3920,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -3946,7 +3940,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>122</v>
       </c>
@@ -3966,7 +3960,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -3986,7 +3980,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -4006,7 +4000,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>131</v>
       </c>
@@ -4026,7 +4020,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -4046,7 +4040,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -4066,7 +4060,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>139</v>
       </c>
@@ -4086,7 +4080,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -4106,7 +4100,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>144</v>
       </c>
@@ -4123,7 +4117,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>147</v>
       </c>
@@ -4140,7 +4134,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>149</v>
       </c>
@@ -4157,7 +4151,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>152</v>
       </c>
@@ -4174,7 +4168,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>154</v>
       </c>
@@ -4191,7 +4185,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>156</v>
       </c>
@@ -4208,7 +4202,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>158</v>
       </c>
@@ -4225,7 +4219,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>160</v>
       </c>
@@ -4242,7 +4236,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>162</v>
       </c>
@@ -4259,7 +4253,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>164</v>
       </c>
@@ -4276,7 +4270,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>166</v>
       </c>
@@ -4293,7 +4287,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>168</v>
       </c>
@@ -4310,7 +4304,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>170</v>
       </c>
@@ -4327,7 +4321,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>172</v>
       </c>
@@ -4344,7 +4338,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>174</v>
       </c>
@@ -4361,7 +4355,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>176</v>
       </c>
@@ -4378,7 +4372,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>178</v>
       </c>
@@ -4395,7 +4389,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>180</v>
       </c>
@@ -4412,7 +4406,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>182</v>
       </c>
@@ -4429,7 +4423,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>184</v>
       </c>
@@ -4446,7 +4440,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>186</v>
       </c>
@@ -4463,7 +4457,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>188</v>
       </c>
@@ -4480,7 +4474,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>190</v>
       </c>
@@ -4497,7 +4491,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>192</v>
       </c>
@@ -4514,7 +4508,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>194</v>
       </c>
@@ -4531,7 +4525,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>196</v>
       </c>
@@ -4548,7 +4542,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>198</v>
       </c>
@@ -4565,7 +4559,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>200</v>
       </c>
@@ -4582,7 +4576,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>202</v>
       </c>
@@ -4599,7 +4593,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>204</v>
       </c>
@@ -4616,7 +4610,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>206</v>
       </c>
@@ -4633,7 +4627,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>208</v>
       </c>
@@ -4650,7 +4644,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>210</v>
       </c>
@@ -4667,7 +4661,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>213</v>
       </c>
@@ -4684,7 +4678,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>216</v>
       </c>
@@ -4701,7 +4695,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>219</v>
       </c>
@@ -4718,7 +4712,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>222</v>
       </c>
@@ -4735,7 +4729,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>224</v>
       </c>
@@ -4752,7 +4746,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>226</v>
       </c>
@@ -4769,7 +4763,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>229</v>
       </c>
@@ -4786,7 +4780,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>485</v>
       </c>
@@ -4803,7 +4797,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>491</v>
       </c>
@@ -4820,7 +4814,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>231</v>
       </c>
@@ -4837,7 +4831,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>234</v>
       </c>
@@ -4854,7 +4848,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>237</v>
       </c>
@@ -4871,7 +4865,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>240</v>
       </c>
@@ -4888,7 +4882,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>242</v>
       </c>
@@ -4905,7 +4899,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>245</v>
       </c>
@@ -4922,7 +4916,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>248</v>
       </c>
@@ -4939,15 +4933,15 @@
         <v>497</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5">
       <c r="E63" s="6"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -4962,7 +4956,7 @@
       </c>
       <c r="E67"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>658</v>
       </c>
@@ -4979,7 +4973,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>660</v>
       </c>
@@ -4996,7 +4990,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>662</v>
       </c>
@@ -5013,7 +5007,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>665</v>
       </c>
@@ -5030,7 +5024,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>136</v>
       </c>
@@ -5047,7 +5041,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>180</v>
       </c>
@@ -5064,7 +5058,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>668</v>
       </c>
@@ -5081,7 +5075,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>216</v>
       </c>
@@ -5098,7 +5092,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>671</v>
       </c>
@@ -5115,7 +5109,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>674</v>
       </c>
@@ -5132,7 +5126,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>676</v>
       </c>
@@ -5149,7 +5143,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>679</v>
       </c>
@@ -5166,7 +5160,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>231</v>
       </c>
@@ -5180,7 +5174,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>681</v>
       </c>
@@ -5197,7 +5191,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>684</v>
       </c>
@@ -5211,7 +5205,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>609</v>
       </c>
@@ -5228,15 +5222,15 @@
         <v>771</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5">
       <c r="E84"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5">
       <c r="A86" s="1" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -5253,7 +5247,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>658</v>
       </c>
@@ -5270,7 +5264,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>141</v>
       </c>
@@ -5287,7 +5281,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>180</v>
       </c>
@@ -5304,7 +5298,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>813</v>
       </c>
@@ -5321,7 +5315,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>816</v>
       </c>
@@ -5338,7 +5332,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>216</v>
       </c>
@@ -5355,7 +5349,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>818</v>
       </c>
@@ -5372,7 +5366,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>821</v>
       </c>
@@ -5389,7 +5383,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>676</v>
       </c>
@@ -5406,7 +5400,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>679</v>
       </c>
@@ -5423,7 +5417,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>231</v>
       </c>
@@ -5440,7 +5434,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>825</v>
       </c>
@@ -5457,7 +5451,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>234</v>
       </c>
@@ -5474,7 +5468,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>829</v>
       </c>
@@ -5491,7 +5485,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>681</v>
       </c>
@@ -5508,7 +5502,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
         <v>832</v>
       </c>
@@ -5525,24 +5519,24 @@
         <v>861</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5">
       <c r="A107" s="11" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5">
       <c r="E108"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5">
       <c r="E109"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5">
       <c r="A110" s="11" t="s">
         <v>912</v>
       </c>
       <c r="E110"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
         <v>0</v>
       </c>
@@ -5557,7 +5551,7 @@
       </c>
       <c r="E111"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5">
       <c r="A112" t="s">
         <v>899</v>
       </c>
@@ -5574,7 +5568,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
         <v>902</v>
       </c>
@@ -5591,7 +5585,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
         <v>904</v>
       </c>
@@ -5608,7 +5602,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
         <v>905</v>
       </c>
@@ -5625,7 +5619,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
         <v>906</v>
       </c>
@@ -5642,7 +5636,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
         <v>908</v>
       </c>
@@ -5659,7 +5653,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
         <v>832</v>
       </c>
@@ -5676,17 +5670,17 @@
         <v>922</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5">
       <c r="A120" s="11" t="s">
         <v>924</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5">
       <c r="A122" s="11" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
         <v>0</v>
       </c>
@@ -5700,7 +5694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
         <v>926</v>
       </c>
@@ -5717,7 +5711,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
         <v>832</v>
       </c>
@@ -5734,7 +5728,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
         <v>930</v>
       </c>
@@ -5748,10 +5742,10 @@
         <v>932</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
         <v>933</v>
       </c>
@@ -5765,10 +5759,10 @@
         <v>932</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128" t="s">
         <v>935</v>
       </c>
@@ -5782,10 +5776,10 @@
         <v>937</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
       <c r="A129" t="s">
         <v>938</v>
       </c>
@@ -5799,10 +5793,10 @@
         <v>937</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130" t="s">
         <v>940</v>
       </c>
@@ -5816,7 +5810,12 @@
         <v>942</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>971</v>
+        <v>968</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" s="11" t="s">
+        <v>970</v>
       </c>
     </row>
   </sheetData>
@@ -5827,13 +5826,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="45.1640625" customWidth="1"/>
     <col min="3" max="3" width="62.33203125" customWidth="1"/>
@@ -5842,7 +5841,7 @@
     <col min="6" max="6" width="30.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5862,7 +5861,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>340</v>
       </c>
@@ -5882,7 +5881,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>343</v>
       </c>
@@ -5902,7 +5901,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>346</v>
       </c>
@@ -5922,7 +5921,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>349</v>
       </c>
@@ -5942,7 +5941,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>351</v>
       </c>
@@ -5962,7 +5961,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>353</v>
       </c>
@@ -5982,7 +5981,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>355</v>
       </c>
@@ -6002,7 +6001,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>358</v>
       </c>
@@ -6022,7 +6021,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>361</v>
       </c>
@@ -6042,7 +6041,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>364</v>
       </c>
@@ -6062,7 +6061,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>366</v>
       </c>
@@ -6082,7 +6081,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>369</v>
       </c>
@@ -6102,7 +6101,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>371</v>
       </c>
@@ -6122,7 +6121,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>334</v>
       </c>
@@ -6142,7 +6141,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>378</v>
       </c>
@@ -6162,18 +6161,18 @@
         <v>527</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -6191,7 +6190,7 @@
       </c>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>639</v>
       </c>
@@ -6211,7 +6210,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>642</v>
       </c>
@@ -6228,7 +6227,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>645</v>
       </c>
@@ -6248,7 +6247,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>648</v>
       </c>
@@ -6268,7 +6267,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>480</v>
       </c>
@@ -6288,7 +6287,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>652</v>
       </c>
@@ -6308,7 +6307,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>654</v>
       </c>
@@ -6328,19 +6327,19 @@
         <v>780</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>868</v>
       </c>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -6360,7 +6359,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>346</v>
       </c>
@@ -6380,7 +6379,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" s="3" customFormat="1">
       <c r="A34" s="3" t="s">
         <v>642</v>
       </c>
@@ -6400,7 +6399,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" s="3" customFormat="1">
       <c r="A35" s="3" t="s">
         <v>835</v>
       </c>
@@ -6420,7 +6419,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" s="3" customFormat="1">
       <c r="A36" s="3" t="s">
         <v>481</v>
       </c>
@@ -6440,7 +6439,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" s="3" customFormat="1">
       <c r="A37" s="3" t="s">
         <v>480</v>
       </c>
@@ -6460,7 +6459,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" s="3" customFormat="1">
       <c r="A38" s="3" t="s">
         <v>837</v>
       </c>
@@ -6480,7 +6479,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" s="3" customFormat="1">
       <c r="A39" s="3" t="s">
         <v>839</v>
       </c>
@@ -6500,7 +6499,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" s="3" customFormat="1">
       <c r="A40" s="3" t="s">
         <v>652</v>
       </c>
@@ -6520,7 +6519,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" s="3" customFormat="1">
       <c r="A41" s="3" t="s">
         <v>654</v>
       </c>
@@ -6540,7 +6539,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" s="3" customFormat="1">
       <c r="A42" s="3" t="s">
         <v>378</v>
       </c>
@@ -6560,7 +6559,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" s="3" customFormat="1">
       <c r="A43" s="3" t="s">
         <v>645</v>
       </c>
@@ -6580,19 +6579,19 @@
         <v>889</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" s="3" customFormat="1">
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" s="3" customFormat="1">
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" s="3" customFormat="1">
       <c r="A46" s="10" t="s">
         <v>890</v>
       </c>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" s="3" customFormat="1">
       <c r="A47" s="3" t="s">
         <v>642</v>
       </c>
@@ -6612,7 +6611,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" s="3" customFormat="1">
       <c r="A48" s="3" t="s">
         <v>837</v>
       </c>
@@ -6632,13 +6631,13 @@
         <v>876</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" s="3" customFormat="1">
       <c r="A50" s="10" t="s">
         <v>893</v>
       </c>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" s="3" customFormat="1">
       <c r="A51" s="3" t="s">
         <v>837</v>
       </c>
@@ -6658,7 +6657,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>894</v>
       </c>
@@ -6678,53 +6677,18 @@
         <v>897</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>898</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6">
       <c r="A58" s="11" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" t="s">
-        <v>7</v>
-      </c>
-      <c r="E59" t="s">
-        <v>8</v>
-      </c>
+        <v>971</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="F59"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>545</v>
-      </c>
-      <c r="B60">
-        <v>3</v>
-      </c>
-      <c r="C60" t="s">
-        <v>957</v>
-      </c>
-      <c r="D60" t="s">
-        <v>958</v>
-      </c>
-      <c r="E60" t="s">
-        <v>959</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>972</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6734,13 +6698,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F154"/>
+  <dimension ref="A1:F156"/>
   <sheetViews>
     <sheetView topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="D159" sqref="D159"/>
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="34.5" customWidth="1"/>
@@ -6749,7 +6713,7 @@
     <col min="6" max="6" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6769,7 +6733,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>251</v>
       </c>
@@ -6789,7 +6753,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>255</v>
       </c>
@@ -6809,7 +6773,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>259</v>
       </c>
@@ -6829,7 +6793,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>263</v>
       </c>
@@ -6849,7 +6813,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>267</v>
       </c>
@@ -6869,7 +6833,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>270</v>
       </c>
@@ -6889,7 +6853,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>272</v>
       </c>
@@ -6909,7 +6873,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>276</v>
       </c>
@@ -6929,7 +6893,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>279</v>
       </c>
@@ -6949,7 +6913,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>282</v>
       </c>
@@ -6969,7 +6933,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>285</v>
       </c>
@@ -6989,7 +6953,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>289</v>
       </c>
@@ -7009,7 +6973,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>292</v>
       </c>
@@ -7029,7 +6993,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>296</v>
       </c>
@@ -7049,7 +7013,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>248</v>
       </c>
@@ -7069,7 +7033,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>301</v>
       </c>
@@ -7089,7 +7053,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>304</v>
       </c>
@@ -7109,7 +7073,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>308</v>
       </c>
@@ -7129,7 +7093,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>310</v>
       </c>
@@ -7149,7 +7113,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>224</v>
       </c>
@@ -7169,7 +7133,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>222</v>
       </c>
@@ -7189,7 +7153,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>316</v>
       </c>
@@ -7209,7 +7173,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>318</v>
       </c>
@@ -7229,7 +7193,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>321</v>
       </c>
@@ -7249,7 +7213,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>324</v>
       </c>
@@ -7269,7 +7233,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>122</v>
       </c>
@@ -7289,7 +7253,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>330</v>
       </c>
@@ -7309,7 +7273,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>333</v>
       </c>
@@ -7329,7 +7293,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>337</v>
       </c>
@@ -7349,12 +7313,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -7371,7 +7335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>251</v>
       </c>
@@ -7391,7 +7355,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>529</v>
       </c>
@@ -7411,7 +7375,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>255</v>
       </c>
@@ -7431,7 +7395,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>534</v>
       </c>
@@ -7451,7 +7415,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>259</v>
       </c>
@@ -7471,7 +7435,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>537</v>
       </c>
@@ -7491,7 +7455,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>541</v>
       </c>
@@ -7511,7 +7475,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>544</v>
       </c>
@@ -7531,7 +7495,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>263</v>
       </c>
@@ -7551,7 +7515,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>267</v>
       </c>
@@ -7571,7 +7535,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>270</v>
       </c>
@@ -7591,7 +7555,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>548</v>
       </c>
@@ -7611,7 +7575,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>272</v>
       </c>
@@ -7631,7 +7595,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>276</v>
       </c>
@@ -7651,7 +7615,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>279</v>
       </c>
@@ -7671,7 +7635,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>553</v>
       </c>
@@ -7691,7 +7655,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>285</v>
       </c>
@@ -7711,7 +7675,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>289</v>
       </c>
@@ -7731,7 +7695,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>558</v>
       </c>
@@ -7751,7 +7715,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>292</v>
       </c>
@@ -7771,7 +7735,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>561</v>
       </c>
@@ -7791,7 +7755,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>296</v>
       </c>
@@ -7811,7 +7775,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>248</v>
       </c>
@@ -7828,7 +7792,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>301</v>
       </c>
@@ -7848,7 +7812,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>304</v>
       </c>
@@ -7868,7 +7832,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>308</v>
       </c>
@@ -7888,7 +7852,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>310</v>
       </c>
@@ -7908,7 +7872,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>316</v>
       </c>
@@ -7928,7 +7892,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>318</v>
       </c>
@@ -7945,7 +7909,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>567</v>
       </c>
@@ -7965,7 +7929,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>569</v>
       </c>
@@ -7985,7 +7949,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>573</v>
       </c>
@@ -8005,7 +7969,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>577</v>
       </c>
@@ -8025,7 +7989,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>580</v>
       </c>
@@ -8045,7 +8009,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>583</v>
       </c>
@@ -8065,7 +8029,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>321</v>
       </c>
@@ -8085,7 +8049,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>324</v>
       </c>
@@ -8105,7 +8069,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>589</v>
       </c>
@@ -8125,7 +8089,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>122</v>
       </c>
@@ -8145,7 +8109,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>592</v>
       </c>
@@ -8165,7 +8129,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>596</v>
       </c>
@@ -8185,7 +8149,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>598</v>
       </c>
@@ -8205,7 +8169,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>600</v>
       </c>
@@ -8225,7 +8189,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>330</v>
       </c>
@@ -8245,7 +8209,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>603</v>
       </c>
@@ -8262,7 +8226,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>512</v>
       </c>
@@ -8282,7 +8246,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>337</v>
       </c>
@@ -8302,12 +8266,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6">
       <c r="A87" s="1" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -8325,7 +8289,7 @@
       </c>
       <c r="F89"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>255</v>
       </c>
@@ -8345,7 +8309,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>688</v>
       </c>
@@ -8365,7 +8329,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>668</v>
       </c>
@@ -8385,7 +8349,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
         <v>693</v>
       </c>
@@ -8405,7 +8369,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>697</v>
       </c>
@@ -8425,7 +8389,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>701</v>
       </c>
@@ -8445,7 +8409,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>272</v>
       </c>
@@ -8465,7 +8429,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>704</v>
       </c>
@@ -8485,7 +8449,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6">
       <c r="A98" t="s">
         <v>707</v>
       </c>
@@ -8505,7 +8469,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6">
       <c r="A99" t="s">
         <v>553</v>
       </c>
@@ -8525,7 +8489,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
         <v>710</v>
       </c>
@@ -8545,7 +8509,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6">
       <c r="A101" t="s">
         <v>289</v>
       </c>
@@ -8565,7 +8529,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6">
       <c r="A102" t="s">
         <v>715</v>
       </c>
@@ -8585,7 +8549,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6">
       <c r="A103" t="s">
         <v>561</v>
       </c>
@@ -8602,7 +8566,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
         <v>718</v>
       </c>
@@ -8622,7 +8586,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
         <v>684</v>
       </c>
@@ -8639,7 +8603,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
         <v>724</v>
       </c>
@@ -8659,7 +8623,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
         <v>569</v>
       </c>
@@ -8676,7 +8640,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6">
       <c r="A108" t="s">
         <v>580</v>
       </c>
@@ -8693,7 +8657,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6">
       <c r="A109" t="s">
         <v>728</v>
       </c>
@@ -8713,7 +8677,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6">
       <c r="A110" t="s">
         <v>324</v>
       </c>
@@ -8733,7 +8697,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6">
       <c r="A111" t="s">
         <v>732</v>
       </c>
@@ -8753,7 +8717,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6">
       <c r="A112" t="s">
         <v>736</v>
       </c>
@@ -8770,7 +8734,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6">
       <c r="A113" t="s">
         <v>738</v>
       </c>
@@ -8790,12 +8754,12 @@
         <v>252</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6">
       <c r="A116" s="1" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -8815,7 +8779,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6">
       <c r="A118" t="s">
         <v>783</v>
       </c>
@@ -8835,7 +8799,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6">
       <c r="A119" t="s">
         <v>732</v>
       </c>
@@ -8855,7 +8819,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
         <v>693</v>
       </c>
@@ -8875,7 +8839,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
         <v>272</v>
       </c>
@@ -8895,7 +8859,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
         <v>787</v>
       </c>
@@ -8915,7 +8879,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6">
       <c r="A123" t="s">
         <v>790</v>
       </c>
@@ -8935,7 +8899,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6">
       <c r="A124" t="s">
         <v>738</v>
       </c>
@@ -8955,7 +8919,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6">
       <c r="A125" t="s">
         <v>869</v>
       </c>
@@ -8975,7 +8939,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6">
       <c r="A126" t="s">
         <v>707</v>
       </c>
@@ -8995,7 +8959,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6">
       <c r="A127" t="s">
         <v>793</v>
       </c>
@@ -9015,7 +8979,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6">
       <c r="A128" t="s">
         <v>715</v>
       </c>
@@ -9035,7 +8999,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6">
       <c r="A129" t="s">
         <v>561</v>
       </c>
@@ -9055,7 +9019,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6">
       <c r="A130" t="s">
         <v>796</v>
       </c>
@@ -9075,7 +9039,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6">
       <c r="A131" t="s">
         <v>798</v>
       </c>
@@ -9095,7 +9059,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6">
       <c r="A132" t="s">
         <v>324</v>
       </c>
@@ -9115,7 +9079,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6">
       <c r="A133" t="s">
         <v>801</v>
       </c>
@@ -9135,7 +9099,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
         <v>589</v>
       </c>
@@ -9155,7 +9119,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6">
       <c r="A135" t="s">
         <v>803</v>
       </c>
@@ -9175,7 +9139,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6">
       <c r="A136" t="s">
         <v>805</v>
       </c>
@@ -9195,7 +9159,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6">
       <c r="A137" t="s">
         <v>808</v>
       </c>
@@ -9215,20 +9179,20 @@
         <v>637</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6">
       <c r="F138"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6">
       <c r="A139" s="1" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6">
       <c r="A142" s="11" t="s">
         <v>912</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6">
       <c r="A143" s="7" t="s">
         <v>0</v>
       </c>
@@ -9245,7 +9209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6">
       <c r="A144" s="7" t="s">
         <v>913</v>
       </c>
@@ -9265,7 +9229,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6">
       <c r="A145" s="7" t="s">
         <v>899</v>
       </c>
@@ -9285,17 +9249,17 @@
         <v>923</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6">
       <c r="A148" s="11" t="s">
         <v>924</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6">
       <c r="A150" s="11" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6">
       <c r="A151" t="s">
         <v>0</v>
       </c>
@@ -9312,7 +9276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6">
       <c r="A152" t="s">
         <v>732</v>
       </c>
@@ -9326,33 +9290,33 @@
         <v>730</v>
       </c>
       <c r="E152" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="F152" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6">
       <c r="A153" t="s">
+        <v>958</v>
+      </c>
+      <c r="B153">
+        <v>2</v>
+      </c>
+      <c r="C153" t="s">
+        <v>959</v>
+      </c>
+      <c r="D153" t="s">
+        <v>960</v>
+      </c>
+      <c r="E153" t="s">
         <v>961</v>
       </c>
-      <c r="B153">
-        <v>2</v>
-      </c>
-      <c r="C153" t="s">
-        <v>962</v>
-      </c>
-      <c r="D153" t="s">
-        <v>963</v>
-      </c>
-      <c r="E153" t="s">
-        <v>964</v>
-      </c>
       <c r="F153" s="2" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
       <c r="A154" t="s">
         <v>935</v>
       </c>
@@ -9360,16 +9324,21 @@
         <v>2</v>
       </c>
       <c r="C154" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="D154" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="E154" t="s">
         <v>937</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>969</v>
+        <v>966</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" s="11" t="s">
+        <v>970</v>
       </c>
     </row>
   </sheetData>
@@ -9381,13 +9350,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="37.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
@@ -9396,7 +9365,7 @@
     <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -9413,7 +9382,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -9430,7 +9399,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -9447,7 +9416,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -9458,7 +9427,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -9469,7 +9438,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -9480,7 +9449,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -9491,7 +9460,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -9505,7 +9474,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -9516,7 +9485,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -9527,7 +9496,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -9544,7 +9513,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -9555,7 +9524,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>87</v>
       </c>
@@ -9572,15 +9541,15 @@
         <v>524</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="D18" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>742</v>
       </c>
@@ -9591,7 +9560,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="7" t="s">
         <v>612</v>
       </c>
@@ -9605,7 +9574,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>747</v>
       </c>
@@ -9616,7 +9585,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>744</v>
       </c>
@@ -9628,10 +9597,10 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -9648,7 +9617,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -9665,7 +9634,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -9679,7 +9648,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>617</v>
       </c>
@@ -9693,10 +9662,10 @@
         <v>758</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>334</v>
       </c>
@@ -9716,17 +9685,17 @@
         <v>855</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="7"/>
       <c r="B33" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
         <v>887</v>
       </c>
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>747</v>
       </c>
@@ -9740,30 +9709,30 @@
         <v>867</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" s="7" t="s">
         <v>891</v>
       </c>
       <c r="B38" s="7"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" s="11" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" s="11"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" s="11" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" s="12" customFormat="1">
       <c r="A44" s="12" t="s">
         <v>948</v>
       </c>
@@ -9777,7 +9746,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>334</v>
       </c>
@@ -9797,7 +9766,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>733</v>
       </c>
@@ -9817,7 +9786,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" s="12" customFormat="1">
       <c r="A49" s="12" t="s">
         <v>955</v>
       </c>
@@ -9828,7 +9797,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -9842,7 +9811,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="B51" t="s">
         <v>55</v>
       </c>
@@ -9850,7 +9819,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -9864,12 +9833,17 @@
         <v>956</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="B53" t="s">
         <v>58</v>
       </c>
       <c r="C53" t="s">
         <v>953</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="11" t="s">
+        <v>970</v>
       </c>
     </row>
   </sheetData>
@@ -9886,14 +9860,14 @@
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="52.33203125" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="2"/>
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -9908,7 +9882,7 @@
       </c>
       <c r="E1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>742</v>
       </c>
@@ -9923,7 +9897,7 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>743</v>
       </c>
@@ -9938,7 +9912,7 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -9953,7 +9927,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -9968,7 +9942,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -9983,7 +9957,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -9998,7 +9972,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -10013,7 +9987,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>614</v>
       </c>
@@ -10028,7 +10002,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>384</v>
       </c>
@@ -10043,7 +10017,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -10058,7 +10032,7 @@
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -10073,7 +10047,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -10088,7 +10062,7 @@
       </c>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>746</v>
       </c>
@@ -10103,7 +10077,7 @@
       </c>
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -10118,7 +10092,7 @@
       </c>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -10133,7 +10107,7 @@
       </c>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -10148,7 +10122,7 @@
       </c>
       <c r="E17"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -10163,7 +10137,7 @@
       </c>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>852</v>
       </c>
@@ -10178,7 +10152,7 @@
       </c>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>846</v>
       </c>
@@ -10193,7 +10167,7 @@
       </c>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>390</v>
       </c>
@@ -10208,7 +10182,7 @@
       </c>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -10223,7 +10197,7 @@
       </c>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -10238,7 +10212,7 @@
       </c>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -10253,7 +10227,7 @@
       </c>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -10268,7 +10242,7 @@
       </c>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -10283,7 +10257,7 @@
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>392</v>
       </c>
@@ -10298,7 +10272,7 @@
       </c>
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -10313,7 +10287,7 @@
       </c>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -10328,7 +10302,7 @@
       </c>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -10343,7 +10317,7 @@
       </c>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -10358,7 +10332,7 @@
       </c>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -10373,7 +10347,7 @@
       </c>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -10388,7 +10362,7 @@
       </c>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>398</v>
       </c>
@@ -10403,7 +10377,7 @@
       </c>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>400</v>
       </c>
@@ -10418,7 +10392,7 @@
       </c>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -10433,7 +10407,7 @@
       </c>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>402</v>
       </c>
@@ -10448,7 +10422,7 @@
       </c>
       <c r="E37"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -10463,7 +10437,7 @@
       </c>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -10478,7 +10452,7 @@
       </c>
       <c r="E39"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -10493,7 +10467,7 @@
       </c>
       <c r="E40"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -10508,7 +10482,7 @@
       </c>
       <c r="E41"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>406</v>
       </c>
@@ -10523,7 +10497,7 @@
       </c>
       <c r="E42"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -10538,7 +10512,7 @@
       </c>
       <c r="E43"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>619</v>
       </c>
@@ -10553,7 +10527,7 @@
       </c>
       <c r="E44"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>408</v>
       </c>
@@ -10568,7 +10542,7 @@
       </c>
       <c r="E45"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>73</v>
       </c>
@@ -10583,7 +10557,7 @@
       </c>
       <c r="E46"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>75</v>
       </c>
@@ -10598,7 +10572,7 @@
       </c>
       <c r="E47"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>77</v>
       </c>
@@ -10613,7 +10587,7 @@
       </c>
       <c r="E48"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>79</v>
       </c>
@@ -10628,7 +10602,7 @@
       </c>
       <c r="E49"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -10643,7 +10617,7 @@
       </c>
       <c r="E50"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -10658,7 +10632,7 @@
       </c>
       <c r="E51"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>412</v>
       </c>
@@ -10673,7 +10647,7 @@
       </c>
       <c r="E52"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -10688,7 +10662,7 @@
       </c>
       <c r="E53"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>395</v>
       </c>
@@ -10703,7 +10677,7 @@
       </c>
       <c r="E54"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>83</v>
       </c>
@@ -10718,7 +10692,7 @@
       </c>
       <c r="E55"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -10733,7 +10707,7 @@
       </c>
       <c r="E56"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>71</v>
       </c>
@@ -10748,7 +10722,7 @@
       </c>
       <c r="E57"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>86</v>
       </c>
@@ -10763,7 +10737,7 @@
       </c>
       <c r="E58"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>84</v>
       </c>
@@ -10778,7 +10752,7 @@
       </c>
       <c r="E59"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>87</v>
       </c>
@@ -10793,7 +10767,7 @@
       </c>
       <c r="E60"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -10808,7 +10782,7 @@
       </c>
       <c r="E61"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="E62"/>
     </row>
   </sheetData>
@@ -10824,16 +10798,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E96E553-B9B7-3A43-9A19-9B2DEFC1133B}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -10843,7 +10817,7 @@
       <c r="E1"/>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -10851,7 +10825,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>742</v>
       </c>
@@ -10859,7 +10833,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>743</v>
       </c>
@@ -10867,7 +10841,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -10875,7 +10849,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -10883,7 +10857,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -10891,7 +10865,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -10899,7 +10873,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -10907,7 +10881,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -10915,7 +10889,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -10923,7 +10897,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -10931,7 +10905,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>852</v>
       </c>
@@ -10939,7 +10913,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>846</v>
       </c>
@@ -10947,7 +10921,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -10955,7 +10929,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>390</v>
       </c>
@@ -10963,7 +10937,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -10971,7 +10945,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -10979,7 +10953,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -10987,7 +10961,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>412</v>
       </c>
@@ -10995,7 +10969,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -11003,7 +10977,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>614</v>
       </c>
@@ -11011,7 +10985,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -11019,7 +10993,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -11027,7 +11001,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -11035,7 +11009,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>384</v>
       </c>
@@ -11043,7 +11017,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>392</v>
       </c>
@@ -11051,7 +11025,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -11059,7 +11033,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>395</v>
       </c>
@@ -11067,7 +11041,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -11075,7 +11049,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -11083,7 +11057,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -11091,7 +11065,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -11099,7 +11073,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -11107,7 +11081,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -11115,7 +11089,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>398</v>
       </c>
@@ -11123,7 +11097,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>400</v>
       </c>
@@ -11131,7 +11105,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -11139,7 +11113,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -11147,7 +11121,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -11155,7 +11129,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>402</v>
       </c>
@@ -11163,7 +11137,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -11171,7 +11145,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -11179,7 +11153,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -11187,7 +11161,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -11195,7 +11169,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>406</v>
       </c>
@@ -11203,7 +11177,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>104</v>
       </c>
@@ -11211,7 +11185,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>30</v>
       </c>
@@ -11219,7 +11193,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -11227,7 +11201,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>32</v>
       </c>
@@ -11235,7 +11209,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>619</v>
       </c>
@@ -11243,7 +11217,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>408</v>
       </c>
@@ -11252,7 +11226,7 @@
       </c>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>73</v>
       </c>
@@ -11262,7 +11236,7 @@
       <c r="C53" s="4"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -11271,7 +11245,7 @@
       </c>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>75</v>
       </c>
@@ -11280,7 +11254,7 @@
       </c>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -11289,7 +11263,7 @@
       </c>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -11297,7 +11271,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -11305,7 +11279,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>79</v>
       </c>
@@ -11313,7 +11287,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
added issues found on 2021-12-14
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85B6505-847F-ED45-8DB7-7ABB09D4718A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C543523-3096-154F-9ABF-829D840E73D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1480" windowWidth="27660" windowHeight="15040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1760" yWindow="3760" windowWidth="22700" windowHeight="12680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="987">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="1015">
   <si>
     <t>sid</t>
   </si>
@@ -2989,13 +2989,97 @@
   </si>
   <si>
     <t>Rechecked on Nov 1st, all known issues are fixed</t>
+  </si>
+  <si>
+    <t>Checked on Dec 14th, identified following issues:</t>
+  </si>
+  <si>
+    <t>OBI_0001620</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Geographic location|Geolocation</t>
+  </si>
+  <si>
+    <t>gates_score_moz | general/general_umsp | gates_score_nig | gates_score_seasonal | gates_score_sm_crt</t>
+  </si>
+  <si>
+    <t>OBI_0001621</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>GAZ_00000448</t>
+  </si>
+  <si>
+    <t>Household|Community|Participant</t>
+  </si>
+  <si>
+    <t>icemr_west_africa | gates_gamin | gates_gems_huas | gates_score_moz | icemr_prism2_border_cohort | gates_gems1a | general/general_umsp | gates_gems | gates_vida | gates_elicit | icemr_india_cx | general/general_kalifabougou | icemr_amazonia_brazil | icemr_india_meghalaya | gates_washb_kenya | gates_washb_bangladesh | gates_score_nig | gates_gems1a_huas | gates_mordor | gates_perch | icemr_malawi | general/general_promote | icemr_india_cohort | gates_score_burundi | icemr_south_asia | gates_vida_hucs_kenya | gates_sip | gates_score_five_country | gates_score_seasonal | icemr_prism2 | gates_score_sm_crt | icemr_india_behavior | icemr_southeast_asia | icemr_prism | gates_provide | gates_score_sm_cohort | icemr_amazonia_peru | icemr_india_severe_malaria | icemr_myanmar | gates_llineup | gates_vida_hucs_gambia_mali | gates_score_rwanda | icemr_southern_africa | gates_maled | gates_ganc | gates_score_zanzibar | icemr_india_fever_surv</t>
+  </si>
+  <si>
+    <t>parent changed in general_umsp.owl and gates_score_seasonal.owl, shall make the same changes to other datasets?</t>
+  </si>
+  <si>
+    <t>under 'Participant' in the icemr_india_fever_surv.owl, is it correct?</t>
+  </si>
+  <si>
+    <t>Checked on Dec 14th, no issue was found</t>
+  </si>
+  <si>
+    <t>Occupation location</t>
+  </si>
+  <si>
+    <t>EUPATH_0050139|EUPATH_0022116</t>
+  </si>
+  <si>
+    <t>Polio serotype 1 titer, by microneutralization result</t>
+  </si>
+  <si>
+    <t>EUPATH_0011290|EUPATH_0036527|EUPATH_0011518</t>
+  </si>
+  <si>
+    <t>Raw antibody titer test result|Maternal blood raw antibody titer test result</t>
+  </si>
+  <si>
+    <t>Polio serotype 2 titer, by microneutralization result</t>
+  </si>
+  <si>
+    <t>EUPATH_0011291|EUPATH_0036528|EUPATH_0011474</t>
+  </si>
+  <si>
+    <t>Polio serotype 3 titer, by microneutralization result</t>
+  </si>
+  <si>
+    <t>EUPATH_0036529|EUPATH_0011292|EUPATH_0011519</t>
+  </si>
+  <si>
+    <t>Maternal blood raw antibody titer test result|Raw antibody titer test result</t>
+  </si>
+  <si>
+    <t>Add comments to redmine: https://redmine.apidb.org/issues/43508</t>
+  </si>
+  <si>
+    <t>Two same label terms with different IDs under 'Raw antibody titer test result'</t>
+  </si>
+  <si>
+    <t>gates_mordor.owl</t>
+  </si>
+  <si>
+    <t>person-day</t>
+  </si>
+  <si>
+    <t>No IRI assigned</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3156,6 +3240,13 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3503,7 +3594,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3517,6 +3608,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3873,10 +3965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5905,6 +5997,11 @@
         <v>982</v>
       </c>
     </row>
+    <row r="140" spans="1:5">
+      <c r="A140" s="11" t="s">
+        <v>999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -5913,10 +6010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6775,7 +6872,113 @@
       </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="F59"/>
+      <c r="A59" s="11"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="11" t="s">
+        <v>987</v>
+      </c>
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D62" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" t="s">
+        <v>633</v>
+      </c>
+      <c r="F62" s="13" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B63">
+        <v>3</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F63" s="13" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B64">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D64" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D65" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>1011</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6785,10 +6988,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F167"/>
+  <dimension ref="A1:F173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="C167" sqref="C167"/>
+    <sheetView topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="A169" sqref="A169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9543,6 +9746,91 @@
         <v>986</v>
       </c>
     </row>
+    <row r="169" spans="1:6">
+      <c r="A169" s="11" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="A170" t="s">
+        <v>0</v>
+      </c>
+      <c r="B170" t="s">
+        <v>10</v>
+      </c>
+      <c r="C170" t="s">
+        <v>2</v>
+      </c>
+      <c r="D170" t="s">
+        <v>11</v>
+      </c>
+      <c r="E170" t="s">
+        <v>3</v>
+      </c>
+      <c r="F170" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="A171" t="s">
+        <v>988</v>
+      </c>
+      <c r="B171">
+        <v>2</v>
+      </c>
+      <c r="C171" t="s">
+        <v>989</v>
+      </c>
+      <c r="D171" t="s">
+        <v>990</v>
+      </c>
+      <c r="E171" t="s">
+        <v>991</v>
+      </c>
+      <c r="F171" s="13" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="A172" t="s">
+        <v>992</v>
+      </c>
+      <c r="B172">
+        <v>2</v>
+      </c>
+      <c r="C172" t="s">
+        <v>993</v>
+      </c>
+      <c r="D172" t="s">
+        <v>990</v>
+      </c>
+      <c r="E172" t="s">
+        <v>991</v>
+      </c>
+      <c r="F172" s="13" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
+      <c r="A173" t="s">
+        <v>994</v>
+      </c>
+      <c r="B173">
+        <v>3</v>
+      </c>
+      <c r="C173" t="s">
+        <v>380</v>
+      </c>
+      <c r="D173" t="s">
+        <v>995</v>
+      </c>
+      <c r="E173" t="s">
+        <v>996</v>
+      </c>
+      <c r="F173" s="13" t="s">
+        <v>998</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F30" xr:uid="{3F2C9002-1B0A-C348-905C-32E2D16BAD66}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9552,10 +9840,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10046,6 +10334,22 @@
     <row r="55" spans="1:5">
       <c r="A55" s="11" t="s">
         <v>936</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="11" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E58" t="s">
+        <v>1014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update PROVIDE and inconsistency issue tracker
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C543523-3096-154F-9ABF-829D840E73D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EFD223-0522-1643-A842-0AA9FA9A1112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="3760" windowWidth="22700" windowHeight="12680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="2300" windowWidth="22700" windowHeight="12680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="1017">
   <si>
     <t>sid</t>
   </si>
@@ -3021,12 +3021,6 @@
     <t>icemr_west_africa | gates_gamin | gates_gems_huas | gates_score_moz | icemr_prism2_border_cohort | gates_gems1a | general/general_umsp | gates_gems | gates_vida | gates_elicit | icemr_india_cx | general/general_kalifabougou | icemr_amazonia_brazil | icemr_india_meghalaya | gates_washb_kenya | gates_washb_bangladesh | gates_score_nig | gates_gems1a_huas | gates_mordor | gates_perch | icemr_malawi | general/general_promote | icemr_india_cohort | gates_score_burundi | icemr_south_asia | gates_vida_hucs_kenya | gates_sip | gates_score_five_country | gates_score_seasonal | icemr_prism2 | gates_score_sm_crt | icemr_india_behavior | icemr_southeast_asia | icemr_prism | gates_provide | gates_score_sm_cohort | icemr_amazonia_peru | icemr_india_severe_malaria | icemr_myanmar | gates_llineup | gates_vida_hucs_gambia_mali | gates_score_rwanda | icemr_southern_africa | gates_maled | gates_ganc | gates_score_zanzibar | icemr_india_fever_surv</t>
   </si>
   <si>
-    <t>parent changed in general_umsp.owl and gates_score_seasonal.owl, shall make the same changes to other datasets?</t>
-  </si>
-  <si>
-    <t>under 'Participant' in the icemr_india_fever_surv.owl, is it correct?</t>
-  </si>
-  <si>
     <t>Checked on Dec 14th, no issue was found</t>
   </si>
   <si>
@@ -3060,12 +3054,6 @@
     <t>Maternal blood raw antibody titer test result|Raw antibody titer test result</t>
   </si>
   <si>
-    <t>Add comments to redmine: https://redmine.apidb.org/issues/43508</t>
-  </si>
-  <si>
-    <t>Two same label terms with different IDs under 'Raw antibody titer test result'</t>
-  </si>
-  <si>
     <t>gates_mordor.owl</t>
   </si>
   <si>
@@ -3073,13 +3061,31 @@
   </si>
   <si>
     <t>No IRI assigned</t>
+  </si>
+  <si>
+    <t>Add comments to redmine: https://redmine.apidb.org/issues/43508; ST - Should be EUPATH_0022116</t>
+  </si>
+  <si>
+    <t>Two same label terms with different IDs under 'Raw antibody titer test result'; ST - term under "Raw antibody titer test result" should be EUPATH_0011290. Please fix in MAL-ED</t>
+  </si>
+  <si>
+    <t>Two same label terms with different IDs under 'Raw antibody titer test result'; ST - term under "Raw antibody titer test result" should be EUPATH_0011291. Please fix in MAL-ED</t>
+  </si>
+  <si>
+    <t>Two same label terms with different IDs under 'Raw antibody titer test result'; ST - term under "Raw antibody titer test result" should be EUPATH_0011292. Please fix in MAL-ED</t>
+  </si>
+  <si>
+    <t>parent changed in general_umsp.owl and gates_score_seasonal.owl, shall make the same changes to other datasets?; ST - yes please</t>
+  </si>
+  <si>
+    <t>under 'Participant' in the icemr_india_fever_surv.owl, is it correct?; ST - No, it should be under Household. Please fix</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3971,7 +3977,7 @@
       <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
@@ -3980,7 +3986,7 @@
     <col min="5" max="5" width="55.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3997,7 +4003,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -4017,7 +4023,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -4037,7 +4043,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -4057,7 +4063,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -4077,7 +4083,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>121</v>
       </c>
@@ -4097,7 +4103,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -4117,7 +4123,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -4137,7 +4143,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -4157,7 +4163,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>133</v>
       </c>
@@ -4177,7 +4183,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>135</v>
       </c>
@@ -4197,7 +4203,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>138</v>
       </c>
@@ -4217,7 +4223,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -4237,7 +4243,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>143</v>
       </c>
@@ -4254,7 +4260,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>146</v>
       </c>
@@ -4271,7 +4277,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>148</v>
       </c>
@@ -4288,7 +4294,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>151</v>
       </c>
@@ -4305,7 +4311,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>153</v>
       </c>
@@ -4322,7 +4328,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>155</v>
       </c>
@@ -4339,7 +4345,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>157</v>
       </c>
@@ -4356,7 +4362,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>159</v>
       </c>
@@ -4373,7 +4379,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>161</v>
       </c>
@@ -4390,7 +4396,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>163</v>
       </c>
@@ -4407,7 +4413,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>165</v>
       </c>
@@ -4424,7 +4430,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>167</v>
       </c>
@@ -4441,7 +4447,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>169</v>
       </c>
@@ -4458,7 +4464,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>171</v>
       </c>
@@ -4475,7 +4481,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>173</v>
       </c>
@@ -4492,7 +4498,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>175</v>
       </c>
@@ -4509,7 +4515,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>177</v>
       </c>
@@ -4526,7 +4532,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>179</v>
       </c>
@@ -4543,7 +4549,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>181</v>
       </c>
@@ -4560,7 +4566,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>183</v>
       </c>
@@ -4577,7 +4583,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>185</v>
       </c>
@@ -4594,7 +4600,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>187</v>
       </c>
@@ -4611,7 +4617,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>189</v>
       </c>
@@ -4628,7 +4634,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>191</v>
       </c>
@@ -4645,7 +4651,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>193</v>
       </c>
@@ -4662,7 +4668,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>195</v>
       </c>
@@ -4679,7 +4685,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>197</v>
       </c>
@@ -4696,7 +4702,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>199</v>
       </c>
@@ -4713,7 +4719,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>201</v>
       </c>
@@ -4730,7 +4736,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>203</v>
       </c>
@@ -4747,7 +4753,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>205</v>
       </c>
@@ -4764,7 +4770,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>207</v>
       </c>
@@ -4781,7 +4787,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>209</v>
       </c>
@@ -4798,7 +4804,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>212</v>
       </c>
@@ -4815,7 +4821,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>215</v>
       </c>
@@ -4832,7 +4838,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>218</v>
       </c>
@@ -4849,7 +4855,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>221</v>
       </c>
@@ -4866,7 +4872,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>223</v>
       </c>
@@ -4883,7 +4889,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>225</v>
       </c>
@@ -4900,7 +4906,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>228</v>
       </c>
@@ -4917,7 +4923,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>475</v>
       </c>
@@ -4934,7 +4940,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>481</v>
       </c>
@@ -4951,7 +4957,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>230</v>
       </c>
@@ -4968,7 +4974,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>233</v>
       </c>
@@ -4985,7 +4991,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>236</v>
       </c>
@@ -5002,7 +5008,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>239</v>
       </c>
@@ -5019,7 +5025,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>241</v>
       </c>
@@ -5036,7 +5042,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>244</v>
       </c>
@@ -5053,7 +5059,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>247</v>
       </c>
@@ -5070,15 +5076,15 @@
         <v>487</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E63" s="6"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -5093,7 +5099,7 @@
       </c>
       <c r="E67"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>641</v>
       </c>
@@ -5110,7 +5116,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>643</v>
       </c>
@@ -5127,7 +5133,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>645</v>
       </c>
@@ -5144,7 +5150,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>648</v>
       </c>
@@ -5161,7 +5167,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>135</v>
       </c>
@@ -5178,7 +5184,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>179</v>
       </c>
@@ -5195,7 +5201,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>651</v>
       </c>
@@ -5212,7 +5218,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>215</v>
       </c>
@@ -5229,7 +5235,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>654</v>
       </c>
@@ -5246,7 +5252,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>657</v>
       </c>
@@ -5263,7 +5269,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>659</v>
       </c>
@@ -5280,7 +5286,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>662</v>
       </c>
@@ -5297,7 +5303,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>230</v>
       </c>
@@ -5311,7 +5317,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>664</v>
       </c>
@@ -5328,7 +5334,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>667</v>
       </c>
@@ -5342,7 +5348,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>599</v>
       </c>
@@ -5359,15 +5365,15 @@
         <v>753</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E84"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -5384,7 +5390,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>641</v>
       </c>
@@ -5401,7 +5407,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>140</v>
       </c>
@@ -5418,7 +5424,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>179</v>
       </c>
@@ -5435,7 +5441,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>795</v>
       </c>
@@ -5452,7 +5458,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>798</v>
       </c>
@@ -5469,7 +5475,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>215</v>
       </c>
@@ -5486,7 +5492,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>800</v>
       </c>
@@ -5503,7 +5509,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>803</v>
       </c>
@@ -5520,7 +5526,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>659</v>
       </c>
@@ -5537,7 +5543,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>662</v>
       </c>
@@ -5554,7 +5560,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>230</v>
       </c>
@@ -5571,7 +5577,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>807</v>
       </c>
@@ -5588,7 +5594,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>233</v>
       </c>
@@ -5605,7 +5611,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>811</v>
       </c>
@@ -5622,7 +5628,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>664</v>
       </c>
@@ -5639,7 +5645,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>814</v>
       </c>
@@ -5656,24 +5662,24 @@
         <v>835</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
         <v>858</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E108"/>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E109"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
         <v>878</v>
       </c>
       <c r="E110"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>0</v>
       </c>
@@ -5688,7 +5694,7 @@
       </c>
       <c r="E111"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>865</v>
       </c>
@@ -5705,7 +5711,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>868</v>
       </c>
@@ -5722,7 +5728,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>870</v>
       </c>
@@ -5739,7 +5745,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>871</v>
       </c>
@@ -5756,7 +5762,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>872</v>
       </c>
@@ -5773,7 +5779,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>874</v>
       </c>
@@ -5790,7 +5796,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>814</v>
       </c>
@@ -5807,17 +5813,17 @@
         <v>888</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
         <v>890</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>0</v>
       </c>
@@ -5831,7 +5837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>892</v>
       </c>
@@ -5848,7 +5854,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>814</v>
       </c>
@@ -5865,7 +5871,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>896</v>
       </c>
@@ -5882,7 +5888,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>899</v>
       </c>
@@ -5899,7 +5905,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>901</v>
       </c>
@@ -5916,7 +5922,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>904</v>
       </c>
@@ -5933,7 +5939,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>906</v>
       </c>
@@ -5950,17 +5956,17 @@
         <v>934</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="11" t="s">
         <v>936</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
         <v>981</v>
       </c>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>0</v>
       </c>
@@ -5975,7 +5981,7 @@
       </c>
       <c r="E136"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>901</v>
       </c>
@@ -5992,14 +5998,14 @@
         <v>932</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>982</v>
       </c>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="11" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
   </sheetData>
@@ -6012,11 +6018,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView topLeftCell="B51" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45.1640625" customWidth="1"/>
     <col min="3" max="3" width="62.33203125" customWidth="1"/>
@@ -6025,7 +6031,7 @@
     <col min="6" max="6" width="30.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -6045,7 +6051,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>339</v>
       </c>
@@ -6065,7 +6071,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>342</v>
       </c>
@@ -6085,7 +6091,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>345</v>
       </c>
@@ -6105,7 +6111,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>348</v>
       </c>
@@ -6125,7 +6131,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>350</v>
       </c>
@@ -6145,7 +6151,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>352</v>
       </c>
@@ -6165,7 +6171,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>354</v>
       </c>
@@ -6185,7 +6191,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>357</v>
       </c>
@@ -6205,7 +6211,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>360</v>
       </c>
@@ -6225,7 +6231,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>363</v>
       </c>
@@ -6245,7 +6251,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>365</v>
       </c>
@@ -6265,7 +6271,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>368</v>
       </c>
@@ -6285,7 +6291,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>370</v>
       </c>
@@ -6305,7 +6311,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>333</v>
       </c>
@@ -6325,7 +6331,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>377</v>
       </c>
@@ -6345,18 +6351,18 @@
         <v>517</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -6374,7 +6380,7 @@
       </c>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>622</v>
       </c>
@@ -6394,7 +6400,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>625</v>
       </c>
@@ -6411,7 +6417,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>628</v>
       </c>
@@ -6431,7 +6437,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>631</v>
       </c>
@@ -6451,7 +6457,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>470</v>
       </c>
@@ -6471,7 +6477,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>635</v>
       </c>
@@ -6491,7 +6497,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>637</v>
       </c>
@@ -6511,19 +6517,19 @@
         <v>762</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>842</v>
       </c>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -6543,7 +6549,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>345</v>
       </c>
@@ -6563,7 +6569,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1">
+    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>625</v>
       </c>
@@ -6583,7 +6589,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1">
+    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>817</v>
       </c>
@@ -6603,7 +6609,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1">
+    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>471</v>
       </c>
@@ -6623,7 +6629,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1">
+    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>470</v>
       </c>
@@ -6643,7 +6649,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1">
+    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>819</v>
       </c>
@@ -6663,7 +6669,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1">
+    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>821</v>
       </c>
@@ -6683,7 +6689,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1">
+    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>635</v>
       </c>
@@ -6703,7 +6709,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1">
+    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>637</v>
       </c>
@@ -6723,7 +6729,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1">
+    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>377</v>
       </c>
@@ -6743,7 +6749,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1">
+    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>628</v>
       </c>
@@ -6763,19 +6769,19 @@
         <v>855</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1">
+    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" s="3" customFormat="1">
+    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" s="3" customFormat="1">
+    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>856</v>
       </c>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" s="3" customFormat="1">
+    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>625</v>
       </c>
@@ -6795,7 +6801,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="3" customFormat="1">
+    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>819</v>
       </c>
@@ -6815,13 +6821,13 @@
         <v>850</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="3" customFormat="1">
+    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
         <v>859</v>
       </c>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" s="3" customFormat="1">
+    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>819</v>
       </c>
@@ -6841,7 +6847,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>860</v>
       </c>
@@ -6861,26 +6867,26 @@
         <v>863</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>864</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="11"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
         <v>987</v>
       </c>
       <c r="F60"/>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -6900,15 +6906,15 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="B62">
         <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="D62" t="s">
         <v>9</v>
@@ -6917,67 +6923,67 @@
         <v>633</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="B63">
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D63" t="s">
         <v>9</v>
       </c>
       <c r="E63" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="B64">
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="D64" t="s">
         <v>9</v>
       </c>
       <c r="E64" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="B65">
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="D65" t="s">
         <v>9</v>
       </c>
       <c r="E65" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>1011</v>
+        <v>1014</v>
       </c>
     </row>
   </sheetData>
@@ -6990,11 +6996,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F173"/>
   <sheetViews>
-    <sheetView topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="A169" sqref="A169"/>
+    <sheetView topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="F174" sqref="F174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="34.5" customWidth="1"/>
@@ -7003,7 +7009,7 @@
     <col min="6" max="6" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7023,7 +7029,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>250</v>
       </c>
@@ -7043,7 +7049,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>254</v>
       </c>
@@ -7063,7 +7069,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>258</v>
       </c>
@@ -7083,7 +7089,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>262</v>
       </c>
@@ -7103,7 +7109,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>266</v>
       </c>
@@ -7123,7 +7129,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>269</v>
       </c>
@@ -7143,7 +7149,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>271</v>
       </c>
@@ -7163,7 +7169,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>275</v>
       </c>
@@ -7183,7 +7189,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>278</v>
       </c>
@@ -7203,7 +7209,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>281</v>
       </c>
@@ -7223,7 +7229,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>284</v>
       </c>
@@ -7243,7 +7249,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>288</v>
       </c>
@@ -7263,7 +7269,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>291</v>
       </c>
@@ -7283,7 +7289,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>295</v>
       </c>
@@ -7303,7 +7309,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>247</v>
       </c>
@@ -7323,7 +7329,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>300</v>
       </c>
@@ -7343,7 +7349,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>303</v>
       </c>
@@ -7363,7 +7369,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>307</v>
       </c>
@@ -7383,7 +7389,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>309</v>
       </c>
@@ -7403,7 +7409,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>223</v>
       </c>
@@ -7423,7 +7429,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>221</v>
       </c>
@@ -7443,7 +7449,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>315</v>
       </c>
@@ -7463,7 +7469,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>317</v>
       </c>
@@ -7483,7 +7489,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>320</v>
       </c>
@@ -7503,7 +7509,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>323</v>
       </c>
@@ -7523,7 +7529,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>121</v>
       </c>
@@ -7543,7 +7549,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>329</v>
       </c>
@@ -7563,7 +7569,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>332</v>
       </c>
@@ -7583,7 +7589,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>336</v>
       </c>
@@ -7603,12 +7609,12 @@
         <v>301</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -7625,7 +7631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>250</v>
       </c>
@@ -7645,7 +7651,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>519</v>
       </c>
@@ -7665,7 +7671,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>254</v>
       </c>
@@ -7685,7 +7691,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>524</v>
       </c>
@@ -7705,7 +7711,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>258</v>
       </c>
@@ -7725,7 +7731,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>527</v>
       </c>
@@ -7745,7 +7751,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>531</v>
       </c>
@@ -7765,7 +7771,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>534</v>
       </c>
@@ -7785,7 +7791,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>262</v>
       </c>
@@ -7805,7 +7811,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>266</v>
       </c>
@@ -7825,7 +7831,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>269</v>
       </c>
@@ -7845,7 +7851,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>538</v>
       </c>
@@ -7865,7 +7871,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>271</v>
       </c>
@@ -7885,7 +7891,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>275</v>
       </c>
@@ -7905,7 +7911,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>278</v>
       </c>
@@ -7925,7 +7931,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>543</v>
       </c>
@@ -7945,7 +7951,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>284</v>
       </c>
@@ -7965,7 +7971,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>288</v>
       </c>
@@ -7985,7 +7991,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>548</v>
       </c>
@@ -8005,7 +8011,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>291</v>
       </c>
@@ -8025,7 +8031,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>551</v>
       </c>
@@ -8045,7 +8051,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>295</v>
       </c>
@@ -8065,7 +8071,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>247</v>
       </c>
@@ -8082,7 +8088,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>300</v>
       </c>
@@ -8102,7 +8108,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>303</v>
       </c>
@@ -8122,7 +8128,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>307</v>
       </c>
@@ -8142,7 +8148,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>309</v>
       </c>
@@ -8162,7 +8168,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>315</v>
       </c>
@@ -8182,7 +8188,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>317</v>
       </c>
@@ -8199,7 +8205,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>557</v>
       </c>
@@ -8219,7 +8225,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>559</v>
       </c>
@@ -8239,7 +8245,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>563</v>
       </c>
@@ -8259,7 +8265,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>567</v>
       </c>
@@ -8279,7 +8285,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>570</v>
       </c>
@@ -8299,7 +8305,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>573</v>
       </c>
@@ -8319,7 +8325,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>320</v>
       </c>
@@ -8339,7 +8345,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>323</v>
       </c>
@@ -8359,7 +8365,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>579</v>
       </c>
@@ -8379,7 +8385,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>121</v>
       </c>
@@ -8399,7 +8405,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>582</v>
       </c>
@@ -8419,7 +8425,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>586</v>
       </c>
@@ -8439,7 +8445,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>588</v>
       </c>
@@ -8459,7 +8465,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>590</v>
       </c>
@@ -8479,7 +8485,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>329</v>
       </c>
@@ -8499,7 +8505,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>593</v>
       </c>
@@ -8516,7 +8522,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>502</v>
       </c>
@@ -8536,7 +8542,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>336</v>
       </c>
@@ -8556,12 +8562,12 @@
         <v>301</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -8579,7 +8585,7 @@
       </c>
       <c r="F89"/>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>254</v>
       </c>
@@ -8599,7 +8605,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>671</v>
       </c>
@@ -8619,7 +8625,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>651</v>
       </c>
@@ -8639,7 +8645,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>676</v>
       </c>
@@ -8659,7 +8665,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>680</v>
       </c>
@@ -8679,7 +8685,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>684</v>
       </c>
@@ -8699,7 +8705,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>271</v>
       </c>
@@ -8719,7 +8725,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>687</v>
       </c>
@@ -8739,7 +8745,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>690</v>
       </c>
@@ -8759,7 +8765,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>543</v>
       </c>
@@ -8779,7 +8785,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>693</v>
       </c>
@@ -8799,7 +8805,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>288</v>
       </c>
@@ -8819,7 +8825,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>698</v>
       </c>
@@ -8839,7 +8845,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>551</v>
       </c>
@@ -8856,7 +8862,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>701</v>
       </c>
@@ -8876,7 +8882,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>667</v>
       </c>
@@ -8893,7 +8899,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>707</v>
       </c>
@@ -8913,7 +8919,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>559</v>
       </c>
@@ -8930,7 +8936,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>570</v>
       </c>
@@ -8947,7 +8953,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>711</v>
       </c>
@@ -8967,7 +8973,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>323</v>
       </c>
@@ -8987,7 +8993,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>715</v>
       </c>
@@ -9007,7 +9013,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>719</v>
       </c>
@@ -9024,7 +9030,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>721</v>
       </c>
@@ -9044,12 +9050,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -9069,7 +9075,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>765</v>
       </c>
@@ -9089,7 +9095,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>715</v>
       </c>
@@ -9109,7 +9115,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>676</v>
       </c>
@@ -9129,7 +9135,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>271</v>
       </c>
@@ -9149,7 +9155,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>769</v>
       </c>
@@ -9169,7 +9175,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>772</v>
       </c>
@@ -9189,7 +9195,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>721</v>
       </c>
@@ -9209,7 +9215,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>843</v>
       </c>
@@ -9229,7 +9235,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>690</v>
       </c>
@@ -9249,7 +9255,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>775</v>
       </c>
@@ -9269,7 +9275,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>698</v>
       </c>
@@ -9289,7 +9295,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>551</v>
       </c>
@@ -9309,7 +9315,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>778</v>
       </c>
@@ -9329,7 +9335,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>780</v>
       </c>
@@ -9349,7 +9355,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>323</v>
       </c>
@@ -9369,7 +9375,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>783</v>
       </c>
@@ -9389,7 +9395,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>579</v>
       </c>
@@ -9409,7 +9415,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>785</v>
       </c>
@@ -9429,7 +9435,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>787</v>
       </c>
@@ -9449,7 +9455,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>790</v>
       </c>
@@ -9469,20 +9475,20 @@
         <v>620</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F138"/>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>858</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="11" t="s">
         <v>878</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="7" t="s">
         <v>0</v>
       </c>
@@ -9499,7 +9505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
         <v>879</v>
       </c>
@@ -9519,7 +9525,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="7" t="s">
         <v>865</v>
       </c>
@@ -9539,17 +9545,17 @@
         <v>889</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="11" t="s">
         <v>890</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="11" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>0</v>
       </c>
@@ -9566,7 +9572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>715</v>
       </c>
@@ -9586,7 +9592,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>924</v>
       </c>
@@ -9606,7 +9612,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>901</v>
       </c>
@@ -9626,17 +9632,17 @@
         <v>932</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="11" t="s">
         <v>936</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="11" t="s">
         <v>975</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>0</v>
       </c>
@@ -9653,7 +9659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>924</v>
       </c>
@@ -9673,7 +9679,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>901</v>
       </c>
@@ -9693,7 +9699,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>976</v>
       </c>
@@ -9713,7 +9719,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>787</v>
       </c>
@@ -9733,7 +9739,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>980</v>
       </c>
@@ -9741,17 +9747,17 @@
         <v>983</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>986</v>
       </c>
     </row>
-    <row r="169" spans="1:6">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="11" t="s">
         <v>987</v>
       </c>
     </row>
-    <row r="170" spans="1:6">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>0</v>
       </c>
@@ -9771,7 +9777,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>988</v>
       </c>
@@ -9788,10 +9794,10 @@
         <v>991</v>
       </c>
       <c r="F171" s="13" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>992</v>
       </c>
@@ -9808,10 +9814,10 @@
         <v>991</v>
       </c>
       <c r="F172" s="13" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>994</v>
       </c>
@@ -9828,7 +9834,7 @@
         <v>996</v>
       </c>
       <c r="F173" s="13" t="s">
-        <v>998</v>
+        <v>1016</v>
       </c>
     </row>
   </sheetData>
@@ -9842,11 +9848,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
@@ -9855,7 +9861,7 @@
     <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -9872,7 +9878,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -9889,7 +9895,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -9906,7 +9912,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -9917,7 +9923,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -9928,7 +9934,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -9939,7 +9945,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -9950,7 +9956,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -9964,7 +9970,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -9975,7 +9981,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -9986,7 +9992,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -10003,7 +10009,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -10014,7 +10020,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -10031,15 +10037,15 @@
         <v>514</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D18" s="5"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>725</v>
       </c>
@@ -10050,7 +10056,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>602</v>
       </c>
@@ -10064,7 +10070,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>730</v>
       </c>
@@ -10075,7 +10081,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>727</v>
       </c>
@@ -10087,10 +10093,10 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -10107,7 +10113,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -10124,7 +10130,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -10138,7 +10144,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>607</v>
       </c>
@@ -10152,10 +10158,10 @@
         <v>740</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>333</v>
       </c>
@@ -10175,17 +10181,17 @@
         <v>829</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" s="3"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>853</v>
       </c>
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>730</v>
       </c>
@@ -10199,30 +10205,30 @@
         <v>841</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>857</v>
       </c>
       <c r="B38" s="7"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>858</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="11"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="12" customFormat="1">
+    <row r="44" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>914</v>
       </c>
@@ -10236,7 +10242,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>333</v>
       </c>
@@ -10256,7 +10262,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>716</v>
       </c>
@@ -10276,7 +10282,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="12" customFormat="1">
+    <row r="49" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="s">
         <v>921</v>
       </c>
@@ -10287,7 +10293,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -10301,7 +10307,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>55</v>
       </c>
@@ -10309,7 +10315,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -10323,7 +10329,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>58</v>
       </c>
@@ -10331,25 +10337,25 @@
         <v>919</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
         <v>936</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
         <v>987</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="C58" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="E58" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
     </row>
   </sheetData>
@@ -10363,10 +10369,10 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
@@ -10375,7 +10381,7 @@
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -10390,7 +10396,7 @@
       </c>
       <c r="E1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>725</v>
       </c>
@@ -10405,7 +10411,7 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>726</v>
       </c>
@@ -10420,7 +10426,7 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -10435,7 +10441,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -10450,7 +10456,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -10465,7 +10471,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -10480,7 +10486,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -10495,7 +10501,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>604</v>
       </c>
@@ -10510,7 +10516,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>383</v>
       </c>
@@ -10525,7 +10531,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -10540,7 +10546,7 @@
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -10555,7 +10561,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -10570,7 +10576,7 @@
       </c>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>729</v>
       </c>
@@ -10585,7 +10591,7 @@
       </c>
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -10600,7 +10606,7 @@
       </c>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -10615,7 +10621,7 @@
       </c>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -10630,7 +10636,7 @@
       </c>
       <c r="E17"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -10645,7 +10651,7 @@
       </c>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>828</v>
       </c>
@@ -10660,7 +10666,7 @@
       </c>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>827</v>
       </c>
@@ -10675,7 +10681,7 @@
       </c>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>387</v>
       </c>
@@ -10690,7 +10696,7 @@
       </c>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -10705,7 +10711,7 @@
       </c>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -10720,7 +10726,7 @@
       </c>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -10735,7 +10741,7 @@
       </c>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -10750,7 +10756,7 @@
       </c>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -10765,7 +10771,7 @@
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>389</v>
       </c>
@@ -10780,7 +10786,7 @@
       </c>
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>101</v>
       </c>
@@ -10795,7 +10801,7 @@
       </c>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>81</v>
       </c>
@@ -10810,7 +10816,7 @@
       </c>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -10825,7 +10831,7 @@
       </c>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -10840,7 +10846,7 @@
       </c>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -10855,7 +10861,7 @@
       </c>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -10870,7 +10876,7 @@
       </c>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>954</v>
       </c>
@@ -10885,7 +10891,7 @@
       </c>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>395</v>
       </c>
@@ -10900,7 +10906,7 @@
       </c>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>397</v>
       </c>
@@ -10915,7 +10921,7 @@
       </c>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -10930,7 +10936,7 @@
       </c>
       <c r="E37"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>399</v>
       </c>
@@ -10945,7 +10951,7 @@
       </c>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -10960,7 +10966,7 @@
       </c>
       <c r="E39"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -10975,7 +10981,7 @@
       </c>
       <c r="E40"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -10990,7 +10996,7 @@
       </c>
       <c r="E41"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>68</v>
       </c>
@@ -11005,7 +11011,7 @@
       </c>
       <c r="E42"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>402</v>
       </c>
@@ -11020,7 +11026,7 @@
       </c>
       <c r="E43"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>103</v>
       </c>
@@ -11035,7 +11041,7 @@
       </c>
       <c r="E44"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>608</v>
       </c>
@@ -11050,7 +11056,7 @@
       </c>
       <c r="E45"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>404</v>
       </c>
@@ -11065,7 +11071,7 @@
       </c>
       <c r="E46"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -11080,7 +11086,7 @@
       </c>
       <c r="E47"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>74</v>
       </c>
@@ -11095,7 +11101,7 @@
       </c>
       <c r="E48"/>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -11110,7 +11116,7 @@
       </c>
       <c r="E49"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -11125,7 +11131,7 @@
       </c>
       <c r="E50"/>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -11140,7 +11146,7 @@
       </c>
       <c r="E51"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -11155,7 +11161,7 @@
       </c>
       <c r="E52"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>405</v>
       </c>
@@ -11170,7 +11176,7 @@
       </c>
       <c r="E53"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -11185,7 +11191,7 @@
       </c>
       <c r="E54"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>392</v>
       </c>
@@ -11200,7 +11206,7 @@
       </c>
       <c r="E55"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>82</v>
       </c>
@@ -11215,7 +11221,7 @@
       </c>
       <c r="E56"/>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -11230,7 +11236,7 @@
       </c>
       <c r="E57"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -11245,7 +11251,7 @@
       </c>
       <c r="E58"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>85</v>
       </c>
@@ -11260,7 +11266,7 @@
       </c>
       <c r="E59"/>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>83</v>
       </c>
@@ -11275,7 +11281,7 @@
       </c>
       <c r="E60"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -11290,7 +11296,7 @@
       </c>
       <c r="E61"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>87</v>
       </c>
@@ -11318,16 +11324,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E96E553-B9B7-3A43-9A19-9B2DEFC1133B}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -11337,7 +11343,7 @@
       <c r="E1"/>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -11345,7 +11351,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>725</v>
       </c>
@@ -11353,7 +11359,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>726</v>
       </c>
@@ -11361,7 +11367,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -11369,7 +11375,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -11377,7 +11383,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -11385,7 +11391,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -11393,7 +11399,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -11401,7 +11407,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -11409,7 +11415,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -11417,7 +11423,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -11425,7 +11431,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>828</v>
       </c>
@@ -11433,7 +11439,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>827</v>
       </c>
@@ -11441,7 +11447,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -11449,7 +11455,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>387</v>
       </c>
@@ -11457,7 +11463,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -11465,7 +11471,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -11473,7 +11479,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -11481,7 +11487,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>405</v>
       </c>
@@ -11489,7 +11495,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -11497,7 +11503,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>604</v>
       </c>
@@ -11505,7 +11511,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -11513,7 +11519,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -11521,7 +11527,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -11529,7 +11535,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>383</v>
       </c>
@@ -11537,7 +11543,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>389</v>
       </c>
@@ -11545,7 +11551,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>101</v>
       </c>
@@ -11553,7 +11559,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>392</v>
       </c>
@@ -11561,7 +11567,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -11569,7 +11575,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -11577,7 +11583,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -11585,7 +11591,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -11593,7 +11599,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -11601,7 +11607,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -11609,7 +11615,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>395</v>
       </c>
@@ -11617,7 +11623,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>397</v>
       </c>
@@ -11625,7 +11631,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -11633,7 +11639,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -11641,7 +11647,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -11649,7 +11655,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>399</v>
       </c>
@@ -11657,7 +11663,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -11665,7 +11671,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -11673,7 +11679,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -11681,7 +11687,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>68</v>
       </c>
@@ -11689,7 +11695,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>402</v>
       </c>
@@ -11697,7 +11703,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -11705,7 +11711,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>30</v>
       </c>
@@ -11713,7 +11719,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -11721,7 +11727,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>32</v>
       </c>
@@ -11729,7 +11735,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>608</v>
       </c>
@@ -11737,7 +11743,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>404</v>
       </c>
@@ -11746,7 +11752,7 @@
       </c>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>72</v>
       </c>
@@ -11756,7 +11762,7 @@
       <c r="C53" s="4"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -11765,7 +11771,7 @@
       </c>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>74</v>
       </c>
@@ -11774,7 +11780,7 @@
       </c>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>87</v>
       </c>
@@ -11783,7 +11789,7 @@
       </c>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -11791,7 +11797,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>76</v>
       </c>
@@ -11799,7 +11805,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -11807,7 +11813,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>86</v>
       </c>

</xml_diff>

<commit_message>
fixed some issues, updated notes
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EFD223-0522-1643-A842-0AA9FA9A1112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5803FC5B-D2E9-DF4C-A26A-AC1BDCBDA8A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="2300" windowWidth="22700" windowHeight="12680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="520" windowWidth="25700" windowHeight="12680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="1017">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="1022">
   <si>
     <t>sid</t>
   </si>
@@ -3079,13 +3079,28 @@
   </si>
   <si>
     <t>under 'Participant' in the icemr_india_fever_surv.owl, is it correct?; ST - No, it should be under Household. Please fix</t>
+  </si>
+  <si>
+    <t>Fixed issues in gates MALED.</t>
+  </si>
+  <si>
+    <t>Will update when work on ICEMR myanmar</t>
+  </si>
+  <si>
+    <t>not change since icemr_india_fever_surv.owl only has 'Participant' and 'Sample' categories.</t>
+  </si>
+  <si>
+    <t>submit the issue to mordor redmine tracker</t>
+  </si>
+  <si>
+    <t>Fixed. Added 'Geolocation' and moved two terms under it in gates_score_moz, gates_score_nig, and gates_score_sm_crt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3600,7 +3615,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3615,6 +3630,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3973,11 +3989,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
+    <sheetView topLeftCell="A133" workbookViewId="0">
       <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
@@ -3986,7 +4002,7 @@
     <col min="5" max="5" width="55.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4003,7 +4019,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -4023,7 +4039,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -4043,7 +4059,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -4063,7 +4079,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -4083,7 +4099,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>121</v>
       </c>
@@ -4103,7 +4119,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -4123,7 +4139,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -4143,7 +4159,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -4163,7 +4179,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>133</v>
       </c>
@@ -4183,7 +4199,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>135</v>
       </c>
@@ -4203,7 +4219,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>138</v>
       </c>
@@ -4223,7 +4239,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -4243,7 +4259,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>143</v>
       </c>
@@ -4260,7 +4276,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>146</v>
       </c>
@@ -4277,7 +4293,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>148</v>
       </c>
@@ -4294,7 +4310,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>151</v>
       </c>
@@ -4311,7 +4327,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>153</v>
       </c>
@@ -4328,7 +4344,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>155</v>
       </c>
@@ -4345,7 +4361,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>157</v>
       </c>
@@ -4362,7 +4378,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>159</v>
       </c>
@@ -4379,7 +4395,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>161</v>
       </c>
@@ -4396,7 +4412,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>163</v>
       </c>
@@ -4413,7 +4429,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>165</v>
       </c>
@@ -4430,7 +4446,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>167</v>
       </c>
@@ -4447,7 +4463,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>169</v>
       </c>
@@ -4464,7 +4480,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>171</v>
       </c>
@@ -4481,7 +4497,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>173</v>
       </c>
@@ -4498,7 +4514,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>175</v>
       </c>
@@ -4515,7 +4531,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>177</v>
       </c>
@@ -4532,7 +4548,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>179</v>
       </c>
@@ -4549,7 +4565,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>181</v>
       </c>
@@ -4566,7 +4582,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>183</v>
       </c>
@@ -4583,7 +4599,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>185</v>
       </c>
@@ -4600,7 +4616,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>187</v>
       </c>
@@ -4617,7 +4633,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>189</v>
       </c>
@@ -4634,7 +4650,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>191</v>
       </c>
@@ -4651,7 +4667,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>193</v>
       </c>
@@ -4668,7 +4684,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>195</v>
       </c>
@@ -4685,7 +4701,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>197</v>
       </c>
@@ -4702,7 +4718,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>199</v>
       </c>
@@ -4719,7 +4735,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>201</v>
       </c>
@@ -4736,7 +4752,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>203</v>
       </c>
@@ -4753,7 +4769,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>205</v>
       </c>
@@ -4770,7 +4786,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>207</v>
       </c>
@@ -4787,7 +4803,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>209</v>
       </c>
@@ -4804,7 +4820,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>212</v>
       </c>
@@ -4821,7 +4837,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>215</v>
       </c>
@@ -4838,7 +4854,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>218</v>
       </c>
@@ -4855,7 +4871,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>221</v>
       </c>
@@ -4872,7 +4888,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>223</v>
       </c>
@@ -4889,7 +4905,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>225</v>
       </c>
@@ -4906,7 +4922,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>228</v>
       </c>
@@ -4923,7 +4939,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>475</v>
       </c>
@@ -4940,7 +4956,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>481</v>
       </c>
@@ -4957,7 +4973,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>230</v>
       </c>
@@ -4974,7 +4990,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>233</v>
       </c>
@@ -4991,7 +5007,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>236</v>
       </c>
@@ -5008,7 +5024,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>239</v>
       </c>
@@ -5025,7 +5041,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>241</v>
       </c>
@@ -5042,7 +5058,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>244</v>
       </c>
@@ -5059,7 +5075,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>247</v>
       </c>
@@ -5076,15 +5092,15 @@
         <v>487</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5">
       <c r="E63" s="6"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -5099,7 +5115,7 @@
       </c>
       <c r="E67"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>641</v>
       </c>
@@ -5116,7 +5132,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>643</v>
       </c>
@@ -5133,7 +5149,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>645</v>
       </c>
@@ -5150,7 +5166,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>648</v>
       </c>
@@ -5167,7 +5183,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>135</v>
       </c>
@@ -5184,7 +5200,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>179</v>
       </c>
@@ -5201,7 +5217,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>651</v>
       </c>
@@ -5218,7 +5234,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>215</v>
       </c>
@@ -5235,7 +5251,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>654</v>
       </c>
@@ -5252,7 +5268,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>657</v>
       </c>
@@ -5269,7 +5285,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>659</v>
       </c>
@@ -5286,7 +5302,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>662</v>
       </c>
@@ -5303,7 +5319,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>230</v>
       </c>
@@ -5317,7 +5333,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>664</v>
       </c>
@@ -5334,7 +5350,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>667</v>
       </c>
@@ -5348,7 +5364,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>599</v>
       </c>
@@ -5365,15 +5381,15 @@
         <v>753</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5">
       <c r="E84"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5">
       <c r="A86" s="1" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -5390,7 +5406,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>641</v>
       </c>
@@ -5407,7 +5423,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>140</v>
       </c>
@@ -5424,7 +5440,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>179</v>
       </c>
@@ -5441,7 +5457,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>795</v>
       </c>
@@ -5458,7 +5474,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>798</v>
       </c>
@@ -5475,7 +5491,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>215</v>
       </c>
@@ -5492,7 +5508,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>800</v>
       </c>
@@ -5509,7 +5525,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>803</v>
       </c>
@@ -5526,7 +5542,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>659</v>
       </c>
@@ -5543,7 +5559,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>662</v>
       </c>
@@ -5560,7 +5576,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>230</v>
       </c>
@@ -5577,7 +5593,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>807</v>
       </c>
@@ -5594,7 +5610,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>233</v>
       </c>
@@ -5611,7 +5627,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>811</v>
       </c>
@@ -5628,7 +5644,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>664</v>
       </c>
@@ -5645,7 +5661,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
         <v>814</v>
       </c>
@@ -5662,24 +5678,24 @@
         <v>835</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5">
       <c r="A107" s="11" t="s">
         <v>858</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5">
       <c r="E108"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5">
       <c r="E109"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5">
       <c r="A110" s="11" t="s">
         <v>878</v>
       </c>
       <c r="E110"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
         <v>0</v>
       </c>
@@ -5694,7 +5710,7 @@
       </c>
       <c r="E111"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5">
       <c r="A112" t="s">
         <v>865</v>
       </c>
@@ -5711,7 +5727,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
         <v>868</v>
       </c>
@@ -5728,7 +5744,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
         <v>870</v>
       </c>
@@ -5745,7 +5761,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
         <v>871</v>
       </c>
@@ -5762,7 +5778,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
         <v>872</v>
       </c>
@@ -5779,7 +5795,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
         <v>874</v>
       </c>
@@ -5796,7 +5812,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
         <v>814</v>
       </c>
@@ -5813,17 +5829,17 @@
         <v>888</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5">
       <c r="A120" s="11" t="s">
         <v>890</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5">
       <c r="A122" s="11" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
         <v>0</v>
       </c>
@@ -5837,7 +5853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
         <v>892</v>
       </c>
@@ -5854,7 +5870,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
         <v>814</v>
       </c>
@@ -5871,7 +5887,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
         <v>896</v>
       </c>
@@ -5888,7 +5904,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
         <v>899</v>
       </c>
@@ -5905,7 +5921,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5">
       <c r="A128" t="s">
         <v>901</v>
       </c>
@@ -5922,7 +5938,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5">
       <c r="A129" t="s">
         <v>904</v>
       </c>
@@ -5939,7 +5955,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5">
       <c r="A130" t="s">
         <v>906</v>
       </c>
@@ -5956,17 +5972,17 @@
         <v>934</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5">
       <c r="A132" s="11" t="s">
         <v>936</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5">
       <c r="A135" s="11" t="s">
         <v>981</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5">
       <c r="A136" t="s">
         <v>0</v>
       </c>
@@ -5981,7 +5997,7 @@
       </c>
       <c r="E136"/>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5">
       <c r="A137" t="s">
         <v>901</v>
       </c>
@@ -5998,12 +6014,12 @@
         <v>932</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5">
       <c r="B138" t="s">
         <v>982</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5">
       <c r="A140" s="11" t="s">
         <v>997</v>
       </c>
@@ -6016,13 +6032,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView topLeftCell="B51" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="45.1640625" customWidth="1"/>
     <col min="3" max="3" width="62.33203125" customWidth="1"/>
@@ -6031,7 +6047,7 @@
     <col min="6" max="6" width="30.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -6051,7 +6067,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>339</v>
       </c>
@@ -6071,7 +6087,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>342</v>
       </c>
@@ -6091,7 +6107,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>345</v>
       </c>
@@ -6111,7 +6127,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>348</v>
       </c>
@@ -6131,7 +6147,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>350</v>
       </c>
@@ -6151,7 +6167,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>352</v>
       </c>
@@ -6171,7 +6187,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>354</v>
       </c>
@@ -6191,7 +6207,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>357</v>
       </c>
@@ -6211,7 +6227,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>360</v>
       </c>
@@ -6231,7 +6247,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>363</v>
       </c>
@@ -6251,7 +6267,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>365</v>
       </c>
@@ -6271,7 +6287,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>368</v>
       </c>
@@ -6291,7 +6307,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>370</v>
       </c>
@@ -6311,7 +6327,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>333</v>
       </c>
@@ -6331,7 +6347,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>377</v>
       </c>
@@ -6351,18 +6367,18 @@
         <v>517</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -6380,7 +6396,7 @@
       </c>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>622</v>
       </c>
@@ -6400,7 +6416,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>625</v>
       </c>
@@ -6417,7 +6433,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>628</v>
       </c>
@@ -6437,7 +6453,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>631</v>
       </c>
@@ -6457,7 +6473,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>470</v>
       </c>
@@ -6477,7 +6493,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>635</v>
       </c>
@@ -6497,7 +6513,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>637</v>
       </c>
@@ -6517,19 +6533,19 @@
         <v>762</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>842</v>
       </c>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -6549,7 +6565,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>345</v>
       </c>
@@ -6569,7 +6585,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" s="3" customFormat="1">
       <c r="A34" s="3" t="s">
         <v>625</v>
       </c>
@@ -6589,7 +6605,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" s="3" customFormat="1">
       <c r="A35" s="3" t="s">
         <v>817</v>
       </c>
@@ -6609,7 +6625,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" s="3" customFormat="1">
       <c r="A36" s="3" t="s">
         <v>471</v>
       </c>
@@ -6629,7 +6645,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" s="3" customFormat="1">
       <c r="A37" s="3" t="s">
         <v>470</v>
       </c>
@@ -6649,7 +6665,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" s="3" customFormat="1">
       <c r="A38" s="3" t="s">
         <v>819</v>
       </c>
@@ -6669,7 +6685,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" s="3" customFormat="1">
       <c r="A39" s="3" t="s">
         <v>821</v>
       </c>
@@ -6689,7 +6705,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" s="3" customFormat="1">
       <c r="A40" s="3" t="s">
         <v>635</v>
       </c>
@@ -6709,7 +6725,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" s="3" customFormat="1">
       <c r="A41" s="3" t="s">
         <v>637</v>
       </c>
@@ -6729,7 +6745,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" s="3" customFormat="1">
       <c r="A42" s="3" t="s">
         <v>377</v>
       </c>
@@ -6749,7 +6765,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" s="3" customFormat="1">
       <c r="A43" s="3" t="s">
         <v>628</v>
       </c>
@@ -6769,19 +6785,19 @@
         <v>855</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" s="3" customFormat="1">
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" s="3" customFormat="1">
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" s="3" customFormat="1">
       <c r="A46" s="10" t="s">
         <v>856</v>
       </c>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" s="3" customFormat="1">
       <c r="A47" s="3" t="s">
         <v>625</v>
       </c>
@@ -6801,7 +6817,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" s="3" customFormat="1">
       <c r="A48" s="3" t="s">
         <v>819</v>
       </c>
@@ -6821,13 +6837,13 @@
         <v>850</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" s="3" customFormat="1">
       <c r="A50" s="10" t="s">
         <v>859</v>
       </c>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" s="3" customFormat="1">
       <c r="A51" s="3" t="s">
         <v>819</v>
       </c>
@@ -6847,7 +6863,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>860</v>
       </c>
@@ -6867,26 +6883,26 @@
         <v>863</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>864</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6">
       <c r="A58" s="11" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6">
       <c r="A59" s="11"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6">
       <c r="A60" s="11" t="s">
         <v>987</v>
       </c>
       <c r="F60"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -6906,7 +6922,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>998</v>
       </c>
@@ -6926,35 +6942,20 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="63" spans="1:6">
+      <c r="F63" s="14" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
         <v>1000</v>
-      </c>
-      <c r="B63">
-        <v>3</v>
-      </c>
-      <c r="C63" t="s">
-        <v>1001</v>
-      </c>
-      <c r="D63" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" t="s">
-        <v>1002</v>
-      </c>
-      <c r="F63" s="13" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>1003</v>
       </c>
       <c r="B64">
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="D64" t="s">
         <v>9</v>
@@ -6963,27 +6964,52 @@
         <v>1002</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="B65">
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="D65" t="s">
         <v>9</v>
       </c>
       <c r="E65" t="s">
+        <v>1002</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D66" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" t="s">
         <v>1007</v>
       </c>
-      <c r="F65" s="13" t="s">
+      <c r="F66" s="13" t="s">
         <v>1014</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="F67" s="14" t="s">
+        <v>1017</v>
       </c>
     </row>
   </sheetData>
@@ -6994,22 +7020,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F173"/>
+  <dimension ref="A1:F175"/>
   <sheetViews>
-    <sheetView topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="F174" sqref="F174"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="34.5" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" customWidth="1"/>
-    <col min="5" max="5" width="51.33203125" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="5" max="5" width="53.83203125" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7029,7 +7055,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>250</v>
       </c>
@@ -7049,7 +7075,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>254</v>
       </c>
@@ -7069,7 +7095,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>258</v>
       </c>
@@ -7089,7 +7115,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>262</v>
       </c>
@@ -7109,7 +7135,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>266</v>
       </c>
@@ -7129,7 +7155,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>269</v>
       </c>
@@ -7149,7 +7175,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>271</v>
       </c>
@@ -7169,7 +7195,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>275</v>
       </c>
@@ -7189,7 +7215,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>278</v>
       </c>
@@ -7209,7 +7235,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>281</v>
       </c>
@@ -7229,7 +7255,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>284</v>
       </c>
@@ -7249,7 +7275,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>288</v>
       </c>
@@ -7269,7 +7295,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>291</v>
       </c>
@@ -7289,7 +7315,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>295</v>
       </c>
@@ -7309,7 +7335,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>247</v>
       </c>
@@ -7329,7 +7355,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>300</v>
       </c>
@@ -7349,7 +7375,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>303</v>
       </c>
@@ -7369,7 +7395,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>307</v>
       </c>
@@ -7389,7 +7415,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>309</v>
       </c>
@@ -7409,7 +7435,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>223</v>
       </c>
@@ -7429,7 +7455,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>221</v>
       </c>
@@ -7449,7 +7475,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>315</v>
       </c>
@@ -7469,7 +7495,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>317</v>
       </c>
@@ -7489,7 +7515,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>320</v>
       </c>
@@ -7509,7 +7535,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>323</v>
       </c>
@@ -7529,7 +7555,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>121</v>
       </c>
@@ -7549,7 +7575,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>329</v>
       </c>
@@ -7569,7 +7595,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>332</v>
       </c>
@@ -7589,7 +7615,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>336</v>
       </c>
@@ -7609,12 +7635,12 @@
         <v>301</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -7631,7 +7657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>250</v>
       </c>
@@ -7651,7 +7677,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>519</v>
       </c>
@@ -7671,7 +7697,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>254</v>
       </c>
@@ -7691,7 +7717,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>524</v>
       </c>
@@ -7711,7 +7737,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>258</v>
       </c>
@@ -7731,7 +7757,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>527</v>
       </c>
@@ -7751,7 +7777,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>531</v>
       </c>
@@ -7771,7 +7797,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>534</v>
       </c>
@@ -7791,7 +7817,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>262</v>
       </c>
@@ -7811,7 +7837,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>266</v>
       </c>
@@ -7831,7 +7857,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>269</v>
       </c>
@@ -7851,7 +7877,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>538</v>
       </c>
@@ -7871,7 +7897,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>271</v>
       </c>
@@ -7891,7 +7917,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>275</v>
       </c>
@@ -7911,7 +7937,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>278</v>
       </c>
@@ -7931,7 +7957,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>543</v>
       </c>
@@ -7951,7 +7977,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>284</v>
       </c>
@@ -7971,7 +7997,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>288</v>
       </c>
@@ -7991,7 +8017,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>548</v>
       </c>
@@ -8011,7 +8037,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>291</v>
       </c>
@@ -8031,7 +8057,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>551</v>
       </c>
@@ -8051,7 +8077,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>295</v>
       </c>
@@ -8071,7 +8097,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>247</v>
       </c>
@@ -8088,7 +8114,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>300</v>
       </c>
@@ -8108,7 +8134,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>303</v>
       </c>
@@ -8128,7 +8154,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>307</v>
       </c>
@@ -8148,7 +8174,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>309</v>
       </c>
@@ -8168,7 +8194,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>315</v>
       </c>
@@ -8188,7 +8214,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>317</v>
       </c>
@@ -8205,7 +8231,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>557</v>
       </c>
@@ -8225,7 +8251,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>559</v>
       </c>
@@ -8245,7 +8271,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>563</v>
       </c>
@@ -8265,7 +8291,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>567</v>
       </c>
@@ -8285,7 +8311,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>570</v>
       </c>
@@ -8305,7 +8331,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>573</v>
       </c>
@@ -8325,7 +8351,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>320</v>
       </c>
@@ -8345,7 +8371,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>323</v>
       </c>
@@ -8365,7 +8391,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>579</v>
       </c>
@@ -8385,7 +8411,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>121</v>
       </c>
@@ -8405,7 +8431,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>582</v>
       </c>
@@ -8425,7 +8451,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>586</v>
       </c>
@@ -8445,7 +8471,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>588</v>
       </c>
@@ -8465,7 +8491,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>590</v>
       </c>
@@ -8485,7 +8511,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>329</v>
       </c>
@@ -8505,7 +8531,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>593</v>
       </c>
@@ -8522,7 +8548,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>502</v>
       </c>
@@ -8542,7 +8568,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>336</v>
       </c>
@@ -8562,12 +8588,12 @@
         <v>301</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6">
       <c r="A87" s="1" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -8585,7 +8611,7 @@
       </c>
       <c r="F89"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>254</v>
       </c>
@@ -8605,7 +8631,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>671</v>
       </c>
@@ -8625,7 +8651,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>651</v>
       </c>
@@ -8645,7 +8671,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
         <v>676</v>
       </c>
@@ -8665,7 +8691,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>680</v>
       </c>
@@ -8685,7 +8711,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>684</v>
       </c>
@@ -8705,7 +8731,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>271</v>
       </c>
@@ -8725,7 +8751,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>687</v>
       </c>
@@ -8745,7 +8771,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6">
       <c r="A98" t="s">
         <v>690</v>
       </c>
@@ -8765,7 +8791,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6">
       <c r="A99" t="s">
         <v>543</v>
       </c>
@@ -8785,7 +8811,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
         <v>693</v>
       </c>
@@ -8805,7 +8831,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6">
       <c r="A101" t="s">
         <v>288</v>
       </c>
@@ -8825,7 +8851,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6">
       <c r="A102" t="s">
         <v>698</v>
       </c>
@@ -8845,7 +8871,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6">
       <c r="A103" t="s">
         <v>551</v>
       </c>
@@ -8862,7 +8888,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
         <v>701</v>
       </c>
@@ -8882,7 +8908,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
         <v>667</v>
       </c>
@@ -8899,7 +8925,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
         <v>707</v>
       </c>
@@ -8919,7 +8945,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
         <v>559</v>
       </c>
@@ -8936,7 +8962,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6">
       <c r="A108" t="s">
         <v>570</v>
       </c>
@@ -8953,7 +8979,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6">
       <c r="A109" t="s">
         <v>711</v>
       </c>
@@ -8973,7 +8999,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6">
       <c r="A110" t="s">
         <v>323</v>
       </c>
@@ -8993,7 +9019,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6">
       <c r="A111" t="s">
         <v>715</v>
       </c>
@@ -9013,7 +9039,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6">
       <c r="A112" t="s">
         <v>719</v>
       </c>
@@ -9030,7 +9056,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6">
       <c r="A113" t="s">
         <v>721</v>
       </c>
@@ -9050,12 +9076,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6">
       <c r="A116" s="1" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -9075,7 +9101,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6">
       <c r="A118" t="s">
         <v>765</v>
       </c>
@@ -9095,7 +9121,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6">
       <c r="A119" t="s">
         <v>715</v>
       </c>
@@ -9115,7 +9141,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
         <v>676</v>
       </c>
@@ -9135,7 +9161,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
         <v>271</v>
       </c>
@@ -9155,7 +9181,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
         <v>769</v>
       </c>
@@ -9175,7 +9201,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6">
       <c r="A123" t="s">
         <v>772</v>
       </c>
@@ -9195,7 +9221,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6">
       <c r="A124" t="s">
         <v>721</v>
       </c>
@@ -9215,7 +9241,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6">
       <c r="A125" t="s">
         <v>843</v>
       </c>
@@ -9235,7 +9261,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6">
       <c r="A126" t="s">
         <v>690</v>
       </c>
@@ -9255,7 +9281,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6">
       <c r="A127" t="s">
         <v>775</v>
       </c>
@@ -9275,7 +9301,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6">
       <c r="A128" t="s">
         <v>698</v>
       </c>
@@ -9295,7 +9321,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6">
       <c r="A129" t="s">
         <v>551</v>
       </c>
@@ -9315,7 +9341,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6">
       <c r="A130" t="s">
         <v>778</v>
       </c>
@@ -9335,7 +9361,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6">
       <c r="A131" t="s">
         <v>780</v>
       </c>
@@ -9355,7 +9381,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6">
       <c r="A132" t="s">
         <v>323</v>
       </c>
@@ -9375,7 +9401,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6">
       <c r="A133" t="s">
         <v>783</v>
       </c>
@@ -9395,7 +9421,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
         <v>579</v>
       </c>
@@ -9415,7 +9441,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6">
       <c r="A135" t="s">
         <v>785</v>
       </c>
@@ -9435,7 +9461,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6">
       <c r="A136" t="s">
         <v>787</v>
       </c>
@@ -9455,7 +9481,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6">
       <c r="A137" t="s">
         <v>790</v>
       </c>
@@ -9475,20 +9501,20 @@
         <v>620</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6">
       <c r="F138"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6">
       <c r="A139" s="1" t="s">
         <v>858</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6">
       <c r="A142" s="11" t="s">
         <v>878</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6">
       <c r="A143" s="7" t="s">
         <v>0</v>
       </c>
@@ -9505,7 +9531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6">
       <c r="A144" s="7" t="s">
         <v>879</v>
       </c>
@@ -9525,7 +9551,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6">
       <c r="A145" s="7" t="s">
         <v>865</v>
       </c>
@@ -9545,17 +9571,17 @@
         <v>889</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6">
       <c r="A148" s="11" t="s">
         <v>890</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6">
       <c r="A150" s="11" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6">
       <c r="A151" t="s">
         <v>0</v>
       </c>
@@ -9572,7 +9598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6">
       <c r="A152" t="s">
         <v>715</v>
       </c>
@@ -9592,7 +9618,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6">
       <c r="A153" t="s">
         <v>924</v>
       </c>
@@ -9612,7 +9638,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6">
       <c r="A154" t="s">
         <v>901</v>
       </c>
@@ -9632,17 +9658,17 @@
         <v>932</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6">
       <c r="A156" s="11" t="s">
         <v>936</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6">
       <c r="A158" s="11" t="s">
         <v>975</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6">
       <c r="A159" t="s">
         <v>0</v>
       </c>
@@ -9659,7 +9685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6">
       <c r="A160" t="s">
         <v>924</v>
       </c>
@@ -9679,7 +9705,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6">
       <c r="A161" t="s">
         <v>901</v>
       </c>
@@ -9699,7 +9725,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6">
       <c r="A162" t="s">
         <v>976</v>
       </c>
@@ -9719,7 +9745,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6">
       <c r="A163" t="s">
         <v>787</v>
       </c>
@@ -9739,7 +9765,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6">
       <c r="A165" t="s">
         <v>980</v>
       </c>
@@ -9747,17 +9773,17 @@
         <v>983</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6">
       <c r="A167" s="1" t="s">
         <v>986</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6">
       <c r="A169" s="11" t="s">
         <v>987</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6">
       <c r="A170" t="s">
         <v>0</v>
       </c>
@@ -9777,7 +9803,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6">
       <c r="A171" t="s">
         <v>988</v>
       </c>
@@ -9797,7 +9823,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6">
       <c r="A172" t="s">
         <v>992</v>
       </c>
@@ -9817,24 +9843,34 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
+    <row r="173" spans="1:6">
+      <c r="F173" s="14" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="A174" t="s">
         <v>994</v>
       </c>
-      <c r="B173">
+      <c r="B174">
         <v>3</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C174" t="s">
         <v>380</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D174" t="s">
         <v>995</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E174" t="s">
         <v>996</v>
       </c>
-      <c r="F173" s="13" t="s">
+      <c r="F174" s="13" t="s">
         <v>1016</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="F175" s="14" t="s">
+        <v>1019</v>
       </c>
     </row>
   </sheetData>
@@ -9848,11 +9884,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="37.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
@@ -9861,7 +9897,7 @@
     <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -9878,7 +9914,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -9895,7 +9931,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -9912,7 +9948,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -9923,7 +9959,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -9934,7 +9970,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -9945,7 +9981,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -9956,7 +9992,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -9970,7 +10006,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -9981,7 +10017,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -9992,7 +10028,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -10009,7 +10045,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -10020,7 +10056,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -10037,15 +10073,15 @@
         <v>514</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="D18" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>725</v>
       </c>
@@ -10056,7 +10092,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="7" t="s">
         <v>602</v>
       </c>
@@ -10070,7 +10106,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>730</v>
       </c>
@@ -10081,7 +10117,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>727</v>
       </c>
@@ -10093,10 +10129,10 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -10113,7 +10149,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -10130,7 +10166,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -10144,7 +10180,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>607</v>
       </c>
@@ -10158,10 +10194,10 @@
         <v>740</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>333</v>
       </c>
@@ -10181,17 +10217,17 @@
         <v>829</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="7"/>
       <c r="B33" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
         <v>853</v>
       </c>
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>730</v>
       </c>
@@ -10205,30 +10241,30 @@
         <v>841</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" s="7" t="s">
         <v>857</v>
       </c>
       <c r="B38" s="7"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" s="11" t="s">
         <v>858</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" s="11"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" s="11" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" s="12" customFormat="1">
       <c r="A44" s="12" t="s">
         <v>914</v>
       </c>
@@ -10242,7 +10278,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>333</v>
       </c>
@@ -10262,7 +10298,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>716</v>
       </c>
@@ -10282,7 +10318,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" s="12" customFormat="1">
       <c r="A49" s="12" t="s">
         <v>921</v>
       </c>
@@ -10293,7 +10329,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -10307,7 +10343,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6">
       <c r="B51" t="s">
         <v>55</v>
       </c>
@@ -10315,7 +10351,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -10329,7 +10365,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6">
       <c r="B53" t="s">
         <v>58</v>
       </c>
@@ -10337,17 +10373,17 @@
         <v>919</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6">
       <c r="A55" s="11" t="s">
         <v>936</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6">
       <c r="A57" s="11" t="s">
         <v>987</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>1009</v>
       </c>
@@ -10356,6 +10392,9 @@
       </c>
       <c r="E58" t="s">
         <v>1010</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>1020</v>
       </c>
     </row>
   </sheetData>
@@ -10372,7 +10411,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
@@ -10381,7 +10420,7 @@
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -10396,7 +10435,7 @@
       </c>
       <c r="E1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>725</v>
       </c>
@@ -10411,7 +10450,7 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>726</v>
       </c>
@@ -10426,7 +10465,7 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -10441,7 +10480,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -10456,7 +10495,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -10471,7 +10510,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -10486,7 +10525,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -10501,7 +10540,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>604</v>
       </c>
@@ -10516,7 +10555,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>383</v>
       </c>
@@ -10531,7 +10570,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -10546,7 +10585,7 @@
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -10561,7 +10600,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -10576,7 +10615,7 @@
       </c>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>729</v>
       </c>
@@ -10591,7 +10630,7 @@
       </c>
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -10606,7 +10645,7 @@
       </c>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -10621,7 +10660,7 @@
       </c>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -10636,7 +10675,7 @@
       </c>
       <c r="E17"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -10651,7 +10690,7 @@
       </c>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>828</v>
       </c>
@@ -10666,7 +10705,7 @@
       </c>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>827</v>
       </c>
@@ -10681,7 +10720,7 @@
       </c>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>387</v>
       </c>
@@ -10696,7 +10735,7 @@
       </c>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -10711,7 +10750,7 @@
       </c>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -10726,7 +10765,7 @@
       </c>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -10741,7 +10780,7 @@
       </c>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -10756,7 +10795,7 @@
       </c>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -10771,7 +10810,7 @@
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>389</v>
       </c>
@@ -10786,7 +10825,7 @@
       </c>
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>101</v>
       </c>
@@ -10801,7 +10840,7 @@
       </c>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>81</v>
       </c>
@@ -10816,7 +10855,7 @@
       </c>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -10831,7 +10870,7 @@
       </c>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -10846,7 +10885,7 @@
       </c>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -10861,7 +10900,7 @@
       </c>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -10876,7 +10915,7 @@
       </c>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>954</v>
       </c>
@@ -10891,7 +10930,7 @@
       </c>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>395</v>
       </c>
@@ -10906,7 +10945,7 @@
       </c>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>397</v>
       </c>
@@ -10921,7 +10960,7 @@
       </c>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -10936,7 +10975,7 @@
       </c>
       <c r="E37"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>399</v>
       </c>
@@ -10951,7 +10990,7 @@
       </c>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -10966,7 +11005,7 @@
       </c>
       <c r="E39"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -10981,7 +11020,7 @@
       </c>
       <c r="E40"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -10996,7 +11035,7 @@
       </c>
       <c r="E41"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>68</v>
       </c>
@@ -11011,7 +11050,7 @@
       </c>
       <c r="E42"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>402</v>
       </c>
@@ -11026,7 +11065,7 @@
       </c>
       <c r="E43"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>103</v>
       </c>
@@ -11041,7 +11080,7 @@
       </c>
       <c r="E44"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>608</v>
       </c>
@@ -11056,7 +11095,7 @@
       </c>
       <c r="E45"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>404</v>
       </c>
@@ -11071,7 +11110,7 @@
       </c>
       <c r="E46"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -11086,7 +11125,7 @@
       </c>
       <c r="E47"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>74</v>
       </c>
@@ -11101,7 +11140,7 @@
       </c>
       <c r="E48"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -11116,7 +11155,7 @@
       </c>
       <c r="E49"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -11131,7 +11170,7 @@
       </c>
       <c r="E50"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -11146,7 +11185,7 @@
       </c>
       <c r="E51"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -11161,7 +11200,7 @@
       </c>
       <c r="E52"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>405</v>
       </c>
@@ -11176,7 +11215,7 @@
       </c>
       <c r="E53"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -11191,7 +11230,7 @@
       </c>
       <c r="E54"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>392</v>
       </c>
@@ -11206,7 +11245,7 @@
       </c>
       <c r="E55"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>82</v>
       </c>
@@ -11221,7 +11260,7 @@
       </c>
       <c r="E56"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -11236,7 +11275,7 @@
       </c>
       <c r="E57"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -11251,7 +11290,7 @@
       </c>
       <c r="E58"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>85</v>
       </c>
@@ -11266,7 +11305,7 @@
       </c>
       <c r="E59"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>83</v>
       </c>
@@ -11281,7 +11320,7 @@
       </c>
       <c r="E60"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -11296,7 +11335,7 @@
       </c>
       <c r="E61"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>87</v>
       </c>
@@ -11328,12 +11367,12 @@
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -11343,7 +11382,7 @@
       <c r="E1"/>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -11351,7 +11390,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>725</v>
       </c>
@@ -11359,7 +11398,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>726</v>
       </c>
@@ -11367,7 +11406,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -11375,7 +11414,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -11383,7 +11422,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -11391,7 +11430,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -11399,7 +11438,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -11407,7 +11446,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -11415,7 +11454,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -11423,7 +11462,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -11431,7 +11470,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>828</v>
       </c>
@@ -11439,7 +11478,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>827</v>
       </c>
@@ -11447,7 +11486,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -11455,7 +11494,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>387</v>
       </c>
@@ -11463,7 +11502,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -11471,7 +11510,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -11479,7 +11518,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -11487,7 +11526,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>405</v>
       </c>
@@ -11495,7 +11534,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -11503,7 +11542,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>604</v>
       </c>
@@ -11511,7 +11550,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -11519,7 +11558,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -11527,7 +11566,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -11535,7 +11574,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>383</v>
       </c>
@@ -11543,7 +11582,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>389</v>
       </c>
@@ -11551,7 +11590,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>101</v>
       </c>
@@ -11559,7 +11598,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>392</v>
       </c>
@@ -11567,7 +11606,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -11575,7 +11614,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -11583,7 +11622,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -11591,7 +11630,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -11599,7 +11638,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -11607,7 +11646,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -11615,7 +11654,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>395</v>
       </c>
@@ -11623,7 +11662,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>397</v>
       </c>
@@ -11631,7 +11670,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -11639,7 +11678,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -11647,7 +11686,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -11655,7 +11694,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>399</v>
       </c>
@@ -11663,7 +11702,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -11671,7 +11710,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -11679,7 +11718,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -11687,7 +11726,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>68</v>
       </c>
@@ -11695,7 +11734,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>402</v>
       </c>
@@ -11703,7 +11742,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -11711,7 +11750,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>30</v>
       </c>
@@ -11719,7 +11758,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -11727,7 +11766,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>32</v>
       </c>
@@ -11735,7 +11774,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>608</v>
       </c>
@@ -11743,7 +11782,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>404</v>
       </c>
@@ -11752,7 +11791,7 @@
       </c>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>72</v>
       </c>
@@ -11762,7 +11801,7 @@
       <c r="C53" s="4"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -11771,7 +11810,7 @@
       </c>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>74</v>
       </c>
@@ -11780,7 +11819,7 @@
       </c>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>87</v>
       </c>
@@ -11789,7 +11828,7 @@
       </c>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -11797,7 +11836,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>76</v>
       </c>
@@ -11805,7 +11844,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -11813,7 +11852,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>86</v>
       </c>

</xml_diff>

<commit_message>
documented Dec 16th checking results
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5803FC5B-D2E9-DF4C-A26A-AC1BDCBDA8A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB0D9E9-75F9-4345-8E6B-AF08211C0899}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="520" windowWidth="25700" windowHeight="12680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="3380" windowWidth="25700" windowHeight="12680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="1022">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="1023">
   <si>
     <t>sid</t>
   </si>
@@ -3084,9 +3084,6 @@
     <t>Fixed issues in gates MALED.</t>
   </si>
   <si>
-    <t>Will update when work on ICEMR myanmar</t>
-  </si>
-  <si>
     <t>not change since icemr_india_fever_surv.owl only has 'Participant' and 'Sample' categories.</t>
   </si>
   <si>
@@ -3094,6 +3091,12 @@
   </si>
   <si>
     <t>Fixed. Added 'Geolocation' and moved two terms under it in gates_score_moz, gates_score_nig, and gates_score_sm_crt</t>
+  </si>
+  <si>
+    <t>Checked on Dec 16th, no issue was found</t>
+  </si>
+  <si>
+    <t>Fixed in ICEMR myanmar</t>
   </si>
 </sst>
 </file>
@@ -3989,8 +3992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6032,10 +6035,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView topLeftCell="B51" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6944,7 +6947,7 @@
     </row>
     <row r="63" spans="1:6">
       <c r="F63" s="14" t="s">
-        <v>1018</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -7010,6 +7013,11 @@
     <row r="67" spans="1:6">
       <c r="F67" s="14" t="s">
         <v>1017</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="11" t="s">
+        <v>1021</v>
       </c>
     </row>
   </sheetData>
@@ -7020,10 +7028,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F175"/>
+  <dimension ref="A1:F177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="C177" sqref="C177"/>
+    <sheetView topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="D180" sqref="D180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9845,7 +9853,7 @@
     </row>
     <row r="173" spans="1:6">
       <c r="F173" s="14" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="174" spans="1:6">
@@ -9870,7 +9878,12 @@
     </row>
     <row r="175" spans="1:6">
       <c r="F175" s="14" t="s">
-        <v>1019</v>
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" s="11" t="s">
+        <v>1021</v>
       </c>
     </row>
   </sheetData>
@@ -9884,8 +9897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10394,7 +10407,7 @@
         <v>1010</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
   </sheetData>
@@ -10407,7 +10420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -11361,10 +11374,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E96E553-B9B7-3A43-9A19-9B2DEFC1133B}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11860,6 +11873,11 @@
         <v>99</v>
       </c>
     </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>1009</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
added inconsistent issues identified on Jan 11, 2022
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB0D9E9-75F9-4345-8E6B-AF08211C0899}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B831D590-7DB2-A04B-A7B4-9AEE24FEF935}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="3380" windowWidth="25700" windowHeight="12680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3100" yWindow="3080" windowWidth="25700" windowHeight="12680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="1023">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="1076">
   <si>
     <t>sid</t>
   </si>
@@ -3097,6 +3097,165 @@
   </si>
   <si>
     <t>Fixed in ICEMR myanmar</t>
+  </si>
+  <si>
+    <t>EUPATH_0000387</t>
+  </si>
+  <si>
+    <t>Traveled in last month | Trips in last month</t>
+  </si>
+  <si>
+    <t>icemr_south_asia | icemr_amazonia_peru</t>
+  </si>
+  <si>
+    <t>EUPATH_0000407</t>
+  </si>
+  <si>
+    <t>District in India | District in Zimbabwe</t>
+  </si>
+  <si>
+    <t>icemr_india_cx | icemr_india_cohort | gates_shine</t>
+  </si>
+  <si>
+    <t>EUPATH_0031266</t>
+  </si>
+  <si>
+    <t>Rotavirus vaccine | Rotavirus vaccine_undocumented</t>
+  </si>
+  <si>
+    <t>gates_vida | gates_vida_hucs_kenya | gates_vida_hucs_gambia_mali | gates_avenir</t>
+  </si>
+  <si>
+    <t>EUPATH_0033175</t>
+  </si>
+  <si>
+    <t>Diphtheria, pertussis, and tetanus (DPT) vaccine status | Diphtheria, pertussis, and tetanus (DPT) vaccine status, undocumented</t>
+  </si>
+  <si>
+    <t>gates_perch | gates_avenir</t>
+  </si>
+  <si>
+    <t>EUPATH_0033225</t>
+  </si>
+  <si>
+    <t>Pneumococcal conjugate vaccine (PCV) status | Pneumococcal conjugate vaccine (PCV) status, undocumented</t>
+  </si>
+  <si>
+    <t>EUPATH_0036100</t>
+  </si>
+  <si>
+    <t>Bacille Calmette-Guerin (BCG) vaccine | BCG vaccine administered | Bacille Calmette-Guerin (BCG) vaccine, undocumented</t>
+  </si>
+  <si>
+    <t>gates_provide | gates_avenir</t>
+  </si>
+  <si>
+    <t>EUPATH_0042044</t>
+  </si>
+  <si>
+    <t>Syphilis test performed | Syphilis sample collected</t>
+  </si>
+  <si>
+    <t>gates_pcs | general/general_promote</t>
+  </si>
+  <si>
+    <t>EUPATH_0042153</t>
+  </si>
+  <si>
+    <t>Treponema pallidum, by rapid test | Treponema p. pallidum, by RDT</t>
+  </si>
+  <si>
+    <t>EUPATH_0047251</t>
+  </si>
+  <si>
+    <t>Baseline date | Baseline survey year</t>
+  </si>
+  <si>
+    <t>gates_shine | gates_ganc</t>
+  </si>
+  <si>
+    <t>EUPATH_0049211</t>
+  </si>
+  <si>
+    <t>Verification of birth date | Verification of birth date,youth</t>
+  </si>
+  <si>
+    <t>gates_gamin | gates_avenir</t>
+  </si>
+  <si>
+    <t>EUPATH_0049212</t>
+  </si>
+  <si>
+    <t>Person providing birth date information | Person providing birth date information, youth</t>
+  </si>
+  <si>
+    <t>Observation details|Demographics</t>
+  </si>
+  <si>
+    <t>gates_gamin | gates_gems_huas | gates_score_moz | icemr_prism2_border_cohort | gates_gems1a | general/general_umsp | gates_gems | gates_vida | gates_elicit | icemr_india_cx | icemr_amazonia_brazil | icemr_india_meghalaya | gates_washb_bangladesh | gates_score_nig | gates_gems1a_huas | gates_perch | general/general_promote | icemr_india_cohort | gates_score_burundi | gates_vida_hucs_kenya | gates_sip | gates_score_five_country | gates_score_seasonal | icemr_prism2 | gates_shine | icemr_india_behavior | icemr_prism | gates_provide | gates_score_sm_cohort | gates_llineup | gates_vida_hucs_gambia_mali | gates_score_rwanda | icemr_southern_africa | gates_avenir | gates_maled | gates_score_zanzibar | icemr_india_fever_surv</t>
+  </si>
+  <si>
+    <t>EUPATH_0042399</t>
+  </si>
+  <si>
+    <t>Child sex</t>
+  </si>
+  <si>
+    <t>Obstetric history|Child demographics</t>
+  </si>
+  <si>
+    <t>EUPATH_0010420</t>
+  </si>
+  <si>
+    <t>Consent for enrollment given</t>
+  </si>
+  <si>
+    <t>Eligibility criteria|Household administrative information</t>
+  </si>
+  <si>
+    <t>gates_gamin | icemr_malawi | gates_avenir</t>
+  </si>
+  <si>
+    <t>EUPATH_0042257</t>
+  </si>
+  <si>
+    <t>Cough</t>
+  </si>
+  <si>
+    <t>Child symptoms|Symptoms</t>
+  </si>
+  <si>
+    <t>general/general_promote | gates_avenir</t>
+  </si>
+  <si>
+    <t>EUPATH_0042260</t>
+  </si>
+  <si>
+    <t>Diarrhea</t>
+  </si>
+  <si>
+    <t>EUPATH_0022088</t>
+  </si>
+  <si>
+    <t>Hospitalization reason</t>
+  </si>
+  <si>
+    <t>Clinical history|Hospitalization</t>
+  </si>
+  <si>
+    <t>icemr_amazonia_brazil | gates_avenir</t>
+  </si>
+  <si>
+    <t>Syphilis test performed|Syphilis sample collected</t>
+  </si>
+  <si>
+    <t>Blood bacteria testing|Blood sample collection process</t>
+  </si>
+  <si>
+    <t>Checked on Jan 11th, 2022, identified following issue:</t>
+  </si>
+  <si>
+    <t>Checked on Jan 11th, 2022, no issue was found</t>
   </si>
 </sst>
 </file>
@@ -3990,17 +4149,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F140"/>
+  <dimension ref="A1:F154"/>
   <sheetViews>
-    <sheetView topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140"/>
+    <sheetView topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" customWidth="1"/>
+    <col min="3" max="3" width="75.5" customWidth="1"/>
     <col min="4" max="4" width="53.83203125" customWidth="1"/>
     <col min="5" max="5" width="55.33203125" style="2" customWidth="1"/>
   </cols>
@@ -6025,6 +6184,179 @@
     <row r="140" spans="1:5">
       <c r="A140" s="11" t="s">
         <v>997</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" s="11" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" t="s">
+        <v>0</v>
+      </c>
+      <c r="B143" t="s">
+        <v>1</v>
+      </c>
+      <c r="C143" t="s">
+        <v>2</v>
+      </c>
+      <c r="D143" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B144">
+        <v>2</v>
+      </c>
+      <c r="C144" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D144" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B145">
+        <v>2</v>
+      </c>
+      <c r="C145" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D145" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B146">
+        <v>2</v>
+      </c>
+      <c r="C146" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D146" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B147">
+        <v>2</v>
+      </c>
+      <c r="C147" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D147" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B148">
+        <v>2</v>
+      </c>
+      <c r="C148" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D148" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B149">
+        <v>3</v>
+      </c>
+      <c r="C149" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D149" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B150">
+        <v>2</v>
+      </c>
+      <c r="C150" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D150" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B151">
+        <v>2</v>
+      </c>
+      <c r="C151" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D151" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B152">
+        <v>2</v>
+      </c>
+      <c r="C152" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D152" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B153">
+        <v>2</v>
+      </c>
+      <c r="C153" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D153" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B154">
+        <v>2</v>
+      </c>
+      <c r="C154" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D154" t="s">
+        <v>1050</v>
       </c>
     </row>
   </sheetData>
@@ -6035,10 +6367,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7020,6 +7352,11 @@
         <v>1021</v>
       </c>
     </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="11" t="s">
+        <v>1075</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -7028,10 +7365,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F177"/>
+  <dimension ref="A1:F188"/>
   <sheetViews>
-    <sheetView topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="D180" sqref="D180"/>
+    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
+      <selection activeCell="C183" sqref="C183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9881,9 +10218,150 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="177" spans="1:1">
+    <row r="177" spans="1:5">
       <c r="A177" s="11" t="s">
         <v>1021</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" s="11" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" t="s">
+        <v>0</v>
+      </c>
+      <c r="B181" t="s">
+        <v>10</v>
+      </c>
+      <c r="C181" t="s">
+        <v>2</v>
+      </c>
+      <c r="D181" t="s">
+        <v>11</v>
+      </c>
+      <c r="E181" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" t="s">
+        <v>502</v>
+      </c>
+      <c r="B182">
+        <v>2</v>
+      </c>
+      <c r="C182" t="s">
+        <v>333</v>
+      </c>
+      <c r="D182" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E182" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B183">
+        <v>2</v>
+      </c>
+      <c r="C183" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D183" t="s">
+        <v>1057</v>
+      </c>
+      <c r="E183" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B184">
+        <v>2</v>
+      </c>
+      <c r="C184" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D184" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E184" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B185">
+        <v>2</v>
+      </c>
+      <c r="C185" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D185" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E185" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B186">
+        <v>2</v>
+      </c>
+      <c r="C186" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D186" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E186" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B187">
+        <v>2</v>
+      </c>
+      <c r="C187" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D187" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E187" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B188">
+        <v>2</v>
+      </c>
+      <c r="C188" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D188" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E188" t="s">
+        <v>1042</v>
       </c>
     </row>
   </sheetData>
@@ -9897,7 +10375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+    <sheetView topLeftCell="A56" workbookViewId="0">
       <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add consistency checking results performed on Feb 17
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36CDD1D-E877-6E41-81CC-81A4148D323A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF73F7E0-107E-F045-8A94-4CE0D9367615}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="500" windowWidth="25700" windowHeight="12680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5680" yWindow="520" windowWidth="25700" windowHeight="12680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="1103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="1168">
   <si>
     <t>sid</t>
   </si>
@@ -3337,6 +3337,201 @@
   </si>
   <si>
     <t>Checked on Jan 14th, 2022, all issues are fixed.</t>
+  </si>
+  <si>
+    <t>EUPATH_0027062</t>
+  </si>
+  <si>
+    <t>Other antibiotics doses per day | Not applicable</t>
+  </si>
+  <si>
+    <t>icemr_west_africa</t>
+  </si>
+  <si>
+    <t>Rotavirus vaccine | Rotavirus vaccine, undocumented</t>
+  </si>
+  <si>
+    <t>EUPATH_0036122</t>
+  </si>
+  <si>
+    <t>Father read with child | Father</t>
+  </si>
+  <si>
+    <t>EUPATH_0036123</t>
+  </si>
+  <si>
+    <t>Father sang with child | Father</t>
+  </si>
+  <si>
+    <t>EUPATH_0036124</t>
+  </si>
+  <si>
+    <t>Father told child stories | Father</t>
+  </si>
+  <si>
+    <t>EUPATH_0036128</t>
+  </si>
+  <si>
+    <t>Mother read with child | Mother</t>
+  </si>
+  <si>
+    <t>EUPATH_0036129</t>
+  </si>
+  <si>
+    <t>Mother sang with child | Mother</t>
+  </si>
+  <si>
+    <t>EUPATH_0036130</t>
+  </si>
+  <si>
+    <t>Mother told child stories | Mother</t>
+  </si>
+  <si>
+    <t>Other adult read with child | Other adult</t>
+  </si>
+  <si>
+    <t>EUPATH_0036133</t>
+  </si>
+  <si>
+    <t>Other adult sang with child | Other adult</t>
+  </si>
+  <si>
+    <t>Other adult told child stories | Other adult</t>
+  </si>
+  <si>
+    <t>Checked on Feb 18th, 2022, identified following issue:</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>EUPATH_0036123|EUPATH_0036122|EUPATH_0036124</t>
+  </si>
+  <si>
+    <t>Family care indicators|Who read with child</t>
+  </si>
+  <si>
+    <t>Mother</t>
+  </si>
+  <si>
+    <t>EUPATH_0036130|EUPATH_0036128|EUPATH_0036129</t>
+  </si>
+  <si>
+    <t>Other adult</t>
+  </si>
+  <si>
+    <t>EUPATH_0036134|EUPATH_0036133|EUPATH_0036132</t>
+  </si>
+  <si>
+    <t>gates_gamin | gates_gems_huas | gates_score_moz | icemr_prism2_border_cohort | gates_gems1a | general/general_umsp | gates_gems | gates_vida | gates_elicit | icemr_india_cx | icemr_amazonia_brazil | icemr_india_meghalaya | gates_score_nig | gates_gems1a_huas | gates_mordor | gates_perch | general/general_promote | icemr_india_cohort | gates_score_burundi | gates_vida_hucs_kenya | gates_sip | gates_score_five_country | gates_score_seasonal | icemr_prism2 | gates_shine | icemr_india_behavior | icemr_prism | gates_provide | gates_score_sm_cohort | icemr_india_daman | gates_llineup | gates_vida_hucs_gambia_mali | gates_score_rwanda | icemr_southern_africa | gates_avenir | gates_maled | gates_score_zanzibar | icemr_india_fever_surv</t>
+  </si>
+  <si>
+    <t>Baseline survey year|Baseline date</t>
+  </si>
+  <si>
+    <t>Observation details|Administrative information</t>
+  </si>
+  <si>
+    <t>EUPATH_0048027</t>
+  </si>
+  <si>
+    <t>Chickens</t>
+  </si>
+  <si>
+    <t>Assets|Animals on property</t>
+  </si>
+  <si>
+    <t>gates_shine | gates_avenir</t>
+  </si>
+  <si>
+    <t>Father read with child|Father</t>
+  </si>
+  <si>
+    <t>gates_pcs | icemr_india_meghalaya | general/general_promote | gates_shine | icemr_india_daman | gates_ganc</t>
+  </si>
+  <si>
+    <t>Household administrative information|Household</t>
+  </si>
+  <si>
+    <t>gates_washb_kenya | gates_washb_bangladesh | gates_shine</t>
+  </si>
+  <si>
+    <t>Mother read with child|Mother</t>
+  </si>
+  <si>
+    <t>Other adult read with child|Other adult</t>
+  </si>
+  <si>
+    <t>Other antibiotics doses per day|Not applicable</t>
+  </si>
+  <si>
+    <t>Treatment|Plasmodium species, by microscopy</t>
+  </si>
+  <si>
+    <t>HP_0031273</t>
+  </si>
+  <si>
+    <t>Shock</t>
+  </si>
+  <si>
+    <t>Severe malaria signs|Symptoms</t>
+  </si>
+  <si>
+    <t>icemr_west_africa | icemr_india_severe_malaria</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000027|UO_0000027</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000015|UO_0000015</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000009|UO_0000009</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000034|NO_IRI</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000036|UO_0000036</t>
+  </si>
+  <si>
+    <t>EUPATH_0000110</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>UO_0000027</t>
+  </si>
+  <si>
+    <t>icemr_india_daman</t>
+  </si>
+  <si>
+    <t>EUPATH_0010075</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>UO_0000015</t>
+  </si>
+  <si>
+    <t>EUPATH_0010084</t>
+  </si>
+  <si>
+    <t>MUAC</t>
+  </si>
+  <si>
+    <t>UO_0000009</t>
+  </si>
+  <si>
+    <t>UO_0000036</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>dataset</t>
   </si>
 </sst>
 </file>
@@ -4239,8 +4434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="C172" sqref="C172:C181"/>
+    <sheetView topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="A159" sqref="A159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6519,24 +6714,219 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
-      <c r="A157" s="11" t="s">
+    <row r="156" spans="1:6">
+      <c r="A156" s="11" t="s">
         <v>1102</v>
       </c>
     </row>
-    <row r="172" spans="3:3">
-      <c r="C172" s="15"/>
-    </row>
-    <row r="173" spans="3:3">
-      <c r="C173" s="15"/>
-    </row>
-    <row r="174" spans="3:3">
+    <row r="159" spans="1:6">
+      <c r="A159" s="11" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" t="s">
+        <v>0</v>
+      </c>
+      <c r="B160" t="s">
+        <v>1</v>
+      </c>
+      <c r="C160" t="s">
+        <v>2</v>
+      </c>
+      <c r="D160" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B161">
+        <v>2</v>
+      </c>
+      <c r="C161" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D161" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B162">
+        <v>2</v>
+      </c>
+      <c r="C162" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D162" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" t="s">
+        <v>599</v>
+      </c>
+      <c r="B163">
+        <v>2</v>
+      </c>
+      <c r="C163" t="s">
+        <v>600</v>
+      </c>
+      <c r="D163" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B164">
+        <v>2</v>
+      </c>
+      <c r="C164" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D164" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B165">
+        <v>2</v>
+      </c>
+      <c r="C165" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D165" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B166">
+        <v>2</v>
+      </c>
+      <c r="C166" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D166" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B167">
+        <v>2</v>
+      </c>
+      <c r="C167" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D167" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B168">
+        <v>2</v>
+      </c>
+      <c r="C168" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D168" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B169">
+        <v>2</v>
+      </c>
+      <c r="C169" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D169" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" t="s">
+        <v>896</v>
+      </c>
+      <c r="B170">
+        <v>2</v>
+      </c>
+      <c r="C170" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D170" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B171">
+        <v>2</v>
+      </c>
+      <c r="C171" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D171" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" t="s">
+        <v>899</v>
+      </c>
+      <c r="B172">
+        <v>2</v>
+      </c>
+      <c r="C172" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D172" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B173">
+        <v>2</v>
+      </c>
+      <c r="C173" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D173" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
       <c r="C174" s="15"/>
     </row>
-    <row r="175" spans="3:3">
+    <row r="175" spans="1:4">
       <c r="C175" s="15"/>
     </row>
-    <row r="176" spans="3:3">
+    <row r="176" spans="1:4">
       <c r="C176" s="15"/>
     </row>
     <row r="177" spans="3:3">
@@ -6562,10 +6952,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7552,6 +7942,101 @@
         <v>1075</v>
       </c>
     </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="11" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F75"/>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" t="s">
+        <v>622</v>
+      </c>
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76" t="s">
+        <v>623</v>
+      </c>
+      <c r="D76" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" t="s">
+        <v>624</v>
+      </c>
+      <c r="F76"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B77">
+        <v>3</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D77" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F77"/>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B78">
+        <v>3</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D78" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F78"/>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B79">
+        <v>3</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D79" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F79"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -7560,9 +8045,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G209"/>
+  <dimension ref="A1:G210"/>
   <sheetViews>
-    <sheetView topLeftCell="A179" workbookViewId="0">
+    <sheetView topLeftCell="A187" workbookViewId="0">
       <selection activeCell="A193" sqref="A193"/>
     </sheetView>
   </sheetViews>
@@ -10613,55 +11098,287 @@
         <v>1102</v>
       </c>
     </row>
+    <row r="191" spans="1:7">
+      <c r="A191" s="11"/>
+    </row>
+    <row r="193" spans="1:6">
+      <c r="A193" s="11" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6">
+      <c r="A194" t="s">
+        <v>0</v>
+      </c>
+      <c r="B194" t="s">
+        <v>10</v>
+      </c>
+      <c r="C194" t="s">
+        <v>2</v>
+      </c>
+      <c r="D194" t="s">
+        <v>11</v>
+      </c>
+      <c r="E194" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6">
+      <c r="A195" t="s">
+        <v>502</v>
+      </c>
+      <c r="B195">
+        <v>2</v>
+      </c>
+      <c r="C195" t="s">
+        <v>333</v>
+      </c>
+      <c r="D195" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E195" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6">
+      <c r="A196" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B196">
+        <v>2</v>
+      </c>
+      <c r="C196" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D196" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E196" t="s">
+        <v>1047</v>
+      </c>
+    </row>
     <row r="197" spans="1:6">
-      <c r="F197"/>
+      <c r="A197" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B197">
+        <v>2</v>
+      </c>
+      <c r="C197" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D197" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E197" t="s">
+        <v>1137</v>
+      </c>
     </row>
     <row r="198" spans="1:6">
+      <c r="A198" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B198">
+        <v>2</v>
+      </c>
+      <c r="C198" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D198" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E198" t="s">
+        <v>1065</v>
+      </c>
       <c r="F198"/>
     </row>
     <row r="199" spans="1:6">
-      <c r="E199" s="2"/>
+      <c r="A199" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B199">
+        <v>2</v>
+      </c>
+      <c r="C199" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D199" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E199" t="s">
+        <v>1065</v>
+      </c>
       <c r="F199"/>
     </row>
     <row r="200" spans="1:6">
-      <c r="E200" s="2"/>
+      <c r="A200" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B200">
+        <v>2</v>
+      </c>
+      <c r="C200" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D200" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E200" t="s">
+        <v>898</v>
+      </c>
       <c r="F200"/>
     </row>
     <row r="201" spans="1:6">
-      <c r="E201" s="2"/>
+      <c r="A201" t="s">
+        <v>543</v>
+      </c>
+      <c r="B201">
+        <v>2</v>
+      </c>
+      <c r="C201" t="s">
+        <v>544</v>
+      </c>
+      <c r="D201" t="s">
+        <v>545</v>
+      </c>
+      <c r="E201" t="s">
+        <v>1139</v>
+      </c>
       <c r="F201"/>
     </row>
     <row r="202" spans="1:6">
-      <c r="E202" s="2"/>
+      <c r="A202" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B202">
+        <v>2</v>
+      </c>
+      <c r="C202" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D202" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E202" t="s">
+        <v>1071</v>
+      </c>
       <c r="F202"/>
     </row>
     <row r="203" spans="1:6">
-      <c r="E203" s="2"/>
+      <c r="A203" t="s">
+        <v>976</v>
+      </c>
+      <c r="B203">
+        <v>2</v>
+      </c>
+      <c r="C203" t="s">
+        <v>977</v>
+      </c>
+      <c r="D203" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E203" t="s">
+        <v>1141</v>
+      </c>
       <c r="F203"/>
     </row>
     <row r="204" spans="1:6">
-      <c r="E204" s="2"/>
+      <c r="A204" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B204">
+        <v>2</v>
+      </c>
+      <c r="C204" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D204" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E204" t="s">
+        <v>898</v>
+      </c>
       <c r="F204"/>
     </row>
     <row r="205" spans="1:6">
-      <c r="A205" s="5"/>
+      <c r="A205" t="s">
+        <v>896</v>
+      </c>
+      <c r="B205">
+        <v>2</v>
+      </c>
+      <c r="C205" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D205" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E205" t="s">
+        <v>898</v>
+      </c>
       <c r="F205"/>
     </row>
     <row r="206" spans="1:6">
-      <c r="A206" s="5"/>
+      <c r="A206" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B206">
+        <v>2</v>
+      </c>
+      <c r="C206" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D206" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E206" t="s">
+        <v>1105</v>
+      </c>
       <c r="F206"/>
     </row>
     <row r="207" spans="1:6">
-      <c r="A207" s="5"/>
+      <c r="A207" t="s">
+        <v>707</v>
+      </c>
+      <c r="B207">
+        <v>2</v>
+      </c>
+      <c r="C207" t="s">
+        <v>708</v>
+      </c>
+      <c r="D207" t="s">
+        <v>627</v>
+      </c>
+      <c r="E207" t="s">
+        <v>709</v>
+      </c>
       <c r="F207"/>
     </row>
     <row r="208" spans="1:6">
-      <c r="A208" s="5"/>
+      <c r="A208" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B208">
+        <v>2</v>
+      </c>
+      <c r="C208" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D208" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E208" t="s">
+        <v>1149</v>
+      </c>
       <c r="F208"/>
     </row>
-    <row r="209" spans="5:6">
-      <c r="E209" s="2"/>
+    <row r="209" spans="1:6">
+      <c r="A209" s="5"/>
       <c r="F209"/>
+    </row>
+    <row r="210" spans="1:6">
+      <c r="E210" s="2"/>
+      <c r="F210"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F30" xr:uid="{3F2C9002-1B0A-C348-905C-32E2D16BAD66}"/>
@@ -10672,10 +11389,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11185,6 +11902,193 @@
       </c>
       <c r="F58" s="2" t="s">
         <v>1019</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="11" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>79</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>80</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>76</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>86</v>
+      </c>
+      <c r="B67">
+        <v>2</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C70" t="s">
+        <v>20</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E70" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C71" t="s">
+        <v>79</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E71" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C72" t="s">
+        <v>79</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E72" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>500</v>
+      </c>
+      <c r="B73" t="s">
+        <v>368</v>
+      </c>
+      <c r="C73" t="s">
+        <v>80</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E73" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>543</v>
+      </c>
+      <c r="B74" t="s">
+        <v>544</v>
+      </c>
+      <c r="C74" t="s">
+        <v>76</v>
+      </c>
+      <c r="E74" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>502</v>
+      </c>
+      <c r="B75" t="s">
+        <v>333</v>
+      </c>
+      <c r="C75" t="s">
+        <v>86</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E75" t="s">
+        <v>1158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed unitIRI issues, refs #45330
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF73F7E0-107E-F045-8A94-4CE0D9367615}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA1AAAD-3039-FB4F-B698-E27229ED3697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5680" yWindow="520" windowWidth="25700" windowHeight="12680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3100" yWindow="520" windowWidth="25700" windowHeight="12680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="1168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2164" uniqueCount="1170">
   <si>
     <t>sid</t>
   </si>
@@ -3399,9 +3399,6 @@
     <t>Other adult told child stories | Other adult</t>
   </si>
   <si>
-    <t>Checked on Feb 18th, 2022, identified following issue:</t>
-  </si>
-  <si>
     <t>Father</t>
   </si>
   <si>
@@ -3532,6 +3529,15 @@
   </si>
   <si>
     <t>dataset</t>
+  </si>
+  <si>
+    <t>wrong IRI</t>
+  </si>
+  <si>
+    <t>All issues fixed. Checked on Feb 18th, 2022</t>
+  </si>
+  <si>
+    <t>Checked on Feb 17th, 2022, identified following issue:</t>
   </si>
 </sst>
 </file>
@@ -4435,7 +4441,7 @@
   <dimension ref="A1:F181"/>
   <sheetViews>
     <sheetView topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="A159" sqref="A159"/>
+      <selection activeCell="B168" sqref="B168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6721,7 +6727,7 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" s="11" t="s">
-        <v>1123</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -6955,7 +6961,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7944,7 +7950,7 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="11" t="s">
-        <v>1123</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -7985,55 +7991,55 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B77">
         <v>3</v>
       </c>
       <c r="C77" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="D77" t="s">
         <v>9</v>
       </c>
       <c r="E77" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="F77"/>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B78">
         <v>3</v>
       </c>
       <c r="C78" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="D78" t="s">
         <v>9</v>
       </c>
       <c r="E78" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="F78"/>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B79">
         <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="D79" t="s">
         <v>9</v>
       </c>
       <c r="E79" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="F79"/>
     </row>
@@ -8047,8 +8053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G210"/>
   <sheetViews>
-    <sheetView topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="A193" sqref="A193"/>
+    <sheetView topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="A200" sqref="A200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11103,7 +11109,7 @@
     </row>
     <row r="193" spans="1:6">
       <c r="A193" s="11" t="s">
-        <v>1123</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="194" spans="1:6">
@@ -11137,7 +11143,7 @@
         <v>1053</v>
       </c>
       <c r="E195" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="196" spans="1:6">
@@ -11148,10 +11154,10 @@
         <v>2</v>
       </c>
       <c r="C196" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D196" t="s">
         <v>1132</v>
-      </c>
-      <c r="D196" t="s">
-        <v>1133</v>
       </c>
       <c r="E196" t="s">
         <v>1047</v>
@@ -11159,19 +11165,19 @@
     </row>
     <row r="197" spans="1:6">
       <c r="A197" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B197">
+        <v>2</v>
+      </c>
+      <c r="C197" t="s">
         <v>1134</v>
       </c>
-      <c r="B197">
-        <v>2</v>
-      </c>
-      <c r="C197" t="s">
+      <c r="D197" t="s">
         <v>1135</v>
       </c>
-      <c r="D197" t="s">
+      <c r="E197" t="s">
         <v>1136</v>
-      </c>
-      <c r="E197" t="s">
-        <v>1137</v>
       </c>
     </row>
     <row r="198" spans="1:6">
@@ -11218,10 +11224,10 @@
         <v>2</v>
       </c>
       <c r="C200" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="D200" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="E200" t="s">
         <v>898</v>
@@ -11242,7 +11248,7 @@
         <v>545</v>
       </c>
       <c r="E201" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="F201"/>
     </row>
@@ -11275,10 +11281,10 @@
         <v>977</v>
       </c>
       <c r="D203" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E203" t="s">
         <v>1140</v>
-      </c>
-      <c r="E203" t="s">
-        <v>1141</v>
       </c>
       <c r="F203"/>
     </row>
@@ -11290,10 +11296,10 @@
         <v>2</v>
       </c>
       <c r="C204" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="D204" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="E204" t="s">
         <v>898</v>
@@ -11308,10 +11314,10 @@
         <v>2</v>
       </c>
       <c r="C205" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="D205" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="E205" t="s">
         <v>898</v>
@@ -11326,10 +11332,10 @@
         <v>2</v>
       </c>
       <c r="C206" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D206" t="s">
         <v>1144</v>
-      </c>
-      <c r="D206" t="s">
-        <v>1145</v>
       </c>
       <c r="E206" t="s">
         <v>1105</v>
@@ -11356,19 +11362,19 @@
     </row>
     <row r="208" spans="1:6">
       <c r="A208" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B208">
+        <v>2</v>
+      </c>
+      <c r="C208" t="s">
         <v>1146</v>
       </c>
-      <c r="B208">
-        <v>2</v>
-      </c>
-      <c r="C208" t="s">
+      <c r="D208" t="s">
         <v>1147</v>
       </c>
-      <c r="D208" t="s">
+      <c r="E208" t="s">
         <v>1148</v>
-      </c>
-      <c r="E208" t="s">
-        <v>1149</v>
       </c>
       <c r="F208"/>
     </row>
@@ -11389,10 +11395,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11906,7 +11912,7 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="11" t="s">
-        <v>1123</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -11928,7 +11934,7 @@
         <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -11939,7 +11945,7 @@
         <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -11950,7 +11956,7 @@
         <v>2</v>
       </c>
       <c r="C65" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -11961,7 +11967,7 @@
         <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -11972,7 +11978,7 @@
         <v>2</v>
       </c>
       <c r="C67" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -11980,7 +11986,7 @@
         <v>915</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>12</v>
@@ -11989,58 +11995,58 @@
         <v>14</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B70" t="s">
         <v>1155</v>
-      </c>
-      <c r="B70" t="s">
-        <v>1156</v>
       </c>
       <c r="C70" t="s">
         <v>20</v>
       </c>
       <c r="D70" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E70" t="s">
         <v>1157</v>
-      </c>
-      <c r="E70" t="s">
-        <v>1158</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B71" t="s">
         <v>1159</v>
-      </c>
-      <c r="B71" t="s">
-        <v>1160</v>
       </c>
       <c r="C71" t="s">
         <v>79</v>
       </c>
       <c r="D71" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="E71" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B72" t="s">
         <v>1162</v>
-      </c>
-      <c r="B72" t="s">
-        <v>1163</v>
       </c>
       <c r="C72" t="s">
         <v>79</v>
       </c>
       <c r="D72" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="E72" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -12054,10 +12060,10 @@
         <v>80</v>
       </c>
       <c r="D73" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="E73" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -12085,10 +12091,34 @@
         <v>86</v>
       </c>
       <c r="D75" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="E75" t="s">
-        <v>1158</v>
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="C76" t="s">
+        <v>727</v>
+      </c>
+      <c r="E76" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="C77" t="s">
+        <v>387</v>
+      </c>
+      <c r="D77" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E77" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="1" t="s">
+        <v>1168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
find some new issues
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7817E904-A0F9-C848-B386-54CFDCB660AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFCFD28-7588-184A-8C9B-76905034B6F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="1280" windowWidth="27900" windowHeight="12680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="1280" windowWidth="27900" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="1210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2271" uniqueCount="1229">
   <si>
     <t>sid</t>
   </si>
@@ -3658,6 +3658,63 @@
   </si>
   <si>
     <t>Changed in provide</t>
+  </si>
+  <si>
+    <t>OBI_0003233</t>
+  </si>
+  <si>
+    <t>Endotracheal tube aspirate test | Endotracheal tube aspirate microbiology test</t>
+  </si>
+  <si>
+    <t>Checked on Feb 23th, 2022, identified following issue:</t>
+  </si>
+  <si>
+    <t>parent_count</t>
+  </si>
+  <si>
+    <t>Cerebrospinal fluid microbiology test|Blood microbiology test|Other sample microbiology test|Induced sputum microbiology test|Endotracheal tube aspirate test|Endotracheal tube aspirate microbiology test|Lung aspirate microbiology test|Pleural fluid microbiology test</t>
+  </si>
+  <si>
+    <t>EUPATH_0038441|EUPATH_0033227|EUPATH_0038599|EUPATH_0033238|EUPATH_0033436|EUPATH_0033443|EUPATH_0033251</t>
+  </si>
+  <si>
+    <t>Organism, by culture</t>
+  </si>
+  <si>
+    <t>Induced sputum microbiology test|Endotracheal tube aspirate test|Endotracheal tube aspirate microbiology test</t>
+  </si>
+  <si>
+    <t>EUPATH_0033236|EUPATH_0033438</t>
+  </si>
+  <si>
+    <t>Organism 3, by culture</t>
+  </si>
+  <si>
+    <t>Pleural fluid microbiology test|Endotracheal tube aspirate test|Endotracheal tube aspirate microbiology test|Lung aspirate microbiology test|Blood microbiology test|Induced sputum microbiology test</t>
+  </si>
+  <si>
+    <t>EUPATH_0033250|EUPATH_0033437|EUPATH_0033444|EUPATH_0033223|EUPATH_0033235</t>
+  </si>
+  <si>
+    <t>Organism 2, by culture</t>
+  </si>
+  <si>
+    <t>Induced sputum test|Endotracheal tube aspirate test|Endotracheal tube aspirate microbiology test</t>
+  </si>
+  <si>
+    <t>EUPATH_0033095|EUPATH_0032393</t>
+  </si>
+  <si>
+    <t>Neutrophils categorization</t>
+  </si>
+  <si>
+    <t>Endotracheal tube aspirate test|Endotracheal tube aspirate microbiology test|Induced sputum test</t>
+  </si>
+  <si>
+    <t>EUPATH_0032385|EUPATH_0033093</t>
+  </si>
+  <si>
+    <t>Epithelial cells categorization</t>
   </si>
 </sst>
 </file>
@@ -4558,19 +4615,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G181"/>
+  <dimension ref="A1:G183"/>
   <sheetViews>
-    <sheetView topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="A175" sqref="A175"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="A179" sqref="A179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
     <col min="3" max="3" width="64.5" customWidth="1"/>
-    <col min="4" max="4" width="53.83203125" customWidth="1"/>
-    <col min="5" max="5" width="31" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -7139,20 +7196,131 @@
     <row r="176" spans="1:7">
       <c r="C176" s="15"/>
     </row>
-    <row r="177" spans="3:3">
+    <row r="177" spans="1:6">
+      <c r="A177" s="11" t="s">
+        <v>1212</v>
+      </c>
       <c r="C177" s="15"/>
     </row>
-    <row r="178" spans="3:3">
-      <c r="C178" s="15"/>
-    </row>
-    <row r="179" spans="3:3">
-      <c r="C179" s="15"/>
-    </row>
-    <row r="180" spans="3:3">
-      <c r="C180" s="15"/>
-    </row>
-    <row r="181" spans="3:3">
-      <c r="C181" s="15"/>
+    <row r="178" spans="1:6">
+      <c r="A178" t="s">
+        <v>4</v>
+      </c>
+      <c r="B178" t="s">
+        <v>5</v>
+      </c>
+      <c r="C178" t="s">
+        <v>6</v>
+      </c>
+      <c r="D178" t="s">
+        <v>7</v>
+      </c>
+      <c r="E178" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F178" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
+      <c r="A179" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B179">
+        <v>2</v>
+      </c>
+      <c r="C179" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D179" t="s">
+        <v>9</v>
+      </c>
+      <c r="E179">
+        <v>3</v>
+      </c>
+      <c r="F179" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="A180" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B180">
+        <v>2</v>
+      </c>
+      <c r="C180" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D180" t="s">
+        <v>9</v>
+      </c>
+      <c r="E180">
+        <v>3</v>
+      </c>
+      <c r="F180" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="A181" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B181">
+        <v>5</v>
+      </c>
+      <c r="C181" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D181" t="s">
+        <v>9</v>
+      </c>
+      <c r="E181">
+        <v>6</v>
+      </c>
+      <c r="F181" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
+      <c r="A182" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B182">
+        <v>2</v>
+      </c>
+      <c r="C182" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D182" t="s">
+        <v>9</v>
+      </c>
+      <c r="E182">
+        <v>3</v>
+      </c>
+      <c r="F182" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
+      <c r="A183" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B183">
+        <v>7</v>
+      </c>
+      <c r="C183" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D183" t="s">
+        <v>9</v>
+      </c>
+      <c r="E183">
+        <v>8</v>
+      </c>
+      <c r="F183" t="s">
+        <v>1214</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8280,17 +8448,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H211"/>
+  <dimension ref="A1:H215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
-      <selection activeCell="A211" sqref="A211"/>
+    <sheetView topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="A213" sqref="A213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.1640625" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
-    <col min="3" max="3" width="34.5" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="66.33203125" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
     <col min="5" max="5" width="53.83203125" customWidth="1"/>
     <col min="6" max="6" width="40.33203125" style="2" customWidth="1"/>
@@ -11710,6 +11878,39 @@
     <row r="211" spans="1:7">
       <c r="A211" s="11" t="s">
         <v>1204</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7">
+      <c r="A213" s="11" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7">
+      <c r="A214" t="s">
+        <v>0</v>
+      </c>
+      <c r="B214" t="s">
+        <v>1</v>
+      </c>
+      <c r="C214" t="s">
+        <v>2</v>
+      </c>
+      <c r="D214" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7">
+      <c r="A215" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B215">
+        <v>2</v>
+      </c>
+      <c r="C215" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D215" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct issues put in wrong worksheet
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFCFD28-7588-184A-8C9B-76905034B6F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D281612-E0E1-A847-80B4-2DB1C560F60E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1280" windowWidth="27900" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="1280" windowWidth="27900" windowHeight="13700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -4615,10 +4615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G183"/>
+  <dimension ref="A1:G176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="A179" sqref="A179"/>
+    <sheetView topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="B186" sqref="B186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7196,132 +7196,6 @@
     <row r="176" spans="1:7">
       <c r="C176" s="15"/>
     </row>
-    <row r="177" spans="1:6">
-      <c r="A177" s="11" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C177" s="15"/>
-    </row>
-    <row r="178" spans="1:6">
-      <c r="A178" t="s">
-        <v>4</v>
-      </c>
-      <c r="B178" t="s">
-        <v>5</v>
-      </c>
-      <c r="C178" t="s">
-        <v>6</v>
-      </c>
-      <c r="D178" t="s">
-        <v>7</v>
-      </c>
-      <c r="E178" t="s">
-        <v>1213</v>
-      </c>
-      <c r="F178" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6">
-      <c r="A179" t="s">
-        <v>1228</v>
-      </c>
-      <c r="B179">
-        <v>2</v>
-      </c>
-      <c r="C179" t="s">
-        <v>1227</v>
-      </c>
-      <c r="D179" t="s">
-        <v>9</v>
-      </c>
-      <c r="E179">
-        <v>3</v>
-      </c>
-      <c r="F179" t="s">
-        <v>1226</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6">
-      <c r="A180" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B180">
-        <v>2</v>
-      </c>
-      <c r="C180" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D180" t="s">
-        <v>9</v>
-      </c>
-      <c r="E180">
-        <v>3</v>
-      </c>
-      <c r="F180" t="s">
-        <v>1223</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6">
-      <c r="A181" t="s">
-        <v>1222</v>
-      </c>
-      <c r="B181">
-        <v>5</v>
-      </c>
-      <c r="C181" t="s">
-        <v>1221</v>
-      </c>
-      <c r="D181" t="s">
-        <v>9</v>
-      </c>
-      <c r="E181">
-        <v>6</v>
-      </c>
-      <c r="F181" t="s">
-        <v>1220</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6">
-      <c r="A182" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B182">
-        <v>2</v>
-      </c>
-      <c r="C182" t="s">
-        <v>1218</v>
-      </c>
-      <c r="D182" t="s">
-        <v>9</v>
-      </c>
-      <c r="E182">
-        <v>3</v>
-      </c>
-      <c r="F182" t="s">
-        <v>1217</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6">
-      <c r="A183" t="s">
-        <v>1216</v>
-      </c>
-      <c r="B183">
-        <v>7</v>
-      </c>
-      <c r="C183" t="s">
-        <v>1215</v>
-      </c>
-      <c r="D183" t="s">
-        <v>9</v>
-      </c>
-      <c r="E183">
-        <v>8</v>
-      </c>
-      <c r="F183" t="s">
-        <v>1214</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -7330,10 +7204,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8435,9 +8309,137 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:6">
       <c r="A81" s="11" t="s">
         <v>1204</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="11" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C83" s="15"/>
+      <c r="E83" s="2"/>
+      <c r="F83"/>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" t="s">
+        <v>4</v>
+      </c>
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F84" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B85">
+        <v>2</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D85" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85">
+        <v>3</v>
+      </c>
+      <c r="F85" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B86">
+        <v>2</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D86" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86">
+        <v>3</v>
+      </c>
+      <c r="F86" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B87">
+        <v>5</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D87" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87">
+        <v>6</v>
+      </c>
+      <c r="F87" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B88">
+        <v>2</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D88" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88">
+        <v>3</v>
+      </c>
+      <c r="F88" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B89">
+        <v>7</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D89" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89">
+        <v>8</v>
+      </c>
+      <c r="F89" t="s">
+        <v>1214</v>
       </c>
     </row>
   </sheetData>
@@ -8450,8 +8452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H215"/>
   <sheetViews>
-    <sheetView topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="A213" sqref="A213"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="C227" sqref="C227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
release of icemr_southern_africa.owl version 2022-03-21
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F4AD02-F921-BA4A-A60D-7824389C02B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919892C5-8B2C-C143-A368-4231C04A6066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="1560" windowWidth="27900" windowHeight="13700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2279" uniqueCount="1232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2293" uniqueCount="1238">
   <si>
     <t>sid</t>
   </si>
@@ -3724,6 +3724,24 @@
   </si>
   <si>
     <t>All issues fixed on Feb 23th.</t>
+  </si>
+  <si>
+    <t>gates_gems_huas | gates_score_moz | icemr_prism2_border_cohort | gates_gems1a | general/general_umsp | gates_gems | gates_vida | gates_ppfp_choices_kenya_pp | gates_score_nig | gates_gems1a_huas | gates_perch | gates_vida_hucs_kenya | gates_score_seasonal | icemr_prism2 | gates_namibia | gates_score_sm_crt | icemr_myanmar | gates_llineup | gates_vida_hucs_gambia_mali</t>
+  </si>
+  <si>
+    <t>UBERON_0009097</t>
+  </si>
+  <si>
+    <t>Pregnant</t>
+  </si>
+  <si>
+    <t>Obstetrics|Pregnancy</t>
+  </si>
+  <si>
+    <t>icemr_west_africa | icemr_prism2_border_cohort | general/general_kalifabougou | icemr_india_meghalaya | icemr_prism2 | gates_namibia | icemr_amazonia_peru | icemr_india_daman | icemr_india_severe_malaria | icemr_myanmar | icemr_southern_africa</t>
+  </si>
+  <si>
+    <t>Checked on Mar 29th, 2022, identified following issue:</t>
   </si>
 </sst>
 </file>
@@ -8479,10 +8497,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H217"/>
+  <dimension ref="A1:H222"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="A219" sqref="A219"/>
+      <selection activeCell="C230" sqref="C230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11950,6 +11968,62 @@
     <row r="217" spans="1:7">
       <c r="A217" s="1" t="s">
         <v>1231</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7">
+      <c r="A219" s="11" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7">
+      <c r="A220" t="s">
+        <v>0</v>
+      </c>
+      <c r="B220" t="s">
+        <v>10</v>
+      </c>
+      <c r="C220" t="s">
+        <v>2</v>
+      </c>
+      <c r="D220" t="s">
+        <v>11</v>
+      </c>
+      <c r="E220" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7">
+      <c r="A221" t="s">
+        <v>336</v>
+      </c>
+      <c r="B221">
+        <v>2</v>
+      </c>
+      <c r="C221" t="s">
+        <v>337</v>
+      </c>
+      <c r="D221" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E221" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7">
+      <c r="A222" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B222">
+        <v>2</v>
+      </c>
+      <c r="C222" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D222" t="s">
+        <v>1235</v>
+      </c>
+      <c r="E222" t="s">
+        <v>1236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added inconsistent issues identified on April 27, 2022
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBDC330-0310-7945-BE75-605D8984B114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8478A91C-75C2-834D-970C-5EE772D6E047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="840" windowWidth="27900" windowHeight="13700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="500" windowWidth="26280" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2296" uniqueCount="1241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2409" uniqueCount="1310">
   <si>
     <t>sid</t>
   </si>
@@ -3751,6 +3751,213 @@
   </si>
   <si>
     <t>All issues fixed on April 1st.</t>
+  </si>
+  <si>
+    <t>Checked on April 27th, 2022, identified following issue:</t>
+  </si>
+  <si>
+    <t>EUPATH_0056602</t>
+  </si>
+  <si>
+    <t>Age at last birthday</t>
+  </si>
+  <si>
+    <t>Demographics|Administrative information</t>
+  </si>
+  <si>
+    <t>gates_jilinde_pe_chv_cohort | gates_jilinde_healthcareprovider_cohort</t>
+  </si>
+  <si>
+    <t>EUPATH_0054344</t>
+  </si>
+  <si>
+    <t>Commercial sex and activity</t>
+  </si>
+  <si>
+    <t>Sexual behavior|Participant</t>
+  </si>
+  <si>
+    <t>gates_jilinde_prospective_cohort | gates_jilinde_retrospective_survey</t>
+  </si>
+  <si>
+    <t>EUPATH_0053050</t>
+  </si>
+  <si>
+    <t>Facility name</t>
+  </si>
+  <si>
+    <t>Administrative information|Clinical history</t>
+  </si>
+  <si>
+    <t>gates_jilinde_prospective_cohort | gates_jilinde_retrospective_survey | gates_jilinde_pe_chv_cohort | gates_namibia | gates_jilinde_healthcareprovider_cohort</t>
+  </si>
+  <si>
+    <t>EUPATH_0035109</t>
+  </si>
+  <si>
+    <t>Mother's age|Maternal age</t>
+  </si>
+  <si>
+    <t>Individuals related to participant|Maternal demographics</t>
+  </si>
+  <si>
+    <t>gates_gamin | gates_elicit | gates_washb_kenya | gates_washb_bangladesh | gates_sip | gates_shine | gates_provide</t>
+  </si>
+  <si>
+    <t>EUPATH_0048083</t>
+  </si>
+  <si>
+    <t>Mother's marital status|Maternal marital status</t>
+  </si>
+  <si>
+    <t>gates_sip | gates_shine</t>
+  </si>
+  <si>
+    <t>EUPATH_0049850</t>
+  </si>
+  <si>
+    <t>Vital status|Child vital status</t>
+  </si>
+  <si>
+    <t>Observation details|Child observation details</t>
+  </si>
+  <si>
+    <t>gates_avenir | gates_ganc</t>
+  </si>
+  <si>
+    <t>Chest X-ray date</t>
+  </si>
+  <si>
+    <t>EUPATH_0038731|EUPATH_0033160</t>
+  </si>
+  <si>
+    <t>Data access group</t>
+  </si>
+  <si>
+    <t>EUPATH_0054057|EUPATH_0053501</t>
+  </si>
+  <si>
+    <t>Have see slogan of 'Jipende JiPrEP'</t>
+  </si>
+  <si>
+    <t>EUPATH_0054651|EUPATH_0054650</t>
+  </si>
+  <si>
+    <t>PrEP</t>
+  </si>
+  <si>
+    <t>Vital status</t>
+  </si>
+  <si>
+    <t>EUPATH_0038398|EUPATH_0049850</t>
+  </si>
+  <si>
+    <t>Physical examination|Observation details|Child observation details</t>
+  </si>
+  <si>
+    <t>Way to cook food</t>
+  </si>
+  <si>
+    <t>FOODON_03450002|EUPATH_0056516</t>
+  </si>
+  <si>
+    <t>When to first hear PrEP</t>
+  </si>
+  <si>
+    <t>EUPATH_0054582|EUPATH_0054583</t>
+  </si>
+  <si>
+    <t>Mother's age | Maternal age</t>
+  </si>
+  <si>
+    <t>Mother's marital status | Maternal marital status</t>
+  </si>
+  <si>
+    <t>Vital status | Child vital status</t>
+  </si>
+  <si>
+    <t>EUPATH_0053511</t>
+  </si>
+  <si>
+    <t>Main reason to initiate PrEP | Reason to initiate PrEP</t>
+  </si>
+  <si>
+    <t>gates_jilinde_awareness_survey | gates_jilinde_retrospective_survey</t>
+  </si>
+  <si>
+    <t>EUPATH_0053512</t>
+  </si>
+  <si>
+    <t>Main reason to initiate PrEP specified | Reason to initiate PrEP  specified</t>
+  </si>
+  <si>
+    <t>EUPATH_0053518</t>
+  </si>
+  <si>
+    <t>Reason to stop taking PrEP specified | Reason of stopping PrEP specified | Main reason to stop taking PrEP  specified</t>
+  </si>
+  <si>
+    <t>gates_jilinde_awareness_survey | gates_jilinde_prospective_cohort | gates_jilinde_retrospective_survey</t>
+  </si>
+  <si>
+    <t>EUPATH_0053519</t>
+  </si>
+  <si>
+    <t>Main reason for stopping or never starting PrEP | Main reason to start or stop taking PrEP | Main reason to stop taking PrEP</t>
+  </si>
+  <si>
+    <t>EUPATH_0053594</t>
+  </si>
+  <si>
+    <t>Reason to stop taking PrEP | Reason of stopping PrEP</t>
+  </si>
+  <si>
+    <t>EUPATH_0054234</t>
+  </si>
+  <si>
+    <t>Other reason to stop PrEP | Reason to stop PrEP due to provider</t>
+  </si>
+  <si>
+    <t>gates_jilinde_prospective_cohort</t>
+  </si>
+  <si>
+    <t>EUPATH_0054253</t>
+  </si>
+  <si>
+    <t>Record creation date | Record create date</t>
+  </si>
+  <si>
+    <t>gates_jilinde_prospective_cohort | gates_jilinde_healthcareprovider_cohort</t>
+  </si>
+  <si>
+    <t>EUPATH_0054279</t>
+  </si>
+  <si>
+    <t>Sex of second partner | Sex of second partner specified</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000099</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0042402</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0050013</t>
+  </si>
+  <si>
+    <t>person-year</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0053215</t>
+  </si>
+  <si>
+    <t>sq km</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C68864</t>
+  </si>
+  <si>
+    <t>Checked on April 27th, 2022, no issue was found.</t>
   </si>
 </sst>
 </file>
@@ -4278,12 +4485,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4651,10 +4857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G176"/>
+  <dimension ref="A1:G189"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="B186" sqref="B186"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="B194" sqref="B194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5684,7 +5890,7 @@
       <c r="D58" t="s">
         <v>238</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="5" t="s">
         <v>483</v>
       </c>
     </row>
@@ -5701,7 +5907,7 @@
       <c r="D59" t="s">
         <v>238</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="E59" s="5" t="s">
         <v>484</v>
       </c>
     </row>
@@ -5718,7 +5924,7 @@
       <c r="D60" t="s">
         <v>243</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="E60" s="5" t="s">
         <v>485</v>
       </c>
     </row>
@@ -5735,7 +5941,7 @@
       <c r="D61" t="s">
         <v>246</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="E61" s="5" t="s">
         <v>486</v>
       </c>
     </row>
@@ -5752,12 +5958,12 @@
       <c r="D62" t="s">
         <v>249</v>
       </c>
-      <c r="E62" s="6" t="s">
+      <c r="E62" s="5" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="E63" s="6"/>
+      <c r="E63" s="5"/>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
@@ -6343,7 +6549,7 @@
       </c>
     </row>
     <row r="107" spans="1:5">
-      <c r="A107" s="11" t="s">
+      <c r="A107" s="10" t="s">
         <v>858</v>
       </c>
     </row>
@@ -6354,7 +6560,7 @@
       <c r="E109"/>
     </row>
     <row r="110" spans="1:5">
-      <c r="A110" s="11" t="s">
+      <c r="A110" s="10" t="s">
         <v>878</v>
       </c>
       <c r="E110"/>
@@ -6494,12 +6700,12 @@
       </c>
     </row>
     <row r="120" spans="1:5">
-      <c r="A120" s="11" t="s">
+      <c r="A120" s="10" t="s">
         <v>890</v>
       </c>
     </row>
     <row r="122" spans="1:5">
-      <c r="A122" s="11" t="s">
+      <c r="A122" s="10" t="s">
         <v>891</v>
       </c>
     </row>
@@ -6637,12 +6843,12 @@
       </c>
     </row>
     <row r="132" spans="1:6">
-      <c r="A132" s="11" t="s">
+      <c r="A132" s="10" t="s">
         <v>936</v>
       </c>
     </row>
     <row r="135" spans="1:6">
-      <c r="A135" s="11" t="s">
+      <c r="A135" s="10" t="s">
         <v>981</v>
       </c>
     </row>
@@ -6684,12 +6890,12 @@
       </c>
     </row>
     <row r="140" spans="1:6">
-      <c r="A140" s="11" t="s">
+      <c r="A140" s="10" t="s">
         <v>997</v>
       </c>
     </row>
     <row r="142" spans="1:6">
-      <c r="A142" s="11" t="s">
+      <c r="A142" s="10" t="s">
         <v>1074</v>
       </c>
     </row>
@@ -6934,12 +7140,12 @@
       </c>
     </row>
     <row r="156" spans="1:6">
-      <c r="A156" s="11" t="s">
+      <c r="A156" s="10" t="s">
         <v>1102</v>
       </c>
     </row>
     <row r="159" spans="1:6">
-      <c r="A159" s="11" t="s">
+      <c r="A159" s="10" t="s">
         <v>1169</v>
       </c>
     </row>
@@ -7013,7 +7219,7 @@
       <c r="E163" s="2" t="s">
         <v>1171</v>
       </c>
-      <c r="F163" s="14" t="s">
+      <c r="F163" s="13" t="s">
         <v>1193</v>
       </c>
       <c r="G163" t="s">
@@ -7221,16 +7427,189 @@
       </c>
     </row>
     <row r="174" spans="1:7">
-      <c r="C174" s="15"/>
+      <c r="C174" s="14"/>
     </row>
     <row r="175" spans="1:7">
-      <c r="A175" s="11" t="s">
+      <c r="A175" s="10" t="s">
         <v>1204</v>
       </c>
-      <c r="C175" s="15"/>
+      <c r="C175" s="14"/>
     </row>
     <row r="176" spans="1:7">
-      <c r="C176" s="15"/>
+      <c r="C176" s="14"/>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" s="10" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" t="s">
+        <v>0</v>
+      </c>
+      <c r="B178" t="s">
+        <v>1</v>
+      </c>
+      <c r="C178" t="s">
+        <v>2</v>
+      </c>
+      <c r="D178" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B179">
+        <v>2</v>
+      </c>
+      <c r="C179" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D179" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B180">
+        <v>2</v>
+      </c>
+      <c r="C180" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D180" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B181">
+        <v>2</v>
+      </c>
+      <c r="C181" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D181" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B182">
+        <v>2</v>
+      </c>
+      <c r="C182" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D182" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B183">
+        <v>2</v>
+      </c>
+      <c r="C183" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D183" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B184">
+        <v>3</v>
+      </c>
+      <c r="C184" t="s">
+        <v>1288</v>
+      </c>
+      <c r="D184" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B185">
+        <v>3</v>
+      </c>
+      <c r="C185" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D185" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B186">
+        <v>2</v>
+      </c>
+      <c r="C186" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D186" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B187">
+        <v>2</v>
+      </c>
+      <c r="C187" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D187" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B188">
+        <v>2</v>
+      </c>
+      <c r="C188" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D188" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B189">
+        <v>2</v>
+      </c>
+      <c r="C189" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D189" t="s">
+        <v>1296</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7240,10 +7619,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7251,7 +7630,7 @@
     <col min="1" max="1" width="45.1640625" customWidth="1"/>
     <col min="3" max="3" width="62.33203125" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="39.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
     <col min="6" max="6" width="30.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7809,7 +8188,7 @@
       <c r="E34" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="5" t="s">
         <v>846</v>
       </c>
     </row>
@@ -7829,7 +8208,7 @@
       <c r="E35" s="3" t="s">
         <v>633</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F35" s="8" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7849,7 +8228,7 @@
       <c r="E36" s="3" t="s">
         <v>511</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" s="5" t="s">
         <v>848</v>
       </c>
     </row>
@@ -7869,7 +8248,7 @@
       <c r="E37" s="3" t="s">
         <v>511</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F37" s="5" t="s">
         <v>849</v>
       </c>
     </row>
@@ -7889,7 +8268,7 @@
       <c r="E38" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F38" s="5" t="s">
         <v>850</v>
       </c>
     </row>
@@ -7909,7 +8288,7 @@
       <c r="E39" s="3" t="s">
         <v>823</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F39" s="5" t="s">
         <v>851</v>
       </c>
     </row>
@@ -7929,7 +8308,7 @@
       <c r="E40" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F40" s="5" t="s">
         <v>845</v>
       </c>
     </row>
@@ -7949,7 +8328,7 @@
       <c r="E41" s="3" t="s">
         <v>640</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="F41" s="5" t="s">
         <v>762</v>
       </c>
     </row>
@@ -7969,7 +8348,7 @@
       <c r="E42" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F42" s="5" t="s">
         <v>517</v>
       </c>
     </row>
@@ -7994,16 +8373,16 @@
       </c>
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1">
-      <c r="F44" s="6"/>
+      <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:6" s="3" customFormat="1">
-      <c r="F45" s="6"/>
+      <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:6" s="3" customFormat="1">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="9" t="s">
         <v>856</v>
       </c>
-      <c r="F46" s="6"/>
+      <c r="F46" s="5"/>
     </row>
     <row r="47" spans="1:6" s="3" customFormat="1">
       <c r="A47" s="3" t="s">
@@ -8021,7 +8400,7 @@
       <c r="E47" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="F47" s="5" t="s">
         <v>846</v>
       </c>
     </row>
@@ -8041,15 +8420,15 @@
       <c r="E48" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="F48" s="5" t="s">
         <v>850</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="3" customFormat="1">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="9" t="s">
         <v>859</v>
       </c>
-      <c r="F50" s="6"/>
+      <c r="F50" s="5"/>
     </row>
     <row r="51" spans="1:6" s="3" customFormat="1">
       <c r="A51" s="3" t="s">
@@ -8067,7 +8446,7 @@
       <c r="E51" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="F51" s="5" t="s">
         <v>862</v>
       </c>
     </row>
@@ -8087,7 +8466,7 @@
       <c r="E52" t="s">
         <v>558</v>
       </c>
-      <c r="F52" s="6" t="s">
+      <c r="F52" s="5" t="s">
         <v>863</v>
       </c>
     </row>
@@ -8097,15 +8476,15 @@
       </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="10" t="s">
         <v>937</v>
       </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="11"/>
+      <c r="A59" s="10"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="10" t="s">
         <v>987</v>
       </c>
       <c r="F60"/>
@@ -8146,12 +8525,12 @@
       <c r="E62" t="s">
         <v>633</v>
       </c>
-      <c r="F62" s="13" t="s">
+      <c r="F62" s="12" t="s">
         <v>1011</v>
       </c>
     </row>
     <row r="63" spans="1:6">
-      <c r="F63" s="14" t="s">
+      <c r="F63" s="13" t="s">
         <v>1022</v>
       </c>
     </row>
@@ -8171,7 +8550,7 @@
       <c r="E64" t="s">
         <v>1002</v>
       </c>
-      <c r="F64" s="13" t="s">
+      <c r="F64" s="12" t="s">
         <v>1012</v>
       </c>
     </row>
@@ -8191,7 +8570,7 @@
       <c r="E65" t="s">
         <v>1002</v>
       </c>
-      <c r="F65" s="13" t="s">
+      <c r="F65" s="12" t="s">
         <v>1013</v>
       </c>
     </row>
@@ -8211,27 +8590,27 @@
       <c r="E66" t="s">
         <v>1007</v>
       </c>
-      <c r="F66" s="13" t="s">
+      <c r="F66" s="12" t="s">
         <v>1014</v>
       </c>
     </row>
     <row r="67" spans="1:7">
-      <c r="F67" s="14" t="s">
+      <c r="F67" s="13" t="s">
         <v>1017</v>
       </c>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="11" t="s">
+      <c r="A69" s="10" t="s">
         <v>1021</v>
       </c>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="10" t="s">
         <v>1075</v>
       </c>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="11" t="s">
+      <c r="A74" s="10" t="s">
         <v>1169</v>
       </c>
     </row>
@@ -8346,15 +8725,15 @@
       </c>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" s="11" t="s">
+      <c r="A81" s="10" t="s">
         <v>1204</v>
       </c>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="11" t="s">
+      <c r="A83" s="10" t="s">
         <v>1212</v>
       </c>
-      <c r="C83" s="15"/>
+      <c r="C83" s="14"/>
       <c r="E83" s="2"/>
       <c r="F83"/>
     </row>
@@ -8496,6 +8875,151 @@
     <row r="91" spans="1:7">
       <c r="A91" s="1" t="s">
         <v>1231</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" s="10" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
+        <v>4</v>
+      </c>
+      <c r="B94" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" t="s">
+        <v>6</v>
+      </c>
+      <c r="D94" t="s">
+        <v>7</v>
+      </c>
+      <c r="E94" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F94" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B95">
+        <v>2</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D95" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B96">
+        <v>2</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D96" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+      <c r="F96" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B97">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D97" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="F97" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B98">
+        <v>2</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D98" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98">
+        <v>3</v>
+      </c>
+      <c r="F98" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B99">
+        <v>2</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1276</v>
+      </c>
+      <c r="D99" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B100">
+        <v>2</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D100" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+      <c r="F100" t="s">
+        <v>1271</v>
       </c>
     </row>
   </sheetData>
@@ -8506,10 +9030,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H224"/>
+  <dimension ref="A1:H234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
-      <selection activeCell="C230" sqref="C230"/>
+    <sheetView topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="A226" sqref="A226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8517,7 +9041,7 @@
     <col min="1" max="1" width="20.1640625" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="66.33203125" customWidth="1"/>
-    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="4" max="4" width="47" customWidth="1"/>
     <col min="5" max="5" width="53.83203125" customWidth="1"/>
     <col min="6" max="6" width="40.33203125" style="2" customWidth="1"/>
   </cols>
@@ -8578,7 +9102,7 @@
       <c r="E3" t="s">
         <v>257</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>621</v>
       </c>
     </row>
@@ -8738,7 +9262,7 @@
       <c r="E11" t="s">
         <v>257</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>621</v>
       </c>
     </row>
@@ -10997,41 +11521,41 @@
       </c>
     </row>
     <row r="142" spans="1:6">
-      <c r="A142" s="11" t="s">
+      <c r="A142" s="10" t="s">
         <v>878</v>
       </c>
     </row>
     <row r="143" spans="1:6">
-      <c r="A143" s="7" t="s">
+      <c r="A143" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B143" s="7" t="s">
+      <c r="B143" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C143" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D143" s="7" t="s">
+      <c r="C143" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D143" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E143" s="7" t="s">
+      <c r="E143" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="144" spans="1:6">
-      <c r="A144" s="7" t="s">
+      <c r="A144" s="6" t="s">
         <v>879</v>
       </c>
-      <c r="B144" s="7">
-        <v>2</v>
-      </c>
-      <c r="C144" s="7" t="s">
+      <c r="B144" s="6">
+        <v>2</v>
+      </c>
+      <c r="C144" s="6" t="s">
         <v>880</v>
       </c>
-      <c r="D144" s="7" t="s">
+      <c r="D144" s="6" t="s">
         <v>561</v>
       </c>
-      <c r="E144" s="7" t="s">
+      <c r="E144" s="6" t="s">
         <v>881</v>
       </c>
       <c r="F144" s="2" t="s">
@@ -11039,19 +11563,19 @@
       </c>
     </row>
     <row r="145" spans="1:6">
-      <c r="A145" s="7" t="s">
+      <c r="A145" s="6" t="s">
         <v>865</v>
       </c>
-      <c r="B145" s="7">
-        <v>2</v>
-      </c>
-      <c r="C145" s="7" t="s">
+      <c r="B145" s="6">
+        <v>2</v>
+      </c>
+      <c r="C145" s="6" t="s">
         <v>882</v>
       </c>
-      <c r="D145" s="7" t="s">
+      <c r="D145" s="6" t="s">
         <v>883</v>
       </c>
-      <c r="E145" s="7" t="s">
+      <c r="E145" s="6" t="s">
         <v>867</v>
       </c>
       <c r="F145" s="2" t="s">
@@ -11059,12 +11583,12 @@
       </c>
     </row>
     <row r="148" spans="1:6">
-      <c r="A148" s="11" t="s">
+      <c r="A148" s="10" t="s">
         <v>890</v>
       </c>
     </row>
     <row r="150" spans="1:6">
-      <c r="A150" s="11" t="s">
+      <c r="A150" s="10" t="s">
         <v>891</v>
       </c>
     </row>
@@ -11146,12 +11670,12 @@
       </c>
     </row>
     <row r="156" spans="1:6">
-      <c r="A156" s="11" t="s">
+      <c r="A156" s="10" t="s">
         <v>936</v>
       </c>
     </row>
     <row r="158" spans="1:6">
-      <c r="A158" s="11" t="s">
+      <c r="A158" s="10" t="s">
         <v>975</v>
       </c>
     </row>
@@ -11266,7 +11790,7 @@
       </c>
     </row>
     <row r="169" spans="1:6">
-      <c r="A169" s="11" t="s">
+      <c r="A169" s="10" t="s">
         <v>987</v>
       </c>
     </row>
@@ -11306,7 +11830,7 @@
       <c r="E171" t="s">
         <v>991</v>
       </c>
-      <c r="F171" s="13" t="s">
+      <c r="F171" s="12" t="s">
         <v>1015</v>
       </c>
     </row>
@@ -11326,12 +11850,12 @@
       <c r="E172" t="s">
         <v>991</v>
       </c>
-      <c r="F172" s="13" t="s">
+      <c r="F172" s="12" t="s">
         <v>1015</v>
       </c>
     </row>
     <row r="173" spans="1:6">
-      <c r="F173" s="14" t="s">
+      <c r="F173" s="13" t="s">
         <v>1020</v>
       </c>
     </row>
@@ -11351,22 +11875,22 @@
       <c r="E174" t="s">
         <v>996</v>
       </c>
-      <c r="F174" s="13" t="s">
+      <c r="F174" s="12" t="s">
         <v>1016</v>
       </c>
     </row>
     <row r="175" spans="1:6">
-      <c r="F175" s="14" t="s">
+      <c r="F175" s="13" t="s">
         <v>1018</v>
       </c>
     </row>
     <row r="177" spans="1:7">
-      <c r="A177" s="11" t="s">
+      <c r="A177" s="10" t="s">
         <v>1021</v>
       </c>
     </row>
     <row r="180" spans="1:7">
-      <c r="A180" s="11" t="s">
+      <c r="A180" s="10" t="s">
         <v>1074</v>
       </c>
     </row>
@@ -11435,7 +11959,7 @@
       <c r="F183" s="2" t="s">
         <v>1092</v>
       </c>
-      <c r="G183" s="14" t="s">
+      <c r="G183" s="13" t="s">
         <v>1101</v>
       </c>
     </row>
@@ -11527,7 +12051,7 @@
       <c r="F187" s="2" t="s">
         <v>1093</v>
       </c>
-      <c r="G187" s="14" t="s">
+      <c r="G187" s="13" t="s">
         <v>1100</v>
       </c>
     </row>
@@ -11555,15 +12079,15 @@
       </c>
     </row>
     <row r="190" spans="1:7">
-      <c r="A190" s="11" t="s">
+      <c r="A190" s="10" t="s">
         <v>1102</v>
       </c>
     </row>
     <row r="191" spans="1:7">
-      <c r="A191" s="11"/>
+      <c r="A191" s="10"/>
     </row>
     <row r="193" spans="1:8">
-      <c r="A193" s="11" t="s">
+      <c r="A193" s="10" t="s">
         <v>1169</v>
       </c>
     </row>
@@ -11761,7 +12285,7 @@
       <c r="F202" s="2" t="s">
         <v>1189</v>
       </c>
-      <c r="G202" s="12" t="s">
+      <c r="G202" s="11" t="s">
         <v>1208</v>
       </c>
       <c r="H202" t="s">
@@ -11925,7 +12449,7 @@
       <c r="F209" s="2" t="s">
         <v>1207</v>
       </c>
-      <c r="G209" s="12" t="s">
+      <c r="G209" s="11" t="s">
         <v>1209</v>
       </c>
     </row>
@@ -11934,12 +12458,12 @@
       <c r="F210"/>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="11" t="s">
+      <c r="A211" s="10" t="s">
         <v>1204</v>
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="11" t="s">
+      <c r="A213" s="10" t="s">
         <v>1212</v>
       </c>
     </row>
@@ -11980,7 +12504,7 @@
       </c>
     </row>
     <row r="219" spans="1:7">
-      <c r="A219" s="11" t="s">
+      <c r="A219" s="10" t="s">
         <v>1237</v>
       </c>
     </row>
@@ -12045,6 +12569,140 @@
       <c r="A224" s="1" t="s">
         <v>1240</v>
       </c>
+    </row>
+    <row r="226" spans="1:6">
+      <c r="A226" s="10" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6">
+      <c r="A227" t="s">
+        <v>0</v>
+      </c>
+      <c r="B227" t="s">
+        <v>10</v>
+      </c>
+      <c r="C227" t="s">
+        <v>2</v>
+      </c>
+      <c r="D227" t="s">
+        <v>11</v>
+      </c>
+      <c r="E227" t="s">
+        <v>3</v>
+      </c>
+      <c r="F227"/>
+    </row>
+    <row r="228" spans="1:6">
+      <c r="A228" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B228">
+        <v>2</v>
+      </c>
+      <c r="C228" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D228" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E228" t="s">
+        <v>1245</v>
+      </c>
+      <c r="F228"/>
+    </row>
+    <row r="229" spans="1:6">
+      <c r="A229" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B229">
+        <v>2</v>
+      </c>
+      <c r="C229" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D229" t="s">
+        <v>1248</v>
+      </c>
+      <c r="E229" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F229"/>
+    </row>
+    <row r="230" spans="1:6">
+      <c r="A230" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B230">
+        <v>2</v>
+      </c>
+      <c r="C230" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D230" t="s">
+        <v>1252</v>
+      </c>
+      <c r="E230" t="s">
+        <v>1253</v>
+      </c>
+      <c r="F230"/>
+    </row>
+    <row r="231" spans="1:6">
+      <c r="A231" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B231">
+        <v>2</v>
+      </c>
+      <c r="C231" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D231" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E231" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F231"/>
+    </row>
+    <row r="232" spans="1:6">
+      <c r="A232" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B232">
+        <v>2</v>
+      </c>
+      <c r="C232" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D232" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E232" t="s">
+        <v>1260</v>
+      </c>
+      <c r="F232"/>
+    </row>
+    <row r="233" spans="1:6">
+      <c r="A233" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B233">
+        <v>2</v>
+      </c>
+      <c r="C233" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D233" t="s">
+        <v>1263</v>
+      </c>
+      <c r="E233" t="s">
+        <v>1264</v>
+      </c>
+      <c r="F233"/>
+    </row>
+    <row r="234" spans="1:6">
+      <c r="F234"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F30" xr:uid="{3F2C9002-1B0A-C348-905C-32E2D16BAD66}"/>
@@ -12055,10 +12713,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12247,7 +12905,7 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="D18" s="5"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
@@ -12266,7 +12924,7 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>602</v>
       </c>
       <c r="B22" t="s">
@@ -12368,13 +13026,13 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="D31" s="5"/>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>333</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="6" t="s">
         <v>502</v>
       </c>
       <c r="C32" t="s">
@@ -12391,7 +13049,7 @@
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="7"/>
+      <c r="A33" s="6"/>
       <c r="B33" s="3"/>
     </row>
     <row r="35" spans="1:6">
@@ -12415,39 +13073,39 @@
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>857</v>
       </c>
-      <c r="B38" s="7"/>
+      <c r="B38" s="6"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="10" t="s">
         <v>858</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="11"/>
+      <c r="A41" s="10"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="10" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="12" customFormat="1">
-      <c r="A44" s="12" t="s">
+    <row r="44" spans="1:6" s="11" customFormat="1">
+      <c r="A44" s="11" t="s">
         <v>914</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="11" t="s">
         <v>915</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="11" t="s">
         <v>916</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="11" t="s">
         <v>917</v>
       </c>
     </row>
@@ -12491,14 +13149,14 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="12" customFormat="1">
-      <c r="A49" s="12" t="s">
+    <row r="49" spans="1:6" s="11" customFormat="1">
+      <c r="A49" s="11" t="s">
         <v>921</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="11" t="s">
         <v>917</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="11" t="s">
         <v>916</v>
       </c>
     </row>
@@ -12547,12 +13205,12 @@
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="10" t="s">
         <v>936</v>
       </c>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="10" t="s">
         <v>987</v>
       </c>
     </row>
@@ -12571,7 +13229,7 @@
       </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="11" t="s">
+      <c r="A61" s="10" t="s">
         <v>1169</v>
       </c>
     </row>
@@ -12779,6 +13437,11 @@
     <row r="79" spans="1:5">
       <c r="A79" s="1" t="s">
         <v>1168</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="10" t="s">
+        <v>1309</v>
       </c>
     </row>
   </sheetData>
@@ -13745,28 +14408,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E96E553-B9B7-3A43-9A19-9B2DEFC1133B}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B67" sqref="A1:B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1"/>
-      <c r="F1"/>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -13774,7 +14435,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>725</v>
       </c>
@@ -13782,7 +14443,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>726</v>
       </c>
@@ -13790,7 +14451,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -13798,236 +14459,236 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>405</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>604</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>828</v>
+        <v>727</v>
       </c>
       <c r="B13" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>827</v>
+        <v>383</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>387</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>388</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>405</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>408</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>604</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>605</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>828</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>411</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>827</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B26" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>389</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>390</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>392</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>393</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="B31" t="s">
-        <v>409</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>389</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>390</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>392</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>393</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -14040,213 +14701,258 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>395</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>396</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>397</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>398</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>409</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>95</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>399</v>
+        <v>912</v>
       </c>
       <c r="B41" t="s">
-        <v>400</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>954</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>395</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>396</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>66</v>
+        <v>397</v>
       </c>
       <c r="B44" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>402</v>
+        <v>60</v>
       </c>
       <c r="B46" t="s">
-        <v>403</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B47" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>30</v>
+        <v>399</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
+        <v>730</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>402</v>
+      </c>
+      <c r="B56" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
         <v>608</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B59" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
         <v>404</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B61" t="s">
         <v>611</v>
       </c>
-      <c r="D52" s="3"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" t="s">
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
         <v>72</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B62" t="s">
         <v>73</v>
       </c>
-      <c r="C53" s="4"/>
-      <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54" t="s">
-        <v>71</v>
-      </c>
-      <c r="D54" s="3"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" t="s">
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
         <v>74</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B63" t="s">
         <v>75</v>
       </c>
-      <c r="D55" s="3"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
         <v>87</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B64" t="s">
         <v>89</v>
       </c>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
-        <v>34</v>
-      </c>
-      <c r="B57" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
         <v>76</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B65" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
         <v>78</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B66" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" t="s">
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
         <v>86</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B67" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" t="s">
-        <v>1009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update consistency issue spreadsheet
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilus-adm/Documents/GitHub/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6D368E-AE3D-2049-84C9-3F452B22B40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8385278D-DE02-614D-9E0C-748CEB7119A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="680" windowWidth="26280" windowHeight="13700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1400" yWindow="2360" windowWidth="32480" windowHeight="22840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -24,11 +24,23 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">termWithDifferentParent!$A$1:$F$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2432" uniqueCount="1317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2435" uniqueCount="1320">
   <si>
     <t>sid</t>
   </si>
@@ -3762,9 +3774,6 @@
     <t>Age at last birthday</t>
   </si>
   <si>
-    <t>Demographics|Administrative information</t>
-  </si>
-  <si>
     <t>gates_jilinde_pe_chv_cohort | gates_jilinde_healthcareprovider_cohort</t>
   </si>
   <si>
@@ -3774,9 +3783,6 @@
     <t>Commercial sex and activity</t>
   </si>
   <si>
-    <t>Sexual behavior|Participant</t>
-  </si>
-  <si>
     <t>gates_jilinde_prospective_cohort | gates_jilinde_retrospective_survey</t>
   </si>
   <si>
@@ -3786,9 +3792,6 @@
     <t>Facility name</t>
   </si>
   <si>
-    <t>Administrative information|Clinical history</t>
-  </si>
-  <si>
     <t>gates_jilinde_prospective_cohort | gates_jilinde_retrospective_survey | gates_jilinde_pe_chv_cohort | gates_namibia | gates_jilinde_healthcareprovider_cohort</t>
   </si>
   <si>
@@ -3979,6 +3982,84 @@
   </si>
   <si>
     <t>Move to Maternal demographics in all studies</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Demographics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>|Administrative information</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sexual behavior</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>|Participant</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Administrative information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>|Clinical history</t>
+    </r>
+  </si>
+  <si>
+    <t>canged to Administrative information</t>
+  </si>
+  <si>
+    <t>changed to Sexual behavior</t>
+  </si>
+  <si>
+    <t>changed to Demographics</t>
   </si>
 </sst>
 </file>
@@ -7480,189 +7561,189 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B179">
+        <v>2</v>
+      </c>
+      <c r="C179" t="s">
+        <v>1276</v>
+      </c>
+      <c r="D179" t="s">
         <v>1254</v>
       </c>
-      <c r="B179">
-        <v>2</v>
-      </c>
-      <c r="C179" t="s">
-        <v>1279</v>
-      </c>
-      <c r="D179" t="s">
-        <v>1257</v>
-      </c>
       <c r="E179" s="2" t="s">
-        <v>1310</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="B180">
         <v>2</v>
       </c>
       <c r="C180" t="s">
-        <v>1280</v>
+        <v>1277</v>
       </c>
       <c r="D180" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>1311</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B181">
+        <v>2</v>
+      </c>
+      <c r="C181" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D181" t="s">
         <v>1261</v>
       </c>
-      <c r="B181">
-        <v>2</v>
-      </c>
-      <c r="C181" t="s">
-        <v>1281</v>
-      </c>
-      <c r="D181" t="s">
-        <v>1264</v>
-      </c>
       <c r="E181" s="2" t="s">
-        <v>1314</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>1282</v>
+        <v>1279</v>
       </c>
       <c r="B182">
         <v>2</v>
       </c>
       <c r="C182" t="s">
-        <v>1283</v>
+        <v>1280</v>
       </c>
       <c r="D182" t="s">
-        <v>1284</v>
+        <v>1281</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>1285</v>
+        <v>1282</v>
       </c>
       <c r="B183">
         <v>2</v>
       </c>
       <c r="C183" t="s">
-        <v>1286</v>
+        <v>1283</v>
       </c>
       <c r="D183" t="s">
-        <v>1284</v>
+        <v>1281</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>1287</v>
+        <v>1284</v>
       </c>
       <c r="B184">
         <v>3</v>
       </c>
       <c r="C184" t="s">
-        <v>1288</v>
+        <v>1285</v>
       </c>
       <c r="D184" t="s">
-        <v>1289</v>
+        <v>1286</v>
       </c>
       <c r="E184" s="2" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>1290</v>
+        <v>1287</v>
       </c>
       <c r="B185">
         <v>3</v>
       </c>
       <c r="C185" t="s">
-        <v>1291</v>
+        <v>1288</v>
       </c>
       <c r="D185" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>1292</v>
+        <v>1289</v>
       </c>
       <c r="B186">
         <v>2</v>
       </c>
       <c r="C186" t="s">
-        <v>1293</v>
+        <v>1290</v>
       </c>
       <c r="D186" t="s">
-        <v>1289</v>
+        <v>1286</v>
       </c>
       <c r="E186" s="2" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>1294</v>
+        <v>1291</v>
       </c>
       <c r="B187">
         <v>2</v>
       </c>
       <c r="C187" t="s">
-        <v>1295</v>
+        <v>1292</v>
       </c>
       <c r="D187" t="s">
-        <v>1296</v>
+        <v>1293</v>
       </c>
       <c r="E187" s="2" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>1297</v>
+        <v>1294</v>
       </c>
       <c r="B188">
         <v>2</v>
       </c>
       <c r="C188" t="s">
-        <v>1298</v>
+        <v>1295</v>
       </c>
       <c r="D188" t="s">
-        <v>1299</v>
+        <v>1296</v>
       </c>
       <c r="E188" s="2" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>1300</v>
+        <v>1297</v>
       </c>
       <c r="B189">
         <v>2</v>
       </c>
       <c r="C189" t="s">
-        <v>1301</v>
+        <v>1298</v>
       </c>
       <c r="D189" t="s">
-        <v>1296</v>
+        <v>1293</v>
       </c>
       <c r="E189" s="2" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
     </row>
   </sheetData>
@@ -8958,13 +9039,13 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>1265</v>
+        <v>1262</v>
       </c>
       <c r="B95">
         <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>1266</v>
+        <v>1263</v>
       </c>
       <c r="D95" t="s">
         <v>9</v>
@@ -8976,18 +9057,18 @@
         <v>755</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>1313</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>1267</v>
+        <v>1264</v>
       </c>
       <c r="B96">
         <v>2</v>
       </c>
       <c r="C96" t="s">
-        <v>1268</v>
+        <v>1265</v>
       </c>
       <c r="D96" t="s">
         <v>9</v>
@@ -8999,18 +9080,18 @@
         <v>251</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>1269</v>
+        <v>1266</v>
       </c>
       <c r="B97">
         <v>2</v>
       </c>
       <c r="C97" t="s">
-        <v>1270</v>
+        <v>1267</v>
       </c>
       <c r="D97" t="s">
         <v>9</v>
@@ -9019,21 +9100,21 @@
         <v>1</v>
       </c>
       <c r="F97" t="s">
-        <v>1271</v>
+        <v>1268</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>1272</v>
+        <v>1269</v>
       </c>
       <c r="B98">
         <v>2</v>
       </c>
       <c r="C98" t="s">
-        <v>1273</v>
+        <v>1270</v>
       </c>
       <c r="D98" t="s">
         <v>9</v>
@@ -9042,21 +9123,21 @@
         <v>3</v>
       </c>
       <c r="F98" t="s">
-        <v>1274</v>
+        <v>1271</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>1314</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>1275</v>
+        <v>1272</v>
       </c>
       <c r="B99">
         <v>2</v>
       </c>
       <c r="C99" t="s">
-        <v>1276</v>
+        <v>1273</v>
       </c>
       <c r="D99" t="s">
         <v>9</v>
@@ -9068,18 +9149,18 @@
         <v>505</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>1277</v>
+        <v>1274</v>
       </c>
       <c r="B100">
         <v>2</v>
       </c>
       <c r="C100" t="s">
-        <v>1278</v>
+        <v>1275</v>
       </c>
       <c r="D100" t="s">
         <v>9</v>
@@ -9088,10 +9169,10 @@
         <v>1</v>
       </c>
       <c r="F100" t="s">
-        <v>1271</v>
+        <v>1268</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
     </row>
   </sheetData>
@@ -9104,8 +9185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D221" workbookViewId="0">
-      <selection activeCell="F238" sqref="F238"/>
+    <sheetView tabSelected="1" topLeftCell="E204" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G230" sqref="G230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9114,7 +9195,7 @@
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="66.33203125" customWidth="1"/>
     <col min="4" max="4" width="47" customWidth="1"/>
-    <col min="5" max="5" width="53.83203125" customWidth="1"/>
+    <col min="5" max="5" width="137.33203125" customWidth="1"/>
     <col min="6" max="6" width="40.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12642,12 +12723,12 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226" s="10" t="s">
         <v>1241</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>0</v>
       </c>
@@ -12665,7 +12746,7 @@
       </c>
       <c r="F227"/>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>1242</v>
       </c>
@@ -12676,116 +12757,125 @@
         <v>1243</v>
       </c>
       <c r="D228" t="s">
+        <v>1314</v>
+      </c>
+      <c r="E228" t="s">
         <v>1244</v>
       </c>
-      <c r="E228" t="s">
+      <c r="F228" s="2" t="s">
+        <v>1312</v>
+      </c>
+      <c r="G228" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
         <v>1245</v>
       </c>
-      <c r="F228" s="2" t="s">
+      <c r="B229">
+        <v>2</v>
+      </c>
+      <c r="C229" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D229" t="s">
         <v>1315</v>
       </c>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A229" t="s">
-        <v>1246</v>
-      </c>
-      <c r="B229">
-        <v>2</v>
-      </c>
-      <c r="C229" t="s">
+      <c r="E229" t="s">
         <v>1247</v>
       </c>
-      <c r="D229" t="s">
+      <c r="F229" s="2" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G229" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
         <v>1248</v>
       </c>
-      <c r="E229" t="s">
+      <c r="B230">
+        <v>2</v>
+      </c>
+      <c r="C230" t="s">
         <v>1249</v>
       </c>
-      <c r="F229" s="2" t="s">
-        <v>1312</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A230" t="s">
+      <c r="D230" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E230" t="s">
         <v>1250</v>
       </c>
-      <c r="B230">
-        <v>2</v>
-      </c>
-      <c r="C230" t="s">
+      <c r="F230" s="2" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G230" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
         <v>1251</v>
       </c>
-      <c r="D230" t="s">
+      <c r="B231">
+        <v>2</v>
+      </c>
+      <c r="C231" t="s">
         <v>1252</v>
       </c>
-      <c r="E230" t="s">
+      <c r="D231" t="s">
         <v>1253</v>
       </c>
-      <c r="F230" s="2" t="s">
-        <v>1312</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A231" t="s">
+      <c r="E231" t="s">
         <v>1254</v>
       </c>
-      <c r="B231">
-        <v>2</v>
-      </c>
-      <c r="C231" t="s">
+      <c r="F231" s="2" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
         <v>1255</v>
       </c>
-      <c r="D231" t="s">
+      <c r="B232">
+        <v>2</v>
+      </c>
+      <c r="C232" t="s">
         <v>1256</v>
       </c>
-      <c r="E231" t="s">
+      <c r="D232" t="s">
+        <v>1253</v>
+      </c>
+      <c r="E232" t="s">
         <v>1257</v>
       </c>
-      <c r="F231" s="2" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A232" t="s">
+      <c r="F232" s="2" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
         <v>1258</v>
       </c>
-      <c r="B232">
-        <v>2</v>
-      </c>
-      <c r="C232" t="s">
+      <c r="B233">
+        <v>2</v>
+      </c>
+      <c r="C233" t="s">
         <v>1259</v>
       </c>
-      <c r="D232" t="s">
-        <v>1256</v>
-      </c>
-      <c r="E232" t="s">
+      <c r="D233" t="s">
         <v>1260</v>
       </c>
-      <c r="F232" s="2" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A233" t="s">
+      <c r="E233" t="s">
         <v>1261</v>
       </c>
-      <c r="B233">
-        <v>2</v>
-      </c>
-      <c r="C233" t="s">
-        <v>1262</v>
-      </c>
-      <c r="D233" t="s">
-        <v>1263</v>
-      </c>
-      <c r="E233" t="s">
-        <v>1264</v>
-      </c>
       <c r="F233" s="2" t="s">
-        <v>1314</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F234"/>
     </row>
   </sheetData>
@@ -13525,7 +13615,7 @@
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>1309</v>
+        <v>1306</v>
       </c>
     </row>
   </sheetData>
@@ -14604,7 +14694,7 @@
         <v>727</v>
       </c>
       <c r="B13" t="s">
-        <v>1302</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -14908,7 +14998,7 @@
         <v>730</v>
       </c>
       <c r="B51" t="s">
-        <v>1303</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -14916,15 +15006,15 @@
         <v>1009</v>
       </c>
       <c r="B52" t="s">
-        <v>1304</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>1305</v>
+        <v>1302</v>
       </c>
       <c r="B53" t="s">
-        <v>1306</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -14961,10 +15051,10 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>1307</v>
+        <v>1304</v>
       </c>
       <c r="B58" t="s">
-        <v>1308</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added new issues identified on 2022-06-07
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52874A2D-407C-6243-994E-24143899B987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BB21B4-6604-C94D-834C-D1034822E1DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="500" windowWidth="23580" windowHeight="15880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4480" yWindow="500" windowWidth="23580" windowHeight="15880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2600" uniqueCount="1367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2635" uniqueCount="1387">
   <si>
     <t>sid</t>
   </si>
@@ -4189,6 +4189,66 @@
   </si>
   <si>
     <t>Checked on May 4th, 2022, all issues fixed.</t>
+  </si>
+  <si>
+    <t>Checked on June 7, 2022, no issue was found</t>
+  </si>
+  <si>
+    <t>EUPATH_0057561</t>
+  </si>
+  <si>
+    <t>Presence of opportunistic infection|Death related to opportunistic infection</t>
+  </si>
+  <si>
+    <t>Contributing cause of death|Signs and symptoms</t>
+  </si>
+  <si>
+    <t>general/general_guatemala_oi_cohort</t>
+  </si>
+  <si>
+    <t>EUPATH_0011936</t>
+  </si>
+  <si>
+    <t>Diphtheria, pertussis, and tetanus (DPT) vaccine dose count | Diphtheria, pertussis, and tetanus (DPT) vaccine dose number</t>
+  </si>
+  <si>
+    <t>gates_avenir | gates_maled</t>
+  </si>
+  <si>
+    <t>EUPATH_0011938</t>
+  </si>
+  <si>
+    <t>Hepatitis B vaccine dose count | Hepatitis B vaccine dose number</t>
+  </si>
+  <si>
+    <t>EUPATH_0011942</t>
+  </si>
+  <si>
+    <t>Measles vaccine dose count | Measles vaccine dose number</t>
+  </si>
+  <si>
+    <t>EUPATH_0011947</t>
+  </si>
+  <si>
+    <t>Pneumococcal conjugate vaccine (PCV) dose count | Pneumococcal conjugate vaccine (PCV) dose number</t>
+  </si>
+  <si>
+    <t>EUPATH_0011949</t>
+  </si>
+  <si>
+    <t>Rotavirus vaccine dose count | Rotavirus vaccine dose number</t>
+  </si>
+  <si>
+    <t>Checked on June 7, 2022, identified following issue:</t>
+  </si>
+  <si>
+    <t>Assigned EUPATH_0057601 to Presence of opportunistic infection</t>
+  </si>
+  <si>
+    <t>Jie's comment</t>
+  </si>
+  <si>
+    <t>Checked on June 7, 2022, the issue was fixed.</t>
   </si>
 </sst>
 </file>
@@ -5088,10 +5148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G220"/>
+  <dimension ref="A1:G228"/>
   <sheetViews>
-    <sheetView topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="A220" sqref="A220"/>
+    <sheetView topLeftCell="A215" workbookViewId="0">
+      <selection activeCell="C230" sqref="C230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8261,6 +8321,95 @@
         <v>1366</v>
       </c>
     </row>
+    <row r="222" spans="1:6">
+      <c r="A222" s="10" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6">
+      <c r="A223" t="s">
+        <v>0</v>
+      </c>
+      <c r="B223" t="s">
+        <v>1</v>
+      </c>
+      <c r="C223" t="s">
+        <v>2</v>
+      </c>
+      <c r="D223" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6">
+      <c r="A224" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B224">
+        <v>2</v>
+      </c>
+      <c r="C224" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D224" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4">
+      <c r="A225" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B225">
+        <v>2</v>
+      </c>
+      <c r="C225" t="s">
+        <v>1376</v>
+      </c>
+      <c r="D225" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4">
+      <c r="A226" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B226">
+        <v>2</v>
+      </c>
+      <c r="C226" t="s">
+        <v>1378</v>
+      </c>
+      <c r="D226" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4">
+      <c r="A227" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B227">
+        <v>2</v>
+      </c>
+      <c r="C227" t="s">
+        <v>1380</v>
+      </c>
+      <c r="D227" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4">
+      <c r="A228" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B228">
+        <v>2</v>
+      </c>
+      <c r="C228" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D228" t="s">
+        <v>1374</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -8269,10 +8418,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H112"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9864,6 +10013,11 @@
         <v>1366</v>
       </c>
     </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="10" t="s">
+        <v>1367</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -9872,10 +10026,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H246"/>
+  <dimension ref="A1:H252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B251" sqref="B251"/>
+    <sheetView topLeftCell="A227" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A253" sqref="A253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -13626,12 +13780,12 @@
       </c>
       <c r="F238"/>
     </row>
-    <row r="241" spans="1:6">
+    <row r="241" spans="1:7">
       <c r="A241" s="10" t="s">
         <v>1355</v>
       </c>
     </row>
-    <row r="242" spans="1:6">
+    <row r="242" spans="1:7">
       <c r="A242" t="s">
         <v>0</v>
       </c>
@@ -13651,7 +13805,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="243" spans="1:6">
+    <row r="243" spans="1:7">
       <c r="A243" t="s">
         <v>1258</v>
       </c>
@@ -13671,7 +13825,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="244" spans="1:6">
+    <row r="244" spans="1:7">
       <c r="A244" t="s">
         <v>1321</v>
       </c>
@@ -13691,9 +13845,62 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="246" spans="1:6">
+    <row r="246" spans="1:7">
       <c r="A246" s="10" t="s">
         <v>1366</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7">
+      <c r="A248" s="10" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7">
+      <c r="A249" t="s">
+        <v>0</v>
+      </c>
+      <c r="B249" t="s">
+        <v>10</v>
+      </c>
+      <c r="C249" t="s">
+        <v>2</v>
+      </c>
+      <c r="D249" t="s">
+        <v>11</v>
+      </c>
+      <c r="E249" t="s">
+        <v>3</v>
+      </c>
+      <c r="F249" s="2" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7">
+      <c r="A250" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B250">
+        <v>2</v>
+      </c>
+      <c r="C250" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D250" t="s">
+        <v>1370</v>
+      </c>
+      <c r="E250" t="s">
+        <v>1371</v>
+      </c>
+      <c r="F250" s="2" t="s">
+        <v>1384</v>
+      </c>
+      <c r="G250" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7">
+      <c r="A252" s="10" t="s">
+        <v>1386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
consistency issues idenfied on Aug 2, 2022
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EECA729-B6FE-E749-934D-5FBAD805BB89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A98F42-90A5-C545-A8DA-138FF7579043}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="500" windowWidth="26600" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2725" uniqueCount="1419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2815" uniqueCount="1469">
   <si>
     <t>sid</t>
   </si>
@@ -4345,6 +4345,156 @@
   </si>
   <si>
     <t>Change SHINE to be under "Clinical history"</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>EUPATH_0000151|EUPATH_0054076</t>
+  </si>
+  <si>
+    <t>Interviewee household head</t>
+  </si>
+  <si>
+    <t>EUPATH_0026005|EUPATH_0058084</t>
+  </si>
+  <si>
+    <t>Individuals related to participant|Household administrative information|Household Administrative information</t>
+  </si>
+  <si>
+    <t>Merozoite surface protein 7, by immunoassay result</t>
+  </si>
+  <si>
+    <t>EUPATH_0057909|EUPATH_0057911</t>
+  </si>
+  <si>
+    <t>Message that see on IEC or promotional materials specified</t>
+  </si>
+  <si>
+    <t>EUPATH_0054932|EUPATH_0058274</t>
+  </si>
+  <si>
+    <t>Where to get last HIV test</t>
+  </si>
+  <si>
+    <t>EUPATH_0058377|EUPATH_0058376</t>
+  </si>
+  <si>
+    <t>HIV/AIDS and STIs</t>
+  </si>
+  <si>
+    <t>Checked on Aug 2nd, 2022, identified following issue:</t>
+  </si>
+  <si>
+    <t>EUPATH_0024156</t>
+  </si>
+  <si>
+    <t>Don't know</t>
+  </si>
+  <si>
+    <t>Household reason for not using a bednet|Reason for not using a bednet</t>
+  </si>
+  <si>
+    <t>icemr_sw_pacific | icemr_southern_africa</t>
+  </si>
+  <si>
+    <t>EUPATH_0024143</t>
+  </si>
+  <si>
+    <t>It is too hot under the net</t>
+  </si>
+  <si>
+    <t>EUPATH_0024148</t>
+  </si>
+  <si>
+    <t>No mosquitoes around</t>
+  </si>
+  <si>
+    <t>EUPATH_0024066</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Household malaria prevention knowledge|Malaria prevention knowledge</t>
+  </si>
+  <si>
+    <t>EUPATH_0024157</t>
+  </si>
+  <si>
+    <t>EUPATH_0038686</t>
+  </si>
+  <si>
+    <t>Other medication</t>
+  </si>
+  <si>
+    <t>Treatment|Clinical history</t>
+  </si>
+  <si>
+    <t>gates_sip | icemr_sw_pacific</t>
+  </si>
+  <si>
+    <t>EUPATH_0024057</t>
+  </si>
+  <si>
+    <t>Sleep under a mosquito net</t>
+  </si>
+  <si>
+    <t>EUPATH_0024058</t>
+  </si>
+  <si>
+    <t>Spray insecticide inside the house</t>
+  </si>
+  <si>
+    <t>EUPATH_0021002</t>
+  </si>
+  <si>
+    <t>Signs and symptoms|Participant</t>
+  </si>
+  <si>
+    <t>icemr_west_africa | gates_gamin | icemr_prism2_border_cohort | gates_gems1a | general_umsp | gates_gems | icemr_india_cx | general_kalifabougou | icemr_amazonia_brazil | icemr_india_meghalaya | gates_perch | icemr_malawi | general_promote | icemr_india_cohort | icemr_south_asia | gates_sip | icemr_prism2 | icemr_india_behavior | icemr_prism | gates_provide | icemr_amazonia_peru | icemr_india_severe_malaria | gates_llineup | icemr_sw_pacific | gates_avenir | icemr_india_fever_surv</t>
+  </si>
+  <si>
+    <t>Household administrative information | Household Administrative information</t>
+  </si>
+  <si>
+    <t>icemr_prism2_border_cohort | gates_washb_bangladesh | icemr_prism2 | gates_shine | gates_namibia | gates_llineup | icemr_sw_pacific | gates_avenir | gates_ganc</t>
+  </si>
+  <si>
+    <t>EUPATH_0025072</t>
+  </si>
+  <si>
+    <t>Health center | Heath center</t>
+  </si>
+  <si>
+    <t>icemr_west_africa | general_umsp | gates_vida | general_guatemala_oi_cohort | icemr_malawi | icemr_myanmar</t>
+  </si>
+  <si>
+    <t>EUPATH_0049007</t>
+  </si>
+  <si>
+    <t>Place visited | Place visited 3</t>
+  </si>
+  <si>
+    <t>icemr_india_meghalaya | icemr_sw_pacific</t>
+  </si>
+  <si>
+    <t>EUPATH_0054076</t>
+  </si>
+  <si>
+    <t>Enrollment date | Enrollment Date</t>
+  </si>
+  <si>
+    <t>general_guatemala_oi_cohort | gates_jilinde_prospective_cohort</t>
+  </si>
+  <si>
+    <t>EUPATH_0054649</t>
+  </si>
+  <si>
+    <t>PrEP source before February 2017  specified | PrEP source before February 2017 specified</t>
+  </si>
+  <si>
+    <t>gates_jilinde_awareness_survey | gates_jilinde_demand_creation_evaluation_questionnaire</t>
   </si>
 </sst>
 </file>
@@ -5244,10 +5394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G244"/>
+  <dimension ref="A1:G252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="C248" sqref="C248"/>
+    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
+      <selection activeCell="A262" sqref="A262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8727,6 +8877,95 @@
         <v>1413</v>
       </c>
     </row>
+    <row r="246" spans="1:5">
+      <c r="A246" s="10" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5">
+      <c r="A247" t="s">
+        <v>0</v>
+      </c>
+      <c r="B247" t="s">
+        <v>1</v>
+      </c>
+      <c r="C247" t="s">
+        <v>2</v>
+      </c>
+      <c r="D247" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5">
+      <c r="A248" t="s">
+        <v>892</v>
+      </c>
+      <c r="B248">
+        <v>2</v>
+      </c>
+      <c r="C248" t="s">
+        <v>1455</v>
+      </c>
+      <c r="D248" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5">
+      <c r="A249" t="s">
+        <v>1457</v>
+      </c>
+      <c r="B249">
+        <v>2</v>
+      </c>
+      <c r="C249" t="s">
+        <v>1458</v>
+      </c>
+      <c r="D249" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5">
+      <c r="A250" t="s">
+        <v>1460</v>
+      </c>
+      <c r="B250">
+        <v>2</v>
+      </c>
+      <c r="C250" t="s">
+        <v>1461</v>
+      </c>
+      <c r="D250" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5">
+      <c r="A251" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B251">
+        <v>2</v>
+      </c>
+      <c r="C251" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D251" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5">
+      <c r="A252" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B252">
+        <v>2</v>
+      </c>
+      <c r="C252" t="s">
+        <v>1467</v>
+      </c>
+      <c r="D252" t="s">
+        <v>1468</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -8735,10 +8974,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H120"/>
+  <dimension ref="A1:H126"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10353,7 +10592,153 @@
       <c r="G119" s="2"/>
     </row>
     <row r="120" spans="1:7">
+      <c r="A120" s="10" t="s">
+        <v>1431</v>
+      </c>
       <c r="F120"/>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>1419</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="B122" s="3">
+        <v>2</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E122" s="3">
+        <v>1</v>
+      </c>
+      <c r="F122" s="3" t="b">
+        <f>EXACT(B122,E122)</f>
+        <v>0</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" s="3" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B123" s="3">
+        <v>2</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123" s="3">
+        <v>3</v>
+      </c>
+      <c r="F123" s="3" t="b">
+        <f>EXACT(B123,E123)</f>
+        <v>0</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" s="3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B124" s="3">
+        <v>2</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124" s="3">
+        <v>1</v>
+      </c>
+      <c r="F124" s="3" t="b">
+        <f>EXACT(B124,E124)</f>
+        <v>0</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" s="3" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B125" s="3">
+        <v>2</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>1427</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E125" s="3">
+        <v>1</v>
+      </c>
+      <c r="F125" s="3" t="b">
+        <f>EXACT(B125,E125)</f>
+        <v>0</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" s="3" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B126" s="3">
+        <v>2</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>1429</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126" s="3">
+        <v>1</v>
+      </c>
+      <c r="F126" s="3" t="b">
+        <f>EXACT(B126,E126)</f>
+        <v>0</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>1430</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10363,10 +10748,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H264"/>
+  <dimension ref="A1:H276"/>
   <sheetViews>
-    <sheetView topLeftCell="A252" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A266" sqref="A266"/>
+    <sheetView topLeftCell="A261" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C278" sqref="C278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10374,7 +10759,7 @@
     <col min="1" max="1" width="20.1640625" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="47.5" customWidth="1"/>
-    <col min="4" max="4" width="47" customWidth="1"/>
+    <col min="4" max="4" width="63.33203125" customWidth="1"/>
     <col min="5" max="5" width="56" customWidth="1"/>
     <col min="6" max="6" width="40.33203125" style="2" customWidth="1"/>
   </cols>
@@ -14361,6 +14746,181 @@
     <row r="264" spans="1:6">
       <c r="A264" s="10" t="s">
         <v>1413</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6">
+      <c r="A266" s="10" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6">
+      <c r="A267" t="s">
+        <v>0</v>
+      </c>
+      <c r="B267" t="s">
+        <v>10</v>
+      </c>
+      <c r="C267" t="s">
+        <v>2</v>
+      </c>
+      <c r="D267" t="s">
+        <v>11</v>
+      </c>
+      <c r="E267" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6">
+      <c r="A268" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B268">
+        <v>2</v>
+      </c>
+      <c r="C268" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D268" t="s">
+        <v>1434</v>
+      </c>
+      <c r="E268" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6">
+      <c r="A269" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B269">
+        <v>2</v>
+      </c>
+      <c r="C269" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D269" t="s">
+        <v>1434</v>
+      </c>
+      <c r="E269" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6">
+      <c r="A270" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B270">
+        <v>2</v>
+      </c>
+      <c r="C270" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D270" t="s">
+        <v>1434</v>
+      </c>
+      <c r="E270" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6">
+      <c r="A271" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B271">
+        <v>2</v>
+      </c>
+      <c r="C271" t="s">
+        <v>1441</v>
+      </c>
+      <c r="D271" t="s">
+        <v>1442</v>
+      </c>
+      <c r="E271" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6">
+      <c r="A272" t="s">
+        <v>1443</v>
+      </c>
+      <c r="B272">
+        <v>2</v>
+      </c>
+      <c r="C272" t="s">
+        <v>1441</v>
+      </c>
+      <c r="D272" t="s">
+        <v>1434</v>
+      </c>
+      <c r="E272" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5">
+      <c r="A273" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B273">
+        <v>2</v>
+      </c>
+      <c r="C273" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D273" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E273" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5">
+      <c r="A274" t="s">
+        <v>1448</v>
+      </c>
+      <c r="B274">
+        <v>2</v>
+      </c>
+      <c r="C274" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D274" t="s">
+        <v>1442</v>
+      </c>
+      <c r="E274" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5">
+      <c r="A275" t="s">
+        <v>1450</v>
+      </c>
+      <c r="B275">
+        <v>2</v>
+      </c>
+      <c r="C275" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D275" t="s">
+        <v>1442</v>
+      </c>
+      <c r="E275" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5">
+      <c r="A276" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B276">
+        <v>2</v>
+      </c>
+      <c r="C276" t="s">
+        <v>620</v>
+      </c>
+      <c r="D276" t="s">
+        <v>1453</v>
+      </c>
+      <c r="E276" t="s">
+        <v>1454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of github.com:VEuPathDB/ApiCommonData"
This reverts commit 40c65a999be6f29f2fa8c10a41008767abacf4b8, reversing
changes made to 15bfe56f095a229b59aa02574ec34586dfe6805c.
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0966BDC2-0A2F-5741-AFD8-F2FEE264AD48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EECA729-B6FE-E749-934D-5FBAD805BB89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="500" windowWidth="26600" windowHeight="14500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2200" yWindow="500" windowWidth="26600" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2852" uniqueCount="1482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2725" uniqueCount="1419">
   <si>
     <t>sid</t>
   </si>
@@ -4345,195 +4345,6 @@
   </si>
   <si>
     <t>Change SHINE to be under "Clinical history"</t>
-  </si>
-  <si>
-    <t>same</t>
-  </si>
-  <si>
-    <t>EUPATH_0000151|EUPATH_0054076</t>
-  </si>
-  <si>
-    <t>Interviewee household head</t>
-  </si>
-  <si>
-    <t>EUPATH_0026005|EUPATH_0058084</t>
-  </si>
-  <si>
-    <t>Individuals related to participant|Household administrative information|Household Administrative information</t>
-  </si>
-  <si>
-    <t>Merozoite surface protein 7, by immunoassay result</t>
-  </si>
-  <si>
-    <t>EUPATH_0057909|EUPATH_0057911</t>
-  </si>
-  <si>
-    <t>Message that see on IEC or promotional materials specified</t>
-  </si>
-  <si>
-    <t>EUPATH_0054932|EUPATH_0058274</t>
-  </si>
-  <si>
-    <t>Where to get last HIV test</t>
-  </si>
-  <si>
-    <t>EUPATH_0058377|EUPATH_0058376</t>
-  </si>
-  <si>
-    <t>HIV/AIDS and STIs</t>
-  </si>
-  <si>
-    <t>Checked on Aug 2nd, 2022, identified following issue:</t>
-  </si>
-  <si>
-    <t>EUPATH_0024156</t>
-  </si>
-  <si>
-    <t>Don't know</t>
-  </si>
-  <si>
-    <t>Household reason for not using a bednet|Reason for not using a bednet</t>
-  </si>
-  <si>
-    <t>icemr_sw_pacific | icemr_southern_africa</t>
-  </si>
-  <si>
-    <t>EUPATH_0024143</t>
-  </si>
-  <si>
-    <t>It is too hot under the net</t>
-  </si>
-  <si>
-    <t>EUPATH_0024148</t>
-  </si>
-  <si>
-    <t>No mosquitoes around</t>
-  </si>
-  <si>
-    <t>EUPATH_0024066</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Household malaria prevention knowledge|Malaria prevention knowledge</t>
-  </si>
-  <si>
-    <t>EUPATH_0024157</t>
-  </si>
-  <si>
-    <t>EUPATH_0038686</t>
-  </si>
-  <si>
-    <t>Other medication</t>
-  </si>
-  <si>
-    <t>Treatment|Clinical history</t>
-  </si>
-  <si>
-    <t>gates_sip | icemr_sw_pacific</t>
-  </si>
-  <si>
-    <t>EUPATH_0024057</t>
-  </si>
-  <si>
-    <t>Sleep under a mosquito net</t>
-  </si>
-  <si>
-    <t>EUPATH_0024058</t>
-  </si>
-  <si>
-    <t>Spray insecticide inside the house</t>
-  </si>
-  <si>
-    <t>EUPATH_0021002</t>
-  </si>
-  <si>
-    <t>Signs and symptoms|Participant</t>
-  </si>
-  <si>
-    <t>icemr_west_africa | gates_gamin | icemr_prism2_border_cohort | gates_gems1a | general_umsp | gates_gems | icemr_india_cx | general_kalifabougou | icemr_amazonia_brazil | icemr_india_meghalaya | gates_perch | icemr_malawi | general_promote | icemr_india_cohort | icemr_south_asia | gates_sip | icemr_prism2 | icemr_india_behavior | icemr_prism | gates_provide | icemr_amazonia_peru | icemr_india_severe_malaria | gates_llineup | icemr_sw_pacific | gates_avenir | icemr_india_fever_surv</t>
-  </si>
-  <si>
-    <t>Household administrative information | Household Administrative information</t>
-  </si>
-  <si>
-    <t>icemr_prism2_border_cohort | gates_washb_bangladesh | icemr_prism2 | gates_shine | gates_namibia | gates_llineup | icemr_sw_pacific | gates_avenir | gates_ganc</t>
-  </si>
-  <si>
-    <t>EUPATH_0025072</t>
-  </si>
-  <si>
-    <t>Health center | Heath center</t>
-  </si>
-  <si>
-    <t>icemr_west_africa | general_umsp | gates_vida | general_guatemala_oi_cohort | icemr_malawi | icemr_myanmar</t>
-  </si>
-  <si>
-    <t>EUPATH_0049007</t>
-  </si>
-  <si>
-    <t>Place visited | Place visited 3</t>
-  </si>
-  <si>
-    <t>icemr_india_meghalaya | icemr_sw_pacific</t>
-  </si>
-  <si>
-    <t>EUPATH_0054076</t>
-  </si>
-  <si>
-    <t>Enrollment date | Enrollment Date</t>
-  </si>
-  <si>
-    <t>general_guatemala_oi_cohort | gates_jilinde_prospective_cohort</t>
-  </si>
-  <si>
-    <t>EUPATH_0054649</t>
-  </si>
-  <si>
-    <t>PrEP source before February 2017  specified | PrEP source before February 2017 specified</t>
-  </si>
-  <si>
-    <t>gates_jilinde_awareness_survey | gates_jilinde_demand_creation_evaluation_questionnaire</t>
-  </si>
-  <si>
-    <t>Label should be "Enrollment date"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label should be "Household administrative information" in sw pacific </t>
-  </si>
-  <si>
-    <t>Label should be "Health center" in Jilinde</t>
-  </si>
-  <si>
-    <t>Label should be "PrEP source before February 2017 specified"</t>
-  </si>
-  <si>
-    <t>Use EUPATH_0000151</t>
-  </si>
-  <si>
-    <t>Change label on EUPATH_0058084 to "Respondant head of household"</t>
-  </si>
-  <si>
-    <t>Use EUPATH_0054932</t>
-  </si>
-  <si>
-    <t>Update EUPATH_0058377 label to say "Where to get last HIV test specified"</t>
-  </si>
-  <si>
-    <t>Create new IRI for sw pacific</t>
-  </si>
-  <si>
-    <t>Move under Signs and symptoms in sw pacfici</t>
-  </si>
-  <si>
-    <t>Label should be "Place visited" in sw_pacific. Need to remap variable so that this IRI has variable  "icemrcambodiaprevalence_data_2022-06-06_2029_sak::scleft1_place_01". Variable "icemrcambodiaprevalence_data_2022-06-06_2029_sak::scleft1_place_03" should be remapped to a new IRI with label "Place visited, 3"</t>
-  </si>
-  <si>
-    <t>Need to check with Sarah. This study hasn't yet undergone owl review</t>
-  </si>
-  <si>
-    <t>Change sw pacific to use 'Other medicine taken'  EUPATH_0053127</t>
   </si>
 </sst>
 </file>
@@ -5433,17 +5244,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G252"/>
+  <dimension ref="A1:G244"/>
   <sheetViews>
-    <sheetView topLeftCell="A231" workbookViewId="0">
-      <selection activeCell="A248" sqref="A248:XFD251"/>
+    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="C248" sqref="C248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="5.1640625" customWidth="1"/>
-    <col min="3" max="3" width="84.5" customWidth="1"/>
+    <col min="3" max="3" width="70.83203125" customWidth="1"/>
     <col min="4" max="4" width="40.33203125" customWidth="1"/>
     <col min="5" max="5" width="53.5" style="2" customWidth="1"/>
   </cols>
@@ -8877,7 +8688,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="241" spans="1:6">
+    <row r="241" spans="1:5">
       <c r="A241" t="s">
         <v>1410</v>
       </c>
@@ -8894,7 +8705,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="242" spans="1:6">
+    <row r="242" spans="1:5">
       <c r="A242" t="s">
         <v>1397</v>
       </c>
@@ -8911,128 +8722,9 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="244" spans="1:6">
+    <row r="244" spans="1:5">
       <c r="A244" s="10" t="s">
         <v>1413</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6">
-      <c r="A246" s="10" t="s">
-        <v>1431</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6">
-      <c r="A247" t="s">
-        <v>0</v>
-      </c>
-      <c r="B247" t="s">
-        <v>1</v>
-      </c>
-      <c r="C247" t="s">
-        <v>2</v>
-      </c>
-      <c r="D247" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6">
-      <c r="A248" t="s">
-        <v>892</v>
-      </c>
-      <c r="B248">
-        <v>2</v>
-      </c>
-      <c r="C248" t="s">
-        <v>1455</v>
-      </c>
-      <c r="D248" t="s">
-        <v>1456</v>
-      </c>
-      <c r="E248" s="2" t="s">
-        <v>1470</v>
-      </c>
-      <c r="F248" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6">
-      <c r="A249" t="s">
-        <v>1457</v>
-      </c>
-      <c r="B249">
-        <v>2</v>
-      </c>
-      <c r="C249" t="s">
-        <v>1458</v>
-      </c>
-      <c r="D249" t="s">
-        <v>1459</v>
-      </c>
-      <c r="E249" s="2" t="s">
-        <v>1471</v>
-      </c>
-      <c r="F249" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6">
-      <c r="A250" t="s">
-        <v>1460</v>
-      </c>
-      <c r="B250">
-        <v>2</v>
-      </c>
-      <c r="C250" t="s">
-        <v>1461</v>
-      </c>
-      <c r="D250" t="s">
-        <v>1462</v>
-      </c>
-      <c r="E250" s="2" t="s">
-        <v>1479</v>
-      </c>
-      <c r="F250" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6">
-      <c r="A251" t="s">
-        <v>1463</v>
-      </c>
-      <c r="B251">
-        <v>2</v>
-      </c>
-      <c r="C251" t="s">
-        <v>1464</v>
-      </c>
-      <c r="D251" t="s">
-        <v>1465</v>
-      </c>
-      <c r="E251" s="2" t="s">
-        <v>1469</v>
-      </c>
-      <c r="F251" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6">
-      <c r="A252" t="s">
-        <v>1466</v>
-      </c>
-      <c r="B252">
-        <v>2</v>
-      </c>
-      <c r="C252" t="s">
-        <v>1467</v>
-      </c>
-      <c r="D252" t="s">
-        <v>1468</v>
-      </c>
-      <c r="E252" s="2" t="s">
-        <v>1472</v>
-      </c>
-      <c r="F252" t="s">
-        <v>829</v>
       </c>
     </row>
   </sheetData>
@@ -9043,10 +8735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I126"/>
+  <dimension ref="A1:H120"/>
   <sheetViews>
-    <sheetView topLeftCell="D115" workbookViewId="0">
-      <selection activeCell="H128" sqref="H128"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9056,7 +8748,6 @@
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="21.1640625" customWidth="1"/>
     <col min="6" max="6" width="30.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="40.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -10639,203 +10330,30 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:7">
       <c r="A114" s="10" t="s">
         <v>1367</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:7">
       <c r="A116" s="10" t="s">
         <v>1400</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:7">
       <c r="A117" s="10"/>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:7">
       <c r="A118" s="10" t="s">
         <v>1413</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:7">
       <c r="F119"/>
       <c r="G119" s="2"/>
     </row>
-    <row r="120" spans="1:9">
-      <c r="A120" s="10" t="s">
-        <v>1431</v>
-      </c>
+    <row r="120" spans="1:7">
       <c r="F120"/>
-    </row>
-    <row r="121" spans="1:9">
-      <c r="A121" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D121" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>1213</v>
-      </c>
-      <c r="F121" s="3" t="s">
-        <v>1419</v>
-      </c>
-      <c r="G121" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9">
-      <c r="A122" s="3" t="s">
-        <v>722</v>
-      </c>
-      <c r="B122" s="3">
-        <v>2</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>1420</v>
-      </c>
-      <c r="D122" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E122" s="3">
-        <v>1</v>
-      </c>
-      <c r="F122" s="3" t="b">
-        <f>EXACT(B122,E122)</f>
-        <v>0</v>
-      </c>
-      <c r="G122" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="H122" s="5" t="s">
-        <v>1473</v>
-      </c>
-      <c r="I122" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9">
-      <c r="A123" s="3" t="s">
-        <v>1421</v>
-      </c>
-      <c r="B123" s="3">
-        <v>2</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>1422</v>
-      </c>
-      <c r="D123" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E123" s="3">
-        <v>3</v>
-      </c>
-      <c r="F123" s="3" t="b">
-        <f>EXACT(B123,E123)</f>
-        <v>0</v>
-      </c>
-      <c r="G123" s="3" t="s">
-        <v>1423</v>
-      </c>
-      <c r="H123" s="5" t="s">
-        <v>1474</v>
-      </c>
-      <c r="I123" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9">
-      <c r="A124" s="3" t="s">
-        <v>1424</v>
-      </c>
-      <c r="B124" s="3">
-        <v>2</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>1425</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E124" s="3">
-        <v>1</v>
-      </c>
-      <c r="F124" s="3" t="b">
-        <f>EXACT(B124,E124)</f>
-        <v>0</v>
-      </c>
-      <c r="G124" s="3" t="s">
-        <v>558</v>
-      </c>
-      <c r="H124" s="2" t="s">
-        <v>1480</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9">
-      <c r="A125" s="3" t="s">
-        <v>1426</v>
-      </c>
-      <c r="B125" s="3">
-        <v>2</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>1427</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E125" s="3">
-        <v>1</v>
-      </c>
-      <c r="F125" s="3" t="b">
-        <f>EXACT(B125,E125)</f>
-        <v>0</v>
-      </c>
-      <c r="G125" s="3" t="s">
-        <v>1268</v>
-      </c>
-      <c r="H125" s="5" t="s">
-        <v>1475</v>
-      </c>
-      <c r="I125" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9">
-      <c r="A126" s="3" t="s">
-        <v>1428</v>
-      </c>
-      <c r="B126" s="3">
-        <v>2</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>1429</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E126" s="3">
-        <v>1</v>
-      </c>
-      <c r="F126" s="3" t="b">
-        <f>EXACT(B126,E126)</f>
-        <v>0</v>
-      </c>
-      <c r="G126" s="3" t="s">
-        <v>1430</v>
-      </c>
-      <c r="H126" s="2" t="s">
-        <v>1476</v>
-      </c>
-      <c r="I126" t="s">
-        <v>829</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10845,10 +10363,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H276"/>
+  <dimension ref="A1:H264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A266" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F279" sqref="F279"/>
+    <sheetView topLeftCell="A252" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A266" sqref="A266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10856,7 +10374,7 @@
     <col min="1" max="1" width="20.1640625" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="47.5" customWidth="1"/>
-    <col min="4" max="4" width="63.33203125" customWidth="1"/>
+    <col min="4" max="4" width="47" customWidth="1"/>
     <col min="5" max="5" width="56" customWidth="1"/>
     <col min="6" max="6" width="40.33203125" style="2" customWidth="1"/>
   </cols>
@@ -14761,7 +14279,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="257" spans="1:7">
+    <row r="257" spans="1:6">
       <c r="A257" t="s">
         <v>1405</v>
       </c>
@@ -14778,12 +14296,12 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="259" spans="1:7">
+    <row r="259" spans="1:6">
       <c r="A259" s="10" t="s">
         <v>1414</v>
       </c>
     </row>
-    <row r="260" spans="1:7">
+    <row r="260" spans="1:6">
       <c r="A260" t="s">
         <v>0</v>
       </c>
@@ -14800,7 +14318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="1:7">
+    <row r="261" spans="1:6">
       <c r="A261" t="s">
         <v>1401</v>
       </c>
@@ -14820,7 +14338,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="262" spans="1:7">
+    <row r="262" spans="1:6">
       <c r="A262" t="s">
         <v>1405</v>
       </c>
@@ -14840,238 +14358,9 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="264" spans="1:7">
+    <row r="264" spans="1:6">
       <c r="A264" s="10" t="s">
         <v>1413</v>
-      </c>
-    </row>
-    <row r="266" spans="1:7">
-      <c r="A266" s="10" t="s">
-        <v>1431</v>
-      </c>
-    </row>
-    <row r="267" spans="1:7">
-      <c r="A267" t="s">
-        <v>0</v>
-      </c>
-      <c r="B267" t="s">
-        <v>10</v>
-      </c>
-      <c r="C267" t="s">
-        <v>2</v>
-      </c>
-      <c r="D267" t="s">
-        <v>11</v>
-      </c>
-      <c r="E267" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="268" spans="1:7">
-      <c r="A268" t="s">
-        <v>1432</v>
-      </c>
-      <c r="B268">
-        <v>2</v>
-      </c>
-      <c r="C268" t="s">
-        <v>1433</v>
-      </c>
-      <c r="D268" t="s">
-        <v>1434</v>
-      </c>
-      <c r="E268" t="s">
-        <v>1435</v>
-      </c>
-      <c r="F268" s="2" t="s">
-        <v>1477</v>
-      </c>
-      <c r="G268" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="269" spans="1:7">
-      <c r="A269" t="s">
-        <v>1436</v>
-      </c>
-      <c r="B269">
-        <v>2</v>
-      </c>
-      <c r="C269" t="s">
-        <v>1437</v>
-      </c>
-      <c r="D269" t="s">
-        <v>1434</v>
-      </c>
-      <c r="E269" t="s">
-        <v>1435</v>
-      </c>
-      <c r="F269" s="2" t="s">
-        <v>1477</v>
-      </c>
-      <c r="G269" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="270" spans="1:7">
-      <c r="A270" t="s">
-        <v>1438</v>
-      </c>
-      <c r="B270">
-        <v>2</v>
-      </c>
-      <c r="C270" t="s">
-        <v>1439</v>
-      </c>
-      <c r="D270" t="s">
-        <v>1434</v>
-      </c>
-      <c r="E270" t="s">
-        <v>1435</v>
-      </c>
-      <c r="F270" s="2" t="s">
-        <v>1477</v>
-      </c>
-      <c r="G270" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="271" spans="1:7">
-      <c r="A271" t="s">
-        <v>1440</v>
-      </c>
-      <c r="B271">
-        <v>2</v>
-      </c>
-      <c r="C271" t="s">
-        <v>1441</v>
-      </c>
-      <c r="D271" t="s">
-        <v>1442</v>
-      </c>
-      <c r="E271" t="s">
-        <v>1435</v>
-      </c>
-      <c r="F271" s="2" t="s">
-        <v>1477</v>
-      </c>
-      <c r="G271" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="272" spans="1:7">
-      <c r="A272" t="s">
-        <v>1443</v>
-      </c>
-      <c r="B272">
-        <v>2</v>
-      </c>
-      <c r="C272" t="s">
-        <v>1441</v>
-      </c>
-      <c r="D272" t="s">
-        <v>1434</v>
-      </c>
-      <c r="E272" t="s">
-        <v>1435</v>
-      </c>
-      <c r="F272" s="2" t="s">
-        <v>1477</v>
-      </c>
-      <c r="G272" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="273" spans="1:7">
-      <c r="A273" t="s">
-        <v>1444</v>
-      </c>
-      <c r="B273">
-        <v>2</v>
-      </c>
-      <c r="C273" t="s">
-        <v>1445</v>
-      </c>
-      <c r="D273" t="s">
-        <v>1446</v>
-      </c>
-      <c r="E273" t="s">
-        <v>1447</v>
-      </c>
-      <c r="F273" s="2" t="s">
-        <v>1481</v>
-      </c>
-      <c r="G273" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="274" spans="1:7">
-      <c r="A274" t="s">
-        <v>1448</v>
-      </c>
-      <c r="B274">
-        <v>2</v>
-      </c>
-      <c r="C274" t="s">
-        <v>1449</v>
-      </c>
-      <c r="D274" t="s">
-        <v>1442</v>
-      </c>
-      <c r="E274" t="s">
-        <v>1435</v>
-      </c>
-      <c r="F274" s="2" t="s">
-        <v>1477</v>
-      </c>
-      <c r="G274" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="275" spans="1:7">
-      <c r="A275" t="s">
-        <v>1450</v>
-      </c>
-      <c r="B275">
-        <v>2</v>
-      </c>
-      <c r="C275" t="s">
-        <v>1451</v>
-      </c>
-      <c r="D275" t="s">
-        <v>1442</v>
-      </c>
-      <c r="E275" t="s">
-        <v>1435</v>
-      </c>
-      <c r="F275" s="2" t="s">
-        <v>1477</v>
-      </c>
-      <c r="G275" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="276" spans="1:7">
-      <c r="A276" t="s">
-        <v>1452</v>
-      </c>
-      <c r="B276">
-        <v>2</v>
-      </c>
-      <c r="C276" t="s">
-        <v>620</v>
-      </c>
-      <c r="D276" t="s">
-        <v>1453</v>
-      </c>
-      <c r="E276" t="s">
-        <v>1454</v>
-      </c>
-      <c r="F276" s="2" t="s">
-        <v>1478</v>
-      </c>
-      <c r="G276" t="s">
-        <v>829</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add checking results on 2022-08-04
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EECA729-B6FE-E749-934D-5FBAD805BB89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F9943B-4DD9-0D46-A9F9-EFF3FCA51112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="500" windowWidth="26600" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="500" windowWidth="26600" windowHeight="14500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2725" uniqueCount="1419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2855" uniqueCount="1482">
   <si>
     <t>sid</t>
   </si>
@@ -3667,9 +3667,6 @@
   </si>
   <si>
     <t>Checked on Feb 23th, 2022, identified following issue:</t>
-  </si>
-  <si>
-    <t>parent_count</t>
   </si>
   <si>
     <t>Cerebrospinal fluid microbiology test|Blood microbiology test|Other sample microbiology test|Induced sputum microbiology test|Endotracheal tube aspirate test|Endotracheal tube aspirate microbiology test|Lung aspirate microbiology test|Pleural fluid microbiology test</t>
@@ -4345,6 +4342,198 @@
   </si>
   <si>
     <t>Change SHINE to be under "Clinical history"</t>
+  </si>
+  <si>
+    <t>EUPATH_0000151|EUPATH_0054076</t>
+  </si>
+  <si>
+    <t>Interviewee household head</t>
+  </si>
+  <si>
+    <t>EUPATH_0026005|EUPATH_0058084</t>
+  </si>
+  <si>
+    <t>Individuals related to participant|Household administrative information|Household Administrative information</t>
+  </si>
+  <si>
+    <t>Merozoite surface protein 7, by immunoassay result</t>
+  </si>
+  <si>
+    <t>EUPATH_0057909|EUPATH_0057911</t>
+  </si>
+  <si>
+    <t>Message that see on IEC or promotional materials specified</t>
+  </si>
+  <si>
+    <t>EUPATH_0054932|EUPATH_0058274</t>
+  </si>
+  <si>
+    <t>Where to get last HIV test</t>
+  </si>
+  <si>
+    <t>EUPATH_0058377|EUPATH_0058376</t>
+  </si>
+  <si>
+    <t>HIV/AIDS and STIs</t>
+  </si>
+  <si>
+    <t>Checked on Aug 2nd, 2022, identified following issue:</t>
+  </si>
+  <si>
+    <t>EUPATH_0024156</t>
+  </si>
+  <si>
+    <t>Don't know</t>
+  </si>
+  <si>
+    <t>Household reason for not using a bednet|Reason for not using a bednet</t>
+  </si>
+  <si>
+    <t>icemr_sw_pacific | icemr_southern_africa</t>
+  </si>
+  <si>
+    <t>EUPATH_0024143</t>
+  </si>
+  <si>
+    <t>It is too hot under the net</t>
+  </si>
+  <si>
+    <t>EUPATH_0024148</t>
+  </si>
+  <si>
+    <t>No mosquitoes around</t>
+  </si>
+  <si>
+    <t>EUPATH_0024066</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Household malaria prevention knowledge|Malaria prevention knowledge</t>
+  </si>
+  <si>
+    <t>EUPATH_0024157</t>
+  </si>
+  <si>
+    <t>EUPATH_0038686</t>
+  </si>
+  <si>
+    <t>Other medication</t>
+  </si>
+  <si>
+    <t>Treatment|Clinical history</t>
+  </si>
+  <si>
+    <t>gates_sip | icemr_sw_pacific</t>
+  </si>
+  <si>
+    <t>EUPATH_0024057</t>
+  </si>
+  <si>
+    <t>Sleep under a mosquito net</t>
+  </si>
+  <si>
+    <t>EUPATH_0024058</t>
+  </si>
+  <si>
+    <t>Spray insecticide inside the house</t>
+  </si>
+  <si>
+    <t>EUPATH_0021002</t>
+  </si>
+  <si>
+    <t>Signs and symptoms|Participant</t>
+  </si>
+  <si>
+    <t>icemr_west_africa | gates_gamin | icemr_prism2_border_cohort | gates_gems1a | general_umsp | gates_gems | icemr_india_cx | general_kalifabougou | icemr_amazonia_brazil | icemr_india_meghalaya | gates_perch | icemr_malawi | general_promote | icemr_india_cohort | icemr_south_asia | gates_sip | icemr_prism2 | icemr_india_behavior | icemr_prism | gates_provide | icemr_amazonia_peru | icemr_india_severe_malaria | gates_llineup | icemr_sw_pacific | gates_avenir | icemr_india_fever_surv</t>
+  </si>
+  <si>
+    <t>Household administrative information | Household Administrative information</t>
+  </si>
+  <si>
+    <t>icemr_prism2_border_cohort | gates_washb_bangladesh | icemr_prism2 | gates_shine | gates_namibia | gates_llineup | icemr_sw_pacific | gates_avenir | gates_ganc</t>
+  </si>
+  <si>
+    <t>EUPATH_0025072</t>
+  </si>
+  <si>
+    <t>Health center | Heath center</t>
+  </si>
+  <si>
+    <t>icemr_west_africa | general_umsp | gates_vida | general_guatemala_oi_cohort | icemr_malawi | icemr_myanmar</t>
+  </si>
+  <si>
+    <t>EUPATH_0049007</t>
+  </si>
+  <si>
+    <t>Place visited | Place visited 3</t>
+  </si>
+  <si>
+    <t>icemr_india_meghalaya | icemr_sw_pacific</t>
+  </si>
+  <si>
+    <t>EUPATH_0054076</t>
+  </si>
+  <si>
+    <t>Enrollment date | Enrollment Date</t>
+  </si>
+  <si>
+    <t>general_guatemala_oi_cohort | gates_jilinde_prospective_cohort</t>
+  </si>
+  <si>
+    <t>EUPATH_0054649</t>
+  </si>
+  <si>
+    <t>PrEP source before February 2017  specified | PrEP source before February 2017 specified</t>
+  </si>
+  <si>
+    <t>gates_jilinde_awareness_survey | gates_jilinde_demand_creation_evaluation_questionnaire</t>
+  </si>
+  <si>
+    <t>Label should be "Enrollment date"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Label should be "Household administrative information" in sw pacific </t>
+  </si>
+  <si>
+    <t>Label should be "Health center" in Jilinde</t>
+  </si>
+  <si>
+    <t>Label should be "PrEP source before February 2017 specified"</t>
+  </si>
+  <si>
+    <t>Use EUPATH_0000151</t>
+  </si>
+  <si>
+    <t>Change label on EUPATH_0058084 to "Respondant head of household"</t>
+  </si>
+  <si>
+    <t>Use EUPATH_0054932</t>
+  </si>
+  <si>
+    <t>Update EUPATH_0058377 label to say "Where to get last HIV test specified"</t>
+  </si>
+  <si>
+    <t>Create new IRI for sw pacific</t>
+  </si>
+  <si>
+    <t>Move under Signs and symptoms in sw pacfici</t>
+  </si>
+  <si>
+    <t>Label should be "Place visited" in sw_pacific. Need to remap variable so that this IRI has variable  "icemrcambodiaprevalence_data_2022-06-06_2029_sak::scleft1_place_01". Variable "icemrcambodiaprevalence_data_2022-06-06_2029_sak::scleft1_place_03" should be remapped to a new IRI with label "Place visited, 3"</t>
+  </si>
+  <si>
+    <t>Need to check with Sarah. This study hasn't yet undergone owl review</t>
+  </si>
+  <si>
+    <t>Change sw pacific to use 'Other medicine taken'  EUPATH_0053127</t>
+  </si>
+  <si>
+    <t>Checked on Aug 4th, 2022, no issue was found</t>
+  </si>
+  <si>
+    <t>Checked on Aug 4th, 2022, only one issue is found.</t>
   </si>
 </sst>
 </file>
@@ -5244,17 +5433,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G244"/>
+  <dimension ref="A1:G254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="C248" sqref="C248"/>
+    <sheetView topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="C239" sqref="C239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="5.1640625" customWidth="1"/>
-    <col min="3" max="3" width="70.83203125" customWidth="1"/>
+    <col min="3" max="3" width="84.5" customWidth="1"/>
     <col min="4" max="4" width="40.33203125" customWidth="1"/>
     <col min="5" max="5" width="53.5" style="2" customWidth="1"/>
   </cols>
@@ -7827,7 +8016,7 @@
     </row>
     <row r="177" spans="1:7">
       <c r="A177" s="10" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="178" spans="1:7">
@@ -7846,19 +8035,19 @@
     </row>
     <row r="179" spans="1:7">
       <c r="A179" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B179">
         <v>2</v>
       </c>
       <c r="C179" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="D179" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="F179" t="s">
         <v>829</v>
@@ -7866,19 +8055,19 @@
     </row>
     <row r="180" spans="1:7">
       <c r="A180" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B180">
         <v>2</v>
       </c>
       <c r="C180" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="D180" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="F180" t="s">
         <v>829</v>
@@ -7886,76 +8075,76 @@
     </row>
     <row r="181" spans="1:7">
       <c r="A181" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B181">
         <v>2</v>
       </c>
       <c r="C181" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="D181" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="182" spans="1:7">
       <c r="A182" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B182">
+        <v>2</v>
+      </c>
+      <c r="C182" t="s">
         <v>1279</v>
       </c>
-      <c r="B182">
-        <v>2</v>
-      </c>
-      <c r="C182" t="s">
+      <c r="D182" t="s">
         <v>1280</v>
       </c>
-      <c r="D182" t="s">
-        <v>1281</v>
-      </c>
       <c r="E182" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F182" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="183" spans="1:7">
       <c r="A183" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B183">
+        <v>2</v>
+      </c>
+      <c r="C183" t="s">
         <v>1282</v>
       </c>
-      <c r="B183">
-        <v>2</v>
-      </c>
-      <c r="C183" t="s">
-        <v>1283</v>
-      </c>
       <c r="D183" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F183" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="184" spans="1:7">
       <c r="A184" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B184">
         <v>3</v>
       </c>
       <c r="C184" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D184" t="s">
         <v>1285</v>
       </c>
-      <c r="D184" t="s">
-        <v>1286</v>
-      </c>
       <c r="E184" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F184" t="s">
         <v>829</v>
@@ -7963,19 +8152,19 @@
     </row>
     <row r="185" spans="1:7">
       <c r="A185" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B185">
         <v>3</v>
       </c>
       <c r="C185" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="D185" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F185" t="s">
         <v>829</v>
@@ -7983,39 +8172,39 @@
     </row>
     <row r="186" spans="1:7">
       <c r="A186" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B186">
+        <v>2</v>
+      </c>
+      <c r="C186" t="s">
         <v>1289</v>
       </c>
-      <c r="B186">
-        <v>2</v>
-      </c>
-      <c r="C186" t="s">
-        <v>1290</v>
-      </c>
       <c r="D186" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="E186" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F186" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="187" spans="1:7">
       <c r="A187" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B187">
+        <v>2</v>
+      </c>
+      <c r="C187" t="s">
         <v>1291</v>
       </c>
-      <c r="B187">
-        <v>2</v>
-      </c>
-      <c r="C187" t="s">
+      <c r="D187" t="s">
         <v>1292</v>
       </c>
-      <c r="D187" t="s">
-        <v>1293</v>
-      </c>
       <c r="E187" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F187" t="s">
         <v>829</v>
@@ -8023,53 +8212,53 @@
     </row>
     <row r="188" spans="1:7">
       <c r="A188" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B188">
+        <v>2</v>
+      </c>
+      <c r="C188" t="s">
         <v>1294</v>
       </c>
-      <c r="B188">
-        <v>2</v>
-      </c>
-      <c r="C188" t="s">
+      <c r="D188" t="s">
         <v>1295</v>
       </c>
-      <c r="D188" t="s">
-        <v>1296</v>
-      </c>
       <c r="E188" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F188" t="s">
         <v>829</v>
       </c>
       <c r="G188" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="189" spans="1:7">
       <c r="A189" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B189">
+        <v>2</v>
+      </c>
+      <c r="C189" t="s">
         <v>1297</v>
       </c>
-      <c r="B189">
-        <v>2</v>
-      </c>
-      <c r="C189" t="s">
-        <v>1298</v>
-      </c>
       <c r="D189" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="E189" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F189" t="s">
         <v>829</v>
       </c>
       <c r="G189" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="191" spans="1:7">
       <c r="A191" s="10" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="192" spans="1:7">
@@ -8088,178 +8277,178 @@
     </row>
     <row r="193" spans="1:5">
       <c r="A193" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B193">
         <v>2</v>
       </c>
       <c r="C193" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="D193" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="E193" s="2" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="194" spans="1:5">
       <c r="A194" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="B194">
         <v>2</v>
       </c>
       <c r="C194" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="D194" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="195" spans="1:5">
       <c r="A195" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B195">
         <v>3</v>
       </c>
       <c r="C195" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D195" t="s">
         <v>1285</v>
-      </c>
-      <c r="D195" t="s">
-        <v>1286</v>
       </c>
     </row>
     <row r="196" spans="1:5">
       <c r="A196" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B196">
         <v>3</v>
       </c>
       <c r="C196" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="D196" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="197" spans="1:5">
       <c r="A197" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B197">
+        <v>2</v>
+      </c>
+      <c r="C197" t="s">
         <v>1326</v>
       </c>
-      <c r="B197">
-        <v>2</v>
-      </c>
-      <c r="C197" t="s">
-        <v>1327</v>
-      </c>
       <c r="D197" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="198" spans="1:5">
       <c r="A198" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B198">
+        <v>2</v>
+      </c>
+      <c r="C198" t="s">
         <v>1328</v>
       </c>
-      <c r="B198">
-        <v>2</v>
-      </c>
-      <c r="C198" t="s">
-        <v>1329</v>
-      </c>
       <c r="D198" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="199" spans="1:5">
       <c r="A199" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B199">
+        <v>2</v>
+      </c>
+      <c r="C199" t="s">
         <v>1330</v>
       </c>
-      <c r="B199">
-        <v>2</v>
-      </c>
-      <c r="C199" t="s">
-        <v>1331</v>
-      </c>
       <c r="D199" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="200" spans="1:5">
       <c r="A200" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B200">
+        <v>2</v>
+      </c>
+      <c r="C200" t="s">
         <v>1332</v>
       </c>
-      <c r="B200">
-        <v>2</v>
-      </c>
-      <c r="C200" t="s">
-        <v>1333</v>
-      </c>
       <c r="D200" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="201" spans="1:5">
       <c r="A201" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B201">
+        <v>2</v>
+      </c>
+      <c r="C201" t="s">
         <v>1291</v>
       </c>
-      <c r="B201">
-        <v>2</v>
-      </c>
-      <c r="C201" t="s">
+      <c r="D201" t="s">
         <v>1292</v>
-      </c>
-      <c r="D201" t="s">
-        <v>1293</v>
       </c>
     </row>
     <row r="202" spans="1:5">
       <c r="A202" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B202">
+        <v>2</v>
+      </c>
+      <c r="C202" t="s">
         <v>1294</v>
       </c>
-      <c r="B202">
-        <v>2</v>
-      </c>
-      <c r="C202" t="s">
+      <c r="D202" t="s">
         <v>1295</v>
-      </c>
-      <c r="D202" t="s">
-        <v>1296</v>
       </c>
     </row>
     <row r="203" spans="1:5">
       <c r="A203" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B203">
+        <v>2</v>
+      </c>
+      <c r="C203" t="s">
         <v>1297</v>
       </c>
-      <c r="B203">
-        <v>2</v>
-      </c>
-      <c r="C203" t="s">
-        <v>1298</v>
-      </c>
       <c r="D203" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="204" spans="1:5">
       <c r="A204" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B204">
+        <v>2</v>
+      </c>
+      <c r="C204" t="s">
         <v>1334</v>
       </c>
-      <c r="B204">
-        <v>2</v>
-      </c>
-      <c r="C204" t="s">
+      <c r="D204" t="s">
         <v>1335</v>
-      </c>
-      <c r="D204" t="s">
-        <v>1336</v>
       </c>
     </row>
     <row r="206" spans="1:5">
       <c r="A206" s="10" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -8281,80 +8470,80 @@
     </row>
     <row r="208" spans="1:5">
       <c r="A208" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B208">
         <v>2</v>
       </c>
       <c r="C208" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="D208" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="E208" s="2" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="209" spans="1:6">
       <c r="A209" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B209">
+        <v>2</v>
+      </c>
+      <c r="C209" t="s">
         <v>1349</v>
       </c>
-      <c r="B209">
-        <v>2</v>
-      </c>
-      <c r="C209" t="s">
-        <v>1350</v>
-      </c>
       <c r="D209" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="E209" s="2" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="210" spans="1:6">
       <c r="A210" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B210">
+        <v>2</v>
+      </c>
+      <c r="C210" t="s">
         <v>1351</v>
       </c>
-      <c r="B210">
-        <v>2</v>
-      </c>
-      <c r="C210" t="s">
-        <v>1352</v>
-      </c>
       <c r="D210" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="E210" s="2" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="211" spans="1:6">
       <c r="A211" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B211">
+        <v>2</v>
+      </c>
+      <c r="C211" t="s">
         <v>1353</v>
       </c>
-      <c r="B211">
-        <v>2</v>
-      </c>
-      <c r="C211" t="s">
-        <v>1354</v>
-      </c>
       <c r="D211" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="E211" s="2" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="213" spans="1:6">
       <c r="A213" s="10" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="215" spans="1:6">
       <c r="A215" s="10" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="216" spans="1:6">
@@ -8374,19 +8563,19 @@
     </row>
     <row r="217" spans="1:6">
       <c r="A217" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B217">
         <v>2</v>
       </c>
       <c r="C217" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="D217" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="E217" s="2" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="F217" t="s">
         <v>829</v>
@@ -8394,19 +8583,19 @@
     </row>
     <row r="218" spans="1:6">
       <c r="A218" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B218">
         <v>2</v>
       </c>
       <c r="C218" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="D218" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="E218" s="2" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="F218" t="s">
         <v>829</v>
@@ -8414,12 +8603,12 @@
     </row>
     <row r="220" spans="1:6">
       <c r="A220" s="10" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="222" spans="1:6">
       <c r="A222" s="10" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="223" spans="1:6">
@@ -8438,19 +8627,19 @@
     </row>
     <row r="224" spans="1:6">
       <c r="A224" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B224">
+        <v>2</v>
+      </c>
+      <c r="C224" t="s">
         <v>1372</v>
       </c>
-      <c r="B224">
-        <v>2</v>
-      </c>
-      <c r="C224" t="s">
+      <c r="D224" t="s">
         <v>1373</v>
       </c>
-      <c r="D224" t="s">
-        <v>1374</v>
-      </c>
       <c r="E224" s="2" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="F224" t="s">
         <v>829</v>
@@ -8458,19 +8647,19 @@
     </row>
     <row r="225" spans="1:6">
       <c r="A225" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B225">
+        <v>2</v>
+      </c>
+      <c r="C225" t="s">
         <v>1375</v>
       </c>
-      <c r="B225">
-        <v>2</v>
-      </c>
-      <c r="C225" t="s">
-        <v>1376</v>
-      </c>
       <c r="D225" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E225" s="2" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="F225" t="s">
         <v>829</v>
@@ -8478,19 +8667,19 @@
     </row>
     <row r="226" spans="1:6">
       <c r="A226" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B226">
+        <v>2</v>
+      </c>
+      <c r="C226" t="s">
         <v>1377</v>
       </c>
-      <c r="B226">
-        <v>2</v>
-      </c>
-      <c r="C226" t="s">
-        <v>1378</v>
-      </c>
       <c r="D226" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E226" s="2" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="F226" t="s">
         <v>829</v>
@@ -8498,19 +8687,19 @@
     </row>
     <row r="227" spans="1:6">
       <c r="A227" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B227">
+        <v>2</v>
+      </c>
+      <c r="C227" t="s">
         <v>1379</v>
       </c>
-      <c r="B227">
-        <v>2</v>
-      </c>
-      <c r="C227" t="s">
-        <v>1380</v>
-      </c>
       <c r="D227" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E227" s="2" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="F227" t="s">
         <v>829</v>
@@ -8518,19 +8707,19 @@
     </row>
     <row r="228" spans="1:6">
       <c r="A228" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B228">
+        <v>2</v>
+      </c>
+      <c r="C228" t="s">
         <v>1381</v>
       </c>
-      <c r="B228">
-        <v>2</v>
-      </c>
-      <c r="C228" t="s">
-        <v>1382</v>
-      </c>
       <c r="D228" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E228" s="2" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="F228" t="s">
         <v>829</v>
@@ -8538,7 +8727,7 @@
     </row>
     <row r="230" spans="1:6">
       <c r="A230" s="10" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="231" spans="1:6">
@@ -8557,19 +8746,19 @@
     </row>
     <row r="232" spans="1:6">
       <c r="A232" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="B232">
         <v>2</v>
       </c>
       <c r="C232" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="D232" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E232" s="2" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="F232" t="s">
         <v>829</v>
@@ -8577,19 +8766,19 @@
     </row>
     <row r="233" spans="1:6">
       <c r="A233" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="B233">
         <v>2</v>
       </c>
       <c r="C233" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="D233" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E233" s="2" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="F233" t="s">
         <v>829</v>
@@ -8597,19 +8786,19 @@
     </row>
     <row r="234" spans="1:6">
       <c r="A234" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="B234">
         <v>2</v>
       </c>
       <c r="C234" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="D234" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E234" s="2" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="F234" t="s">
         <v>829</v>
@@ -8617,19 +8806,19 @@
     </row>
     <row r="235" spans="1:6">
       <c r="A235" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="B235">
         <v>2</v>
       </c>
       <c r="C235" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="D235" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E235" s="2" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="F235" t="s">
         <v>829</v>
@@ -8637,19 +8826,19 @@
     </row>
     <row r="236" spans="1:6">
       <c r="A236" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="B236">
         <v>2</v>
       </c>
       <c r="C236" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D236" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E236" s="2" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="F236" t="s">
         <v>829</v>
@@ -8657,21 +8846,21 @@
     </row>
     <row r="237" spans="1:6">
       <c r="A237" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B237">
+        <v>2</v>
+      </c>
+      <c r="C237" t="s">
         <v>1397</v>
       </c>
-      <c r="B237">
-        <v>2</v>
-      </c>
-      <c r="C237" t="s">
-        <v>1398</v>
-      </c>
       <c r="D237" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="239" spans="1:6">
       <c r="A239" s="10" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="240" spans="1:6">
@@ -8688,43 +8877,167 @@
         <v>3</v>
       </c>
     </row>
-    <row r="241" spans="1:5">
+    <row r="241" spans="1:6">
       <c r="A241" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B241">
+        <v>2</v>
+      </c>
+      <c r="C241" t="s">
         <v>1410</v>
       </c>
-      <c r="B241">
-        <v>2</v>
-      </c>
-      <c r="C241" t="s">
-        <v>1411</v>
-      </c>
       <c r="D241" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E241" s="2" t="s">
-        <v>1416</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6">
       <c r="A242" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B242">
+        <v>2</v>
+      </c>
+      <c r="C242" t="s">
         <v>1397</v>
       </c>
-      <c r="B242">
-        <v>2</v>
-      </c>
-      <c r="C242" t="s">
-        <v>1398</v>
-      </c>
       <c r="D242" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="E242" s="2" t="s">
-        <v>1415</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6">
       <c r="A244" s="10" t="s">
-        <v>1413</v>
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6">
+      <c r="A246" s="10" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6">
+      <c r="A247" t="s">
+        <v>0</v>
+      </c>
+      <c r="B247" t="s">
+        <v>1</v>
+      </c>
+      <c r="C247" t="s">
+        <v>2</v>
+      </c>
+      <c r="D247" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6">
+      <c r="A248" t="s">
+        <v>892</v>
+      </c>
+      <c r="B248">
+        <v>2</v>
+      </c>
+      <c r="C248" t="s">
+        <v>1453</v>
+      </c>
+      <c r="D248" t="s">
+        <v>1454</v>
+      </c>
+      <c r="E248" s="2" t="s">
+        <v>1468</v>
+      </c>
+      <c r="F248" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6">
+      <c r="A249" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B249">
+        <v>2</v>
+      </c>
+      <c r="C249" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D249" t="s">
+        <v>1457</v>
+      </c>
+      <c r="E249" s="2" t="s">
+        <v>1469</v>
+      </c>
+      <c r="F249" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6">
+      <c r="A250" t="s">
+        <v>1458</v>
+      </c>
+      <c r="B250">
+        <v>2</v>
+      </c>
+      <c r="C250" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D250" t="s">
+        <v>1460</v>
+      </c>
+      <c r="E250" s="2" t="s">
+        <v>1477</v>
+      </c>
+      <c r="F250" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6">
+      <c r="A251" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B251">
+        <v>2</v>
+      </c>
+      <c r="C251" t="s">
+        <v>1462</v>
+      </c>
+      <c r="D251" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E251" s="2" t="s">
+        <v>1467</v>
+      </c>
+      <c r="F251" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6">
+      <c r="A252" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B252">
+        <v>2</v>
+      </c>
+      <c r="C252" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D252" t="s">
+        <v>1466</v>
+      </c>
+      <c r="E252" s="2" t="s">
+        <v>1470</v>
+      </c>
+      <c r="F252" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6">
+      <c r="A254" s="10" t="s">
+        <v>1480</v>
       </c>
     </row>
   </sheetData>
@@ -8735,10 +9048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H120"/>
+  <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8748,6 +9061,7 @@
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="21.1640625" customWidth="1"/>
     <col min="6" max="6" width="30.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="40.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -9840,12 +10154,12 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:7">
       <c r="A81" s="10" t="s">
         <v>1204</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:7">
       <c r="A83" s="10" t="s">
         <v>1212</v>
       </c>
@@ -9853,7 +10167,7 @@
       <c r="E83" s="2"/>
       <c r="F83"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
         <v>4</v>
       </c>
@@ -9867,138 +10181,121 @@
         <v>7</v>
       </c>
       <c r="E84" t="s">
-        <v>1213</v>
-      </c>
-      <c r="F84" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="85" spans="1:8">
+      <c r="F84"/>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B85">
         <v>2</v>
       </c>
       <c r="C85" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="D85" t="s">
         <v>9</v>
       </c>
-      <c r="E85">
-        <v>3</v>
-      </c>
-      <c r="F85" t="s">
-        <v>1226</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
+      <c r="E85" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B86">
         <v>2</v>
       </c>
       <c r="C86" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="D86" t="s">
         <v>9</v>
       </c>
-      <c r="E86">
-        <v>3</v>
-      </c>
-      <c r="F86" t="s">
-        <v>1223</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
+      <c r="E86" t="s">
+        <v>1222</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B87">
         <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="D87" t="s">
         <v>9</v>
       </c>
-      <c r="E87">
-        <v>6</v>
-      </c>
-      <c r="F87" t="s">
-        <v>1220</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
+      <c r="E87" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B88">
         <v>2</v>
       </c>
       <c r="C88" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="D88" t="s">
         <v>9</v>
       </c>
-      <c r="E88">
-        <v>3</v>
-      </c>
-      <c r="F88" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
+      <c r="E88" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B89">
         <v>7</v>
       </c>
       <c r="C89" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="D89" t="s">
         <v>9</v>
       </c>
-      <c r="E89">
-        <v>8</v>
-      </c>
-      <c r="F89" t="s">
-        <v>1214</v>
-      </c>
-      <c r="G89" s="2" t="s">
+      <c r="E89" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="1" t="s">
         <v>1230</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
-      <c r="A91" s="1" t="s">
-        <v>1231</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:7">
       <c r="A93" s="10" t="s">
-        <v>1241</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
         <v>4</v>
       </c>
@@ -10012,159 +10309,139 @@
         <v>7</v>
       </c>
       <c r="E94" t="s">
-        <v>1213</v>
-      </c>
-      <c r="F94" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="95" spans="1:8">
+      <c r="F94"/>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B95">
+        <v>2</v>
+      </c>
+      <c r="C95" t="s">
         <v>1262</v>
-      </c>
-      <c r="B95">
-        <v>2</v>
-      </c>
-      <c r="C95" t="s">
-        <v>1263</v>
       </c>
       <c r="D95" t="s">
         <v>9</v>
       </c>
-      <c r="E95">
-        <v>1</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="E95" t="s">
         <v>755</v>
       </c>
-      <c r="G95" s="2" t="s">
-        <v>1310</v>
-      </c>
-      <c r="H95" t="s">
+      <c r="F95" s="2" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G95" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B96">
+        <v>2</v>
+      </c>
+      <c r="C96" t="s">
         <v>1264</v>
-      </c>
-      <c r="B96">
-        <v>2</v>
-      </c>
-      <c r="C96" t="s">
-        <v>1265</v>
       </c>
       <c r="D96" t="s">
         <v>9</v>
       </c>
-      <c r="E96">
-        <v>1</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="E96" t="s">
         <v>251</v>
       </c>
-      <c r="G96" s="2" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7">
+      <c r="F96" s="2" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B97">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
         <v>1266</v>
-      </c>
-      <c r="B97">
-        <v>2</v>
-      </c>
-      <c r="C97" t="s">
-        <v>1267</v>
       </c>
       <c r="D97" t="s">
         <v>9</v>
       </c>
-      <c r="E97">
-        <v>1</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="E97" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" t="s">
         <v>1268</v>
       </c>
-      <c r="G97" s="2" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7">
-      <c r="A98" t="s">
+      <c r="B98">
+        <v>2</v>
+      </c>
+      <c r="C98" t="s">
         <v>1269</v>
-      </c>
-      <c r="B98">
-        <v>2</v>
-      </c>
-      <c r="C98" t="s">
-        <v>1270</v>
       </c>
       <c r="D98" t="s">
         <v>9</v>
       </c>
-      <c r="E98">
-        <v>3</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="E98" t="s">
+        <v>1270</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" t="s">
         <v>1271</v>
       </c>
-      <c r="G98" s="2" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7">
-      <c r="A99" t="s">
+      <c r="B99">
+        <v>2</v>
+      </c>
+      <c r="C99" t="s">
         <v>1272</v>
-      </c>
-      <c r="B99">
-        <v>2</v>
-      </c>
-      <c r="C99" t="s">
-        <v>1273</v>
       </c>
       <c r="D99" t="s">
         <v>9</v>
       </c>
-      <c r="E99">
-        <v>1</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="E99" t="s">
         <v>505</v>
       </c>
-      <c r="G99" s="2" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7">
+      <c r="F99" s="2" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B100">
+        <v>2</v>
+      </c>
+      <c r="C100" t="s">
         <v>1274</v>
-      </c>
-      <c r="B100">
-        <v>2</v>
-      </c>
-      <c r="C100" t="s">
-        <v>1275</v>
       </c>
       <c r="D100" t="s">
         <v>9</v>
       </c>
-      <c r="E100">
-        <v>1</v>
-      </c>
-      <c r="F100" t="s">
-        <v>1268</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7">
+      <c r="E100" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
       <c r="A103" s="10" t="s">
-        <v>1337</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
         <v>4</v>
       </c>
@@ -10178,166 +10455,145 @@
         <v>7</v>
       </c>
       <c r="E104" t="s">
-        <v>1213</v>
-      </c>
-      <c r="F104" t="s">
         <v>8</v>
       </c>
-      <c r="G104" s="2" t="s">
+      <c r="F104" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B105">
         <v>2</v>
       </c>
       <c r="C105" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="D105" t="s">
         <v>9</v>
       </c>
-      <c r="E105">
-        <v>1</v>
-      </c>
-      <c r="F105" t="s">
+      <c r="E105" t="s">
         <v>276</v>
       </c>
-      <c r="G105" s="2" t="s">
-        <v>1347</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7">
+      <c r="F105" s="2" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B106">
+        <v>2</v>
+      </c>
+      <c r="C106" t="s">
         <v>1264</v>
-      </c>
-      <c r="B106">
-        <v>2</v>
-      </c>
-      <c r="C106" t="s">
-        <v>1265</v>
       </c>
       <c r="D106" t="s">
         <v>9</v>
       </c>
-      <c r="E106">
-        <v>1</v>
-      </c>
-      <c r="F106" t="s">
+      <c r="E106" t="s">
         <v>251</v>
       </c>
-      <c r="G106" s="2" t="s">
-        <v>1346</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7">
+      <c r="F106" s="2" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B107">
+        <v>2</v>
+      </c>
+      <c r="C107" t="s">
         <v>1266</v>
-      </c>
-      <c r="B107">
-        <v>2</v>
-      </c>
-      <c r="C107" t="s">
-        <v>1267</v>
       </c>
       <c r="D107" t="s">
         <v>9</v>
       </c>
-      <c r="E107">
-        <v>1</v>
-      </c>
-      <c r="F107" t="s">
+      <c r="E107" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" t="s">
         <v>1268</v>
       </c>
-      <c r="G107" s="2" t="s">
-        <v>1345</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7">
-      <c r="A108" t="s">
+      <c r="B108">
+        <v>2</v>
+      </c>
+      <c r="C108" t="s">
         <v>1269</v>
-      </c>
-      <c r="B108">
-        <v>2</v>
-      </c>
-      <c r="C108" t="s">
-        <v>1270</v>
       </c>
       <c r="D108" t="s">
         <v>9</v>
       </c>
-      <c r="E108">
-        <v>3</v>
-      </c>
-      <c r="F108" t="s">
+      <c r="E108" t="s">
+        <v>1270</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" t="s">
         <v>1271</v>
       </c>
-      <c r="G108" s="2" t="s">
-        <v>1344</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7">
-      <c r="A109" t="s">
+      <c r="B109">
+        <v>2</v>
+      </c>
+      <c r="C109" t="s">
         <v>1272</v>
-      </c>
-      <c r="B109">
-        <v>2</v>
-      </c>
-      <c r="C109" t="s">
-        <v>1273</v>
       </c>
       <c r="D109" t="s">
         <v>9</v>
       </c>
-      <c r="E109">
-        <v>1</v>
-      </c>
-      <c r="F109" t="s">
+      <c r="E109" t="s">
         <v>505</v>
       </c>
-      <c r="G109" s="2" t="s">
-        <v>1343</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7">
+      <c r="F109" s="2" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
       <c r="A110" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B110">
+        <v>2</v>
+      </c>
+      <c r="C110" t="s">
         <v>1274</v>
-      </c>
-      <c r="B110">
-        <v>2</v>
-      </c>
-      <c r="C110" t="s">
-        <v>1275</v>
       </c>
       <c r="D110" t="s">
         <v>9</v>
       </c>
-      <c r="E110">
-        <v>1</v>
-      </c>
-      <c r="F110" t="s">
-        <v>1268</v>
-      </c>
-      <c r="G110" s="2" t="s">
-        <v>1342</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7">
+      <c r="E110" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="A112" s="10" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="10" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="116" spans="1:7">
       <c r="A116" s="10" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -10345,7 +10601,7 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="10" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -10353,7 +10609,169 @@
       <c r="G119" s="2"/>
     </row>
     <row r="120" spans="1:7">
+      <c r="A120" s="10" t="s">
+        <v>1429</v>
+      </c>
       <c r="F120"/>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F121"/>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="B122" s="3">
+        <v>2</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>1471</v>
+      </c>
+      <c r="G122" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" s="3" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B123" s="3">
+        <v>2</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>1421</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>1472</v>
+      </c>
+      <c r="G123" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" s="3" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B124" s="3">
+        <v>2</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" s="3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B125" s="3">
+        <v>2</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>1473</v>
+      </c>
+      <c r="G125" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" s="3" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B126" s="3">
+        <v>2</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>1427</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>1428</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>1474</v>
+      </c>
+      <c r="G126" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
+      <c r="F127"/>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" s="10" t="s">
+        <v>1481</v>
+      </c>
+      <c r="F128"/>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="3" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B129" s="3">
+        <v>2</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>1478</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10363,10 +10781,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H264"/>
+  <dimension ref="A1:H278"/>
   <sheetViews>
-    <sheetView topLeftCell="A252" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A266" sqref="A266"/>
+    <sheetView topLeftCell="A264" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A278" sqref="A278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10374,7 +10792,7 @@
     <col min="1" max="1" width="20.1640625" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="47.5" customWidth="1"/>
-    <col min="4" max="4" width="47" customWidth="1"/>
+    <col min="4" max="4" width="63.33203125" customWidth="1"/>
     <col min="5" max="5" width="56" customWidth="1"/>
     <col min="6" max="6" width="40.33203125" style="2" customWidth="1"/>
   </cols>
@@ -13828,17 +14246,17 @@
         <v>386</v>
       </c>
       <c r="F215" s="2" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="217" spans="1:7">
       <c r="A217" s="1" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="219" spans="1:7">
       <c r="A219" s="10" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="220" spans="1:7">
@@ -13872,40 +14290,40 @@
         <v>1053</v>
       </c>
       <c r="E221" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="F221" s="2" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="222" spans="1:7">
       <c r="A222" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B222">
+        <v>2</v>
+      </c>
+      <c r="C222" t="s">
         <v>1233</v>
       </c>
-      <c r="B222">
-        <v>2</v>
-      </c>
-      <c r="C222" t="s">
+      <c r="D222" t="s">
         <v>1234</v>
       </c>
-      <c r="D222" t="s">
+      <c r="E222" t="s">
         <v>1235</v>
       </c>
-      <c r="E222" t="s">
-        <v>1236</v>
-      </c>
       <c r="F222" s="2" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="224" spans="1:7">
       <c r="A224" s="1" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="226" spans="1:7">
       <c r="A226" s="10" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="227" spans="1:7">
@@ -13928,131 +14346,131 @@
     </row>
     <row r="228" spans="1:7">
       <c r="A228" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B228">
+        <v>2</v>
+      </c>
+      <c r="C228" t="s">
         <v>1242</v>
       </c>
-      <c r="B228">
-        <v>2</v>
-      </c>
-      <c r="C228" t="s">
+      <c r="D228" t="s">
+        <v>1313</v>
+      </c>
+      <c r="E228" t="s">
         <v>1243</v>
       </c>
-      <c r="D228" t="s">
-        <v>1314</v>
-      </c>
-      <c r="E228" t="s">
-        <v>1244</v>
-      </c>
       <c r="F228" s="2" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G228" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="229" spans="1:7">
       <c r="A229" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B229">
+        <v>2</v>
+      </c>
+      <c r="C229" t="s">
         <v>1245</v>
       </c>
-      <c r="B229">
-        <v>2</v>
-      </c>
-      <c r="C229" t="s">
+      <c r="D229" t="s">
+        <v>1314</v>
+      </c>
+      <c r="E229" t="s">
         <v>1246</v>
       </c>
-      <c r="D229" t="s">
-        <v>1315</v>
-      </c>
-      <c r="E229" t="s">
-        <v>1247</v>
-      </c>
       <c r="F229" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G229" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="230" spans="1:7">
       <c r="A230" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B230">
+        <v>2</v>
+      </c>
+      <c r="C230" t="s">
         <v>1248</v>
       </c>
-      <c r="B230">
-        <v>2</v>
-      </c>
-      <c r="C230" t="s">
+      <c r="D230" t="s">
+        <v>1315</v>
+      </c>
+      <c r="E230" t="s">
         <v>1249</v>
       </c>
-      <c r="D230" t="s">
-        <v>1316</v>
-      </c>
-      <c r="E230" t="s">
-        <v>1250</v>
-      </c>
       <c r="F230" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G230" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="231" spans="1:7">
       <c r="A231" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B231">
+        <v>2</v>
+      </c>
+      <c r="C231" t="s">
         <v>1251</v>
       </c>
-      <c r="B231">
-        <v>2</v>
-      </c>
-      <c r="C231" t="s">
+      <c r="D231" t="s">
         <v>1252</v>
       </c>
-      <c r="D231" t="s">
+      <c r="E231" t="s">
         <v>1253</v>
       </c>
-      <c r="E231" t="s">
-        <v>1254</v>
-      </c>
       <c r="F231" s="2" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="232" spans="1:7">
       <c r="A232" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B232">
+        <v>2</v>
+      </c>
+      <c r="C232" t="s">
         <v>1255</v>
       </c>
-      <c r="B232">
-        <v>2</v>
-      </c>
-      <c r="C232" t="s">
+      <c r="D232" t="s">
+        <v>1252</v>
+      </c>
+      <c r="E232" t="s">
         <v>1256</v>
       </c>
-      <c r="D232" t="s">
-        <v>1253</v>
-      </c>
-      <c r="E232" t="s">
-        <v>1257</v>
-      </c>
       <c r="F232" s="2" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="233" spans="1:7">
       <c r="A233" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B233">
+        <v>2</v>
+      </c>
+      <c r="C233" t="s">
         <v>1258</v>
       </c>
-      <c r="B233">
-        <v>2</v>
-      </c>
-      <c r="C233" t="s">
+      <c r="D233" t="s">
         <v>1259</v>
       </c>
-      <c r="D233" t="s">
+      <c r="E233" t="s">
         <v>1260</v>
       </c>
-      <c r="E233" t="s">
-        <v>1261</v>
-      </c>
       <c r="F233" s="2" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="234" spans="1:7">
@@ -14060,7 +14478,7 @@
     </row>
     <row r="235" spans="1:7">
       <c r="A235" s="10" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="236" spans="1:7">
@@ -14083,43 +14501,43 @@
     </row>
     <row r="237" spans="1:7">
       <c r="A237" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B237">
+        <v>2</v>
+      </c>
+      <c r="C237" t="s">
         <v>1321</v>
       </c>
-      <c r="B237">
-        <v>2</v>
-      </c>
-      <c r="C237" t="s">
+      <c r="D237" t="s">
         <v>1322</v>
       </c>
-      <c r="D237" t="s">
+      <c r="E237" t="s">
         <v>1323</v>
-      </c>
-      <c r="E237" t="s">
-        <v>1324</v>
       </c>
       <c r="F237"/>
     </row>
     <row r="238" spans="1:7">
       <c r="A238" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B238">
+        <v>2</v>
+      </c>
+      <c r="C238" t="s">
         <v>1258</v>
       </c>
-      <c r="B238">
-        <v>2</v>
-      </c>
-      <c r="C238" t="s">
+      <c r="D238" t="s">
         <v>1259</v>
       </c>
-      <c r="D238" t="s">
+      <c r="E238" t="s">
         <v>1260</v>
-      </c>
-      <c r="E238" t="s">
-        <v>1261</v>
       </c>
       <c r="F238"/>
     </row>
     <row r="241" spans="1:7">
       <c r="A241" s="10" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="242" spans="1:7">
@@ -14139,57 +14557,57 @@
         <v>3</v>
       </c>
       <c r="F242" s="2" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="243" spans="1:7">
       <c r="A243" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B243">
         <v>2</v>
       </c>
       <c r="C243" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="D243" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E243" t="s">
         <v>1260</v>
       </c>
-      <c r="E243" t="s">
-        <v>1261</v>
-      </c>
       <c r="F243" s="2" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="244" spans="1:7">
       <c r="A244" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B244">
+        <v>2</v>
+      </c>
+      <c r="C244" t="s">
         <v>1321</v>
       </c>
-      <c r="B244">
-        <v>2</v>
-      </c>
-      <c r="C244" t="s">
+      <c r="D244" t="s">
         <v>1322</v>
       </c>
-      <c r="D244" t="s">
+      <c r="E244" t="s">
         <v>1323</v>
       </c>
-      <c r="E244" t="s">
-        <v>1324</v>
-      </c>
       <c r="F244" s="2" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="246" spans="1:7">
       <c r="A246" s="10" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="248" spans="1:7">
       <c r="A248" s="10" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -14209,27 +14627,27 @@
         <v>3</v>
       </c>
       <c r="F249" s="2" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="250" spans="1:7">
       <c r="A250" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B250">
+        <v>2</v>
+      </c>
+      <c r="C250" t="s">
         <v>1368</v>
       </c>
-      <c r="B250">
-        <v>2</v>
-      </c>
-      <c r="C250" t="s">
+      <c r="D250" t="s">
         <v>1369</v>
       </c>
-      <c r="D250" t="s">
+      <c r="E250" t="s">
         <v>1370</v>
       </c>
-      <c r="E250" t="s">
-        <v>1371</v>
-      </c>
       <c r="F250" s="2" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="G250" t="s">
         <v>829</v>
@@ -14237,12 +14655,12 @@
     </row>
     <row r="252" spans="1:7">
       <c r="A252" s="10" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="254" spans="1:7">
       <c r="A254" s="10" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="255" spans="1:7">
@@ -14264,44 +14682,44 @@
     </row>
     <row r="256" spans="1:7">
       <c r="A256" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B256">
+        <v>2</v>
+      </c>
+      <c r="C256" t="s">
         <v>1401</v>
       </c>
-      <c r="B256">
-        <v>2</v>
-      </c>
-      <c r="C256" t="s">
+      <c r="D256" t="s">
         <v>1402</v>
       </c>
-      <c r="D256" t="s">
+      <c r="E256" t="s">
         <v>1403</v>
       </c>
-      <c r="E256" t="s">
+    </row>
+    <row r="257" spans="1:7">
+      <c r="A257" t="s">
         <v>1404</v>
       </c>
-    </row>
-    <row r="257" spans="1:6">
-      <c r="A257" t="s">
+      <c r="B257">
+        <v>2</v>
+      </c>
+      <c r="C257" t="s">
         <v>1405</v>
       </c>
-      <c r="B257">
-        <v>2</v>
-      </c>
-      <c r="C257" t="s">
+      <c r="D257" t="s">
         <v>1406</v>
       </c>
-      <c r="D257" t="s">
+      <c r="E257" t="s">
         <v>1407</v>
       </c>
-      <c r="E257" t="s">
-        <v>1408</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6">
+    </row>
+    <row r="259" spans="1:7">
       <c r="A259" s="10" t="s">
-        <v>1414</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7">
       <c r="A260" t="s">
         <v>0</v>
       </c>
@@ -14318,49 +14736,283 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="1:6">
+    <row r="261" spans="1:7">
       <c r="A261" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B261">
+        <v>2</v>
+      </c>
+      <c r="C261" t="s">
         <v>1401</v>
       </c>
-      <c r="B261">
-        <v>2</v>
-      </c>
-      <c r="C261" t="s">
+      <c r="D261" t="s">
         <v>1402</v>
       </c>
-      <c r="D261" t="s">
+      <c r="E261" t="s">
         <v>1403</v>
       </c>
-      <c r="E261" t="s">
+      <c r="F261" s="2" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7">
+      <c r="A262" t="s">
         <v>1404</v>
       </c>
-      <c r="F261" s="2" t="s">
+      <c r="B262">
+        <v>2</v>
+      </c>
+      <c r="C262" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D262" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E262" t="s">
+        <v>1407</v>
+      </c>
+      <c r="F262" s="2" t="s">
         <v>1417</v>
       </c>
     </row>
-    <row r="262" spans="1:6">
-      <c r="A262" t="s">
-        <v>1405</v>
-      </c>
-      <c r="B262">
-        <v>2</v>
-      </c>
-      <c r="C262" t="s">
-        <v>1406</v>
-      </c>
-      <c r="D262" t="s">
-        <v>1407</v>
-      </c>
-      <c r="E262" t="s">
-        <v>1408</v>
-      </c>
-      <c r="F262" s="2" t="s">
-        <v>1418</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6">
+    <row r="264" spans="1:7">
       <c r="A264" s="10" t="s">
-        <v>1413</v>
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7">
+      <c r="A266" s="10" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7">
+      <c r="A267" t="s">
+        <v>0</v>
+      </c>
+      <c r="B267" t="s">
+        <v>10</v>
+      </c>
+      <c r="C267" t="s">
+        <v>2</v>
+      </c>
+      <c r="D267" t="s">
+        <v>11</v>
+      </c>
+      <c r="E267" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7">
+      <c r="A268" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B268">
+        <v>2</v>
+      </c>
+      <c r="C268" t="s">
+        <v>1431</v>
+      </c>
+      <c r="D268" t="s">
+        <v>1432</v>
+      </c>
+      <c r="E268" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F268" s="2" t="s">
+        <v>1475</v>
+      </c>
+      <c r="G268" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7">
+      <c r="A269" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B269">
+        <v>2</v>
+      </c>
+      <c r="C269" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D269" t="s">
+        <v>1432</v>
+      </c>
+      <c r="E269" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F269" s="2" t="s">
+        <v>1475</v>
+      </c>
+      <c r="G269" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7">
+      <c r="A270" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B270">
+        <v>2</v>
+      </c>
+      <c r="C270" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D270" t="s">
+        <v>1432</v>
+      </c>
+      <c r="E270" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F270" s="2" t="s">
+        <v>1475</v>
+      </c>
+      <c r="G270" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7">
+      <c r="A271" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B271">
+        <v>2</v>
+      </c>
+      <c r="C271" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D271" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E271" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F271" s="2" t="s">
+        <v>1475</v>
+      </c>
+      <c r="G271" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7">
+      <c r="A272" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B272">
+        <v>2</v>
+      </c>
+      <c r="C272" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D272" t="s">
+        <v>1432</v>
+      </c>
+      <c r="E272" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F272" s="2" t="s">
+        <v>1475</v>
+      </c>
+      <c r="G272" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7">
+      <c r="A273" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B273">
+        <v>2</v>
+      </c>
+      <c r="C273" t="s">
+        <v>1443</v>
+      </c>
+      <c r="D273" t="s">
+        <v>1444</v>
+      </c>
+      <c r="E273" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F273" s="2" t="s">
+        <v>1479</v>
+      </c>
+      <c r="G273" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7">
+      <c r="A274" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B274">
+        <v>2</v>
+      </c>
+      <c r="C274" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D274" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E274" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F274" s="2" t="s">
+        <v>1475</v>
+      </c>
+      <c r="G274" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7">
+      <c r="A275" t="s">
+        <v>1448</v>
+      </c>
+      <c r="B275">
+        <v>2</v>
+      </c>
+      <c r="C275" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D275" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E275" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F275" s="2" t="s">
+        <v>1475</v>
+      </c>
+      <c r="G275" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7">
+      <c r="A276" t="s">
+        <v>1450</v>
+      </c>
+      <c r="B276">
+        <v>2</v>
+      </c>
+      <c r="C276" t="s">
+        <v>620</v>
+      </c>
+      <c r="D276" t="s">
+        <v>1451</v>
+      </c>
+      <c r="E276" t="s">
+        <v>1452</v>
+      </c>
+      <c r="F276" s="2" t="s">
+        <v>1476</v>
+      </c>
+      <c r="G276" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7">
+      <c r="A278" s="10" t="s">
+        <v>1480</v>
       </c>
     </row>
   </sheetData>
@@ -15100,7 +15752,7 @@
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="10" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
   </sheetData>
@@ -16179,7 +16831,7 @@
         <v>727</v>
       </c>
       <c r="B13" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -16483,7 +17135,7 @@
         <v>730</v>
       </c>
       <c r="B51" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -16491,15 +17143,15 @@
         <v>1009</v>
       </c>
       <c r="B52" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B53" t="s">
         <v>1302</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1303</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -16536,10 +17188,10 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B58" t="s">
         <v>1304</v>
-      </c>
-      <c r="B58" t="s">
-        <v>1305</v>
       </c>
     </row>
     <row r="59" spans="1:2">

</xml_diff>

<commit_message>
updated the file to commit 7baf853603e0338a4fc01a572c4813d1070f5e63
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0966BDC2-0A2F-5741-AFD8-F2FEE264AD48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F9943B-4DD9-0D46-A9F9-EFF3FCA51112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="500" windowWidth="26600" windowHeight="14500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="500" windowWidth="26600" windowHeight="14500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2852" uniqueCount="1482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2855" uniqueCount="1482">
   <si>
     <t>sid</t>
   </si>
@@ -3667,9 +3667,6 @@
   </si>
   <si>
     <t>Checked on Feb 23th, 2022, identified following issue:</t>
-  </si>
-  <si>
-    <t>parent_count</t>
   </si>
   <si>
     <t>Cerebrospinal fluid microbiology test|Blood microbiology test|Other sample microbiology test|Induced sputum microbiology test|Endotracheal tube aspirate test|Endotracheal tube aspirate microbiology test|Lung aspirate microbiology test|Pleural fluid microbiology test</t>
@@ -4347,9 +4344,6 @@
     <t>Change SHINE to be under "Clinical history"</t>
   </si>
   <si>
-    <t>same</t>
-  </si>
-  <si>
     <t>EUPATH_0000151|EUPATH_0054076</t>
   </si>
   <si>
@@ -4534,6 +4528,12 @@
   </si>
   <si>
     <t>Change sw pacific to use 'Other medicine taken'  EUPATH_0053127</t>
+  </si>
+  <si>
+    <t>Checked on Aug 4th, 2022, no issue was found</t>
+  </si>
+  <si>
+    <t>Checked on Aug 4th, 2022, only one issue is found.</t>
   </si>
 </sst>
 </file>
@@ -5433,10 +5433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G252"/>
+  <dimension ref="A1:G254"/>
   <sheetViews>
-    <sheetView topLeftCell="A231" workbookViewId="0">
-      <selection activeCell="A248" sqref="A248:XFD251"/>
+    <sheetView topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="C239" sqref="C239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8016,7 +8016,7 @@
     </row>
     <row r="177" spans="1:7">
       <c r="A177" s="10" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="178" spans="1:7">
@@ -8035,19 +8035,19 @@
     </row>
     <row r="179" spans="1:7">
       <c r="A179" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B179">
         <v>2</v>
       </c>
       <c r="C179" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="D179" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="F179" t="s">
         <v>829</v>
@@ -8055,19 +8055,19 @@
     </row>
     <row r="180" spans="1:7">
       <c r="A180" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B180">
         <v>2</v>
       </c>
       <c r="C180" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="D180" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="F180" t="s">
         <v>829</v>
@@ -8075,76 +8075,76 @@
     </row>
     <row r="181" spans="1:7">
       <c r="A181" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B181">
         <v>2</v>
       </c>
       <c r="C181" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="D181" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="182" spans="1:7">
       <c r="A182" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B182">
+        <v>2</v>
+      </c>
+      <c r="C182" t="s">
         <v>1279</v>
       </c>
-      <c r="B182">
-        <v>2</v>
-      </c>
-      <c r="C182" t="s">
+      <c r="D182" t="s">
         <v>1280</v>
       </c>
-      <c r="D182" t="s">
-        <v>1281</v>
-      </c>
       <c r="E182" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F182" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="183" spans="1:7">
       <c r="A183" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B183">
+        <v>2</v>
+      </c>
+      <c r="C183" t="s">
         <v>1282</v>
       </c>
-      <c r="B183">
-        <v>2</v>
-      </c>
-      <c r="C183" t="s">
-        <v>1283</v>
-      </c>
       <c r="D183" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F183" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="184" spans="1:7">
       <c r="A184" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B184">
         <v>3</v>
       </c>
       <c r="C184" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D184" t="s">
         <v>1285</v>
       </c>
-      <c r="D184" t="s">
-        <v>1286</v>
-      </c>
       <c r="E184" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F184" t="s">
         <v>829</v>
@@ -8152,19 +8152,19 @@
     </row>
     <row r="185" spans="1:7">
       <c r="A185" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B185">
         <v>3</v>
       </c>
       <c r="C185" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="D185" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F185" t="s">
         <v>829</v>
@@ -8172,39 +8172,39 @@
     </row>
     <row r="186" spans="1:7">
       <c r="A186" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B186">
+        <v>2</v>
+      </c>
+      <c r="C186" t="s">
         <v>1289</v>
       </c>
-      <c r="B186">
-        <v>2</v>
-      </c>
-      <c r="C186" t="s">
-        <v>1290</v>
-      </c>
       <c r="D186" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="E186" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F186" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="187" spans="1:7">
       <c r="A187" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B187">
+        <v>2</v>
+      </c>
+      <c r="C187" t="s">
         <v>1291</v>
       </c>
-      <c r="B187">
-        <v>2</v>
-      </c>
-      <c r="C187" t="s">
+      <c r="D187" t="s">
         <v>1292</v>
       </c>
-      <c r="D187" t="s">
-        <v>1293</v>
-      </c>
       <c r="E187" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F187" t="s">
         <v>829</v>
@@ -8212,53 +8212,53 @@
     </row>
     <row r="188" spans="1:7">
       <c r="A188" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B188">
+        <v>2</v>
+      </c>
+      <c r="C188" t="s">
         <v>1294</v>
       </c>
-      <c r="B188">
-        <v>2</v>
-      </c>
-      <c r="C188" t="s">
+      <c r="D188" t="s">
         <v>1295</v>
       </c>
-      <c r="D188" t="s">
-        <v>1296</v>
-      </c>
       <c r="E188" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F188" t="s">
         <v>829</v>
       </c>
       <c r="G188" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="189" spans="1:7">
       <c r="A189" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B189">
+        <v>2</v>
+      </c>
+      <c r="C189" t="s">
         <v>1297</v>
       </c>
-      <c r="B189">
-        <v>2</v>
-      </c>
-      <c r="C189" t="s">
-        <v>1298</v>
-      </c>
       <c r="D189" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="E189" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F189" t="s">
         <v>829</v>
       </c>
       <c r="G189" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="191" spans="1:7">
       <c r="A191" s="10" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="192" spans="1:7">
@@ -8277,178 +8277,178 @@
     </row>
     <row r="193" spans="1:5">
       <c r="A193" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B193">
         <v>2</v>
       </c>
       <c r="C193" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="D193" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="E193" s="2" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="194" spans="1:5">
       <c r="A194" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="B194">
         <v>2</v>
       </c>
       <c r="C194" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="D194" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="195" spans="1:5">
       <c r="A195" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B195">
         <v>3</v>
       </c>
       <c r="C195" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D195" t="s">
         <v>1285</v>
-      </c>
-      <c r="D195" t="s">
-        <v>1286</v>
       </c>
     </row>
     <row r="196" spans="1:5">
       <c r="A196" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B196">
         <v>3</v>
       </c>
       <c r="C196" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="D196" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="197" spans="1:5">
       <c r="A197" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B197">
+        <v>2</v>
+      </c>
+      <c r="C197" t="s">
         <v>1326</v>
       </c>
-      <c r="B197">
-        <v>2</v>
-      </c>
-      <c r="C197" t="s">
-        <v>1327</v>
-      </c>
       <c r="D197" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="198" spans="1:5">
       <c r="A198" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B198">
+        <v>2</v>
+      </c>
+      <c r="C198" t="s">
         <v>1328</v>
       </c>
-      <c r="B198">
-        <v>2</v>
-      </c>
-      <c r="C198" t="s">
-        <v>1329</v>
-      </c>
       <c r="D198" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="199" spans="1:5">
       <c r="A199" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B199">
+        <v>2</v>
+      </c>
+      <c r="C199" t="s">
         <v>1330</v>
       </c>
-      <c r="B199">
-        <v>2</v>
-      </c>
-      <c r="C199" t="s">
-        <v>1331</v>
-      </c>
       <c r="D199" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="200" spans="1:5">
       <c r="A200" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B200">
+        <v>2</v>
+      </c>
+      <c r="C200" t="s">
         <v>1332</v>
       </c>
-      <c r="B200">
-        <v>2</v>
-      </c>
-      <c r="C200" t="s">
-        <v>1333</v>
-      </c>
       <c r="D200" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="201" spans="1:5">
       <c r="A201" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B201">
+        <v>2</v>
+      </c>
+      <c r="C201" t="s">
         <v>1291</v>
       </c>
-      <c r="B201">
-        <v>2</v>
-      </c>
-      <c r="C201" t="s">
+      <c r="D201" t="s">
         <v>1292</v>
-      </c>
-      <c r="D201" t="s">
-        <v>1293</v>
       </c>
     </row>
     <row r="202" spans="1:5">
       <c r="A202" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B202">
+        <v>2</v>
+      </c>
+      <c r="C202" t="s">
         <v>1294</v>
       </c>
-      <c r="B202">
-        <v>2</v>
-      </c>
-      <c r="C202" t="s">
+      <c r="D202" t="s">
         <v>1295</v>
-      </c>
-      <c r="D202" t="s">
-        <v>1296</v>
       </c>
     </row>
     <row r="203" spans="1:5">
       <c r="A203" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B203">
+        <v>2</v>
+      </c>
+      <c r="C203" t="s">
         <v>1297</v>
       </c>
-      <c r="B203">
-        <v>2</v>
-      </c>
-      <c r="C203" t="s">
-        <v>1298</v>
-      </c>
       <c r="D203" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="204" spans="1:5">
       <c r="A204" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B204">
+        <v>2</v>
+      </c>
+      <c r="C204" t="s">
         <v>1334</v>
       </c>
-      <c r="B204">
-        <v>2</v>
-      </c>
-      <c r="C204" t="s">
+      <c r="D204" t="s">
         <v>1335</v>
-      </c>
-      <c r="D204" t="s">
-        <v>1336</v>
       </c>
     </row>
     <row r="206" spans="1:5">
       <c r="A206" s="10" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -8470,80 +8470,80 @@
     </row>
     <row r="208" spans="1:5">
       <c r="A208" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B208">
         <v>2</v>
       </c>
       <c r="C208" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="D208" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="E208" s="2" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="209" spans="1:6">
       <c r="A209" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B209">
+        <v>2</v>
+      </c>
+      <c r="C209" t="s">
         <v>1349</v>
       </c>
-      <c r="B209">
-        <v>2</v>
-      </c>
-      <c r="C209" t="s">
-        <v>1350</v>
-      </c>
       <c r="D209" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="E209" s="2" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="210" spans="1:6">
       <c r="A210" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B210">
+        <v>2</v>
+      </c>
+      <c r="C210" t="s">
         <v>1351</v>
       </c>
-      <c r="B210">
-        <v>2</v>
-      </c>
-      <c r="C210" t="s">
-        <v>1352</v>
-      </c>
       <c r="D210" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="E210" s="2" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="211" spans="1:6">
       <c r="A211" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B211">
+        <v>2</v>
+      </c>
+      <c r="C211" t="s">
         <v>1353</v>
       </c>
-      <c r="B211">
-        <v>2</v>
-      </c>
-      <c r="C211" t="s">
-        <v>1354</v>
-      </c>
       <c r="D211" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="E211" s="2" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="213" spans="1:6">
       <c r="A213" s="10" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="215" spans="1:6">
       <c r="A215" s="10" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="216" spans="1:6">
@@ -8563,19 +8563,19 @@
     </row>
     <row r="217" spans="1:6">
       <c r="A217" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B217">
         <v>2</v>
       </c>
       <c r="C217" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="D217" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="E217" s="2" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="F217" t="s">
         <v>829</v>
@@ -8583,19 +8583,19 @@
     </row>
     <row r="218" spans="1:6">
       <c r="A218" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B218">
         <v>2</v>
       </c>
       <c r="C218" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="D218" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="E218" s="2" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="F218" t="s">
         <v>829</v>
@@ -8603,12 +8603,12 @@
     </row>
     <row r="220" spans="1:6">
       <c r="A220" s="10" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="222" spans="1:6">
       <c r="A222" s="10" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="223" spans="1:6">
@@ -8627,19 +8627,19 @@
     </row>
     <row r="224" spans="1:6">
       <c r="A224" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B224">
+        <v>2</v>
+      </c>
+      <c r="C224" t="s">
         <v>1372</v>
       </c>
-      <c r="B224">
-        <v>2</v>
-      </c>
-      <c r="C224" t="s">
+      <c r="D224" t="s">
         <v>1373</v>
       </c>
-      <c r="D224" t="s">
-        <v>1374</v>
-      </c>
       <c r="E224" s="2" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="F224" t="s">
         <v>829</v>
@@ -8647,19 +8647,19 @@
     </row>
     <row r="225" spans="1:6">
       <c r="A225" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B225">
+        <v>2</v>
+      </c>
+      <c r="C225" t="s">
         <v>1375</v>
       </c>
-      <c r="B225">
-        <v>2</v>
-      </c>
-      <c r="C225" t="s">
-        <v>1376</v>
-      </c>
       <c r="D225" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E225" s="2" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="F225" t="s">
         <v>829</v>
@@ -8667,19 +8667,19 @@
     </row>
     <row r="226" spans="1:6">
       <c r="A226" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B226">
+        <v>2</v>
+      </c>
+      <c r="C226" t="s">
         <v>1377</v>
       </c>
-      <c r="B226">
-        <v>2</v>
-      </c>
-      <c r="C226" t="s">
-        <v>1378</v>
-      </c>
       <c r="D226" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E226" s="2" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="F226" t="s">
         <v>829</v>
@@ -8687,19 +8687,19 @@
     </row>
     <row r="227" spans="1:6">
       <c r="A227" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B227">
+        <v>2</v>
+      </c>
+      <c r="C227" t="s">
         <v>1379</v>
       </c>
-      <c r="B227">
-        <v>2</v>
-      </c>
-      <c r="C227" t="s">
-        <v>1380</v>
-      </c>
       <c r="D227" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E227" s="2" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="F227" t="s">
         <v>829</v>
@@ -8707,19 +8707,19 @@
     </row>
     <row r="228" spans="1:6">
       <c r="A228" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B228">
+        <v>2</v>
+      </c>
+      <c r="C228" t="s">
         <v>1381</v>
       </c>
-      <c r="B228">
-        <v>2</v>
-      </c>
-      <c r="C228" t="s">
-        <v>1382</v>
-      </c>
       <c r="D228" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E228" s="2" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="F228" t="s">
         <v>829</v>
@@ -8727,7 +8727,7 @@
     </row>
     <row r="230" spans="1:6">
       <c r="A230" s="10" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="231" spans="1:6">
@@ -8746,19 +8746,19 @@
     </row>
     <row r="232" spans="1:6">
       <c r="A232" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="B232">
         <v>2</v>
       </c>
       <c r="C232" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="D232" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E232" s="2" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="F232" t="s">
         <v>829</v>
@@ -8766,19 +8766,19 @@
     </row>
     <row r="233" spans="1:6">
       <c r="A233" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="B233">
         <v>2</v>
       </c>
       <c r="C233" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="D233" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E233" s="2" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="F233" t="s">
         <v>829</v>
@@ -8786,19 +8786,19 @@
     </row>
     <row r="234" spans="1:6">
       <c r="A234" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="B234">
         <v>2</v>
       </c>
       <c r="C234" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="D234" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E234" s="2" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="F234" t="s">
         <v>829</v>
@@ -8806,19 +8806,19 @@
     </row>
     <row r="235" spans="1:6">
       <c r="A235" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="B235">
         <v>2</v>
       </c>
       <c r="C235" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="D235" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E235" s="2" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="F235" t="s">
         <v>829</v>
@@ -8826,19 +8826,19 @@
     </row>
     <row r="236" spans="1:6">
       <c r="A236" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="B236">
         <v>2</v>
       </c>
       <c r="C236" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D236" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E236" s="2" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="F236" t="s">
         <v>829</v>
@@ -8846,21 +8846,21 @@
     </row>
     <row r="237" spans="1:6">
       <c r="A237" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B237">
+        <v>2</v>
+      </c>
+      <c r="C237" t="s">
         <v>1397</v>
       </c>
-      <c r="B237">
-        <v>2</v>
-      </c>
-      <c r="C237" t="s">
-        <v>1398</v>
-      </c>
       <c r="D237" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="239" spans="1:6">
       <c r="A239" s="10" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="240" spans="1:6">
@@ -8879,46 +8879,46 @@
     </row>
     <row r="241" spans="1:6">
       <c r="A241" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B241">
+        <v>2</v>
+      </c>
+      <c r="C241" t="s">
         <v>1410</v>
       </c>
-      <c r="B241">
-        <v>2</v>
-      </c>
-      <c r="C241" t="s">
-        <v>1411</v>
-      </c>
       <c r="D241" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E241" s="2" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="242" spans="1:6">
       <c r="A242" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B242">
+        <v>2</v>
+      </c>
+      <c r="C242" t="s">
         <v>1397</v>
       </c>
-      <c r="B242">
-        <v>2</v>
-      </c>
-      <c r="C242" t="s">
-        <v>1398</v>
-      </c>
       <c r="D242" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="E242" s="2" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="244" spans="1:6">
       <c r="A244" s="10" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="246" spans="1:6">
       <c r="A246" s="10" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="247" spans="1:6">
@@ -8943,13 +8943,13 @@
         <v>2</v>
       </c>
       <c r="C248" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="D248" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="E248" s="2" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="F248" t="s">
         <v>829</v>
@@ -8957,19 +8957,19 @@
     </row>
     <row r="249" spans="1:6">
       <c r="A249" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B249">
+        <v>2</v>
+      </c>
+      <c r="C249" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D249" t="s">
         <v>1457</v>
       </c>
-      <c r="B249">
-        <v>2</v>
-      </c>
-      <c r="C249" t="s">
-        <v>1458</v>
-      </c>
-      <c r="D249" t="s">
-        <v>1459</v>
-      </c>
       <c r="E249" s="2" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="F249" t="s">
         <v>829</v>
@@ -8977,19 +8977,19 @@
     </row>
     <row r="250" spans="1:6">
       <c r="A250" t="s">
+        <v>1458</v>
+      </c>
+      <c r="B250">
+        <v>2</v>
+      </c>
+      <c r="C250" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D250" t="s">
         <v>1460</v>
       </c>
-      <c r="B250">
-        <v>2</v>
-      </c>
-      <c r="C250" t="s">
-        <v>1461</v>
-      </c>
-      <c r="D250" t="s">
-        <v>1462</v>
-      </c>
       <c r="E250" s="2" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="F250" t="s">
         <v>829</v>
@@ -8997,19 +8997,19 @@
     </row>
     <row r="251" spans="1:6">
       <c r="A251" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B251">
+        <v>2</v>
+      </c>
+      <c r="C251" t="s">
+        <v>1462</v>
+      </c>
+      <c r="D251" t="s">
         <v>1463</v>
       </c>
-      <c r="B251">
-        <v>2</v>
-      </c>
-      <c r="C251" t="s">
-        <v>1464</v>
-      </c>
-      <c r="D251" t="s">
-        <v>1465</v>
-      </c>
       <c r="E251" s="2" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="F251" t="s">
         <v>829</v>
@@ -9017,22 +9017,27 @@
     </row>
     <row r="252" spans="1:6">
       <c r="A252" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B252">
+        <v>2</v>
+      </c>
+      <c r="C252" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D252" t="s">
         <v>1466</v>
       </c>
-      <c r="B252">
-        <v>2</v>
-      </c>
-      <c r="C252" t="s">
-        <v>1467</v>
-      </c>
-      <c r="D252" t="s">
-        <v>1468</v>
-      </c>
       <c r="E252" s="2" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="F252" t="s">
         <v>829</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6">
+      <c r="A254" s="10" t="s">
+        <v>1480</v>
       </c>
     </row>
   </sheetData>
@@ -9043,10 +9048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I126"/>
+  <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView topLeftCell="D115" workbookViewId="0">
-      <selection activeCell="H128" sqref="H128"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10149,12 +10154,12 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:7">
       <c r="A81" s="10" t="s">
         <v>1204</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:7">
       <c r="A83" s="10" t="s">
         <v>1212</v>
       </c>
@@ -10162,7 +10167,7 @@
       <c r="E83" s="2"/>
       <c r="F83"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
         <v>4</v>
       </c>
@@ -10176,138 +10181,121 @@
         <v>7</v>
       </c>
       <c r="E84" t="s">
-        <v>1213</v>
-      </c>
-      <c r="F84" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="85" spans="1:8">
+      <c r="F84"/>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B85">
         <v>2</v>
       </c>
       <c r="C85" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="D85" t="s">
         <v>9</v>
       </c>
-      <c r="E85">
-        <v>3</v>
-      </c>
-      <c r="F85" t="s">
-        <v>1226</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
+      <c r="E85" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B86">
         <v>2</v>
       </c>
       <c r="C86" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="D86" t="s">
         <v>9</v>
       </c>
-      <c r="E86">
-        <v>3</v>
-      </c>
-      <c r="F86" t="s">
-        <v>1223</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
+      <c r="E86" t="s">
+        <v>1222</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B87">
         <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="D87" t="s">
         <v>9</v>
       </c>
-      <c r="E87">
-        <v>6</v>
-      </c>
-      <c r="F87" t="s">
-        <v>1220</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
+      <c r="E87" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B88">
         <v>2</v>
       </c>
       <c r="C88" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="D88" t="s">
         <v>9</v>
       </c>
-      <c r="E88">
-        <v>3</v>
-      </c>
-      <c r="F88" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
+      <c r="E88" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B89">
         <v>7</v>
       </c>
       <c r="C89" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="D89" t="s">
         <v>9</v>
       </c>
-      <c r="E89">
-        <v>8</v>
-      </c>
-      <c r="F89" t="s">
-        <v>1214</v>
-      </c>
-      <c r="G89" s="2" t="s">
+      <c r="E89" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="1" t="s">
         <v>1230</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
-      <c r="A91" s="1" t="s">
-        <v>1231</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:7">
       <c r="A93" s="10" t="s">
-        <v>1241</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
         <v>4</v>
       </c>
@@ -10321,159 +10309,139 @@
         <v>7</v>
       </c>
       <c r="E94" t="s">
-        <v>1213</v>
-      </c>
-      <c r="F94" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="95" spans="1:8">
+      <c r="F94"/>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B95">
+        <v>2</v>
+      </c>
+      <c r="C95" t="s">
         <v>1262</v>
-      </c>
-      <c r="B95">
-        <v>2</v>
-      </c>
-      <c r="C95" t="s">
-        <v>1263</v>
       </c>
       <c r="D95" t="s">
         <v>9</v>
       </c>
-      <c r="E95">
-        <v>1</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="E95" t="s">
         <v>755</v>
       </c>
-      <c r="G95" s="2" t="s">
-        <v>1310</v>
-      </c>
-      <c r="H95" t="s">
+      <c r="F95" s="2" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G95" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B96">
+        <v>2</v>
+      </c>
+      <c r="C96" t="s">
         <v>1264</v>
-      </c>
-      <c r="B96">
-        <v>2</v>
-      </c>
-      <c r="C96" t="s">
-        <v>1265</v>
       </c>
       <c r="D96" t="s">
         <v>9</v>
       </c>
-      <c r="E96">
-        <v>1</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="E96" t="s">
         <v>251</v>
       </c>
-      <c r="G96" s="2" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7">
+      <c r="F96" s="2" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B97">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
         <v>1266</v>
-      </c>
-      <c r="B97">
-        <v>2</v>
-      </c>
-      <c r="C97" t="s">
-        <v>1267</v>
       </c>
       <c r="D97" t="s">
         <v>9</v>
       </c>
-      <c r="E97">
-        <v>1</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="E97" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" t="s">
         <v>1268</v>
       </c>
-      <c r="G97" s="2" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7">
-      <c r="A98" t="s">
+      <c r="B98">
+        <v>2</v>
+      </c>
+      <c r="C98" t="s">
         <v>1269</v>
-      </c>
-      <c r="B98">
-        <v>2</v>
-      </c>
-      <c r="C98" t="s">
-        <v>1270</v>
       </c>
       <c r="D98" t="s">
         <v>9</v>
       </c>
-      <c r="E98">
-        <v>3</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="E98" t="s">
+        <v>1270</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" t="s">
         <v>1271</v>
       </c>
-      <c r="G98" s="2" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7">
-      <c r="A99" t="s">
+      <c r="B99">
+        <v>2</v>
+      </c>
+      <c r="C99" t="s">
         <v>1272</v>
-      </c>
-      <c r="B99">
-        <v>2</v>
-      </c>
-      <c r="C99" t="s">
-        <v>1273</v>
       </c>
       <c r="D99" t="s">
         <v>9</v>
       </c>
-      <c r="E99">
-        <v>1</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="E99" t="s">
         <v>505</v>
       </c>
-      <c r="G99" s="2" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7">
+      <c r="F99" s="2" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B100">
+        <v>2</v>
+      </c>
+      <c r="C100" t="s">
         <v>1274</v>
-      </c>
-      <c r="B100">
-        <v>2</v>
-      </c>
-      <c r="C100" t="s">
-        <v>1275</v>
       </c>
       <c r="D100" t="s">
         <v>9</v>
       </c>
-      <c r="E100">
-        <v>1</v>
-      </c>
-      <c r="F100" t="s">
-        <v>1268</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7">
+      <c r="E100" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
       <c r="A103" s="10" t="s">
-        <v>1337</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
         <v>4</v>
       </c>
@@ -10487,187 +10455,166 @@
         <v>7</v>
       </c>
       <c r="E104" t="s">
-        <v>1213</v>
-      </c>
-      <c r="F104" t="s">
         <v>8</v>
       </c>
-      <c r="G104" s="2" t="s">
+      <c r="F104" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B105">
         <v>2</v>
       </c>
       <c r="C105" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="D105" t="s">
         <v>9</v>
       </c>
-      <c r="E105">
-        <v>1</v>
-      </c>
-      <c r="F105" t="s">
+      <c r="E105" t="s">
         <v>276</v>
       </c>
-      <c r="G105" s="2" t="s">
-        <v>1347</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7">
+      <c r="F105" s="2" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B106">
+        <v>2</v>
+      </c>
+      <c r="C106" t="s">
         <v>1264</v>
-      </c>
-      <c r="B106">
-        <v>2</v>
-      </c>
-      <c r="C106" t="s">
-        <v>1265</v>
       </c>
       <c r="D106" t="s">
         <v>9</v>
       </c>
-      <c r="E106">
-        <v>1</v>
-      </c>
-      <c r="F106" t="s">
+      <c r="E106" t="s">
         <v>251</v>
       </c>
-      <c r="G106" s="2" t="s">
-        <v>1346</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7">
+      <c r="F106" s="2" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B107">
+        <v>2</v>
+      </c>
+      <c r="C107" t="s">
         <v>1266</v>
-      </c>
-      <c r="B107">
-        <v>2</v>
-      </c>
-      <c r="C107" t="s">
-        <v>1267</v>
       </c>
       <c r="D107" t="s">
         <v>9</v>
       </c>
-      <c r="E107">
-        <v>1</v>
-      </c>
-      <c r="F107" t="s">
+      <c r="E107" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" t="s">
         <v>1268</v>
       </c>
-      <c r="G107" s="2" t="s">
-        <v>1345</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7">
-      <c r="A108" t="s">
+      <c r="B108">
+        <v>2</v>
+      </c>
+      <c r="C108" t="s">
         <v>1269</v>
-      </c>
-      <c r="B108">
-        <v>2</v>
-      </c>
-      <c r="C108" t="s">
-        <v>1270</v>
       </c>
       <c r="D108" t="s">
         <v>9</v>
       </c>
-      <c r="E108">
-        <v>3</v>
-      </c>
-      <c r="F108" t="s">
+      <c r="E108" t="s">
+        <v>1270</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" t="s">
         <v>1271</v>
       </c>
-      <c r="G108" s="2" t="s">
-        <v>1344</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7">
-      <c r="A109" t="s">
+      <c r="B109">
+        <v>2</v>
+      </c>
+      <c r="C109" t="s">
         <v>1272</v>
-      </c>
-      <c r="B109">
-        <v>2</v>
-      </c>
-      <c r="C109" t="s">
-        <v>1273</v>
       </c>
       <c r="D109" t="s">
         <v>9</v>
       </c>
-      <c r="E109">
-        <v>1</v>
-      </c>
-      <c r="F109" t="s">
+      <c r="E109" t="s">
         <v>505</v>
       </c>
-      <c r="G109" s="2" t="s">
-        <v>1343</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7">
+      <c r="F109" s="2" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
       <c r="A110" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B110">
+        <v>2</v>
+      </c>
+      <c r="C110" t="s">
         <v>1274</v>
-      </c>
-      <c r="B110">
-        <v>2</v>
-      </c>
-      <c r="C110" t="s">
-        <v>1275</v>
       </c>
       <c r="D110" t="s">
         <v>9</v>
       </c>
-      <c r="E110">
-        <v>1</v>
-      </c>
-      <c r="F110" t="s">
-        <v>1268</v>
-      </c>
-      <c r="G110" s="2" t="s">
-        <v>1342</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7">
+      <c r="E110" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="A112" s="10" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" s="10" t="s">
         <v>1366</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
-      <c r="A114" s="10" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:7">
       <c r="A116" s="10" t="s">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
       <c r="A117" s="10"/>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:7">
       <c r="A118" s="10" t="s">
-        <v>1413</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
       <c r="F119"/>
       <c r="G119" s="2"/>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:7">
       <c r="A120" s="10" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="F120"/>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:7">
       <c r="A121" s="3" t="s">
         <v>4</v>
       </c>
@@ -10681,16 +10628,11 @@
         <v>7</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>1213</v>
-      </c>
-      <c r="F121" s="3" t="s">
-        <v>1419</v>
-      </c>
-      <c r="G121" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="122" spans="1:9">
+      <c r="F121"/>
+    </row>
+    <row r="122" spans="1:7">
       <c r="A122" s="3" t="s">
         <v>722</v>
       </c>
@@ -10698,143 +10640,137 @@
         <v>2</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E122" s="3">
-        <v>1</v>
-      </c>
-      <c r="F122" s="3" t="b">
-        <f>EXACT(B122,E122)</f>
-        <v>0</v>
-      </c>
-      <c r="G122" s="3" t="s">
+      <c r="E122" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="H122" s="5" t="s">
-        <v>1473</v>
-      </c>
-      <c r="I122" t="s">
+      <c r="F122" s="5" t="s">
+        <v>1471</v>
+      </c>
+      <c r="G122" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:7">
       <c r="A123" s="3" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="B123" s="3">
         <v>2</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E123" s="3">
-        <v>3</v>
-      </c>
-      <c r="F123" s="3" t="b">
-        <f>EXACT(B123,E123)</f>
-        <v>0</v>
-      </c>
-      <c r="G123" s="3" t="s">
+      <c r="E123" s="3" t="s">
+        <v>1421</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>1472</v>
+      </c>
+      <c r="G123" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" s="3" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B124" s="3">
+        <v>2</v>
+      </c>
+      <c r="C124" s="3" t="s">
         <v>1423</v>
-      </c>
-      <c r="H123" s="5" t="s">
-        <v>1474</v>
-      </c>
-      <c r="I123" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9">
-      <c r="A124" s="3" t="s">
-        <v>1424</v>
-      </c>
-      <c r="B124" s="3">
-        <v>2</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>1425</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E124" s="3">
-        <v>1</v>
-      </c>
-      <c r="F124" s="3" t="b">
-        <f>EXACT(B124,E124)</f>
-        <v>0</v>
-      </c>
-      <c r="G124" s="3" t="s">
+      <c r="E124" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="H124" s="2" t="s">
-        <v>1480</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9">
+      <c r="F124" s="2" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
       <c r="A125" s="3" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="B125" s="3">
         <v>2</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E125" s="3">
-        <v>1</v>
-      </c>
-      <c r="F125" s="3" t="b">
-        <f>EXACT(B125,E125)</f>
-        <v>0</v>
-      </c>
-      <c r="G125" s="3" t="s">
-        <v>1268</v>
-      </c>
-      <c r="H125" s="5" t="s">
-        <v>1475</v>
-      </c>
-      <c r="I125" t="s">
+      <c r="E125" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>1473</v>
+      </c>
+      <c r="G125" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:7">
       <c r="A126" s="3" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
       <c r="B126" s="3">
         <v>2</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E126" s="3">
-        <v>1</v>
-      </c>
-      <c r="F126" s="3" t="b">
-        <f>EXACT(B126,E126)</f>
-        <v>0</v>
-      </c>
-      <c r="G126" s="3" t="s">
-        <v>1430</v>
-      </c>
-      <c r="H126" s="2" t="s">
-        <v>1476</v>
-      </c>
-      <c r="I126" t="s">
+      <c r="E126" s="3" t="s">
+        <v>1428</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>1474</v>
+      </c>
+      <c r="G126" t="s">
         <v>829</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
+      <c r="F127"/>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" s="10" t="s">
+        <v>1481</v>
+      </c>
+      <c r="F128"/>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="3" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B129" s="3">
+        <v>2</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>1478</v>
       </c>
     </row>
   </sheetData>
@@ -10845,10 +10781,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H276"/>
+  <dimension ref="A1:H278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A266" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F279" sqref="F279"/>
+    <sheetView topLeftCell="A264" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A278" sqref="A278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14310,17 +14246,17 @@
         <v>386</v>
       </c>
       <c r="F215" s="2" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="217" spans="1:7">
       <c r="A217" s="1" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="219" spans="1:7">
       <c r="A219" s="10" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="220" spans="1:7">
@@ -14354,40 +14290,40 @@
         <v>1053</v>
       </c>
       <c r="E221" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="F221" s="2" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="222" spans="1:7">
       <c r="A222" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B222">
+        <v>2</v>
+      </c>
+      <c r="C222" t="s">
         <v>1233</v>
       </c>
-      <c r="B222">
-        <v>2</v>
-      </c>
-      <c r="C222" t="s">
+      <c r="D222" t="s">
         <v>1234</v>
       </c>
-      <c r="D222" t="s">
+      <c r="E222" t="s">
         <v>1235</v>
       </c>
-      <c r="E222" t="s">
-        <v>1236</v>
-      </c>
       <c r="F222" s="2" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="224" spans="1:7">
       <c r="A224" s="1" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="226" spans="1:7">
       <c r="A226" s="10" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="227" spans="1:7">
@@ -14410,131 +14346,131 @@
     </row>
     <row r="228" spans="1:7">
       <c r="A228" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B228">
+        <v>2</v>
+      </c>
+      <c r="C228" t="s">
         <v>1242</v>
       </c>
-      <c r="B228">
-        <v>2</v>
-      </c>
-      <c r="C228" t="s">
+      <c r="D228" t="s">
+        <v>1313</v>
+      </c>
+      <c r="E228" t="s">
         <v>1243</v>
       </c>
-      <c r="D228" t="s">
-        <v>1314</v>
-      </c>
-      <c r="E228" t="s">
-        <v>1244</v>
-      </c>
       <c r="F228" s="2" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G228" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="229" spans="1:7">
       <c r="A229" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B229">
+        <v>2</v>
+      </c>
+      <c r="C229" t="s">
         <v>1245</v>
       </c>
-      <c r="B229">
-        <v>2</v>
-      </c>
-      <c r="C229" t="s">
+      <c r="D229" t="s">
+        <v>1314</v>
+      </c>
+      <c r="E229" t="s">
         <v>1246</v>
       </c>
-      <c r="D229" t="s">
-        <v>1315</v>
-      </c>
-      <c r="E229" t="s">
-        <v>1247</v>
-      </c>
       <c r="F229" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G229" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="230" spans="1:7">
       <c r="A230" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B230">
+        <v>2</v>
+      </c>
+      <c r="C230" t="s">
         <v>1248</v>
       </c>
-      <c r="B230">
-        <v>2</v>
-      </c>
-      <c r="C230" t="s">
+      <c r="D230" t="s">
+        <v>1315</v>
+      </c>
+      <c r="E230" t="s">
         <v>1249</v>
       </c>
-      <c r="D230" t="s">
-        <v>1316</v>
-      </c>
-      <c r="E230" t="s">
-        <v>1250</v>
-      </c>
       <c r="F230" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G230" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="231" spans="1:7">
       <c r="A231" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B231">
+        <v>2</v>
+      </c>
+      <c r="C231" t="s">
         <v>1251</v>
       </c>
-      <c r="B231">
-        <v>2</v>
-      </c>
-      <c r="C231" t="s">
+      <c r="D231" t="s">
         <v>1252</v>
       </c>
-      <c r="D231" t="s">
+      <c r="E231" t="s">
         <v>1253</v>
       </c>
-      <c r="E231" t="s">
-        <v>1254</v>
-      </c>
       <c r="F231" s="2" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="232" spans="1:7">
       <c r="A232" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B232">
+        <v>2</v>
+      </c>
+      <c r="C232" t="s">
         <v>1255</v>
       </c>
-      <c r="B232">
-        <v>2</v>
-      </c>
-      <c r="C232" t="s">
+      <c r="D232" t="s">
+        <v>1252</v>
+      </c>
+      <c r="E232" t="s">
         <v>1256</v>
       </c>
-      <c r="D232" t="s">
-        <v>1253</v>
-      </c>
-      <c r="E232" t="s">
-        <v>1257</v>
-      </c>
       <c r="F232" s="2" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="233" spans="1:7">
       <c r="A233" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B233">
+        <v>2</v>
+      </c>
+      <c r="C233" t="s">
         <v>1258</v>
       </c>
-      <c r="B233">
-        <v>2</v>
-      </c>
-      <c r="C233" t="s">
+      <c r="D233" t="s">
         <v>1259</v>
       </c>
-      <c r="D233" t="s">
+      <c r="E233" t="s">
         <v>1260</v>
       </c>
-      <c r="E233" t="s">
-        <v>1261</v>
-      </c>
       <c r="F233" s="2" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="234" spans="1:7">
@@ -14542,7 +14478,7 @@
     </row>
     <row r="235" spans="1:7">
       <c r="A235" s="10" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="236" spans="1:7">
@@ -14565,43 +14501,43 @@
     </row>
     <row r="237" spans="1:7">
       <c r="A237" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B237">
+        <v>2</v>
+      </c>
+      <c r="C237" t="s">
         <v>1321</v>
       </c>
-      <c r="B237">
-        <v>2</v>
-      </c>
-      <c r="C237" t="s">
+      <c r="D237" t="s">
         <v>1322</v>
       </c>
-      <c r="D237" t="s">
+      <c r="E237" t="s">
         <v>1323</v>
-      </c>
-      <c r="E237" t="s">
-        <v>1324</v>
       </c>
       <c r="F237"/>
     </row>
     <row r="238" spans="1:7">
       <c r="A238" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B238">
+        <v>2</v>
+      </c>
+      <c r="C238" t="s">
         <v>1258</v>
       </c>
-      <c r="B238">
-        <v>2</v>
-      </c>
-      <c r="C238" t="s">
+      <c r="D238" t="s">
         <v>1259</v>
       </c>
-      <c r="D238" t="s">
+      <c r="E238" t="s">
         <v>1260</v>
-      </c>
-      <c r="E238" t="s">
-        <v>1261</v>
       </c>
       <c r="F238"/>
     </row>
     <row r="241" spans="1:7">
       <c r="A241" s="10" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="242" spans="1:7">
@@ -14621,57 +14557,57 @@
         <v>3</v>
       </c>
       <c r="F242" s="2" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="243" spans="1:7">
       <c r="A243" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B243">
         <v>2</v>
       </c>
       <c r="C243" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="D243" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E243" t="s">
         <v>1260</v>
       </c>
-      <c r="E243" t="s">
-        <v>1261</v>
-      </c>
       <c r="F243" s="2" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="244" spans="1:7">
       <c r="A244" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B244">
+        <v>2</v>
+      </c>
+      <c r="C244" t="s">
         <v>1321</v>
       </c>
-      <c r="B244">
-        <v>2</v>
-      </c>
-      <c r="C244" t="s">
+      <c r="D244" t="s">
         <v>1322</v>
       </c>
-      <c r="D244" t="s">
+      <c r="E244" t="s">
         <v>1323</v>
       </c>
-      <c r="E244" t="s">
-        <v>1324</v>
-      </c>
       <c r="F244" s="2" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="246" spans="1:7">
       <c r="A246" s="10" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="248" spans="1:7">
       <c r="A248" s="10" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -14691,27 +14627,27 @@
         <v>3</v>
       </c>
       <c r="F249" s="2" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="250" spans="1:7">
       <c r="A250" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B250">
+        <v>2</v>
+      </c>
+      <c r="C250" t="s">
         <v>1368</v>
       </c>
-      <c r="B250">
-        <v>2</v>
-      </c>
-      <c r="C250" t="s">
+      <c r="D250" t="s">
         <v>1369</v>
       </c>
-      <c r="D250" t="s">
+      <c r="E250" t="s">
         <v>1370</v>
       </c>
-      <c r="E250" t="s">
-        <v>1371</v>
-      </c>
       <c r="F250" s="2" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="G250" t="s">
         <v>829</v>
@@ -14719,12 +14655,12 @@
     </row>
     <row r="252" spans="1:7">
       <c r="A252" s="10" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="254" spans="1:7">
       <c r="A254" s="10" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="255" spans="1:7">
@@ -14746,41 +14682,41 @@
     </row>
     <row r="256" spans="1:7">
       <c r="A256" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B256">
+        <v>2</v>
+      </c>
+      <c r="C256" t="s">
         <v>1401</v>
       </c>
-      <c r="B256">
-        <v>2</v>
-      </c>
-      <c r="C256" t="s">
+      <c r="D256" t="s">
         <v>1402</v>
       </c>
-      <c r="D256" t="s">
+      <c r="E256" t="s">
         <v>1403</v>
-      </c>
-      <c r="E256" t="s">
-        <v>1404</v>
       </c>
     </row>
     <row r="257" spans="1:7">
       <c r="A257" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B257">
+        <v>2</v>
+      </c>
+      <c r="C257" t="s">
         <v>1405</v>
       </c>
-      <c r="B257">
-        <v>2</v>
-      </c>
-      <c r="C257" t="s">
+      <c r="D257" t="s">
         <v>1406</v>
       </c>
-      <c r="D257" t="s">
+      <c r="E257" t="s">
         <v>1407</v>
-      </c>
-      <c r="E257" t="s">
-        <v>1408</v>
       </c>
     </row>
     <row r="259" spans="1:7">
       <c r="A259" s="10" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="260" spans="1:7">
@@ -14802,52 +14738,52 @@
     </row>
     <row r="261" spans="1:7">
       <c r="A261" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B261">
+        <v>2</v>
+      </c>
+      <c r="C261" t="s">
         <v>1401</v>
       </c>
-      <c r="B261">
-        <v>2</v>
-      </c>
-      <c r="C261" t="s">
+      <c r="D261" t="s">
         <v>1402</v>
       </c>
-      <c r="D261" t="s">
+      <c r="E261" t="s">
         <v>1403</v>
       </c>
-      <c r="E261" t="s">
-        <v>1404</v>
-      </c>
       <c r="F261" s="2" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="262" spans="1:7">
       <c r="A262" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B262">
+        <v>2</v>
+      </c>
+      <c r="C262" t="s">
         <v>1405</v>
       </c>
-      <c r="B262">
-        <v>2</v>
-      </c>
-      <c r="C262" t="s">
+      <c r="D262" t="s">
         <v>1406</v>
       </c>
-      <c r="D262" t="s">
+      <c r="E262" t="s">
         <v>1407</v>
       </c>
-      <c r="E262" t="s">
-        <v>1408</v>
-      </c>
       <c r="F262" s="2" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="264" spans="1:7">
       <c r="A264" s="10" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="266" spans="1:7">
       <c r="A266" s="10" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="267" spans="1:7">
@@ -14869,22 +14805,22 @@
     </row>
     <row r="268" spans="1:7">
       <c r="A268" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B268">
+        <v>2</v>
+      </c>
+      <c r="C268" t="s">
+        <v>1431</v>
+      </c>
+      <c r="D268" t="s">
         <v>1432</v>
       </c>
-      <c r="B268">
-        <v>2</v>
-      </c>
-      <c r="C268" t="s">
+      <c r="E268" t="s">
         <v>1433</v>
       </c>
-      <c r="D268" t="s">
-        <v>1434</v>
-      </c>
-      <c r="E268" t="s">
-        <v>1435</v>
-      </c>
       <c r="F268" s="2" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="G268" t="s">
         <v>829</v>
@@ -14892,22 +14828,22 @@
     </row>
     <row r="269" spans="1:7">
       <c r="A269" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="B269">
         <v>2</v>
       </c>
       <c r="C269" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="D269" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="E269" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="F269" s="2" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="G269" t="s">
         <v>829</v>
@@ -14915,22 +14851,22 @@
     </row>
     <row r="270" spans="1:7">
       <c r="A270" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B270">
         <v>2</v>
       </c>
       <c r="C270" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="D270" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="E270" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="F270" s="2" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="G270" t="s">
         <v>829</v>
@@ -14938,22 +14874,22 @@
     </row>
     <row r="271" spans="1:7">
       <c r="A271" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B271">
+        <v>2</v>
+      </c>
+      <c r="C271" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D271" t="s">
         <v>1440</v>
       </c>
-      <c r="B271">
-        <v>2</v>
-      </c>
-      <c r="C271" t="s">
-        <v>1441</v>
-      </c>
-      <c r="D271" t="s">
-        <v>1442</v>
-      </c>
       <c r="E271" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="F271" s="2" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="G271" t="s">
         <v>829</v>
@@ -14961,22 +14897,22 @@
     </row>
     <row r="272" spans="1:7">
       <c r="A272" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="B272">
         <v>2</v>
       </c>
       <c r="C272" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="D272" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="E272" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="F272" s="2" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="G272" t="s">
         <v>829</v>
@@ -14984,22 +14920,22 @@
     </row>
     <row r="273" spans="1:7">
       <c r="A273" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B273">
+        <v>2</v>
+      </c>
+      <c r="C273" t="s">
+        <v>1443</v>
+      </c>
+      <c r="D273" t="s">
         <v>1444</v>
       </c>
-      <c r="B273">
-        <v>2</v>
-      </c>
-      <c r="C273" t="s">
+      <c r="E273" t="s">
         <v>1445</v>
       </c>
-      <c r="D273" t="s">
-        <v>1446</v>
-      </c>
-      <c r="E273" t="s">
-        <v>1447</v>
-      </c>
       <c r="F273" s="2" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="G273" t="s">
         <v>829</v>
@@ -15007,22 +14943,22 @@
     </row>
     <row r="274" spans="1:7">
       <c r="A274" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="B274">
         <v>2</v>
       </c>
       <c r="C274" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="D274" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="E274" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="F274" s="2" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="G274" t="s">
         <v>829</v>
@@ -15030,22 +14966,22 @@
     </row>
     <row r="275" spans="1:7">
       <c r="A275" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="B275">
         <v>2</v>
       </c>
       <c r="C275" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="D275" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="E275" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="F275" s="2" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="G275" t="s">
         <v>829</v>
@@ -15053,7 +14989,7 @@
     </row>
     <row r="276" spans="1:7">
       <c r="A276" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="B276">
         <v>2</v>
@@ -15062,16 +14998,21 @@
         <v>620</v>
       </c>
       <c r="D276" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="E276" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="F276" s="2" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="G276" t="s">
         <v>829</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7">
+      <c r="A278" s="10" t="s">
+        <v>1480</v>
       </c>
     </row>
   </sheetData>
@@ -15811,7 +15752,7 @@
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="10" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
   </sheetData>
@@ -16890,7 +16831,7 @@
         <v>727</v>
       </c>
       <c r="B13" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -17194,7 +17135,7 @@
         <v>730</v>
       </c>
       <c r="B51" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -17202,15 +17143,15 @@
         <v>1009</v>
       </c>
       <c r="B52" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B53" t="s">
         <v>1302</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1303</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -17247,10 +17188,10 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B58" t="s">
         <v>1304</v>
-      </c>
-      <c r="B58" t="s">
-        <v>1305</v>
       </c>
     </row>
     <row r="59" spans="1:2">

</xml_diff>

<commit_message>
added issues found on Aug 16, 2022
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F9943B-4DD9-0D46-A9F9-EFF3FCA51112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783ADF84-371B-CD48-B467-72066A18C238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="500" windowWidth="26600" windowHeight="14500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4960" yWindow="2500" windowWidth="26600" windowHeight="12380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2855" uniqueCount="1482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2905" uniqueCount="1508">
   <si>
     <t>sid</t>
   </si>
@@ -4534,6 +4534,84 @@
   </si>
   <si>
     <t>Checked on Aug 4th, 2022, only one issue is found.</t>
+  </si>
+  <si>
+    <t>changed to EUPATH_0000151</t>
+  </si>
+  <si>
+    <t>Was there sexual behavior change since take PrEP|Sexual behavior change since take PrEP</t>
+  </si>
+  <si>
+    <t>PrEP|Sexual behavior</t>
+  </si>
+  <si>
+    <t>EUPATH_0053214</t>
+  </si>
+  <si>
+    <t>Sprayed against mosquitoes in past 12 months | Sprayed in past 12 months</t>
+  </si>
+  <si>
+    <t>gates_namibia | icemr_sw_pacific</t>
+  </si>
+  <si>
+    <t>Was there sexual behavior change since take PrEP | Sexual behavior change since take PrEP</t>
+  </si>
+  <si>
+    <t>Reason to stop taking PrEP | Reason you stopped taking PrEP</t>
+  </si>
+  <si>
+    <t>gates_jilinde_awareness_survey | gates_jilinde_prospective_cohort | gates_jilinde_retrospective_survey | gates_jilinde_demand_creation_evaluation_questionnaire</t>
+  </si>
+  <si>
+    <t>What did you do with extra tablets after stopping PrEP | Extra tablets after stop taking PrEP</t>
+  </si>
+  <si>
+    <t>Other use of extra tablets after stopping PrEP specified | Extra tablets after stop taking PrEP specified</t>
+  </si>
+  <si>
+    <t>Live together with spouse or partner | Live with partner</t>
+  </si>
+  <si>
+    <t>gates_jilinde_awareness_survey | gates_jilinde_prospective_cohort | gates_jilinde_demand_creation_evaluation_questionnaire</t>
+  </si>
+  <si>
+    <t>EUPATH_0054169</t>
+  </si>
+  <si>
+    <t>Other main reason for agreeing to offer of PrEP specified | Main reason for agreeing to offer of PrEP</t>
+  </si>
+  <si>
+    <t>EUPATH_0054175</t>
+  </si>
+  <si>
+    <t>Main reason for stopping PrEP after prior use | Other main reason for stopping PrEP after prior use</t>
+  </si>
+  <si>
+    <t>EUPATH_0054248</t>
+  </si>
+  <si>
+    <t>Other reason of reconsidering taking PrEP specified | Reason of reconsidering taking PrEP</t>
+  </si>
+  <si>
+    <t>EUPATH_0054330</t>
+  </si>
+  <si>
+    <t>Whether have child | Have children</t>
+  </si>
+  <si>
+    <t>Sex work | Commercial sex and activity</t>
+  </si>
+  <si>
+    <t>gates_jilinde_prospective_cohort | gates_jilinde_retrospective_survey | gates_jilinde_demand_creation_evaluation_questionnaire</t>
+  </si>
+  <si>
+    <t>Checked on Aug 16th, 2022, one issue is found.</t>
+  </si>
+  <si>
+    <t>Checked on Aug 16th, 2022, one issue is found</t>
+  </si>
+  <si>
+    <t>Checked on Aug 16th, 2022, identified following issue:</t>
   </si>
 </sst>
 </file>
@@ -5433,10 +5511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G254"/>
+  <dimension ref="A1:G268"/>
   <sheetViews>
-    <sheetView topLeftCell="A234" workbookViewId="0">
-      <selection activeCell="C239" sqref="C239"/>
+    <sheetView tabSelected="1" topLeftCell="A242" workbookViewId="0">
+      <selection activeCell="C257" sqref="C257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9040,6 +9118,179 @@
         <v>1480</v>
       </c>
     </row>
+    <row r="256" spans="1:6">
+      <c r="A256" s="10" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4">
+      <c r="A257" t="s">
+        <v>0</v>
+      </c>
+      <c r="B257" t="s">
+        <v>1</v>
+      </c>
+      <c r="C257" t="s">
+        <v>2</v>
+      </c>
+      <c r="D257" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4">
+      <c r="A258" t="s">
+        <v>1485</v>
+      </c>
+      <c r="B258">
+        <v>2</v>
+      </c>
+      <c r="C258" t="s">
+        <v>1486</v>
+      </c>
+      <c r="D258" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4">
+      <c r="A259" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B259">
+        <v>2</v>
+      </c>
+      <c r="C259" t="s">
+        <v>1488</v>
+      </c>
+      <c r="D259" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4">
+      <c r="A260" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B260">
+        <v>2</v>
+      </c>
+      <c r="C260" t="s">
+        <v>1489</v>
+      </c>
+      <c r="D260" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4">
+      <c r="A261" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B261">
+        <v>2</v>
+      </c>
+      <c r="C261" t="s">
+        <v>1491</v>
+      </c>
+      <c r="D261" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4">
+      <c r="A262" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B262">
+        <v>2</v>
+      </c>
+      <c r="C262" t="s">
+        <v>1492</v>
+      </c>
+      <c r="D262" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4">
+      <c r="A263" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B263">
+        <v>2</v>
+      </c>
+      <c r="C263" t="s">
+        <v>1493</v>
+      </c>
+      <c r="D263" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4">
+      <c r="A264" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B264">
+        <v>2</v>
+      </c>
+      <c r="C264" t="s">
+        <v>1496</v>
+      </c>
+      <c r="D264" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4">
+      <c r="A265" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B265">
+        <v>2</v>
+      </c>
+      <c r="C265" t="s">
+        <v>1498</v>
+      </c>
+      <c r="D265" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4">
+      <c r="A266" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B266">
+        <v>2</v>
+      </c>
+      <c r="C266" t="s">
+        <v>1500</v>
+      </c>
+      <c r="D266" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4">
+      <c r="A267" t="s">
+        <v>1501</v>
+      </c>
+      <c r="B267">
+        <v>2</v>
+      </c>
+      <c r="C267" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D267" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4">
+      <c r="A268" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B268">
+        <v>2</v>
+      </c>
+      <c r="C268" t="s">
+        <v>1503</v>
+      </c>
+      <c r="D268" t="s">
+        <v>1504</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -9048,10 +9299,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136"/>
+    <sheetView topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10753,7 +11004,7 @@
       </c>
       <c r="F128"/>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:7">
       <c r="A129" s="3" t="s">
         <v>1422</v>
       </c>
@@ -10772,6 +11023,37 @@
       <c r="F129" s="2" t="s">
         <v>1478</v>
       </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" s="10" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" t="s">
+        <v>722</v>
+      </c>
+      <c r="B132">
+        <v>2</v>
+      </c>
+      <c r="C132" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D132" t="s">
+        <v>9</v>
+      </c>
+      <c r="E132" t="s">
+        <v>251</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>1482</v>
+      </c>
+      <c r="G132" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="F133"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10781,10 +11063,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H278"/>
+  <dimension ref="A1:H281"/>
   <sheetViews>
-    <sheetView topLeftCell="A264" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A278" sqref="A278"/>
+    <sheetView topLeftCell="A270" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C284" sqref="C284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15014,6 +15296,29 @@
       <c r="A278" s="10" t="s">
         <v>1480</v>
       </c>
+    </row>
+    <row r="280" spans="1:7">
+      <c r="A280" s="10" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7">
+      <c r="A281" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B281">
+        <v>2</v>
+      </c>
+      <c r="C281" t="s">
+        <v>1483</v>
+      </c>
+      <c r="D281" t="s">
+        <v>1484</v>
+      </c>
+      <c r="E281" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F281"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F30" xr:uid="{3F2C9002-1B0A-C348-905C-32E2D16BAD66}"/>

</xml_diff>

<commit_message>
add issues found on Oct 21st, 2022
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14870DD-B7AC-FC4B-8868-10CFF49E0C2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290A5314-F0C4-7142-9B74-28577320E6A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="520" windowWidth="24820" windowHeight="15880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3400" yWindow="500" windowWidth="24820" windowHeight="15880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2970" uniqueCount="1537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3068" uniqueCount="1592">
   <si>
     <t>sid</t>
   </si>
@@ -4699,6 +4699,171 @@
   </si>
   <si>
     <t>Checked on Aug 16th, 2022, all issues are fixed</t>
+  </si>
+  <si>
+    <t>Checked on Oct 21st, 2022, identified following issue:</t>
+  </si>
+  <si>
+    <t>EUPATH_0000001</t>
+  </si>
+  <si>
+    <t>Building material | Respiratory and asthma control score (TRACK)</t>
+  </si>
+  <si>
+    <t>icemr_india_cx | gates_crypto | icemr_india_cohort | icemr_india_severe_malaria</t>
+  </si>
+  <si>
+    <t>EUPATH_0010533</t>
+  </si>
+  <si>
+    <t>Loose stools in day count | Loose stools in day count, caregiver report</t>
+  </si>
+  <si>
+    <t>gates_crypto | gates_provide | gates_maled</t>
+  </si>
+  <si>
+    <t>EUPATH_0015040</t>
+  </si>
+  <si>
+    <t>Unprotected spring | Unprotected dug well or spring</t>
+  </si>
+  <si>
+    <t>gates_gems1a | gates_gems | gates_vida | gates_jilinde_costing_survey</t>
+  </si>
+  <si>
+    <t>EUPATH_0015050</t>
+  </si>
+  <si>
+    <t>Bore hole | Protected shallow well or borehole</t>
+  </si>
+  <si>
+    <t>EUPATH_0025047</t>
+  </si>
+  <si>
+    <t>Roof material type | Roof material categorization</t>
+  </si>
+  <si>
+    <t>gates_washb_kenya | icemr_malawi | general_promote | gates_shine</t>
+  </si>
+  <si>
+    <t>EUPATH_0036053</t>
+  </si>
+  <si>
+    <t>Stool consistencys | Stool consistency, caregiver report</t>
+  </si>
+  <si>
+    <t>gates_crypto | gates_provide</t>
+  </si>
+  <si>
+    <t>EUPATH_0036210</t>
+  </si>
+  <si>
+    <t>Household expenditures in local currency | Family expenditures in local currency</t>
+  </si>
+  <si>
+    <t>EUPATH_0051964</t>
+  </si>
+  <si>
+    <t>Health care | Healthcare</t>
+  </si>
+  <si>
+    <t>gates_ppfp_choices_kenya_pp | gates_jilinde_costing_survey</t>
+  </si>
+  <si>
+    <t>EUPATH_0054676</t>
+  </si>
+  <si>
+    <t>Read newspapers | Read newspaper</t>
+  </si>
+  <si>
+    <t>gates_jilinde_awareness_survey | gates_jilinde_costing_survey | gates_jilinde_demand_creation_evaluation_questionnaire</t>
+  </si>
+  <si>
+    <t>EUPATH_0054747</t>
+  </si>
+  <si>
+    <t>Whether listen to radio | Listen to radio</t>
+  </si>
+  <si>
+    <t>EUPATH_0054787</t>
+  </si>
+  <si>
+    <t>Whether watch TV | Watch television</t>
+  </si>
+  <si>
+    <t>Checked on Oct 21st, 2022, no issue was found</t>
+  </si>
+  <si>
+    <t>Bore hole|Protected shallow well or borehole</t>
+  </si>
+  <si>
+    <t>Drinking water source|Water source</t>
+  </si>
+  <si>
+    <t>Building material|Respiratory and asthma control score (TRACK)</t>
+  </si>
+  <si>
+    <t>Dwelling characteristics|Signs and symptoms</t>
+  </si>
+  <si>
+    <t>Child observation details|Child physical exam</t>
+  </si>
+  <si>
+    <t>gates_ganc | gates_betterbirth</t>
+  </si>
+  <si>
+    <t>Loose stools in day count, caregiver report|Loose stools in day count</t>
+  </si>
+  <si>
+    <t>Symptoms|Symptoms by caregiver report</t>
+  </si>
+  <si>
+    <t>EUPATH_0015049</t>
+  </si>
+  <si>
+    <t>Other water source</t>
+  </si>
+  <si>
+    <t>EUPATH_0015038</t>
+  </si>
+  <si>
+    <t>Protected spring</t>
+  </si>
+  <si>
+    <t>EUPATH_0015046</t>
+  </si>
+  <si>
+    <t>Rainwater</t>
+  </si>
+  <si>
+    <t>Read newspapers|Read newspaper</t>
+  </si>
+  <si>
+    <t>Activity|Use of media at least once a week</t>
+  </si>
+  <si>
+    <t>Stool consistency, caregiver report|Stool consistencys</t>
+  </si>
+  <si>
+    <t>EUPATH_0031313</t>
+  </si>
+  <si>
+    <t>Surface water</t>
+  </si>
+  <si>
+    <t>gates_vida | gates_jilinde_costing_survey</t>
+  </si>
+  <si>
+    <t>Unprotected spring|Unprotected dug well or spring</t>
+  </si>
+  <si>
+    <t>Whether listen to radio|Listen to radio</t>
+  </si>
+  <si>
+    <t>Whether watch TV|Watch television</t>
+  </si>
+  <si>
+    <t>Might due to different terms but assigned same ID</t>
   </si>
 </sst>
 </file>
@@ -5598,10 +5763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G277"/>
+  <dimension ref="A1:G291"/>
   <sheetViews>
-    <sheetView topLeftCell="A255" workbookViewId="0">
-      <selection activeCell="A277" sqref="A277"/>
+    <sheetView topLeftCell="A261" workbookViewId="0">
+      <selection activeCell="A279" sqref="A279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9530,6 +9695,179 @@
         <v>1536</v>
       </c>
     </row>
+    <row r="279" spans="1:4">
+      <c r="A279" s="10" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4">
+      <c r="A280" t="s">
+        <v>0</v>
+      </c>
+      <c r="B280" t="s">
+        <v>1</v>
+      </c>
+      <c r="C280" t="s">
+        <v>2</v>
+      </c>
+      <c r="D280" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4">
+      <c r="A281" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B281">
+        <v>2</v>
+      </c>
+      <c r="C281" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D281" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4">
+      <c r="A282" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B282">
+        <v>2</v>
+      </c>
+      <c r="C282" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D282" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4">
+      <c r="A283" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B283">
+        <v>2</v>
+      </c>
+      <c r="C283" t="s">
+        <v>1545</v>
+      </c>
+      <c r="D283" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4">
+      <c r="A284" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B284">
+        <v>2</v>
+      </c>
+      <c r="C284" t="s">
+        <v>1548</v>
+      </c>
+      <c r="D284" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4">
+      <c r="A285" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B285">
+        <v>2</v>
+      </c>
+      <c r="C285" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D285" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4">
+      <c r="A286" t="s">
+        <v>1552</v>
+      </c>
+      <c r="B286">
+        <v>2</v>
+      </c>
+      <c r="C286" t="s">
+        <v>1553</v>
+      </c>
+      <c r="D286" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4">
+      <c r="A287" t="s">
+        <v>1555</v>
+      </c>
+      <c r="B287">
+        <v>2</v>
+      </c>
+      <c r="C287" t="s">
+        <v>1556</v>
+      </c>
+      <c r="D287" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4">
+      <c r="A288" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B288">
+        <v>2</v>
+      </c>
+      <c r="C288" t="s">
+        <v>1558</v>
+      </c>
+      <c r="D288" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4">
+      <c r="A289" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B289">
+        <v>2</v>
+      </c>
+      <c r="C289" t="s">
+        <v>1561</v>
+      </c>
+      <c r="D289" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4">
+      <c r="A290" t="s">
+        <v>1563</v>
+      </c>
+      <c r="B290">
+        <v>2</v>
+      </c>
+      <c r="C290" t="s">
+        <v>1564</v>
+      </c>
+      <c r="D290" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4">
+      <c r="A291" t="s">
+        <v>1565</v>
+      </c>
+      <c r="B291">
+        <v>2</v>
+      </c>
+      <c r="C291" t="s">
+        <v>1566</v>
+      </c>
+      <c r="D291" t="s">
+        <v>1562</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -9538,10 +9876,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G133"/>
+  <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11294,6 +11632,11 @@
     <row r="133" spans="1:7">
       <c r="F133"/>
     </row>
+    <row r="134" spans="1:7">
+      <c r="A134" s="10" t="s">
+        <v>1567</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -11302,10 +11645,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H290"/>
+  <dimension ref="A1:H308"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A271" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B293" sqref="B293"/>
+    <sheetView tabSelected="1" topLeftCell="A289" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C310" sqref="C310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15649,9 +15992,271 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="290" spans="1:1">
+    <row r="290" spans="1:6">
       <c r="A290" s="10" t="s">
         <v>1536</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6">
+      <c r="A292" s="10" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6">
+      <c r="A293" t="s">
+        <v>0</v>
+      </c>
+      <c r="B293" t="s">
+        <v>10</v>
+      </c>
+      <c r="C293" t="s">
+        <v>2</v>
+      </c>
+      <c r="D293" t="s">
+        <v>11</v>
+      </c>
+      <c r="E293" t="s">
+        <v>3</v>
+      </c>
+      <c r="F293"/>
+    </row>
+    <row r="294" spans="1:6">
+      <c r="A294" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B294">
+        <v>2</v>
+      </c>
+      <c r="C294" t="s">
+        <v>1568</v>
+      </c>
+      <c r="D294" t="s">
+        <v>1569</v>
+      </c>
+      <c r="E294" t="s">
+        <v>1546</v>
+      </c>
+      <c r="F294"/>
+    </row>
+    <row r="295" spans="1:6">
+      <c r="A295" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B295">
+        <v>2</v>
+      </c>
+      <c r="C295" t="s">
+        <v>1570</v>
+      </c>
+      <c r="D295" t="s">
+        <v>1571</v>
+      </c>
+      <c r="E295" t="s">
+        <v>1540</v>
+      </c>
+      <c r="F295"/>
+    </row>
+    <row r="296" spans="1:6">
+      <c r="A296" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B296">
+        <v>2</v>
+      </c>
+      <c r="C296" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D296" t="s">
+        <v>1572</v>
+      </c>
+      <c r="E296" t="s">
+        <v>1573</v>
+      </c>
+      <c r="F296"/>
+    </row>
+    <row r="297" spans="1:6">
+      <c r="A297" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B297">
+        <v>2</v>
+      </c>
+      <c r="C297" t="s">
+        <v>1574</v>
+      </c>
+      <c r="D297" t="s">
+        <v>1575</v>
+      </c>
+      <c r="E297" t="s">
+        <v>1543</v>
+      </c>
+      <c r="F297"/>
+    </row>
+    <row r="298" spans="1:6">
+      <c r="A298" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B298">
+        <v>2</v>
+      </c>
+      <c r="C298" t="s">
+        <v>1577</v>
+      </c>
+      <c r="D298" t="s">
+        <v>1569</v>
+      </c>
+      <c r="E298" t="s">
+        <v>1546</v>
+      </c>
+      <c r="F298"/>
+    </row>
+    <row r="299" spans="1:6">
+      <c r="A299" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B299">
+        <v>2</v>
+      </c>
+      <c r="C299" t="s">
+        <v>1579</v>
+      </c>
+      <c r="D299" t="s">
+        <v>1569</v>
+      </c>
+      <c r="E299" t="s">
+        <v>1546</v>
+      </c>
+      <c r="F299"/>
+    </row>
+    <row r="300" spans="1:6">
+      <c r="A300" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B300">
+        <v>2</v>
+      </c>
+      <c r="C300" t="s">
+        <v>1581</v>
+      </c>
+      <c r="D300" t="s">
+        <v>1569</v>
+      </c>
+      <c r="E300" t="s">
+        <v>1546</v>
+      </c>
+      <c r="F300"/>
+    </row>
+    <row r="301" spans="1:6">
+      <c r="A301" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B301">
+        <v>2</v>
+      </c>
+      <c r="C301" t="s">
+        <v>1582</v>
+      </c>
+      <c r="D301" t="s">
+        <v>1583</v>
+      </c>
+      <c r="E301" t="s">
+        <v>1562</v>
+      </c>
+      <c r="F301"/>
+    </row>
+    <row r="302" spans="1:6">
+      <c r="A302" t="s">
+        <v>1552</v>
+      </c>
+      <c r="B302">
+        <v>2</v>
+      </c>
+      <c r="C302" t="s">
+        <v>1584</v>
+      </c>
+      <c r="D302" t="s">
+        <v>1575</v>
+      </c>
+      <c r="E302" t="s">
+        <v>1554</v>
+      </c>
+      <c r="F302"/>
+    </row>
+    <row r="303" spans="1:6">
+      <c r="A303" t="s">
+        <v>1585</v>
+      </c>
+      <c r="B303">
+        <v>2</v>
+      </c>
+      <c r="C303" t="s">
+        <v>1586</v>
+      </c>
+      <c r="D303" t="s">
+        <v>1569</v>
+      </c>
+      <c r="E303" t="s">
+        <v>1587</v>
+      </c>
+      <c r="F303"/>
+    </row>
+    <row r="304" spans="1:6">
+      <c r="A304" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B304">
+        <v>2</v>
+      </c>
+      <c r="C304" t="s">
+        <v>1588</v>
+      </c>
+      <c r="D304" t="s">
+        <v>1569</v>
+      </c>
+      <c r="E304" t="s">
+        <v>1546</v>
+      </c>
+      <c r="F304"/>
+    </row>
+    <row r="305" spans="1:6">
+      <c r="A305" t="s">
+        <v>1563</v>
+      </c>
+      <c r="B305">
+        <v>2</v>
+      </c>
+      <c r="C305" t="s">
+        <v>1589</v>
+      </c>
+      <c r="D305" t="s">
+        <v>1583</v>
+      </c>
+      <c r="E305" t="s">
+        <v>1562</v>
+      </c>
+      <c r="F305"/>
+    </row>
+    <row r="306" spans="1:6">
+      <c r="A306" t="s">
+        <v>1565</v>
+      </c>
+      <c r="B306">
+        <v>2</v>
+      </c>
+      <c r="C306" t="s">
+        <v>1590</v>
+      </c>
+      <c r="D306" t="s">
+        <v>1583</v>
+      </c>
+      <c r="E306" t="s">
+        <v>1562</v>
+      </c>
+      <c r="F306"/>
+    </row>
+    <row r="308" spans="1:6">
+      <c r="A308" t="s">
+        <v>1591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
issue identified on Dec 7th, 2022
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A48EAFB-C8F7-104C-AF05-430D48ADAA74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3602D03F-86CB-6D4E-B408-B019A596D9C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7100" yWindow="1400" windowWidth="21660" windowHeight="14560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-200" yWindow="500" windowWidth="21660" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3093" uniqueCount="1608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3112" uniqueCount="1615">
   <si>
     <t>sid</t>
   </si>
@@ -4912,6 +4912,27 @@
   </si>
   <si>
     <t>Checked on Oct 24th, 2022, all issues are fixed.</t>
+  </si>
+  <si>
+    <t>Checked on Dec 7th, 2022, identified following issue:</t>
+  </si>
+  <si>
+    <t>EUPATH_0011652</t>
+  </si>
+  <si>
+    <t>Feedings yesterday|Lipid-based nutrient supplement feedings yesterday count</t>
+  </si>
+  <si>
+    <t>Feeding|Diet</t>
+  </si>
+  <si>
+    <t>gates_shine | gates_maled</t>
+  </si>
+  <si>
+    <t>Lipid-based nutrient supplement feedings yesterday count | Feedings yesterday</t>
+  </si>
+  <si>
+    <t>Checked on Dec 7th, 2022, no issue was found</t>
   </si>
 </sst>
 </file>
@@ -5811,10 +5832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G293"/>
+  <dimension ref="A1:G297"/>
   <sheetViews>
-    <sheetView topLeftCell="A271" workbookViewId="0">
-      <selection activeCell="C298" sqref="C298"/>
+    <sheetView tabSelected="1" topLeftCell="A282" workbookViewId="0">
+      <selection activeCell="B303" sqref="B303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9954,6 +9975,39 @@
         <v>1607</v>
       </c>
     </row>
+    <row r="295" spans="1:5">
+      <c r="A295" s="10" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5">
+      <c r="A296" t="s">
+        <v>0</v>
+      </c>
+      <c r="B296" t="s">
+        <v>1</v>
+      </c>
+      <c r="C296" t="s">
+        <v>2</v>
+      </c>
+      <c r="D296" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5">
+      <c r="A297" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B297">
+        <v>2</v>
+      </c>
+      <c r="C297" t="s">
+        <v>1613</v>
+      </c>
+      <c r="D297" t="s">
+        <v>1612</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -9962,10 +10016,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G134"/>
+  <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11723,6 +11777,11 @@
         <v>1567</v>
       </c>
     </row>
+    <row r="136" spans="1:7">
+      <c r="A136" s="10" t="s">
+        <v>1614</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -11733,8 +11792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A300" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B311" sqref="B311"/>
+    <sheetView topLeftCell="A296" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A310" sqref="A310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -16372,12 +16431,45 @@
       </c>
     </row>
     <row r="310" spans="1:6">
+      <c r="A310" s="10" t="s">
+        <v>1608</v>
+      </c>
       <c r="F310"/>
     </row>
     <row r="311" spans="1:6">
+      <c r="A311" t="s">
+        <v>0</v>
+      </c>
+      <c r="B311" t="s">
+        <v>10</v>
+      </c>
+      <c r="C311" t="s">
+        <v>2</v>
+      </c>
+      <c r="D311" t="s">
+        <v>11</v>
+      </c>
+      <c r="E311" t="s">
+        <v>3</v>
+      </c>
       <c r="F311"/>
     </row>
     <row r="312" spans="1:6">
+      <c r="A312" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B312">
+        <v>2</v>
+      </c>
+      <c r="C312" t="s">
+        <v>1610</v>
+      </c>
+      <c r="D312" t="s">
+        <v>1611</v>
+      </c>
+      <c r="E312" t="s">
+        <v>1612</v>
+      </c>
       <c r="F312"/>
     </row>
     <row r="313" spans="1:6">

</xml_diff>

<commit_message>
added new issues found on Dec 9th, 2022
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52DA7DD-05CC-594E-99D1-780D4C162151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E085CF61-17F0-3D42-ABFF-987605B2BE64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="2200" windowWidth="23760" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6240" yWindow="500" windowWidth="23760" windowHeight="14560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3115" uniqueCount="1618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3134" uniqueCount="1626">
   <si>
     <t>sid</t>
   </si>
@@ -4941,7 +4941,31 @@
     <t>Give a new IRI to the SHINE term and leave where it is</t>
   </si>
   <si>
-    <t>Assigned ID: EUPATH_0048294, fixed issue</t>
+    <t>Assigned new ID: EUPATH_0048294, fixed issue</t>
+  </si>
+  <si>
+    <t>Checked on Dec 9th, 2022, found new issue:</t>
+  </si>
+  <si>
+    <t>EUPATH_0000350</t>
+  </si>
+  <si>
+    <t>Days worked every week | Time spent in occupation every week</t>
+  </si>
+  <si>
+    <t>gates_jilinde_costing_survey | icemr_amazonia_peru</t>
+  </si>
+  <si>
+    <t>EUPATH_0050506</t>
+  </si>
+  <si>
+    <t>Facility type</t>
+  </si>
+  <si>
+    <t>Administrative information|Clinical history</t>
+  </si>
+  <si>
+    <t>gates_jilinde_costing_survey | gates_avenir</t>
   </si>
 </sst>
 </file>
@@ -5841,17 +5865,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G297"/>
+  <dimension ref="A1:G301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A287" workbookViewId="0">
-      <selection activeCell="A298" sqref="A298"/>
+    <sheetView topLeftCell="A284" workbookViewId="0">
+      <selection activeCell="A299" sqref="A299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="5.1640625" customWidth="1"/>
-    <col min="3" max="3" width="84.5" customWidth="1"/>
+    <col min="3" max="3" width="72.5" customWidth="1"/>
     <col min="4" max="4" width="83.33203125" customWidth="1"/>
     <col min="5" max="5" width="53.5" style="2" customWidth="1"/>
   </cols>
@@ -10021,6 +10045,39 @@
       </c>
       <c r="F297" t="s">
         <v>1617</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6">
+      <c r="A299" s="10" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6">
+      <c r="A300" t="s">
+        <v>0</v>
+      </c>
+      <c r="B300" t="s">
+        <v>1</v>
+      </c>
+      <c r="C300" t="s">
+        <v>2</v>
+      </c>
+      <c r="D300" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6">
+      <c r="A301" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B301">
+        <v>2</v>
+      </c>
+      <c r="C301" t="s">
+        <v>1620</v>
+      </c>
+      <c r="D301" t="s">
+        <v>1621</v>
       </c>
     </row>
   </sheetData>
@@ -11807,8 +11864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H321"/>
   <sheetViews>
-    <sheetView topLeftCell="D300" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F313" sqref="F313"/>
+    <sheetView tabSelected="1" topLeftCell="A301" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B321" sqref="B321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -16400,7 +16457,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="305" spans="1:6">
+    <row r="305" spans="1:7">
       <c r="A305" t="s">
         <v>1563</v>
       </c>
@@ -16420,7 +16477,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="306" spans="1:6">
+    <row r="306" spans="1:7">
       <c r="A306" t="s">
         <v>1565</v>
       </c>
@@ -16440,18 +16497,18 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="308" spans="1:6">
+    <row r="308" spans="1:7">
       <c r="A308" s="10" t="s">
         <v>1607</v>
       </c>
     </row>
-    <row r="310" spans="1:6">
+    <row r="310" spans="1:7">
       <c r="A310" s="10" t="s">
         <v>1608</v>
       </c>
       <c r="F310"/>
     </row>
-    <row r="311" spans="1:6">
+    <row r="311" spans="1:7">
       <c r="A311" t="s">
         <v>0</v>
       </c>
@@ -16469,7 +16526,7 @@
       </c>
       <c r="F311"/>
     </row>
-    <row r="312" spans="1:6">
+    <row r="312" spans="1:7">
       <c r="A312" t="s">
         <v>1609</v>
       </c>
@@ -16488,29 +16545,65 @@
       <c r="F312" t="s">
         <v>1616</v>
       </c>
-    </row>
-    <row r="313" spans="1:6">
+      <c r="G312" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7">
       <c r="F313"/>
     </row>
-    <row r="314" spans="1:6">
+    <row r="314" spans="1:7">
+      <c r="A314" s="10" t="s">
+        <v>1618</v>
+      </c>
       <c r="F314"/>
     </row>
-    <row r="315" spans="1:6">
+    <row r="315" spans="1:7">
+      <c r="A315" t="s">
+        <v>0</v>
+      </c>
+      <c r="B315" t="s">
+        <v>10</v>
+      </c>
+      <c r="C315" t="s">
+        <v>2</v>
+      </c>
+      <c r="D315" t="s">
+        <v>11</v>
+      </c>
+      <c r="E315" t="s">
+        <v>3</v>
+      </c>
       <c r="F315"/>
     </row>
-    <row r="316" spans="1:6">
+    <row r="316" spans="1:7">
+      <c r="A316" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B316">
+        <v>2</v>
+      </c>
+      <c r="C316" t="s">
+        <v>1623</v>
+      </c>
+      <c r="D316" t="s">
+        <v>1624</v>
+      </c>
+      <c r="E316" t="s">
+        <v>1625</v>
+      </c>
       <c r="F316"/>
     </row>
-    <row r="317" spans="1:6">
+    <row r="317" spans="1:7">
       <c r="F317"/>
     </row>
-    <row r="318" spans="1:6">
+    <row r="318" spans="1:7">
       <c r="F318"/>
     </row>
-    <row r="319" spans="1:6">
+    <row r="319" spans="1:7">
       <c r="F319"/>
     </row>
-    <row r="320" spans="1:6">
+    <row r="320" spans="1:7">
       <c r="F320"/>
     </row>
     <row r="321" spans="6:6">

</xml_diff>

<commit_message>
Ontology updates + icemr2 sea idMap
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/Documents/GitHub/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nupur/Documents/GitHub/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A0D74E-9EFD-DF48-BD56-3751DEF078AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4331151C-7D62-4D43-AC7D-751B17C44DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3189" uniqueCount="1664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3201" uniqueCount="1676">
   <si>
     <t>sid</t>
   </si>
@@ -5080,6 +5080,42 @@
   </si>
   <si>
     <t>Checked on February 9, 2023 and found no unit issues.</t>
+  </si>
+  <si>
+    <t>Jilinde costing should be "Time spent in occupation every week"</t>
+  </si>
+  <si>
+    <t>Icemr_amazonia_peru_cx should be "Car or truck"</t>
+  </si>
+  <si>
+    <t>Icemr_amazonia_peru_cx should be "Animals indoors"</t>
+  </si>
+  <si>
+    <t>General_promote should be "Full term deliveries count"</t>
+  </si>
+  <si>
+    <t>Icemr_amazonia_peru_cx should be "Visible feces in yard"?</t>
+  </si>
+  <si>
+    <t>Icemr_amazonia_peru_cx should be "Out of bed time"?</t>
+  </si>
+  <si>
+    <t>Icemr_llineup2 should be "Healthcare"</t>
+  </si>
+  <si>
+    <t>Which term is better?</t>
+  </si>
+  <si>
+    <t>Two different IRIs for Fatigue and 1 for Malaise. Malaise refers to an overall feeling of discomfort and lack of well-being. Fatigue is extreme tiredness and lack of energy or motivation for everyday activities.</t>
+  </si>
+  <si>
+    <t>Demographics is the right parent?</t>
+  </si>
+  <si>
+    <t>Move in Icemr_amazonia_peru_cx to under "Income"</t>
+  </si>
+  <si>
+    <t>Which is the right parent?</t>
   </si>
 </sst>
 </file>
@@ -5607,7 +5643,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5618,6 +5654,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5976,8 +6013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G314"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="C322" sqref="C322"/>
+    <sheetView topLeftCell="A290" workbookViewId="0">
+      <selection activeCell="C311" sqref="C311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5985,7 +6022,7 @@
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="5.1640625" customWidth="1"/>
     <col min="3" max="3" width="72.5" customWidth="1"/>
-    <col min="4" max="4" width="83.33203125" customWidth="1"/>
+    <col min="4" max="4" width="83.33203125" style="10" customWidth="1"/>
     <col min="5" max="5" width="53.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5999,7 +6036,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -6016,7 +6053,7 @@
       <c r="C2" t="s">
         <v>110</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="10" t="s">
         <v>111</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -6036,7 +6073,7 @@
       <c r="C3" t="s">
         <v>113</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="10" t="s">
         <v>114</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -6056,7 +6093,7 @@
       <c r="C4" t="s">
         <v>116</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -6076,7 +6113,7 @@
       <c r="C5" t="s">
         <v>119</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="10" t="s">
         <v>120</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -6096,7 +6133,7 @@
       <c r="C6" t="s">
         <v>122</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -6116,7 +6153,7 @@
       <c r="C7" t="s">
         <v>125</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="10" t="s">
         <v>126</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -6136,7 +6173,7 @@
       <c r="C8" t="s">
         <v>128</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="10" t="s">
         <v>129</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -6156,7 +6193,7 @@
       <c r="C9" t="s">
         <v>131</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="10" t="s">
         <v>132</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -6176,7 +6213,7 @@
       <c r="C10" t="s">
         <v>134</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="10" t="s">
         <v>132</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -6196,7 +6233,7 @@
       <c r="C11" t="s">
         <v>136</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="10" t="s">
         <v>137</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -6216,7 +6253,7 @@
       <c r="C12" t="s">
         <v>139</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="10" t="s">
         <v>132</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -6236,7 +6273,7 @@
       <c r="C13" t="s">
         <v>141</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="10" t="s">
         <v>142</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -6256,7 +6293,7 @@
       <c r="C14" t="s">
         <v>144</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -6273,7 +6310,7 @@
       <c r="C15" t="s">
         <v>147</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -6290,7 +6327,7 @@
       <c r="C16" t="s">
         <v>149</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -6307,7 +6344,7 @@
       <c r="C17" t="s">
         <v>152</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -6324,7 +6361,7 @@
       <c r="C18" t="s">
         <v>154</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -6341,7 +6378,7 @@
       <c r="C19" t="s">
         <v>156</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -6358,7 +6395,7 @@
       <c r="C20" t="s">
         <v>158</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -6375,7 +6412,7 @@
       <c r="C21" t="s">
         <v>160</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -6392,7 +6429,7 @@
       <c r="C22" t="s">
         <v>162</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -6409,7 +6446,7 @@
       <c r="C23" t="s">
         <v>164</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -6426,7 +6463,7 @@
       <c r="C24" t="s">
         <v>166</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -6443,7 +6480,7 @@
       <c r="C25" t="s">
         <v>168</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -6460,7 +6497,7 @@
       <c r="C26" t="s">
         <v>170</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -6477,7 +6514,7 @@
       <c r="C27" t="s">
         <v>172</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -6494,7 +6531,7 @@
       <c r="C28" t="s">
         <v>174</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -6511,7 +6548,7 @@
       <c r="C29" t="s">
         <v>176</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -6528,7 +6565,7 @@
       <c r="C30" t="s">
         <v>178</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -6545,7 +6582,7 @@
       <c r="C31" t="s">
         <v>180</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E31" s="2" t="s">
@@ -6562,7 +6599,7 @@
       <c r="C32" t="s">
         <v>182</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E32" s="2" t="s">
@@ -6579,7 +6616,7 @@
       <c r="C33" t="s">
         <v>184</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E33" s="2" t="s">
@@ -6596,7 +6633,7 @@
       <c r="C34" t="s">
         <v>186</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E34" s="2" t="s">
@@ -6613,7 +6650,7 @@
       <c r="C35" t="s">
         <v>188</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -6630,7 +6667,7 @@
       <c r="C36" t="s">
         <v>190</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E36" s="2" t="s">
@@ -6647,7 +6684,7 @@
       <c r="C37" t="s">
         <v>192</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E37" s="2" t="s">
@@ -6664,7 +6701,7 @@
       <c r="C38" t="s">
         <v>194</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E38" s="2" t="s">
@@ -6681,7 +6718,7 @@
       <c r="C39" t="s">
         <v>196</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -6698,7 +6735,7 @@
       <c r="C40" t="s">
         <v>198</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E40" s="2" t="s">
@@ -6715,7 +6752,7 @@
       <c r="C41" t="s">
         <v>200</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E41" s="2" t="s">
@@ -6732,7 +6769,7 @@
       <c r="C42" t="s">
         <v>202</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E42" s="2" t="s">
@@ -6749,7 +6786,7 @@
       <c r="C43" t="s">
         <v>204</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E43" s="2" t="s">
@@ -6766,7 +6803,7 @@
       <c r="C44" t="s">
         <v>206</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E44" s="2" t="s">
@@ -6783,7 +6820,7 @@
       <c r="C45" t="s">
         <v>208</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="10" t="s">
         <v>150</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -6800,7 +6837,7 @@
       <c r="C46" t="s">
         <v>210</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="10" t="s">
         <v>211</v>
       </c>
       <c r="E46" s="2" t="s">
@@ -6817,7 +6854,7 @@
       <c r="C47" t="s">
         <v>213</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="10" t="s">
         <v>214</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -6834,7 +6871,7 @@
       <c r="C48" t="s">
         <v>216</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="10" t="s">
         <v>217</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -6851,7 +6888,7 @@
       <c r="C49" t="s">
         <v>219</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="10" t="s">
         <v>220</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -6868,7 +6905,7 @@
       <c r="C50" t="s">
         <v>222</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E50" s="2" t="s">
@@ -6885,7 +6922,7 @@
       <c r="C51" t="s">
         <v>224</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E51" s="2" t="s">
@@ -6902,7 +6939,7 @@
       <c r="C52" t="s">
         <v>226</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="10" t="s">
         <v>227</v>
       </c>
       <c r="E52" s="2" t="s">
@@ -6919,7 +6956,7 @@
       <c r="C53" t="s">
         <v>229</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="10" t="s">
         <v>227</v>
       </c>
       <c r="E53" s="2" t="s">
@@ -6936,7 +6973,7 @@
       <c r="C54" t="s">
         <v>476</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="10" t="s">
         <v>478</v>
       </c>
       <c r="E54" s="2" t="s">
@@ -6953,7 +6990,7 @@
       <c r="C55" t="s">
         <v>479</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="10" t="s">
         <v>478</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -6970,7 +7007,7 @@
       <c r="C56" t="s">
         <v>231</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="10" t="s">
         <v>232</v>
       </c>
       <c r="E56" s="2" t="s">
@@ -6987,7 +7024,7 @@
       <c r="C57" t="s">
         <v>234</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="10" t="s">
         <v>235</v>
       </c>
       <c r="E57" s="2" t="s">
@@ -7004,7 +7041,7 @@
       <c r="C58" t="s">
         <v>237</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="10" t="s">
         <v>238</v>
       </c>
       <c r="E58" s="2" t="s">
@@ -7021,7 +7058,7 @@
       <c r="C59" t="s">
         <v>240</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="10" t="s">
         <v>238</v>
       </c>
       <c r="E59" s="2" t="s">
@@ -7038,7 +7075,7 @@
       <c r="C60" t="s">
         <v>242</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="10" t="s">
         <v>243</v>
       </c>
       <c r="E60" s="2" t="s">
@@ -7055,7 +7092,7 @@
       <c r="C61" t="s">
         <v>245</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="10" t="s">
         <v>246</v>
       </c>
       <c r="E61" s="2" t="s">
@@ -7072,7 +7109,7 @@
       <c r="C62" t="s">
         <v>248</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="10" t="s">
         <v>249</v>
       </c>
       <c r="E62" s="2" t="s">
@@ -7094,7 +7131,7 @@
       <c r="C67" t="s">
         <v>2</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E67"/>
@@ -7109,7 +7146,7 @@
       <c r="C68" t="s">
         <v>642</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="10" t="s">
         <v>541</v>
       </c>
       <c r="E68" s="2" t="s">
@@ -7126,7 +7163,7 @@
       <c r="C69" t="s">
         <v>644</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E69" s="2" t="s">
@@ -7143,7 +7180,7 @@
       <c r="C70" t="s">
         <v>646</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="10" t="s">
         <v>647</v>
       </c>
       <c r="E70" s="2" t="s">
@@ -7160,7 +7197,7 @@
       <c r="C71" t="s">
         <v>649</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="10" t="s">
         <v>647</v>
       </c>
       <c r="E71" s="2" t="s">
@@ -7177,7 +7214,7 @@
       <c r="C72" t="s">
         <v>650</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="10" t="s">
         <v>137</v>
       </c>
       <c r="E72" s="2" t="s">
@@ -7194,7 +7231,7 @@
       <c r="C73" t="s">
         <v>598</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E73" s="2" t="s">
@@ -7211,7 +7248,7 @@
       <c r="C74" t="s">
         <v>652</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="10" t="s">
         <v>653</v>
       </c>
       <c r="E74" s="2" t="s">
@@ -7228,7 +7265,7 @@
       <c r="C75" t="s">
         <v>216</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="10" t="s">
         <v>217</v>
       </c>
       <c r="E75" s="2" t="s">
@@ -7245,7 +7282,7 @@
       <c r="C76" t="s">
         <v>655</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="10" t="s">
         <v>656</v>
       </c>
       <c r="E76" s="2" t="s">
@@ -7262,7 +7299,7 @@
       <c r="C77" t="s">
         <v>658</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="10" t="s">
         <v>656</v>
       </c>
       <c r="E77" s="2" t="s">
@@ -7279,7 +7316,7 @@
       <c r="C78" t="s">
         <v>660</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="10" t="s">
         <v>661</v>
       </c>
       <c r="E78" s="2" t="s">
@@ -7296,7 +7333,7 @@
       <c r="C79" t="s">
         <v>663</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="10" t="s">
         <v>661</v>
       </c>
       <c r="E79" s="2" t="s">
@@ -7313,7 +7350,7 @@
       <c r="C80" t="s">
         <v>231</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="10" t="s">
         <v>232</v>
       </c>
     </row>
@@ -7327,7 +7364,7 @@
       <c r="C81" t="s">
         <v>665</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="10" t="s">
         <v>666</v>
       </c>
       <c r="E81" s="2" t="s">
@@ -7344,7 +7381,7 @@
       <c r="C82" t="s">
         <v>668</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -7358,7 +7395,7 @@
       <c r="C83" t="s">
         <v>600</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="10" t="s">
         <v>601</v>
       </c>
       <c r="E83" s="2" t="s">
@@ -7383,7 +7420,7 @@
       <c r="C88" t="s">
         <v>2</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E88" s="2" t="s">
@@ -7400,7 +7437,7 @@
       <c r="C89" t="s">
         <v>642</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="10" t="s">
         <v>541</v>
       </c>
       <c r="E89" s="2" t="s">
@@ -7417,7 +7454,7 @@
       <c r="C90" t="s">
         <v>793</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="10" t="s">
         <v>794</v>
       </c>
       <c r="E90" s="2" t="s">
@@ -7434,7 +7471,7 @@
       <c r="C91" t="s">
         <v>598</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E91" s="2" t="s">
@@ -7451,7 +7488,7 @@
       <c r="C92" t="s">
         <v>796</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="10" t="s">
         <v>797</v>
       </c>
       <c r="E92" s="2" t="s">
@@ -7468,7 +7505,7 @@
       <c r="C93" t="s">
         <v>799</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="10" t="s">
         <v>592</v>
       </c>
       <c r="E93" s="2" t="s">
@@ -7485,7 +7522,7 @@
       <c r="C94" t="s">
         <v>216</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="10" t="s">
         <v>217</v>
       </c>
       <c r="E94" s="2" t="s">
@@ -7502,7 +7539,7 @@
       <c r="C95" t="s">
         <v>801</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="10" t="s">
         <v>802</v>
       </c>
       <c r="E95" s="2" t="s">
@@ -7519,7 +7556,7 @@
       <c r="C96" t="s">
         <v>804</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="10" t="s">
         <v>802</v>
       </c>
       <c r="E96" s="2" t="s">
@@ -7536,7 +7573,7 @@
       <c r="C97" t="s">
         <v>660</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="10" t="s">
         <v>805</v>
       </c>
       <c r="E97" s="2" t="s">
@@ -7553,7 +7590,7 @@
       <c r="C98" t="s">
         <v>663</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="10" t="s">
         <v>805</v>
       </c>
       <c r="E98" s="2" t="s">
@@ -7570,7 +7607,7 @@
       <c r="C99" t="s">
         <v>806</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="10" t="s">
         <v>232</v>
       </c>
       <c r="E99" s="2" t="s">
@@ -7587,7 +7624,7 @@
       <c r="C100" t="s">
         <v>808</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="10" t="s">
         <v>809</v>
       </c>
       <c r="E100" s="2" t="s">
@@ -7604,7 +7641,7 @@
       <c r="C101" t="s">
         <v>810</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="10" t="s">
         <v>235</v>
       </c>
       <c r="E101" s="2" t="s">
@@ -7621,7 +7658,7 @@
       <c r="C102" t="s">
         <v>812</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="10" t="s">
         <v>813</v>
       </c>
       <c r="E102" s="2" t="s">
@@ -7638,7 +7675,7 @@
       <c r="C103" t="s">
         <v>665</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="10" t="s">
         <v>666</v>
       </c>
       <c r="E103" s="2" t="s">
@@ -7655,7 +7692,7 @@
       <c r="C104" t="s">
         <v>815</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="10" t="s">
         <v>581</v>
       </c>
       <c r="E104" s="2" t="s">
@@ -7689,7 +7726,7 @@
       <c r="C111" t="s">
         <v>2</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E111"/>
@@ -7704,7 +7741,7 @@
       <c r="C112" t="s">
         <v>866</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="10" t="s">
         <v>867</v>
       </c>
       <c r="E112" s="2" t="s">
@@ -7721,7 +7758,7 @@
       <c r="C113" t="s">
         <v>869</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="10" t="s">
         <v>132</v>
       </c>
       <c r="E113" s="2" t="s">
@@ -7738,7 +7775,7 @@
       <c r="C114" t="s">
         <v>869</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="10" t="s">
         <v>132</v>
       </c>
       <c r="E114" s="2" t="s">
@@ -7755,7 +7792,7 @@
       <c r="C115" t="s">
         <v>869</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D115" s="10" t="s">
         <v>132</v>
       </c>
       <c r="E115" s="2" t="s">
@@ -7772,7 +7809,7 @@
       <c r="C116" t="s">
         <v>873</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="10" t="s">
         <v>802</v>
       </c>
       <c r="E116" s="2" t="s">
@@ -7789,7 +7826,7 @@
       <c r="C117" t="s">
         <v>875</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117" s="10" t="s">
         <v>211</v>
       </c>
       <c r="E117" s="2" t="s">
@@ -7806,7 +7843,7 @@
       <c r="C118" t="s">
         <v>876</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D118" s="10" t="s">
         <v>877</v>
       </c>
       <c r="E118" s="2" t="s">
@@ -7833,7 +7870,7 @@
       <c r="C123" t="s">
         <v>2</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D123" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7847,7 +7884,7 @@
       <c r="C124" t="s">
         <v>893</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D124" s="10" t="s">
         <v>894</v>
       </c>
       <c r="E124" s="2" t="s">
@@ -7864,7 +7901,7 @@
       <c r="C125" t="s">
         <v>895</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D125" s="10" t="s">
         <v>877</v>
       </c>
       <c r="E125" s="2" t="s">
@@ -7881,7 +7918,7 @@
       <c r="C126" t="s">
         <v>897</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126" s="10" t="s">
         <v>898</v>
       </c>
       <c r="E126" s="2" t="s">
@@ -7898,7 +7935,7 @@
       <c r="C127" t="s">
         <v>900</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D127" s="10" t="s">
         <v>898</v>
       </c>
       <c r="E127" s="2" t="s">
@@ -7915,7 +7952,7 @@
       <c r="C128" t="s">
         <v>902</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="10" t="s">
         <v>903</v>
       </c>
       <c r="E128" s="2" t="s">
@@ -7932,7 +7969,7 @@
       <c r="C129" t="s">
         <v>905</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="10" t="s">
         <v>903</v>
       </c>
       <c r="E129" s="2" t="s">
@@ -7949,7 +7986,7 @@
       <c r="C130" t="s">
         <v>907</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D130" s="10" t="s">
         <v>908</v>
       </c>
       <c r="E130" s="2" t="s">
@@ -7976,7 +8013,7 @@
       <c r="C136" t="s">
         <v>2</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D136" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E136"/>
@@ -7991,7 +8028,7 @@
       <c r="C137" t="s">
         <v>902</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D137" s="10" t="s">
         <v>903</v>
       </c>
       <c r="E137" s="2" t="s">
@@ -8023,7 +8060,7 @@
       <c r="C143" t="s">
         <v>2</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D143" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E143" s="2" t="s">
@@ -8043,7 +8080,7 @@
       <c r="C144" t="s">
         <v>1024</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D144" s="10" t="s">
         <v>1025</v>
       </c>
       <c r="E144" s="2" t="s">
@@ -8063,7 +8100,7 @@
       <c r="C145" t="s">
         <v>1027</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D145" s="10" t="s">
         <v>1028</v>
       </c>
       <c r="E145" s="2" t="s">
@@ -8083,7 +8120,7 @@
       <c r="C146" t="s">
         <v>1030</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D146" s="10" t="s">
         <v>1031</v>
       </c>
       <c r="E146" s="2" t="s">
@@ -8103,7 +8140,7 @@
       <c r="C147" t="s">
         <v>1033</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D147" s="10" t="s">
         <v>1034</v>
       </c>
       <c r="E147" s="2" t="s">
@@ -8123,7 +8160,7 @@
       <c r="C148" t="s">
         <v>1036</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D148" s="10" t="s">
         <v>1034</v>
       </c>
       <c r="E148" s="2" t="s">
@@ -8143,7 +8180,7 @@
       <c r="C149" t="s">
         <v>1038</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D149" s="10" t="s">
         <v>1039</v>
       </c>
       <c r="E149" s="2" t="s">
@@ -8163,7 +8200,7 @@
       <c r="C150" t="s">
         <v>1041</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D150" s="10" t="s">
         <v>1042</v>
       </c>
       <c r="E150" s="2" t="s">
@@ -8183,7 +8220,7 @@
       <c r="C151" t="s">
         <v>1044</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D151" s="10" t="s">
         <v>1042</v>
       </c>
       <c r="E151" s="2" t="s">
@@ -8203,7 +8240,7 @@
       <c r="C152" t="s">
         <v>1046</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D152" s="10" t="s">
         <v>1047</v>
       </c>
       <c r="E152" s="2" t="s">
@@ -8223,7 +8260,7 @@
       <c r="C153" t="s">
         <v>1049</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D153" s="10" t="s">
         <v>1050</v>
       </c>
       <c r="E153" s="2" t="s">
@@ -8243,7 +8280,7 @@
       <c r="C154" t="s">
         <v>1052</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D154" s="10" t="s">
         <v>1050</v>
       </c>
       <c r="E154" s="2" t="s">
@@ -8273,7 +8310,7 @@
       <c r="C160" t="s">
         <v>2</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D160" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8287,7 +8324,7 @@
       <c r="C161" t="s">
         <v>1104</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D161" s="10" t="s">
         <v>1105</v>
       </c>
       <c r="E161" s="2" t="s">
@@ -8307,7 +8344,7 @@
       <c r="C162" t="s">
         <v>1106</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D162" s="10" t="s">
         <v>1031</v>
       </c>
       <c r="E162" s="2" t="s">
@@ -8327,7 +8364,7 @@
       <c r="C163" t="s">
         <v>600</v>
       </c>
-      <c r="D163" t="s">
+      <c r="D163" s="10" t="s">
         <v>601</v>
       </c>
       <c r="E163" s="2" t="s">
@@ -8350,7 +8387,7 @@
       <c r="C164" t="s">
         <v>1108</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D164" s="10" t="s">
         <v>898</v>
       </c>
       <c r="E164" s="2" t="s">
@@ -8370,7 +8407,7 @@
       <c r="C165" t="s">
         <v>1110</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="10" t="s">
         <v>898</v>
       </c>
       <c r="E165" s="2" t="s">
@@ -8390,7 +8427,7 @@
       <c r="C166" t="s">
         <v>1112</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="10" t="s">
         <v>898</v>
       </c>
       <c r="E166" s="2" t="s">
@@ -8410,7 +8447,7 @@
       <c r="C167" t="s">
         <v>1114</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="10" t="s">
         <v>898</v>
       </c>
       <c r="E167" s="2" t="s">
@@ -8430,7 +8467,7 @@
       <c r="C168" t="s">
         <v>1116</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="10" t="s">
         <v>898</v>
       </c>
       <c r="E168" s="2" t="s">
@@ -8450,7 +8487,7 @@
       <c r="C169" t="s">
         <v>1118</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="10" t="s">
         <v>898</v>
       </c>
       <c r="E169" s="2" t="s">
@@ -8470,7 +8507,7 @@
       <c r="C170" t="s">
         <v>1119</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="10" t="s">
         <v>898</v>
       </c>
       <c r="E170" s="2" t="s">
@@ -8490,7 +8527,7 @@
       <c r="C171" t="s">
         <v>1121</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="10" t="s">
         <v>898</v>
       </c>
       <c r="E171" s="2" t="s">
@@ -8510,7 +8547,7 @@
       <c r="C172" t="s">
         <v>1122</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="10" t="s">
         <v>898</v>
       </c>
       <c r="E172" s="2" t="s">
@@ -8530,7 +8567,7 @@
       <c r="C173" t="s">
         <v>1046</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="10" t="s">
         <v>1047</v>
       </c>
       <c r="E173" s="2" t="s">
@@ -8567,7 +8604,7 @@
       <c r="C178" t="s">
         <v>2</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8581,7 +8618,7 @@
       <c r="C179" t="s">
         <v>1275</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="10" t="s">
         <v>1253</v>
       </c>
       <c r="E179" s="2" t="s">
@@ -8601,7 +8638,7 @@
       <c r="C180" t="s">
         <v>1276</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="10" t="s">
         <v>1256</v>
       </c>
       <c r="E180" s="2" t="s">
@@ -8621,7 +8658,7 @@
       <c r="C181" t="s">
         <v>1277</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="10" t="s">
         <v>1260</v>
       </c>
       <c r="E181" s="2" t="s">
@@ -8638,7 +8675,7 @@
       <c r="C182" t="s">
         <v>1279</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="10" t="s">
         <v>1280</v>
       </c>
       <c r="E182" s="2" t="s">
@@ -8658,7 +8695,7 @@
       <c r="C183" t="s">
         <v>1282</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="10" t="s">
         <v>1280</v>
       </c>
       <c r="E183" s="2" t="s">
@@ -8678,7 +8715,7 @@
       <c r="C184" t="s">
         <v>1284</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="10" t="s">
         <v>1285</v>
       </c>
       <c r="E184" s="2" t="s">
@@ -8698,7 +8735,7 @@
       <c r="C185" t="s">
         <v>1287</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="10" t="s">
         <v>1246</v>
       </c>
       <c r="E185" s="2" t="s">
@@ -8718,7 +8755,7 @@
       <c r="C186" t="s">
         <v>1289</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="10" t="s">
         <v>1285</v>
       </c>
       <c r="E186" s="2" t="s">
@@ -8738,7 +8775,7 @@
       <c r="C187" t="s">
         <v>1291</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="10" t="s">
         <v>1292</v>
       </c>
       <c r="E187" s="2" t="s">
@@ -8758,7 +8795,7 @@
       <c r="C188" t="s">
         <v>1294</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="10" t="s">
         <v>1295</v>
       </c>
       <c r="E188" s="2" t="s">
@@ -8781,7 +8818,7 @@
       <c r="C189" t="s">
         <v>1297</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="10" t="s">
         <v>1292</v>
       </c>
       <c r="E189" s="2" t="s">
@@ -8809,7 +8846,7 @@
       <c r="C192" t="s">
         <v>2</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -8823,7 +8860,7 @@
       <c r="C193" t="s">
         <v>1277</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="10" t="s">
         <v>1260</v>
       </c>
       <c r="E193" s="2" t="s">
@@ -8840,7 +8877,7 @@
       <c r="C194" t="s">
         <v>1324</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="10" t="s">
         <v>1280</v>
       </c>
     </row>
@@ -8854,7 +8891,7 @@
       <c r="C195" t="s">
         <v>1284</v>
       </c>
-      <c r="D195" t="s">
+      <c r="D195" s="10" t="s">
         <v>1285</v>
       </c>
     </row>
@@ -8868,7 +8905,7 @@
       <c r="C196" t="s">
         <v>1287</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="10" t="s">
         <v>1246</v>
       </c>
     </row>
@@ -8882,7 +8919,7 @@
       <c r="C197" t="s">
         <v>1326</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="10" t="s">
         <v>1246</v>
       </c>
     </row>
@@ -8896,7 +8933,7 @@
       <c r="C198" t="s">
         <v>1328</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="10" t="s">
         <v>1246</v>
       </c>
     </row>
@@ -8910,7 +8947,7 @@
       <c r="C199" t="s">
         <v>1330</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="10" t="s">
         <v>1246</v>
       </c>
     </row>
@@ -8924,7 +8961,7 @@
       <c r="C200" t="s">
         <v>1332</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="10" t="s">
         <v>1292</v>
       </c>
     </row>
@@ -8938,7 +8975,7 @@
       <c r="C201" t="s">
         <v>1291</v>
       </c>
-      <c r="D201" t="s">
+      <c r="D201" s="10" t="s">
         <v>1292</v>
       </c>
     </row>
@@ -8952,7 +8989,7 @@
       <c r="C202" t="s">
         <v>1294</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="10" t="s">
         <v>1295</v>
       </c>
     </row>
@@ -8966,7 +9003,7 @@
       <c r="C203" t="s">
         <v>1297</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="10" t="s">
         <v>1292</v>
       </c>
     </row>
@@ -8980,7 +9017,7 @@
       <c r="C204" t="s">
         <v>1334</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="10" t="s">
         <v>1335</v>
       </c>
     </row>
@@ -8999,7 +9036,7 @@
       <c r="C207" t="s">
         <v>2</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E207" s="2" t="s">
@@ -9016,7 +9053,7 @@
       <c r="C208" t="s">
         <v>1347</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="10" t="s">
         <v>1246</v>
       </c>
       <c r="E208" s="2" t="s">
@@ -9033,7 +9070,7 @@
       <c r="C209" t="s">
         <v>1349</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="10" t="s">
         <v>1295</v>
       </c>
       <c r="E209" s="2" t="s">
@@ -9050,7 +9087,7 @@
       <c r="C210" t="s">
         <v>1351</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="10" t="s">
         <v>1295</v>
       </c>
       <c r="E210" s="2" t="s">
@@ -9067,7 +9104,7 @@
       <c r="C211" t="s">
         <v>1353</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="10" t="s">
         <v>1295</v>
       </c>
       <c r="E211" s="2" t="s">
@@ -9094,7 +9131,7 @@
       <c r="C216" t="s">
         <v>2</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E216"/>
@@ -9109,7 +9146,7 @@
       <c r="C217" t="s">
         <v>1275</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="10" t="s">
         <v>1253</v>
       </c>
       <c r="E217" s="2" t="s">
@@ -9129,7 +9166,7 @@
       <c r="C218" t="s">
         <v>1276</v>
       </c>
-      <c r="D218" t="s">
+      <c r="D218" s="10" t="s">
         <v>1256</v>
       </c>
       <c r="E218" s="2" t="s">
@@ -9159,7 +9196,7 @@
       <c r="C223" t="s">
         <v>2</v>
       </c>
-      <c r="D223" t="s">
+      <c r="D223" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9173,7 +9210,7 @@
       <c r="C224" t="s">
         <v>1372</v>
       </c>
-      <c r="D224" t="s">
+      <c r="D224" s="10" t="s">
         <v>1373</v>
       </c>
       <c r="E224" s="2" t="s">
@@ -9193,7 +9230,7 @@
       <c r="C225" t="s">
         <v>1375</v>
       </c>
-      <c r="D225" t="s">
+      <c r="D225" s="10" t="s">
         <v>1373</v>
       </c>
       <c r="E225" s="2" t="s">
@@ -9213,7 +9250,7 @@
       <c r="C226" t="s">
         <v>1377</v>
       </c>
-      <c r="D226" t="s">
+      <c r="D226" s="10" t="s">
         <v>1373</v>
       </c>
       <c r="E226" s="2" t="s">
@@ -9233,7 +9270,7 @@
       <c r="C227" t="s">
         <v>1379</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D227" s="10" t="s">
         <v>1373</v>
       </c>
       <c r="E227" s="2" t="s">
@@ -9253,7 +9290,7 @@
       <c r="C228" t="s">
         <v>1381</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D228" s="10" t="s">
         <v>1373</v>
       </c>
       <c r="E228" s="2" t="s">
@@ -9278,7 +9315,7 @@
       <c r="C231" t="s">
         <v>2</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D231" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9292,7 +9329,7 @@
       <c r="C232" t="s">
         <v>1391</v>
       </c>
-      <c r="D232" t="s">
+      <c r="D232" s="10" t="s">
         <v>1373</v>
       </c>
       <c r="E232" s="2" t="s">
@@ -9312,7 +9349,7 @@
       <c r="C233" t="s">
         <v>1392</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D233" s="10" t="s">
         <v>1373</v>
       </c>
       <c r="E233" s="2" t="s">
@@ -9332,7 +9369,7 @@
       <c r="C234" t="s">
         <v>1393</v>
       </c>
-      <c r="D234" t="s">
+      <c r="D234" s="10" t="s">
         <v>1373</v>
       </c>
       <c r="E234" s="2" t="s">
@@ -9352,7 +9389,7 @@
       <c r="C235" t="s">
         <v>1394</v>
       </c>
-      <c r="D235" t="s">
+      <c r="D235" s="10" t="s">
         <v>1373</v>
       </c>
       <c r="E235" s="2" t="s">
@@ -9372,7 +9409,7 @@
       <c r="C236" t="s">
         <v>1395</v>
       </c>
-      <c r="D236" t="s">
+      <c r="D236" s="10" t="s">
         <v>1373</v>
       </c>
       <c r="E236" s="2" t="s">
@@ -9392,7 +9429,7 @@
       <c r="C237" t="s">
         <v>1397</v>
       </c>
-      <c r="D237" t="s">
+      <c r="D237" s="10" t="s">
         <v>1256</v>
       </c>
     </row>
@@ -9411,7 +9448,7 @@
       <c r="C240" t="s">
         <v>2</v>
       </c>
-      <c r="D240" t="s">
+      <c r="D240" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9425,7 +9462,7 @@
       <c r="C241" t="s">
         <v>1410</v>
       </c>
-      <c r="D241" t="s">
+      <c r="D241" s="10" t="s">
         <v>1373</v>
       </c>
       <c r="E241" s="2" t="s">
@@ -9442,7 +9479,7 @@
       <c r="C242" t="s">
         <v>1397</v>
       </c>
-      <c r="D242" t="s">
+      <c r="D242" s="10" t="s">
         <v>1256</v>
       </c>
       <c r="E242" s="2" t="s">
@@ -9469,7 +9506,7 @@
       <c r="C247" t="s">
         <v>2</v>
       </c>
-      <c r="D247" t="s">
+      <c r="D247" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9483,7 +9520,7 @@
       <c r="C248" t="s">
         <v>1453</v>
       </c>
-      <c r="D248" t="s">
+      <c r="D248" s="10" t="s">
         <v>1454</v>
       </c>
       <c r="E248" s="2" t="s">
@@ -9503,7 +9540,7 @@
       <c r="C249" t="s">
         <v>1456</v>
       </c>
-      <c r="D249" t="s">
+      <c r="D249" s="10" t="s">
         <v>1457</v>
       </c>
       <c r="E249" s="2" t="s">
@@ -9523,7 +9560,7 @@
       <c r="C250" t="s">
         <v>1459</v>
       </c>
-      <c r="D250" t="s">
+      <c r="D250" s="10" t="s">
         <v>1460</v>
       </c>
       <c r="E250" s="2" t="s">
@@ -9543,7 +9580,7 @@
       <c r="C251" t="s">
         <v>1462</v>
       </c>
-      <c r="D251" t="s">
+      <c r="D251" s="10" t="s">
         <v>1463</v>
       </c>
       <c r="E251" s="2" t="s">
@@ -9563,7 +9600,7 @@
       <c r="C252" t="s">
         <v>1465</v>
       </c>
-      <c r="D252" t="s">
+      <c r="D252" s="10" t="s">
         <v>1466</v>
       </c>
       <c r="E252" s="2" t="s">
@@ -9593,7 +9630,7 @@
       <c r="C257" t="s">
         <v>2</v>
       </c>
-      <c r="D257" t="s">
+      <c r="D257" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9607,7 +9644,7 @@
       <c r="C258" t="s">
         <v>1486</v>
       </c>
-      <c r="D258" t="s">
+      <c r="D258" s="10" t="s">
         <v>1487</v>
       </c>
       <c r="E258" s="2" t="s">
@@ -9627,7 +9664,7 @@
       <c r="C259" t="s">
         <v>1488</v>
       </c>
-      <c r="D259" t="s">
+      <c r="D259" s="10" t="s">
         <v>1246</v>
       </c>
       <c r="E259" s="2" t="s">
@@ -9647,7 +9684,7 @@
       <c r="C260" t="s">
         <v>1489</v>
       </c>
-      <c r="D260" t="s">
+      <c r="D260" s="10" t="s">
         <v>1490</v>
       </c>
       <c r="E260" s="2" t="s">
@@ -9667,7 +9704,7 @@
       <c r="C261" t="s">
         <v>1491</v>
       </c>
-      <c r="D261" t="s">
+      <c r="D261" s="10" t="s">
         <v>1246</v>
       </c>
       <c r="E261" s="2" t="s">
@@ -9687,7 +9724,7 @@
       <c r="C262" t="s">
         <v>1492</v>
       </c>
-      <c r="D262" t="s">
+      <c r="D262" s="10" t="s">
         <v>1246</v>
       </c>
       <c r="E262" s="2" t="s">
@@ -9707,7 +9744,7 @@
       <c r="C263" t="s">
         <v>1493</v>
       </c>
-      <c r="D263" t="s">
+      <c r="D263" s="10" t="s">
         <v>1494</v>
       </c>
       <c r="E263" s="2" t="s">
@@ -9727,7 +9764,7 @@
       <c r="C264" t="s">
         <v>1496</v>
       </c>
-      <c r="D264" t="s">
+      <c r="D264" s="10" t="s">
         <v>1292</v>
       </c>
       <c r="E264" s="2" t="s">
@@ -9747,7 +9784,7 @@
       <c r="C265" t="s">
         <v>1498</v>
       </c>
-      <c r="D265" t="s">
+      <c r="D265" s="10" t="s">
         <v>1292</v>
       </c>
       <c r="E265" s="2" t="s">
@@ -9767,7 +9804,7 @@
       <c r="C266" t="s">
         <v>1509</v>
       </c>
-      <c r="D266" t="s">
+      <c r="D266" s="10" t="s">
         <v>1510</v>
       </c>
       <c r="E266" s="2" t="s">
@@ -9787,7 +9824,7 @@
       <c r="C267" t="s">
         <v>1500</v>
       </c>
-      <c r="D267" t="s">
+      <c r="D267" s="10" t="s">
         <v>1292</v>
       </c>
       <c r="E267" s="2" t="s">
@@ -9807,7 +9844,7 @@
       <c r="C268" t="s">
         <v>1502</v>
       </c>
-      <c r="D268" t="s">
+      <c r="D268" s="10" t="s">
         <v>1494</v>
       </c>
       <c r="E268" s="2" t="s">
@@ -9827,7 +9864,7 @@
       <c r="C269" t="s">
         <v>1503</v>
       </c>
-      <c r="D269" t="s">
+      <c r="D269" s="10" t="s">
         <v>1504</v>
       </c>
       <c r="E269" s="2" t="s">
@@ -9852,7 +9889,7 @@
       <c r="C272" t="s">
         <v>2</v>
       </c>
-      <c r="D272" t="s">
+      <c r="D272" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9866,7 +9903,7 @@
       <c r="C273" t="s">
         <v>1524</v>
       </c>
-      <c r="D273" t="s">
+      <c r="D273" s="10" t="s">
         <v>1292</v>
       </c>
     </row>
@@ -9880,7 +9917,7 @@
       <c r="C274" t="s">
         <v>1526</v>
       </c>
-      <c r="D274" t="s">
+      <c r="D274" s="10" t="s">
         <v>1292</v>
       </c>
     </row>
@@ -9894,7 +9931,7 @@
       <c r="C275" t="s">
         <v>1528</v>
       </c>
-      <c r="D275" t="s">
+      <c r="D275" s="10" t="s">
         <v>1292</v>
       </c>
     </row>
@@ -9918,7 +9955,7 @@
       <c r="C280" t="s">
         <v>2</v>
       </c>
-      <c r="D280" t="s">
+      <c r="D280" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9932,7 +9969,7 @@
       <c r="C281" t="s">
         <v>1539</v>
       </c>
-      <c r="D281" t="s">
+      <c r="D281" s="10" t="s">
         <v>1540</v>
       </c>
       <c r="E281" s="2" t="s">
@@ -9949,7 +9986,7 @@
       <c r="C282" t="s">
         <v>1542</v>
       </c>
-      <c r="D282" t="s">
+      <c r="D282" s="10" t="s">
         <v>1543</v>
       </c>
       <c r="E282" s="2" t="s">
@@ -9966,7 +10003,7 @@
       <c r="C283" t="s">
         <v>1545</v>
       </c>
-      <c r="D283" t="s">
+      <c r="D283" s="10" t="s">
         <v>1546</v>
       </c>
       <c r="E283" s="2" t="s">
@@ -9983,7 +10020,7 @@
       <c r="C284" t="s">
         <v>1548</v>
       </c>
-      <c r="D284" t="s">
+      <c r="D284" s="10" t="s">
         <v>1546</v>
       </c>
       <c r="E284" s="2" t="s">
@@ -10000,7 +10037,7 @@
       <c r="C285" t="s">
         <v>1550</v>
       </c>
-      <c r="D285" t="s">
+      <c r="D285" s="10" t="s">
         <v>1551</v>
       </c>
       <c r="E285" s="2" t="s">
@@ -10017,7 +10054,7 @@
       <c r="C286" t="s">
         <v>1553</v>
       </c>
-      <c r="D286" t="s">
+      <c r="D286" s="10" t="s">
         <v>1554</v>
       </c>
       <c r="E286" s="2" t="s">
@@ -10034,7 +10071,7 @@
       <c r="C287" t="s">
         <v>1556</v>
       </c>
-      <c r="D287" t="s">
+      <c r="D287" s="10" t="s">
         <v>1554</v>
       </c>
       <c r="E287" s="2" t="s">
@@ -10051,7 +10088,7 @@
       <c r="C288" t="s">
         <v>1558</v>
       </c>
-      <c r="D288" t="s">
+      <c r="D288" s="10" t="s">
         <v>1559</v>
       </c>
       <c r="E288" s="2" t="s">
@@ -10068,7 +10105,7 @@
       <c r="C289" t="s">
         <v>1561</v>
       </c>
-      <c r="D289" t="s">
+      <c r="D289" s="10" t="s">
         <v>1562</v>
       </c>
       <c r="E289" s="2" t="s">
@@ -10085,7 +10122,7 @@
       <c r="C290" t="s">
         <v>1564</v>
       </c>
-      <c r="D290" t="s">
+      <c r="D290" s="10" t="s">
         <v>1562</v>
       </c>
       <c r="E290" s="2" t="s">
@@ -10102,7 +10139,7 @@
       <c r="C291" t="s">
         <v>1566</v>
       </c>
-      <c r="D291" t="s">
+      <c r="D291" s="10" t="s">
         <v>1562</v>
       </c>
       <c r="E291" s="2" t="s">
@@ -10129,7 +10166,7 @@
       <c r="C296" t="s">
         <v>2</v>
       </c>
-      <c r="D296" t="s">
+      <c r="D296" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10143,7 +10180,7 @@
       <c r="C297" t="s">
         <v>1613</v>
       </c>
-      <c r="D297" t="s">
+      <c r="D297" s="10" t="s">
         <v>1612</v>
       </c>
       <c r="E297" s="2" t="s">
@@ -10168,7 +10205,7 @@
       <c r="C300" t="s">
         <v>2</v>
       </c>
-      <c r="D300" t="s">
+      <c r="D300" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10182,7 +10219,7 @@
       <c r="C301" t="s">
         <v>1620</v>
       </c>
-      <c r="D301" t="s">
+      <c r="D301" s="10" t="s">
         <v>1621</v>
       </c>
       <c r="E301" s="2" t="s">
@@ -10199,7 +10236,7 @@
         <v>1652</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>0</v>
       </c>
@@ -10209,11 +10246,11 @@
       <c r="C305" t="s">
         <v>2</v>
       </c>
-      <c r="D305" t="s">
+      <c r="D305" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>1630</v>
       </c>
@@ -10223,11 +10260,14 @@
       <c r="C306" t="s">
         <v>1631</v>
       </c>
-      <c r="D306" t="s">
+      <c r="D306" s="10" t="s">
         <v>1632</v>
       </c>
-    </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E306" s="2" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>1619</v>
       </c>
@@ -10237,11 +10277,14 @@
       <c r="C307" t="s">
         <v>1620</v>
       </c>
-      <c r="D307" t="s">
+      <c r="D307" s="10" t="s">
         <v>1621</v>
       </c>
-    </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E307" s="2" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>1633</v>
       </c>
@@ -10251,11 +10294,14 @@
       <c r="C308" t="s">
         <v>1634</v>
       </c>
-      <c r="D308" t="s">
+      <c r="D308" s="10" t="s">
         <v>1635</v>
       </c>
-    </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E308" s="2" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>307</v>
       </c>
@@ -10265,11 +10311,14 @@
       <c r="C309" t="s">
         <v>1636</v>
       </c>
-      <c r="D309" t="s">
+      <c r="D309" s="10" t="s">
         <v>1637</v>
       </c>
-    </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E309" s="2" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>1638</v>
       </c>
@@ -10279,11 +10328,14 @@
       <c r="C310" t="s">
         <v>1639</v>
       </c>
-      <c r="D310" t="s">
+      <c r="D310" s="10" t="s">
         <v>1640</v>
       </c>
-    </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E310" s="2" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>1641</v>
       </c>
@@ -10293,11 +10345,14 @@
       <c r="C311" t="s">
         <v>1642</v>
       </c>
-      <c r="D311" t="s">
+      <c r="D311" s="10" t="s">
         <v>1643</v>
       </c>
-    </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E311" s="2" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>1557</v>
       </c>
@@ -10307,11 +10362,14 @@
       <c r="C312" t="s">
         <v>1644</v>
       </c>
-      <c r="D312" t="s">
+      <c r="D312" s="10" t="s">
         <v>1645</v>
       </c>
-    </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E312" s="2" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>1646</v>
       </c>
@@ -10321,11 +10379,14 @@
       <c r="C313" t="s">
         <v>1647</v>
       </c>
-      <c r="D313" t="s">
+      <c r="D313" s="10" t="s">
         <v>1648</v>
       </c>
-    </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E313" s="2" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>1649</v>
       </c>
@@ -10335,8 +10396,11 @@
       <c r="C314" t="s">
         <v>1650</v>
       </c>
-      <c r="D314" t="s">
+      <c r="D314" s="10" t="s">
         <v>1651</v>
+      </c>
+      <c r="E314" s="2" t="s">
+        <v>1672</v>
       </c>
     </row>
   </sheetData>
@@ -12115,8 +12179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H322"/>
   <sheetViews>
-    <sheetView topLeftCell="A301" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C325" sqref="C325"/>
+    <sheetView tabSelected="1" topLeftCell="A303" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F318" sqref="F318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16893,7 +16957,9 @@
       <c r="E320" t="s">
         <v>1655</v>
       </c>
-      <c r="F320"/>
+      <c r="F320" s="2" t="s">
+        <v>1673</v>
+      </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
@@ -16911,7 +16977,9 @@
       <c r="E321" t="s">
         <v>1659</v>
       </c>
-      <c r="F321"/>
+      <c r="F321" s="2" t="s">
+        <v>1674</v>
+      </c>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
@@ -16928,6 +16996,9 @@
       </c>
       <c r="E322" t="s">
         <v>1662</v>
+      </c>
+      <c r="F322" s="2" t="s">
+        <v>1675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inconsistency fixes, redmine 45330
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nupur/Documents/GitHub/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/Documents/GitHub/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2155C7B-451A-B44E-B96D-9EA2543E151F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88B1CDC-2023-7E47-AA33-B9ED146215AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33240" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMulitpleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3201" uniqueCount="1676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3204" uniqueCount="1678">
   <si>
     <t>sid</t>
   </si>
@@ -5117,12 +5117,18 @@
   <si>
     <t>Change parent to "Treatment"</t>
   </si>
+  <si>
+    <t>Fixed on Feb 16, 2023.</t>
+  </si>
+  <si>
+    <t>Checked on Feb 9, 2023; no issue was found.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5299,6 +5305,13 @@
       <color rgb="FFB42419"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -5643,7 +5656,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5654,6 +5667,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6010,10 +6024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G314"/>
+  <dimension ref="A1:G316"/>
   <sheetViews>
-    <sheetView topLeftCell="A291" workbookViewId="0">
-      <selection activeCell="D317" sqref="D317"/>
+    <sheetView tabSelected="1" topLeftCell="A288" workbookViewId="0">
+      <selection activeCell="A316" sqref="A316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10262,7 +10276,7 @@
       <c r="D306" t="s">
         <v>1632</v>
       </c>
-      <c r="E306" s="2" t="s">
+      <c r="E306" s="10" t="s">
         <v>1665</v>
       </c>
     </row>
@@ -10279,7 +10293,7 @@
       <c r="D307" t="s">
         <v>1621</v>
       </c>
-      <c r="E307" s="2" t="s">
+      <c r="E307" s="10" t="s">
         <v>1666</v>
       </c>
     </row>
@@ -10296,7 +10310,7 @@
       <c r="D308" t="s">
         <v>1635</v>
       </c>
-      <c r="E308" s="2" t="s">
+      <c r="E308" s="10" t="s">
         <v>1664</v>
       </c>
     </row>
@@ -10313,7 +10327,7 @@
       <c r="D309" t="s">
         <v>1637</v>
       </c>
-      <c r="E309" s="2" t="s">
+      <c r="E309" s="10" t="s">
         <v>1667</v>
       </c>
     </row>
@@ -10330,7 +10344,7 @@
       <c r="D310" t="s">
         <v>1640</v>
       </c>
-      <c r="E310" s="2" t="s">
+      <c r="E310" s="10" t="s">
         <v>1668</v>
       </c>
     </row>
@@ -10347,7 +10361,7 @@
       <c r="D311" t="s">
         <v>1643</v>
       </c>
-      <c r="E311" s="2" t="s">
+      <c r="E311" s="10" t="s">
         <v>1669</v>
       </c>
     </row>
@@ -10364,7 +10378,7 @@
       <c r="D312" t="s">
         <v>1645</v>
       </c>
-      <c r="E312" s="2" t="s">
+      <c r="E312" s="10" t="s">
         <v>1670</v>
       </c>
     </row>
@@ -10381,7 +10395,7 @@
       <c r="D313" t="s">
         <v>1648</v>
       </c>
-      <c r="E313" s="2" t="s">
+      <c r="E313" s="10" t="s">
         <v>1671</v>
       </c>
     </row>
@@ -10398,8 +10412,13 @@
       <c r="D314" t="s">
         <v>1651</v>
       </c>
-      <c r="E314" s="2" t="s">
+      <c r="E314" s="10" t="s">
         <v>1672</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A316" s="1" t="s">
+        <v>1676</v>
       </c>
     </row>
   </sheetData>
@@ -10410,10 +10429,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G136"/>
+  <dimension ref="A1:G138"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12168,6 +12187,11 @@
         <v>1614</v>
       </c>
     </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>1677</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -12176,10 +12200,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H322"/>
+  <dimension ref="A1:H324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A297" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F331" sqref="F331"/>
+    <sheetView topLeftCell="A305" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A324" sqref="A324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16956,7 +16980,7 @@
       <c r="E320" t="s">
         <v>1655</v>
       </c>
-      <c r="F320" s="2" t="s">
+      <c r="F320" s="10" t="s">
         <v>1673</v>
       </c>
     </row>
@@ -16976,7 +17000,7 @@
       <c r="E321" t="s">
         <v>1659</v>
       </c>
-      <c r="F321" s="2" t="s">
+      <c r="F321" s="10" t="s">
         <v>1674</v>
       </c>
     </row>
@@ -16996,8 +17020,13 @@
       <c r="E322" t="s">
         <v>1662</v>
       </c>
-      <c r="F322" s="2" t="s">
+      <c r="F322" s="10" t="s">
         <v>1675</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A324" s="1" t="s">
+        <v>1676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Crypto update for consistency & missing units. QC update.
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nupur/Documents/GitHub/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/Documents/GitHub/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FCE405-D6F9-4248-B581-A2EDA77DCA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C17AD7C-DBDF-E546-89EB-50E1B39EC99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6108,7 +6108,7 @@
   <dimension ref="A1:G323"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A299" workbookViewId="0">
-      <selection activeCell="E327" sqref="E327"/>
+      <selection activeCell="E323" sqref="E323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10534,7 +10534,7 @@
       <c r="D320" t="s">
         <v>1613</v>
       </c>
-      <c r="E320" s="2" t="s">
+      <c r="E320" s="10" t="s">
         <v>1658</v>
       </c>
     </row>
@@ -10551,7 +10551,7 @@
       <c r="D321" t="s">
         <v>1546</v>
       </c>
-      <c r="E321" s="2" t="s">
+      <c r="E321" s="10" t="s">
         <v>1701</v>
       </c>
     </row>
@@ -10568,7 +10568,7 @@
       <c r="D322" t="s">
         <v>1675</v>
       </c>
-      <c r="E322" s="2" t="s">
+      <c r="E322" s="10" t="s">
         <v>1703</v>
       </c>
     </row>
@@ -10585,7 +10585,7 @@
       <c r="D323" t="s">
         <v>1675</v>
       </c>
-      <c r="E323" s="2" t="s">
+      <c r="E323" s="10" t="s">
         <v>1704</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Consistency fix JILINDE Costing Survey
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/Documents/GitHub/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C17AD7C-DBDF-E546-89EB-50E1B39EC99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF36CCC-E175-7F4A-8BE0-FCE78FB2BDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMultipleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3248" uniqueCount="1705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3250" uniqueCount="1706">
   <si>
     <t>sid</t>
   </si>
@@ -5203,6 +5203,9 @@
   </si>
   <si>
     <t>gates_crypto should have a new IRI assigned for "Period start date" under the parent "Observation details"</t>
+  </si>
+  <si>
+    <t>Fixed Feb 17, 2023.</t>
   </si>
 </sst>
 </file>
@@ -6105,10 +6108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G323"/>
+  <dimension ref="A1:G325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A299" workbookViewId="0">
-      <selection activeCell="E323" sqref="E323"/>
+    <sheetView topLeftCell="A296" workbookViewId="0">
+      <selection activeCell="A325" sqref="A325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10587,6 +10590,11 @@
       </c>
       <c r="E323" s="10" t="s">
         <v>1704</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A325" s="1" t="s">
+        <v>1705</v>
       </c>
     </row>
   </sheetData>
@@ -17219,10 +17227,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84351FC9-A5B2-F24D-8B55-E6051DA9E552}">
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88:D89"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18007,6 +18015,11 @@
       </c>
       <c r="E89" t="s">
         <v>1698</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>1705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed known issues and found some new ones
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
+++ b/Load/ontology/harmonization/clinEpi_eda_inconsistencyIssues.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nupur/Documents/GitHub/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C69555-83DD-7749-9229-D45CD21B3E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8FBEC9-258C-514A-855F-0A0D2DC5D460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4820" yWindow="500" windowWidth="24040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termsWithMultipleLabels" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3305" uniqueCount="1736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3351" uniqueCount="1741">
   <si>
     <t>sid</t>
   </si>
@@ -5296,6 +5296,21 @@
   </si>
   <si>
     <t>Please change gates_avenir to "Total rotavirus vaccine doses"</t>
+  </si>
+  <si>
+    <t>icemr_prism2 | icemr_prism | gates_vida_hucs_gambia_mali | gates_jilinde_demand_creation_evaluation_questionnaire | gates_gems1a | gates_jilinde_awareness_survey | gates_jilinde_pe_chv_cohort | gates_vida_hucs_kenya | gates_llineup_rct | gates_jilinde_costing_survey | gates_ganc | gates_vida | general_promote | gates_jilinde_healthcareprovider_cohort | icemr_amazonia_brazil | icemr_llineup2 | gates_gems_huas | gates_washb_kenya | icemr_malawi | icemr_prism2_border_cohort | gates_shine | icemr_amazonia_peru_cx | gates_gems</t>
+  </si>
+  <si>
+    <t>Checked on Mar 29th, 2023, found new issues:</t>
+  </si>
+  <si>
+    <t>Household administrative information|Administrative information</t>
+  </si>
+  <si>
+    <t>Cannot make change in 'gates_jilinde_retrospective_survey' since no 'Household' category. Do you want to add the category with only one term under it?</t>
+  </si>
+  <si>
+    <t>See comments above, 'Cannot make change in 'gates_jilinde_retrospective_survey' since no 'Household' category. Do you want to add the category with only one term under it?'</t>
   </si>
 </sst>
 </file>
@@ -6198,10 +6213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G334"/>
+  <dimension ref="A1:G341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="E342" sqref="E342"/>
+    <sheetView topLeftCell="A312" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="A336" sqref="A336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10631,7 +10646,7 @@
         <v>1658</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>1671</v>
       </c>
@@ -10648,7 +10663,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>1673</v>
       </c>
@@ -10665,7 +10680,7 @@
         <v>1703</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>1676</v>
       </c>
@@ -10682,17 +10697,17 @@
         <v>1704</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A325" s="1" t="s">
         <v>1705</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A327" s="1" t="s">
         <v>1706</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>0</v>
       </c>
@@ -10706,7 +10721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>578</v>
       </c>
@@ -10722,8 +10737,11 @@
       <c r="E329" s="2" t="s">
         <v>1731</v>
       </c>
-    </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F329" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>1401</v>
       </c>
@@ -10739,8 +10757,11 @@
       <c r="E330" s="2" t="s">
         <v>1732</v>
       </c>
-    </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F330" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>1710</v>
       </c>
@@ -10756,8 +10777,11 @@
       <c r="E331" s="2" t="s">
         <v>1733</v>
       </c>
-    </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F331" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>580</v>
       </c>
@@ -10773,8 +10797,11 @@
       <c r="E332" s="2" t="s">
         <v>1734</v>
       </c>
-    </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F332" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>582</v>
       </c>
@@ -10790,8 +10817,11 @@
       <c r="E333" s="2" t="s">
         <v>1735</v>
       </c>
-    </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F333" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>1547</v>
       </c>
@@ -10807,6 +10837,89 @@
       <c r="E334" s="2" t="s">
         <v>1730</v>
       </c>
+      <c r="F334" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A336" s="1" t="s">
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A337" t="s">
+        <v>0</v>
+      </c>
+      <c r="B337" t="s">
+        <v>1</v>
+      </c>
+      <c r="C337" t="s">
+        <v>2</v>
+      </c>
+      <c r="D337" t="s">
+        <v>3</v>
+      </c>
+      <c r="E337"/>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A338" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B338">
+        <v>2</v>
+      </c>
+      <c r="C338" t="s">
+        <v>1623</v>
+      </c>
+      <c r="D338" t="s">
+        <v>1736</v>
+      </c>
+      <c r="E338"/>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A339" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B339">
+        <v>2</v>
+      </c>
+      <c r="C339" t="s">
+        <v>1626</v>
+      </c>
+      <c r="D339" t="s">
+        <v>1627</v>
+      </c>
+      <c r="E339"/>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A340" t="s">
+        <v>301</v>
+      </c>
+      <c r="B340">
+        <v>2</v>
+      </c>
+      <c r="C340" t="s">
+        <v>1628</v>
+      </c>
+      <c r="D340" t="s">
+        <v>1629</v>
+      </c>
+      <c r="E340"/>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A341" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B341">
+        <v>2</v>
+      </c>
+      <c r="C341" t="s">
+        <v>1634</v>
+      </c>
+      <c r="D341" t="s">
+        <v>1635</v>
+      </c>
+      <c r="E341"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12592,10 +12705,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H332"/>
+  <dimension ref="A1:H338"/>
   <sheetViews>
-    <sheetView topLeftCell="A313" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E337" sqref="E337"/>
+    <sheetView tabSelected="1" topLeftCell="A316" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F337" sqref="F337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12604,7 +12717,7 @@
     <col min="2" max="2" width="8.5" customWidth="1"/>
     <col min="3" max="3" width="42" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
-    <col min="5" max="5" width="44.33203125" customWidth="1"/>
+    <col min="5" max="5" width="75.6640625" customWidth="1"/>
     <col min="6" max="6" width="40.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17376,7 +17489,7 @@
         <v>1665</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>1648</v>
       </c>
@@ -17396,7 +17509,7 @@
         <v>1666</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>1652</v>
       </c>
@@ -17416,22 +17529,22 @@
         <v>1667</v>
       </c>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A324" s="1" t="s">
         <v>1668</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A325" s="1" t="s">
         <v>1678</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A327" s="1" t="s">
         <v>1706</v>
       </c>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>0</v>
       </c>
@@ -17448,7 +17561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>1645</v>
       </c>
@@ -17467,8 +17580,11 @@
       <c r="F329" s="2" t="s">
         <v>1665</v>
       </c>
-    </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G329" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>1718</v>
       </c>
@@ -17487,8 +17603,11 @@
       <c r="F330" s="2" t="s">
         <v>1665</v>
       </c>
-    </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G330" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>1722</v>
       </c>
@@ -17507,8 +17626,11 @@
       <c r="F331" s="2" t="s">
         <v>1728</v>
       </c>
-    </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G331" t="s">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>1547</v>
       </c>
@@ -17527,6 +17649,88 @@
       <c r="F332" s="2" t="s">
         <v>1729</v>
       </c>
+      <c r="G332" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A334" s="1" t="s">
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A335" t="s">
+        <v>0</v>
+      </c>
+      <c r="B335" t="s">
+        <v>10</v>
+      </c>
+      <c r="C335" t="s">
+        <v>2</v>
+      </c>
+      <c r="D335" t="s">
+        <v>11</v>
+      </c>
+      <c r="E335" t="s">
+        <v>3</v>
+      </c>
+      <c r="F335"/>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A336" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B336">
+        <v>2</v>
+      </c>
+      <c r="C336" t="s">
+        <v>1723</v>
+      </c>
+      <c r="D336" t="s">
+        <v>1738</v>
+      </c>
+      <c r="E336" t="s">
+        <v>1725</v>
+      </c>
+      <c r="F336" t="s">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A337" t="s">
+        <v>1648</v>
+      </c>
+      <c r="B337">
+        <v>2</v>
+      </c>
+      <c r="C337" t="s">
+        <v>1649</v>
+      </c>
+      <c r="D337" t="s">
+        <v>1650</v>
+      </c>
+      <c r="E337" t="s">
+        <v>1651</v>
+      </c>
+      <c r="F337"/>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A338" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B338">
+        <v>2</v>
+      </c>
+      <c r="C338" t="s">
+        <v>1653</v>
+      </c>
+      <c r="D338" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E338" t="s">
+        <v>1654</v>
+      </c>
+      <c r="F338"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F30" xr:uid="{3F2C9002-1B0A-C348-905C-32E2D16BAD66}"/>

</xml_diff>